<commit_message>
convocazioni chiuse colosseo agosto
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stefa\Link-clan\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7D43993-37AF-40D7-B96F-081E6422CD74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C5A0E50-C6EF-4542-A5AA-083D73F9759E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{FECCDA54-7594-4EB7-ABFB-2C408C6461DD}"/>
   </bookViews>
@@ -827,13 +827,13 @@
     <t>Attivo</t>
   </si>
   <si>
-    <t>si</t>
-  </si>
-  <si>
     <t>ＡＲ♠️Ｍｉｃｈａｅｌ</t>
   </si>
   <si>
     <t>@Micro723</t>
+  </si>
+  <si>
+    <t>no</t>
   </si>
 </sst>
 </file>
@@ -1699,8 +1699,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EE2B0F9-AC31-464B-B046-53CB033C8615}">
   <dimension ref="A1:D142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A125" workbookViewId="0">
-      <selection activeCell="D142" sqref="D142"/>
+    <sheetView tabSelected="1" topLeftCell="A126" workbookViewId="0">
+      <selection activeCell="C130" sqref="C130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1741,7 +1741,7 @@
         <v>3</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -1755,7 +1755,7 @@
         <v>3</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -1769,7 +1769,7 @@
         <v>3</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -1783,7 +1783,7 @@
         <v>3</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -1797,7 +1797,7 @@
         <v>3</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -1811,7 +1811,7 @@
         <v>3</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -1825,7 +1825,7 @@
         <v>3</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -1839,7 +1839,7 @@
         <v>3</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -1853,7 +1853,7 @@
         <v>3</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -1867,7 +1867,7 @@
         <v>3</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -1881,7 +1881,7 @@
         <v>3</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -1895,7 +1895,7 @@
         <v>3</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -1909,7 +1909,7 @@
         <v>3</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
@@ -1923,7 +1923,7 @@
         <v>3</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
@@ -1937,7 +1937,7 @@
         <v>3</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
@@ -1951,7 +1951,7 @@
         <v>3</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
@@ -1965,7 +1965,7 @@
         <v>3</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
@@ -1979,7 +1979,7 @@
         <v>3</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
@@ -1993,7 +1993,7 @@
         <v>3</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
@@ -2007,7 +2007,7 @@
         <v>3</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
@@ -2021,7 +2021,7 @@
         <v>3</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
@@ -2035,7 +2035,7 @@
         <v>3</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
@@ -2049,7 +2049,7 @@
         <v>3</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
@@ -2063,7 +2063,7 @@
         <v>3</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
@@ -2077,7 +2077,7 @@
         <v>3</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
@@ -2091,7 +2091,7 @@
         <v>3</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
@@ -2105,7 +2105,7 @@
         <v>3</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
@@ -2119,7 +2119,7 @@
         <v>3</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
@@ -2133,7 +2133,7 @@
         <v>3</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
@@ -2147,7 +2147,7 @@
         <v>3</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
@@ -2161,7 +2161,7 @@
         <v>3</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
@@ -2175,7 +2175,7 @@
         <v>3</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
@@ -2189,7 +2189,7 @@
         <v>3</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
@@ -2203,7 +2203,7 @@
         <v>3</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
@@ -2217,7 +2217,7 @@
         <v>3</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
@@ -2231,7 +2231,7 @@
         <v>165</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
@@ -2245,7 +2245,7 @@
         <v>165</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
@@ -2259,7 +2259,7 @@
         <v>165</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
@@ -2273,7 +2273,7 @@
         <v>165</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
@@ -2287,7 +2287,7 @@
         <v>165</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
@@ -2301,7 +2301,7 @@
         <v>165</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
@@ -2312,7 +2312,7 @@
         <v>165</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
@@ -2326,7 +2326,7 @@
         <v>165</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
@@ -2340,7 +2340,7 @@
         <v>165</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
@@ -2354,7 +2354,7 @@
         <v>165</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
@@ -2365,7 +2365,7 @@
         <v>165</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
@@ -2376,7 +2376,7 @@
         <v>165</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
@@ -2390,7 +2390,7 @@
         <v>165</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
@@ -2404,7 +2404,7 @@
         <v>165</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
@@ -2418,7 +2418,7 @@
         <v>165</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
@@ -2432,7 +2432,7 @@
         <v>165</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
@@ -2446,7 +2446,7 @@
         <v>165</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
@@ -2460,7 +2460,7 @@
         <v>165</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
@@ -2474,7 +2474,7 @@
         <v>165</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
@@ -2485,7 +2485,7 @@
         <v>165</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
@@ -2499,7 +2499,7 @@
         <v>165</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
@@ -2510,7 +2510,7 @@
         <v>165</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
@@ -2524,7 +2524,7 @@
         <v>165</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
@@ -2535,7 +2535,7 @@
         <v>165</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
@@ -2549,7 +2549,7 @@
         <v>165</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
@@ -2563,7 +2563,7 @@
         <v>165</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
@@ -2577,7 +2577,7 @@
         <v>165</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
@@ -2588,7 +2588,7 @@
         <v>165</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
@@ -2602,7 +2602,7 @@
         <v>165</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
@@ -2616,7 +2616,7 @@
         <v>165</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
@@ -2630,7 +2630,7 @@
         <v>165</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
@@ -2644,7 +2644,7 @@
         <v>165</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
@@ -2658,7 +2658,7 @@
         <v>165</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
@@ -2672,7 +2672,7 @@
         <v>165</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
@@ -2686,7 +2686,7 @@
         <v>165</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
@@ -2697,7 +2697,7 @@
         <v>165</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
@@ -2711,7 +2711,7 @@
         <v>165</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
@@ -2725,7 +2725,7 @@
         <v>165</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
@@ -2739,7 +2739,7 @@
         <v>165</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
@@ -2753,7 +2753,7 @@
         <v>165</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
@@ -2767,7 +2767,7 @@
         <v>165</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
@@ -2781,7 +2781,7 @@
         <v>165</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
@@ -2795,7 +2795,7 @@
         <v>165</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
@@ -2809,7 +2809,7 @@
         <v>165</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.3">
@@ -2823,7 +2823,7 @@
         <v>165</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.3">
@@ -2837,7 +2837,7 @@
         <v>165</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.3">
@@ -2851,7 +2851,7 @@
         <v>165</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.3">
@@ -2865,7 +2865,7 @@
         <v>165</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.3">
@@ -2879,7 +2879,7 @@
         <v>165</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.3">
@@ -2893,7 +2893,7 @@
         <v>165</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.3">
@@ -2907,7 +2907,7 @@
         <v>165</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.3">
@@ -2921,7 +2921,7 @@
         <v>165</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.3">
@@ -2935,7 +2935,7 @@
         <v>264</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.3">
@@ -2949,7 +2949,7 @@
         <v>264</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.3">
@@ -2963,7 +2963,7 @@
         <v>264</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.3">
@@ -2977,7 +2977,7 @@
         <v>264</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.3">
@@ -2991,7 +2991,7 @@
         <v>264</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.3">
@@ -3005,7 +3005,7 @@
         <v>264</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.3">
@@ -3019,7 +3019,7 @@
         <v>264</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.3">
@@ -3033,7 +3033,7 @@
         <v>264</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.3">
@@ -3047,7 +3047,7 @@
         <v>264</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.3">
@@ -3061,7 +3061,7 @@
         <v>264</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.3">
@@ -3075,7 +3075,7 @@
         <v>264</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.3">
@@ -3089,7 +3089,7 @@
         <v>264</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.3">
@@ -3103,7 +3103,7 @@
         <v>264</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.3">
@@ -3117,7 +3117,7 @@
         <v>264</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.3">
@@ -3131,7 +3131,7 @@
         <v>264</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.3">
@@ -3145,7 +3145,7 @@
         <v>264</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.3">
@@ -3159,7 +3159,7 @@
         <v>264</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.3">
@@ -3173,7 +3173,7 @@
         <v>264</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.3">
@@ -3187,7 +3187,7 @@
         <v>264</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.3">
@@ -3201,7 +3201,7 @@
         <v>264</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.3">
@@ -3215,7 +3215,7 @@
         <v>264</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.3">
@@ -3229,7 +3229,7 @@
         <v>264</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.3">
@@ -3243,7 +3243,7 @@
         <v>264</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.3">
@@ -3254,7 +3254,7 @@
         <v>264</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.3">
@@ -3268,7 +3268,7 @@
         <v>264</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.3">
@@ -3282,7 +3282,7 @@
         <v>264</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.3">
@@ -3296,7 +3296,7 @@
         <v>264</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.3">
@@ -3310,7 +3310,7 @@
         <v>264</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.3">
@@ -3324,7 +3324,7 @@
         <v>264</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.3">
@@ -3338,7 +3338,7 @@
         <v>264</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.3">
@@ -3352,7 +3352,7 @@
         <v>264</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.3">
@@ -3366,7 +3366,7 @@
         <v>264</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.3">
@@ -3380,7 +3380,7 @@
         <v>264</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.3">
@@ -3394,7 +3394,7 @@
         <v>264</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.3">
@@ -3408,7 +3408,7 @@
         <v>264</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.3">
@@ -3422,7 +3422,7 @@
         <v>264</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.3">
@@ -3436,7 +3436,7 @@
         <v>264</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.3">
@@ -3450,7 +3450,7 @@
         <v>264</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.3">
@@ -3464,7 +3464,7 @@
         <v>264</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.3">
@@ -3478,7 +3478,7 @@
         <v>264</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.3">
@@ -3489,7 +3489,7 @@
         <v>264</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.3">
@@ -3500,7 +3500,7 @@
         <v>264</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.3">
@@ -3514,7 +3514,7 @@
         <v>264</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.3">
@@ -3528,7 +3528,7 @@
         <v>264</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.3">
@@ -3542,7 +3542,7 @@
         <v>264</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.3">
@@ -3556,7 +3556,7 @@
         <v>264</v>
       </c>
       <c r="D134" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.3">
@@ -3570,7 +3570,7 @@
         <v>264</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.3">
@@ -3584,7 +3584,7 @@
         <v>264</v>
       </c>
       <c r="D136" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.3">
@@ -3598,7 +3598,7 @@
         <v>264</v>
       </c>
       <c r="D137" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.3">
@@ -3612,7 +3612,7 @@
         <v>264</v>
       </c>
       <c r="D138" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.3">
@@ -3626,7 +3626,7 @@
         <v>264</v>
       </c>
       <c r="D139" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.3">
@@ -3640,7 +3640,7 @@
         <v>264</v>
       </c>
       <c r="D140" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.3">
@@ -3654,21 +3654,21 @@
         <v>264</v>
       </c>
       <c r="D141" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A142" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C142" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D142" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
convocazioni 3 settimana settembre
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stefa\Link-clan\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93C38519-29ED-4902-9F40-00A533C5E1AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FC3AA61-BC9C-4A92-85E1-4F0AE80AC0F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{FECCDA54-7594-4EB7-ABFB-2C408C6461DD}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{FECCDA54-7594-4EB7-ABFB-2C408C6461DD}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="639" uniqueCount="286">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="629" uniqueCount="382">
   <si>
     <t>TagTelegram</t>
   </si>
@@ -153,9 +153,6 @@
     <t>FORTEX</t>
   </si>
   <si>
-    <t>@FORTEX09</t>
-  </si>
-  <si>
     <t>MARCHIO</t>
   </si>
   <si>
@@ -687,9 +684,6 @@
     <t/>
   </si>
   <si>
-    <t>@sunnering41</t>
-  </si>
-  <si>
     <t>AR♦️Matteo</t>
   </si>
   <si>
@@ -892,6 +886,300 @@
   </si>
   <si>
     <t>@Haroldpain69</t>
+  </si>
+  <si>
+    <t>@sunnering</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ＡＲ♠️Ɛ Ɩ ɪ Ơ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ＡＲ♦️Ｂｌａｚｏｒ１１１ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  aleman(statale) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ＡＲ♠️＠ｌｅｍａｎ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Ａｒ❤️Ｓａｍｕｅｌｅ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  geeno </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ＡＲ ❤️ＡＬＥＸ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  AR♣️OMA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  crezyred </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Damo </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> robu </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Qliff </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> MARCHIO </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ＡＲ♠️Ｏｘｈａｔｒｅｓ</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ＡＲ♣️Ｒｉｃｃａｌｓｏ </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> bo </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> BrokerTony </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ＡＲ♥️Ｍａｚｚｉｔｏ </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> sid </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> DOCCC </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> mrdeath75 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ahmed </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Uchiha Madara </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> bughy </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> J.O.K.E.R.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Davide.Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> AR♠️alfone </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Daniele </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ＡＲ♦️Ｅ＄</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> dino </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> alabatia89 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> dani_lanc </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Peppone91 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> OhAnd4 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> YATO51 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Kekko03 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Sandiokan </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> $!B!N </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ＡＲ♠️Ｆｅｄｅ </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ＡＲ♠️ＢＡＣ </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ＡＲ♦️道路軍Wåyne </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> AR ♦️Goldenboy </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ＡＲ♣️Ｃｉｃｃｉｏ </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> AR♣️Severens</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Nico </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> cicciovolley91 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Begghich </t>
+  </si>
+  <si>
+    <t>@GoofyGooberr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  AR♦️Matteo </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Arsenio </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Lore_98 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  simo99 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  AR♦️Nico </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Angeloxf7 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  tala </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Don Michele </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  vinz </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> nevio lostirato </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> coraz </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bombazza </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> REMIDA </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Luca </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Luigi13 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> zumpy </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ＡＲ♣️Ｓｕｎｄｒｉｐｓ </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> TexWiller </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> LATIN WARRIOR™ </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ＡＲ❤️♣️ＧＯＤ９８♠️♦️ </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> pro </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> gigio </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> •fury™• </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Lubbro95 C.B  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Just_Dodo </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> christian98 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ⭐️Marco⭐️ </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> AnUbIs </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> random guy </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Enriic </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Big </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> orso86 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Zokum </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> AR♦️ᴍᴀᴛᴛᴇᴏ </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> riccardo </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> DonPunta </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Domenico </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Pinguino </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> OneLeggedJack </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> lil_wally </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SistemaS</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> sebabigo </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> \GuyFawkes/ </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ⚡️MAJOR⚡️ </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> frankye73 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ar♦️KingSupremo </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> kingmike </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> El Peko </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Wolfdale </t>
   </si>
 </sst>
 </file>
@@ -1758,7 +2046,7 @@
   <dimension ref="A1:D99"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C48" sqref="C2:C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1786,1323 +2074,1317 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B2" t="s">
-        <v>215</v>
+      <c r="B2" s="1" t="s">
+        <v>285</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B3" t="s">
-        <v>19</v>
+      <c r="B3" s="1" t="s">
+        <v>286</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B4" t="s">
-        <v>4</v>
+      <c r="B4" s="1" t="s">
+        <v>287</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B5" t="s">
-        <v>9</v>
+      <c r="B5" s="1" t="s">
+        <v>288</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>39</v>
-      </c>
-      <c r="B6" t="s">
-        <v>38</v>
+      <c r="A6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>289</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>23</v>
-      </c>
-      <c r="B7" t="s">
-        <v>210</v>
+      <c r="A7" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>290</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>115</v>
-      </c>
-      <c r="B8" t="s">
-        <v>211</v>
+      <c r="A8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>291</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>51</v>
+      <c r="A9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>292</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" t="s">
-        <v>13</v>
+      <c r="A10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>293</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>31</v>
-      </c>
-      <c r="B11" t="s">
-        <v>30</v>
+      <c r="A11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>294</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>33</v>
-      </c>
-      <c r="B12" t="s">
-        <v>32</v>
+      <c r="A12" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>295</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>49</v>
-      </c>
-      <c r="B13" t="s">
-        <v>48</v>
+      <c r="A13" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>296</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>47</v>
-      </c>
-      <c r="B14" t="s">
-        <v>46</v>
+      <c r="A14" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>297</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>41</v>
-      </c>
-      <c r="B15" t="s">
-        <v>40</v>
+      <c r="B15" s="1" t="s">
+        <v>298</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>216</v>
-      </c>
-      <c r="B16" t="s">
-        <v>153</v>
+      <c r="A16" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>299</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>16</v>
-      </c>
-      <c r="B17" t="s">
-        <v>15</v>
+      <c r="A17" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>300</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>25</v>
-      </c>
-      <c r="B18" t="s">
-        <v>24</v>
+      <c r="A18" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>301</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>27</v>
-      </c>
-      <c r="B19" t="s">
-        <v>26</v>
+      <c r="A19" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>302</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>18</v>
-      </c>
-      <c r="B20" t="s">
-        <v>17</v>
+      <c r="A20" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>303</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>146</v>
-      </c>
-      <c r="B21" t="s">
-        <v>145</v>
+      <c r="A21" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>304</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>140</v>
-      </c>
-      <c r="B22" t="s">
-        <v>139</v>
+      <c r="A22" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>305</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>43</v>
-      </c>
-      <c r="B23" t="s">
-        <v>42</v>
+      <c r="A23" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>306</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>7</v>
-      </c>
-      <c r="B24" t="s">
-        <v>6</v>
+      <c r="A24" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>307</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>50</v>
-      </c>
-      <c r="B25" t="s">
-        <v>52</v>
+      <c r="A25" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>308</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>29</v>
-      </c>
-      <c r="B26" t="s">
-        <v>28</v>
+      <c r="A26" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>309</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>117</v>
-      </c>
-      <c r="B27" t="s">
-        <v>116</v>
+      <c r="A27" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>310</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>37</v>
-      </c>
-      <c r="B28" t="s">
-        <v>36</v>
+      <c r="A28" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>311</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>100</v>
-      </c>
-      <c r="B29" t="s">
-        <v>99</v>
+      <c r="A29" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>312</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>35</v>
-      </c>
-      <c r="B30" t="s">
-        <v>34</v>
+      <c r="A30" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>313</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>91</v>
-      </c>
-      <c r="B31" t="s">
-        <v>90</v>
+      <c r="A31" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>314</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>217</v>
-      </c>
-      <c r="B32" t="s">
-        <v>212</v>
+      <c r="A32" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>315</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>144</v>
-      </c>
-      <c r="B33" t="s">
-        <v>143</v>
+      <c r="A33" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>316</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>123</v>
-      </c>
-      <c r="B34" t="s">
-        <v>122</v>
+      <c r="A34" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>317</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>45</v>
-      </c>
-      <c r="B35" t="s">
-        <v>44</v>
+      <c r="A35" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>318</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
-        <v>138</v>
-      </c>
-      <c r="B36" t="s">
-        <v>137</v>
+      <c r="A36" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>319</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
-        <v>97</v>
-      </c>
-      <c r="B37" t="s">
-        <v>96</v>
+      <c r="A37" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>320</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>121</v>
-      </c>
-      <c r="B38" t="s">
-        <v>120</v>
+      <c r="A38" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>321</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>165</v>
-      </c>
-      <c r="B39" t="s">
-        <v>158</v>
+      <c r="A39" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>322</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
-        <v>163</v>
-      </c>
-      <c r="B40" t="s">
-        <v>159</v>
+      <c r="A40" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>323</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>12</v>
-      </c>
-      <c r="B41" t="s">
-        <v>11</v>
+      <c r="A41" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>324</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
-        <v>164</v>
-      </c>
-      <c r="B42" t="s">
-        <v>160</v>
+      <c r="A42" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>325</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
-        <v>22</v>
-      </c>
-      <c r="B43" t="s">
-        <v>21</v>
+      <c r="A43" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>326</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
+      <c r="A44" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="B44" t="s">
-        <v>161</v>
+      <c r="B44" s="1" t="s">
+        <v>327</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
-        <v>167</v>
-      </c>
-      <c r="B45" t="s">
-        <v>162</v>
+      <c r="B45" s="1" t="s">
+        <v>328</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
-        <v>209</v>
-      </c>
-      <c r="B46" t="s">
-        <v>213</v>
+      <c r="A46" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>329</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
-        <v>67</v>
-      </c>
-      <c r="B47" t="s">
-        <v>66</v>
+      <c r="A47" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>330</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
-        <v>92</v>
-      </c>
-      <c r="B48" t="s">
-        <v>208</v>
+      <c r="A48" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>331</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>127</v>
-      </c>
-      <c r="B49" t="s">
-        <v>214</v>
+        <v>274</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>333</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>3</v>
+        <v>94</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>276</v>
+        <v>154</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>218</v>
+        <v>334</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>155</v>
+        <v>103</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>70</v>
+        <v>335</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>104</v>
+        <v>124</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>103</v>
+        <v>336</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>125</v>
+        <v>135</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>124</v>
+        <v>337</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>136</v>
+        <v>101</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>150</v>
+        <v>338</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>101</v>
+        <v>339</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>89</v>
+        <v>275</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>88</v>
+        <v>340</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>277</v>
+        <v>141</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>274</v>
+        <v>341</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>142</v>
+        <v>97</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>141</v>
+        <v>342</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>98</v>
+        <v>276</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>147</v>
+        <v>343</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>278</v>
+        <v>71</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>229</v>
+        <v>344</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>72</v>
+        <v>133</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>71</v>
+        <v>345</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>134</v>
+        <v>63</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>133</v>
+        <v>346</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>63</v>
+        <v>347</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>60</v>
+        <v>277</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>59</v>
+        <v>348</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>279</v>
+        <v>128</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>235</v>
+        <v>349</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>129</v>
+        <v>57</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>128</v>
+        <v>350</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>58</v>
+        <v>129</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>57</v>
+        <v>351</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>151</v>
+        <v>352</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>130</v>
+        <v>61</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>148</v>
+        <v>353</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>105</v>
+        <v>354</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>62</v>
+        <v>155</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>61</v>
+        <v>355</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>111</v>
+        <v>86</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>110</v>
+        <v>356</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>156</v>
+        <v>73</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>112</v>
+        <v>357</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>87</v>
+        <v>53</v>
       </c>
       <c r="B74" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="C74" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="C74" s="1" t="s">
-        <v>95</v>
-      </c>
       <c r="D74" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>74</v>
+        <v>106</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>73</v>
+        <v>359</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>54</v>
+        <v>108</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>53</v>
+        <v>360</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>107</v>
+        <v>64</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>247</v>
+        <v>361</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>109</v>
+        <v>131</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>108</v>
+        <v>362</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>93</v>
+        <v>363</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>132</v>
+        <v>85</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>131</v>
+        <v>364</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>56</v>
+        <v>81</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>55</v>
+        <v>365</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>85</v>
+        <v>366</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>81</v>
+        <v>367</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>83</v>
+        <v>368</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>69</v>
+        <v>113</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>68</v>
+        <v>369</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>78</v>
+        <v>118</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>77</v>
+        <v>370</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>114</v>
+        <v>75</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>113</v>
+        <v>371</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>119</v>
+        <v>278</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>118</v>
+        <v>372</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>76</v>
+        <v>215</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>75</v>
+        <v>373</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>261</v>
+        <v>374</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>209</v>
+        <v>332</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>152</v>
+        <v>375</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="92" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>281</v>
+        <v>134</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>262</v>
+        <v>376</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>157</v>
+        <v>79</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>154</v>
+        <v>377</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>135</v>
+        <v>280</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>265</v>
+        <v>378</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>80</v>
+        <v>281</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>79</v>
+        <v>379</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.3">
@@ -3110,13 +3392,13 @@
         <v>282</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>267</v>
+        <v>380</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.3">
@@ -3124,42 +3406,20 @@
         <v>283</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>269</v>
+        <v>381</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A98" t="s">
-        <v>284</v>
-      </c>
-      <c r="B98" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="C98" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="D98" s="1" t="s">
-        <v>168</v>
-      </c>
+      <c r="A98"/>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A99" t="s">
-        <v>285</v>
-      </c>
-      <c r="B99" s="1" t="s">
-        <v>272</v>
-      </c>
-      <c r="C99" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="D99" s="1" t="s">
-        <v>168</v>
-      </c>
+      <c r="A99"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3190,23 +3450,23 @@
         <v>1</v>
       </c>
       <c r="F4" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="H4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="I4" t="str">
-        <f>_xlfn.CONCAT(H4:H4)</f>
+        <f t="shared" ref="I4:I51" si="0">_xlfn.CONCAT(H4:H4)</f>
         <v>elioo_06</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="Q4" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="R4" s="1" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="S4" t="str">
         <f>_xlfn.CONCAT(Q4:R4)</f>
@@ -3222,23 +3482,23 @@
         <v>19</v>
       </c>
       <c r="H5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="I5" t="str">
-        <f>_xlfn.CONCAT(H5:H5)</f>
+        <f t="shared" si="0"/>
         <v>Blazor111</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="Q5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="R5" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="S5" t="str">
-        <f t="shared" ref="Q5:S53" si="0">_xlfn.CONCAT(Q5:R5)</f>
+        <f t="shared" ref="S5:S53" si="1">_xlfn.CONCAT(Q5:R5)</f>
         <v>@arsenlupin10arsenlupin10</v>
       </c>
     </row>
@@ -3251,23 +3511,23 @@
         <v>4</v>
       </c>
       <c r="H6" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="I6" t="str">
-        <f>_xlfn.CONCAT(H6:H6)</f>
+        <f t="shared" si="0"/>
         <v>aleman7273</v>
       </c>
       <c r="P6" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q6" t="s">
         <v>103</v>
       </c>
-      <c r="Q6" t="s">
-        <v>104</v>
-      </c>
       <c r="R6" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="S6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>@L0R3NZ098L0R3NZ098</v>
       </c>
     </row>
@@ -3280,23 +3540,23 @@
         <v>9</v>
       </c>
       <c r="H7" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="I7" t="str">
-        <f>_xlfn.CONCAT(H7:H7)</f>
+        <f t="shared" si="0"/>
         <v>aleman7273</v>
       </c>
       <c r="P7" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="Q7" t="s">
         <v>124</v>
       </c>
-      <c r="Q7" t="s">
-        <v>125</v>
-      </c>
       <c r="R7" s="1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="S7" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>@ilConte1999ilConte1999</v>
       </c>
     </row>
@@ -3309,23 +3569,23 @@
         <v>38</v>
       </c>
       <c r="H8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="I8" t="str">
-        <f>_xlfn.CONCAT(H8:H8)</f>
+        <f t="shared" si="0"/>
         <v>FORTEX09</v>
       </c>
       <c r="P8" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="Q8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="R8" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="S8" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>@Nicopasse00Nicopasse00</v>
       </c>
     </row>
@@ -3335,26 +3595,26 @@
       </c>
       <c r="E9" s="1"/>
       <c r="F9" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="H9" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="I9" t="str">
-        <f>_xlfn.CONCAT(H9:H9)</f>
+        <f t="shared" si="0"/>
         <v>BuldzS</v>
       </c>
       <c r="P9" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="Q9" t="s">
         <v>101</v>
       </c>
-      <c r="Q9" t="s">
-        <v>102</v>
-      </c>
       <c r="R9" s="1" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="S9" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>@angang37angang37</v>
       </c>
     </row>
@@ -3364,26 +3624,26 @@
       </c>
       <c r="E10" s="1"/>
       <c r="F10" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="H10" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="I10" t="str">
-        <f>_xlfn.CONCAT(H10:H10)</f>
+        <f t="shared" si="0"/>
         <v>Alestrega22</v>
       </c>
       <c r="P10" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q10" t="s">
         <v>88</v>
       </c>
-      <c r="Q10" t="s">
-        <v>89</v>
-      </c>
       <c r="R10" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="S10" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>@Tala91111Tala91111</v>
       </c>
     </row>
@@ -3393,26 +3653,26 @@
       </c>
       <c r="E11" s="1"/>
       <c r="F11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H11" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="I11" t="str">
-        <f>_xlfn.CONCAT(H11:H11)</f>
+        <f t="shared" si="0"/>
         <v>Ale_Mare93</v>
       </c>
       <c r="P11" s="1" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="Q11" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="R11" s="1" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="S11" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>@Don_Michele_RoyaleDon_Michele_Royale</v>
       </c>
     </row>
@@ -3425,23 +3685,23 @@
         <v>13</v>
       </c>
       <c r="H12" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="I12" t="str">
-        <f>_xlfn.CONCAT(H12:H12)</f>
+        <f t="shared" si="0"/>
         <v>Romas10</v>
       </c>
       <c r="P12" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="Q12" t="s">
         <v>141</v>
       </c>
-      <c r="Q12" t="s">
-        <v>142</v>
-      </c>
       <c r="R12" s="1" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="S12" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>@vinz9898vinz9898</v>
       </c>
     </row>
@@ -3457,20 +3717,20 @@
         <v>30</v>
       </c>
       <c r="I13" t="str">
-        <f>_xlfn.CONCAT(H13:H13)</f>
+        <f t="shared" si="0"/>
         <v>crezyred</v>
       </c>
       <c r="P13" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="Q13" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="R13" s="1" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="S13" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>@kvaradona997kvaradona997</v>
       </c>
     </row>
@@ -3483,23 +3743,23 @@
         <v>32</v>
       </c>
       <c r="H14" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I14" t="str">
-        <f>_xlfn.CONCAT(H14:H14)</f>
+        <f t="shared" si="0"/>
         <v>DaMoops</v>
       </c>
       <c r="P14" s="1" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="Q14" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="R14" s="1" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="S14" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>@coraaaazcoraaaaz</v>
       </c>
     </row>
@@ -3509,26 +3769,26 @@
       </c>
       <c r="E15" s="1"/>
       <c r="F15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H15" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I15" t="str">
-        <f>_xlfn.CONCAT(H15:H15)</f>
+        <f t="shared" si="0"/>
         <v>Robu99</v>
       </c>
       <c r="P15" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q15" t="s">
         <v>71</v>
       </c>
-      <c r="Q15" t="s">
-        <v>72</v>
-      </c>
       <c r="R15" s="1" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="S15" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>@nicola3194nicola3194</v>
       </c>
     </row>
@@ -3538,26 +3798,26 @@
       </c>
       <c r="E16" s="1"/>
       <c r="F16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H16" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I16" t="str">
-        <f>_xlfn.CONCAT(H16:H16)</f>
+        <f t="shared" si="0"/>
         <v>Punk_ake</v>
       </c>
       <c r="P16" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="Q16" t="s">
         <v>133</v>
       </c>
-      <c r="Q16" t="s">
-        <v>134</v>
-      </c>
       <c r="R16" s="1" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="S16" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>@RemidaRemida</v>
       </c>
     </row>
@@ -3567,26 +3827,26 @@
       </c>
       <c r="E17" s="1"/>
       <c r="F17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H17" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I17" t="str">
-        <f>_xlfn.CONCAT(H17:H17)</f>
+        <f t="shared" si="0"/>
         <v>Marchio04</v>
       </c>
       <c r="P17" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q17" t="s">
         <v>63</v>
       </c>
-      <c r="Q17" t="s">
-        <v>64</v>
-      </c>
       <c r="R17" s="1" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="S17" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>@Lucaa123Lucaa123</v>
       </c>
     </row>
@@ -3596,23 +3856,23 @@
       </c>
       <c r="E18" s="1"/>
       <c r="F18" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="I18" t="str">
-        <f>_xlfn.CONCAT(H18:H18)</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="P18" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q18" t="s">
         <v>59</v>
       </c>
-      <c r="Q18" t="s">
-        <v>60</v>
-      </c>
       <c r="R18" s="1" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="S18" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>@luigi134luigi134</v>
       </c>
     </row>
@@ -3625,23 +3885,23 @@
         <v>15</v>
       </c>
       <c r="H19" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I19" t="str">
-        <f>_xlfn.CONCAT(H19:H19)</f>
+        <f t="shared" si="0"/>
         <v>riccalso</v>
       </c>
       <c r="P19" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="Q19" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="R19" s="1" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="S19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>@FabioZumpy77FabioZumpy77</v>
       </c>
     </row>
@@ -3654,23 +3914,23 @@
         <v>24</v>
       </c>
       <c r="H20" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="I20" t="str">
-        <f>_xlfn.CONCAT(H20:H20)</f>
+        <f t="shared" si="0"/>
         <v>BO_CRL</v>
       </c>
       <c r="P20" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q20" t="s">
         <v>128</v>
       </c>
-      <c r="Q20" t="s">
-        <v>129</v>
-      </c>
       <c r="R20" s="1" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="S20" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>@SUNDRIPSYTSUNDRIPSYT</v>
       </c>
     </row>
@@ -3686,20 +3946,20 @@
         <v>26</v>
       </c>
       <c r="I21" t="str">
-        <f>_xlfn.CONCAT(H21:H21)</f>
+        <f t="shared" si="0"/>
         <v>BrokerTony</v>
       </c>
       <c r="P21" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q21" t="s">
         <v>57</v>
       </c>
-      <c r="Q21" t="s">
-        <v>58</v>
-      </c>
       <c r="R21" s="1" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="S21" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>@dm996mazzdm996mazz</v>
       </c>
     </row>
@@ -3712,23 +3972,23 @@
         <v>17</v>
       </c>
       <c r="H22" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="I22" t="str">
-        <f>_xlfn.CONCAT(H22:H22)</f>
+        <f t="shared" si="0"/>
         <v>Mazzito</v>
       </c>
       <c r="P22" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="Q22" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="R22" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="S22" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>@ralfone01ralfone01</v>
       </c>
     </row>
@@ -3738,26 +3998,26 @@
       </c>
       <c r="E23" s="1"/>
       <c r="F23" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H23" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I23" t="str">
-        <f>_xlfn.CONCAT(H23:H23)</f>
+        <f t="shared" si="0"/>
         <v>NicoSkev98</v>
       </c>
       <c r="P23" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="Q23" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="R23" s="1" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="S23" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>@LatinoCcHLatinoCcH</v>
       </c>
     </row>
@@ -3767,26 +4027,26 @@
       </c>
       <c r="E24" s="1"/>
       <c r="F24" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H24" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="I24" t="str">
-        <f>_xlfn.CONCAT(H24:H24)</f>
+        <f t="shared" si="0"/>
         <v>pietro_actis</v>
       </c>
       <c r="P24" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="Q24" t="s">
         <v>105</v>
       </c>
-      <c r="Q24" t="s">
-        <v>106</v>
-      </c>
       <c r="R24" s="1" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="S24" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>@ARGOD98ARGOD98</v>
       </c>
     </row>
@@ -3796,26 +4056,26 @@
       </c>
       <c r="E25" s="1"/>
       <c r="F25" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H25" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I25" t="str">
-        <f>_xlfn.CONCAT(H25:H25)</f>
+        <f t="shared" si="0"/>
         <v>mrdeath75</v>
       </c>
       <c r="P25" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q25" t="s">
         <v>61</v>
       </c>
-      <c r="Q25" t="s">
-        <v>62</v>
-      </c>
       <c r="R25" s="1" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="S25" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>@moretti000moretti000</v>
       </c>
     </row>
@@ -3828,23 +4088,23 @@
         <v>6</v>
       </c>
       <c r="H26" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="I26" t="str">
-        <f>_xlfn.CONCAT(H26:H26)</f>
+        <f t="shared" si="0"/>
         <v>Ahmed_Eliow</v>
       </c>
       <c r="P26" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q26" t="s">
         <v>110</v>
       </c>
-      <c r="Q26" t="s">
-        <v>111</v>
-      </c>
       <c r="R26" s="1" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="S26" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>@LuigiVallomeLuigiVallome</v>
       </c>
     </row>
@@ -3854,26 +4114,26 @@
       </c>
       <c r="E27" s="1"/>
       <c r="F27" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H27" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="I27" t="str">
-        <f>_xlfn.CONCAT(H27:H27)</f>
+        <f t="shared" si="0"/>
         <v>Madara_2912</v>
       </c>
       <c r="P27" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="Q27" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="R27" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="S27" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>@emanuelnaemanuelna</v>
       </c>
     </row>
@@ -3886,23 +4146,23 @@
         <v>28</v>
       </c>
       <c r="H28" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="I28" t="str">
-        <f>_xlfn.CONCAT(H28:H28)</f>
+        <f t="shared" si="0"/>
         <v>ArBughy</v>
       </c>
       <c r="P28" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="Q28" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="R28" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="S28" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>@Lucaser95Lucaser95</v>
       </c>
     </row>
@@ -3912,26 +4172,26 @@
       </c>
       <c r="E29" s="1"/>
       <c r="F29" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H29" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="I29" t="str">
-        <f>_xlfn.CONCAT(H29:H29)</f>
+        <f t="shared" si="0"/>
         <v>Tanjim041</v>
       </c>
       <c r="P29" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q29" t="s">
         <v>73</v>
       </c>
-      <c r="Q29" t="s">
-        <v>74</v>
-      </c>
       <c r="R29" s="1" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="S29" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>@edoogrigoedoogrigo</v>
       </c>
     </row>
@@ -3944,23 +4204,23 @@
         <v>36</v>
       </c>
       <c r="H30" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="I30" t="str">
-        <f>_xlfn.CONCAT(H30:H30)</f>
+        <f t="shared" si="0"/>
         <v>Sz66603</v>
       </c>
       <c r="P30" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q30" t="s">
         <v>53</v>
       </c>
-      <c r="Q30" t="s">
-        <v>54</v>
-      </c>
       <c r="R30" s="1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="S30" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>@chri98757chri98757</v>
       </c>
     </row>
@@ -3970,26 +4230,26 @@
       </c>
       <c r="E31" s="1"/>
       <c r="F31" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H31" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="I31" t="str">
-        <f>_xlfn.CONCAT(H31:H31)</f>
+        <f t="shared" si="0"/>
         <v>ralfone01</v>
       </c>
       <c r="P31" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="Q31" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="R31" s="1" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="S31" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>@MarcoP_PMMarcoP_PM</v>
       </c>
     </row>
@@ -4002,23 +4262,23 @@
         <v>34</v>
       </c>
       <c r="H32" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I32" t="str">
-        <f>_xlfn.CONCAT(H32:H32)</f>
+        <f t="shared" si="0"/>
         <v>yvngdanyy</v>
       </c>
       <c r="P32" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q32" t="s">
         <v>108</v>
       </c>
-      <c r="Q32" t="s">
-        <v>109</v>
-      </c>
       <c r="R32" s="1" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="S32" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>@RusuA24RusuA24</v>
       </c>
     </row>
@@ -4028,26 +4288,26 @@
       </c>
       <c r="E33" s="1"/>
       <c r="F33" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H33" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I33" t="str">
-        <f>_xlfn.CONCAT(H33:H33)</f>
+        <f t="shared" si="0"/>
         <v>rkomi99</v>
       </c>
       <c r="P33" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="Q33" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="R33" s="1" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="S33" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>@Davide438Davide438</v>
       </c>
     </row>
@@ -4057,26 +4317,26 @@
       </c>
       <c r="E34" s="1"/>
       <c r="F34" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="H34" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="I34" t="str">
-        <f>_xlfn.CONCAT(H34:H34)</f>
+        <f t="shared" si="0"/>
         <v>sunnering41</v>
       </c>
       <c r="P34" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="Q34" t="s">
         <v>131</v>
       </c>
-      <c r="Q34" t="s">
-        <v>132</v>
-      </c>
       <c r="R34" s="1" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="S34" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>@iherriiherri</v>
       </c>
     </row>
@@ -4086,26 +4346,26 @@
       </c>
       <c r="E35" s="1"/>
       <c r="F35" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H35" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="I35" t="str">
-        <f>_xlfn.CONCAT(H35:H35)</f>
+        <f t="shared" si="0"/>
         <v>alabatia89</v>
       </c>
       <c r="P35" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q35" t="s">
         <v>55</v>
       </c>
-      <c r="Q35" t="s">
-        <v>56</v>
-      </c>
       <c r="R35" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="S35" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>@WTHBIGWTHBIG</v>
       </c>
     </row>
@@ -4115,26 +4375,26 @@
       </c>
       <c r="E36" s="1"/>
       <c r="F36" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H36" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="I36" t="str">
-        <f>_xlfn.CONCAT(H36:H36)</f>
+        <f t="shared" si="0"/>
         <v>asso_nr</v>
       </c>
       <c r="P36" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q36" t="s">
         <v>85</v>
       </c>
-      <c r="Q36" t="s">
-        <v>86</v>
-      </c>
       <c r="R36" s="1" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="S36" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>@orso_86orso_86</v>
       </c>
     </row>
@@ -4144,26 +4404,26 @@
       </c>
       <c r="E37" s="1"/>
       <c r="F37" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H37" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I37" t="str">
-        <f>_xlfn.CONCAT(H37:H37)</f>
+        <f t="shared" si="0"/>
         <v>PepponeB91</v>
       </c>
       <c r="P37" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q37" t="s">
         <v>81</v>
       </c>
-      <c r="Q37" t="s">
-        <v>82</v>
-      </c>
       <c r="R37" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="S37" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>@GiovicorGiovicor</v>
       </c>
     </row>
@@ -4173,26 +4433,26 @@
       </c>
       <c r="E38" s="1"/>
       <c r="F38" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H38" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="I38" t="str">
-        <f>_xlfn.CONCAT(H38:H38)</f>
+        <f t="shared" si="0"/>
         <v>OhAnd4</v>
       </c>
       <c r="P38" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q38" t="s">
         <v>83</v>
       </c>
-      <c r="Q38" t="s">
-        <v>84</v>
-      </c>
       <c r="R38" s="1" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="S38" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>@xmatte0xxmatte0x</v>
       </c>
     </row>
@@ -4202,26 +4462,26 @@
       </c>
       <c r="E39" s="1"/>
       <c r="F39" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H39" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="I39" t="str">
-        <f>_xlfn.CONCAT(H39:H39)</f>
+        <f t="shared" si="0"/>
         <v>Lilyan51</v>
       </c>
       <c r="P39" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q39" t="s">
         <v>68</v>
       </c>
-      <c r="Q39" t="s">
-        <v>69</v>
-      </c>
       <c r="R39" s="1" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="S39" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>@torodeitori14torodeitori14</v>
       </c>
     </row>
@@ -4230,26 +4490,26 @@
         <v>38</v>
       </c>
       <c r="F40" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H40" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="I40" t="str">
-        <f>_xlfn.CONCAT(H40:H40)</f>
+        <f t="shared" si="0"/>
         <v>K3kk07</v>
       </c>
       <c r="P40" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q40" t="s">
         <v>77</v>
       </c>
-      <c r="Q40" t="s">
-        <v>78</v>
-      </c>
       <c r="R40" s="1" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="S40" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>@Wazito888Wazito888</v>
       </c>
     </row>
@@ -4258,26 +4518,26 @@
         <v>39</v>
       </c>
       <c r="F41" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H41" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="I41" t="str">
-        <f>_xlfn.CONCAT(H41:H41)</f>
+        <f t="shared" si="0"/>
         <v>Mastrolivo</v>
       </c>
       <c r="P41" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="Q41" t="s">
         <v>113</v>
       </c>
-      <c r="Q41" t="s">
-        <v>114</v>
-      </c>
       <c r="R41" s="1" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="S41" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>@domenico_9domenico_9</v>
       </c>
     </row>
@@ -4286,26 +4546,26 @@
         <v>40</v>
       </c>
       <c r="F42" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H42" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="I42" t="str">
-        <f>_xlfn.CONCAT(H42:H42)</f>
+        <f t="shared" si="0"/>
         <v>Sibinpopzz</v>
       </c>
       <c r="P42" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q42" t="s">
         <v>118</v>
       </c>
-      <c r="Q42" t="s">
-        <v>119</v>
-      </c>
       <c r="R42" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="S42" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>@lorenzocastaldiilorenzocastaldii</v>
       </c>
     </row>
@@ -4317,23 +4577,23 @@
         <v>11</v>
       </c>
       <c r="H43" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="I43" t="str">
-        <f>_xlfn.CONCAT(H43:H43)</f>
+        <f t="shared" si="0"/>
         <v>FedericoBello03</v>
       </c>
       <c r="P43" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q43" t="s">
         <v>75</v>
       </c>
-      <c r="Q43" t="s">
-        <v>76</v>
-      </c>
       <c r="R43" s="1" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="S43" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>@JackgioncoJackgionco</v>
       </c>
     </row>
@@ -4342,26 +4602,26 @@
         <v>42</v>
       </c>
       <c r="F44" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H44" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="I44" t="str">
-        <f>_xlfn.CONCAT(H44:H44)</f>
+        <f t="shared" si="0"/>
         <v>BACWasTaken</v>
       </c>
       <c r="P44" s="1" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="Q44" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="R44" s="1" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="S44" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>@lil_wallylil_wally</v>
       </c>
     </row>
@@ -4373,21 +4633,21 @@
         <v>21</v>
       </c>
       <c r="H45" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="I45" t="str">
-        <f>_xlfn.CONCAT(H45:H45)</f>
+        <f t="shared" si="0"/>
         <v>wa1n8</v>
       </c>
       <c r="P45" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="Q45" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="R45" s="1"/>
       <c r="S45" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>@</v>
       </c>
     </row>
@@ -4396,26 +4656,26 @@
         <v>44</v>
       </c>
       <c r="F46" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="H46" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="I46" t="str">
-        <f>_xlfn.CONCAT(H46:H46)</f>
+        <f t="shared" si="0"/>
         <v>aless_io98</v>
       </c>
       <c r="P46" s="1" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="Q46" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="R46" s="1" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="S46" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>@BonziferBonzifer</v>
       </c>
     </row>
@@ -4424,26 +4684,26 @@
         <v>45</v>
       </c>
       <c r="F47" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="H47" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="I47" t="str">
-        <f>_xlfn.CONCAT(H47:H47)</f>
+        <f t="shared" si="0"/>
         <v>MaspicDigital</v>
       </c>
       <c r="P47" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="Q47" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="R47" s="1" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="S47" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>@donche97donche97</v>
       </c>
     </row>
@@ -4452,23 +4712,23 @@
         <v>46</v>
       </c>
       <c r="F48" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="I48" t="str">
-        <f>_xlfn.CONCAT(H48:H48)</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="P48" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="Q48" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="R48" s="1" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="S48" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>@MAJOR992MAJOR992</v>
       </c>
     </row>
@@ -4477,26 +4737,26 @@
         <v>47</v>
       </c>
       <c r="F49" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H49" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="I49" t="str">
-        <f>_xlfn.CONCAT(H49:H49)</f>
+        <f t="shared" si="0"/>
         <v>niflash</v>
       </c>
       <c r="P49" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q49" t="s">
         <v>79</v>
       </c>
-      <c r="Q49" t="s">
-        <v>80</v>
-      </c>
       <c r="R49" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="S49" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>@frankye73frankye73</v>
       </c>
     </row>
@@ -4505,26 +4765,26 @@
         <v>48</v>
       </c>
       <c r="F50" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="H50" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="I50" t="str">
-        <f>_xlfn.CONCAT(H50:H50)</f>
+        <f t="shared" si="0"/>
         <v>cicciovolley91</v>
       </c>
       <c r="P50" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="Q50" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="R50" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="S50" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>@mattiaframarinmattiaframarin</v>
       </c>
     </row>
@@ -4533,58 +4793,58 @@
         <v>49</v>
       </c>
       <c r="F51" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="H51" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I51" t="str">
-        <f>_xlfn.CONCAT(H51:H51)</f>
+        <f t="shared" si="0"/>
         <v>begghich</v>
       </c>
       <c r="P51" s="1" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="Q51" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="R51" s="1" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="S51" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>@Kingmike1592Kingmike1592</v>
       </c>
     </row>
     <row r="52" spans="1:19" x14ac:dyDescent="0.3">
       <c r="F52" s="1"/>
       <c r="P52" s="1" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="Q52" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="R52" s="1" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="S52" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>@ADr_aicaADr_aica</v>
       </c>
     </row>
     <row r="53" spans="1:19" x14ac:dyDescent="0.3">
       <c r="F53" s="1"/>
       <c r="P53" s="1" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="Q53" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="R53" s="1" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="S53" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>@Haroldpain69Haroldpain69</v>
       </c>
     </row>

</xml_diff>

<commit_message>
convocazioni 4 settimana settembre
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stefa\Link-clan\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FC3AA61-BC9C-4A92-85E1-4F0AE80AC0F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BAE1CBF-1A29-4FCC-A476-12A9872EC070}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{FECCDA54-7594-4EB7-ABFB-2C408C6461DD}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="629" uniqueCount="382">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="650" uniqueCount="400">
   <si>
     <t>TagTelegram</t>
   </si>
@@ -522,12 +522,6 @@
     <t>ＡＲ♣️Ｃｉｃｃｉｏ</t>
   </si>
   <si>
-    <t>@Sibinpopzz</t>
-  </si>
-  <si>
-    <t>@BACWasTaken</t>
-  </si>
-  <si>
     <t>@Mastrolivo</t>
   </si>
   <si>
@@ -888,298 +882,358 @@
     <t>@Haroldpain69</t>
   </si>
   <si>
-    <t>@sunnering</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  ＡＲ♠️Ɛ Ɩ ɪ Ơ </t>
-  </si>
-  <si>
-    <t xml:space="preserve">  ＡＲ♦️Ｂｌａｚｏｒ１１１ </t>
-  </si>
-  <si>
-    <t xml:space="preserve">  aleman(statale) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">  ＡＲ♠️＠ｌｅｍａｎ </t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Ａｒ❤️Ｓａｍｕｅｌｅ </t>
-  </si>
-  <si>
-    <t xml:space="preserve">  geeno </t>
-  </si>
-  <si>
-    <t xml:space="preserve">  ＡＲ ❤️ＡＬＥＸ </t>
-  </si>
-  <si>
-    <t xml:space="preserve">  AR♣️OMA </t>
-  </si>
-  <si>
-    <t xml:space="preserve">  crezyred </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Damo </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> robu </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Qliff </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> MARCHIO </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ＡＲ♠️Ｏｘｈａｔｒｅｓ</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ＡＲ♣️Ｒｉｃｃａｌｓｏ </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> bo </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> BrokerTony </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ＡＲ♥️Ｍａｚｚｉｔｏ </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> sid </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> DOCCC </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> mrdeath75 </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Ahmed </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Uchiha Madara </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> bughy </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> J.O.K.E.R.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Davide.Z</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> AR♠️alfone </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Daniele </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ＡＲ♦️Ｅ＄</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> dino </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> alabatia89 </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> dani_lanc </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Peppone91 </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> OhAnd4 </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> YATO51 </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Kekko03 </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Sandiokan </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> $!B!N </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ＡＲ♠️Ｆｅｄｅ </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ＡＲ♠️ＢＡＣ </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ＡＲ♦️道路軍Wåyne </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> AR ♦️Goldenboy </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ＡＲ♣️Ｃｉｃｃｉｏ </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> AR♣️Severens</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Nico </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> cicciovolley91 </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Begghich </t>
-  </si>
-  <si>
     <t>@GoofyGooberr</t>
   </si>
   <si>
-    <t xml:space="preserve">  AR♦️Matteo </t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Arsenio </t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Lore_98 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">  simo99 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">  AR♦️Nico </t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Angeloxf7 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">  tala </t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Don Michele </t>
-  </si>
-  <si>
-    <t xml:space="preserve">  vinz </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> nevio lostirato </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> coraz </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Bombazza </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> REMIDA </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Luca </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Luigi13 </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> zumpy </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ＡＲ♣️Ｓｕｎｄｒｉｐｓ </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> TexWiller </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> LATIN WARRIOR™ </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ＡＲ❤️♣️ＧＯＤ９８♠️♦️ </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> pro </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> gigio </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> •fury™• </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Lubbro95 C.B  </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Just_Dodo </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> christian98 </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ⭐️Marco⭐️ </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> AnUbIs </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> random guy </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Enriic </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Big </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> orso86 </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Zokum </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> AR♦️ᴍᴀᴛᴛᴇᴏ </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> riccardo </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> DonPunta </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Domenico </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Pinguino </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> OneLeggedJack </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> lil_wally </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> SistemaS</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> sebabigo </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> \GuyFawkes/ </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ⚡️MAJOR⚡️ </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> frankye73 </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Ar♦️KingSupremo </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> kingmike </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> El Peko </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Wolfdale </t>
+    <t xml:space="preserve">Antonio96 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">_SINA22_ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thor⚡️ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">begghich </t>
+  </si>
+  <si>
+    <t xml:space="preserve">simo99 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kekko03 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Domenico </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Don Michele </t>
+  </si>
+  <si>
+    <t xml:space="preserve">\GuyFawkes/ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ＡＲ♦️Ｎｉｃｏ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">gigio </t>
+  </si>
+  <si>
+    <t xml:space="preserve">tala </t>
+  </si>
+  <si>
+    <t xml:space="preserve">LATIN WARRIOR™ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AR♣️OMA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ＡＲ♠️Ｆｅｄｅ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uchiha Madara </t>
+  </si>
+  <si>
+    <t xml:space="preserve">GaiaScienza </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lore_98 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">christian98 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">shinigami </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ＡＲ♠️Ɛ Ɩ ɪ Ơ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Daniele </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Qliff </t>
+  </si>
+  <si>
+    <t xml:space="preserve">mrdeath75 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sandiokan </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AR ♦️Goldenboy </t>
+  </si>
+  <si>
+    <t xml:space="preserve">crezyred </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ＡＲ♥️Ｍａｚｚｉｔｏ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Geeno </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ＡＲ♣️Ｒｉｃｃａｌｓｏ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">aleman(statale) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Damo </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ＡＲ♠️Ｏｘｈａｔｒｅｓ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">DOCCC </t>
+  </si>
+  <si>
+    <t xml:space="preserve">bughy </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AR♣️Ciccio </t>
+  </si>
+  <si>
+    <t xml:space="preserve">bo </t>
+  </si>
+  <si>
+    <t xml:space="preserve">MARCHIO </t>
+  </si>
+  <si>
+    <t xml:space="preserve">BrokerTony </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ａｒ❤️Ｓａｍｕｅｌｅ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ＡＲ ❤️ＡＬＥＸ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ＡＲ♦️Ｅ＄ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ＡＲ♦️Ｂｌａｚｏｒ１１１ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">alabatia89 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peppone91 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Davide.Z </t>
+  </si>
+  <si>
+    <t xml:space="preserve">sid </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Luigi13 </t>
+  </si>
+  <si>
+    <t>HTL I EBDP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">coraz </t>
+  </si>
+  <si>
+    <t>@totino96</t>
+  </si>
+  <si>
+    <t>@RickySina22</t>
+  </si>
+  <si>
+    <t>@Gaia951</t>
+  </si>
+  <si>
+    <t>@Balliver</t>
+  </si>
+  <si>
+    <t>@Mannito92</t>
+  </si>
+  <si>
+    <t>@luca3689</t>
+  </si>
+  <si>
+    <t>@Freenk8</t>
+  </si>
+  <si>
+    <t>@MerMet92</t>
+  </si>
+  <si>
+    <t>@T0N1003</t>
+  </si>
+  <si>
+    <t>@ciuler</t>
+  </si>
+  <si>
+    <t>@Sas0800</t>
+  </si>
+  <si>
+    <t>@arsenapoli</t>
+  </si>
+  <si>
+    <t>@superfede2</t>
+  </si>
+  <si>
+    <t>@Oneleggedjack</t>
+  </si>
+  <si>
+    <t>@Manu2365</t>
+  </si>
+  <si>
+    <t>@usernamepersonalee</t>
+  </si>
+  <si>
+    <t>@srd_rce</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ahmed </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wolfdale </t>
+  </si>
+  <si>
+    <t xml:space="preserve">robu </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cry </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AR♠️alfone </t>
+  </si>
+  <si>
+    <t xml:space="preserve">YATO51 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Big </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Luca01 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;c5&gt;OhAnd4 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cicciovolley91 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Frenk8 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Meru </t>
+  </si>
+  <si>
+    <t xml:space="preserve">lord Tony </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nico </t>
+  </si>
+  <si>
+    <t xml:space="preserve">dani_lanc </t>
+  </si>
+  <si>
+    <t xml:space="preserve">khmer BM⚡️ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">TexWiller </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ar♦️KingSupremo </t>
+  </si>
+  <si>
+    <t xml:space="preserve">vinz </t>
+  </si>
+  <si>
+    <t xml:space="preserve">⭐️Marco⭐️ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">J.O.K.E.R </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ＡＲ❤️♣️ＧＯＤ９８♠️♦️ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AR♦️ᴍᴀᴛᴛᴇᴏ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bombazza </t>
+  </si>
+  <si>
+    <t xml:space="preserve">●SUMATRA● </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AnUbIs </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arsenio </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Angeloxf7 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ＡＲ♣️Ｓｕｎｄｒｉｐｓ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ＢＲ♠️ＤｏＮ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">nevio lostirato </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lubbro95 C.B. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">lil_wally </t>
+  </si>
+  <si>
+    <t xml:space="preserve">pro </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zokum </t>
+  </si>
+  <si>
+    <t xml:space="preserve">⚡️MAJOR⚡️ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">superfede </t>
+  </si>
+  <si>
+    <t xml:space="preserve">sebabigo </t>
+  </si>
+  <si>
+    <t xml:space="preserve">OneLeggedJack </t>
+  </si>
+  <si>
+    <t xml:space="preserve">•fury™• </t>
+  </si>
+  <si>
+    <t xml:space="preserve">random guy </t>
+  </si>
+  <si>
+    <t xml:space="preserve">frankye73 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zumpy </t>
+  </si>
+  <si>
+    <t xml:space="preserve">REMIDA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">kingmike </t>
+  </si>
+  <si>
+    <t xml:space="preserve">orso86 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lore </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eric </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Just_Dodo </t>
+  </si>
+  <si>
+    <t xml:space="preserve">DonPunta </t>
   </si>
 </sst>
 </file>
@@ -2043,16 +2097,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EE2B0F9-AC31-464B-B046-53CB033C8615}">
-  <dimension ref="A1:D99"/>
+  <dimension ref="A1:D102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C48" sqref="C2:C48"/>
+      <selection activeCell="A96" sqref="A96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.77734375" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.88671875" style="1"/>
@@ -2079,1347 +2133,1414 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>10</v>
+        <v>333</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>20</v>
+        <v>334</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>5</v>
+        <v>126</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>23</v>
+        <v>124</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>8</v>
+        <v>113</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>14</v>
+        <v>273</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>31</v>
+        <v>282</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>33</v>
+        <v>135</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>48</v>
+        <v>110</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>46</v>
+        <v>88</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>40</v>
+        <v>129</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="B15" s="1" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>25</v>
+        <v>49</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>27</v>
+        <v>335</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>18</v>
+        <v>103</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>145</v>
+        <v>53</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>139</v>
+        <v>12</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>42</v>
+        <v>10</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>7</v>
+        <v>35</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>116</v>
+        <v>162</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>37</v>
+        <v>163</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>99</v>
+        <v>31</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>90</v>
+        <v>114</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>284</v>
+        <v>16</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>143</v>
+        <v>5</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>122</v>
+        <v>33</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>44</v>
+        <v>336</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>96</v>
+        <v>29</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
-        <v>120</v>
+        <v>164</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>164</v>
+        <v>25</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
-        <v>162</v>
+        <v>40</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
-        <v>163</v>
+        <v>23</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
-        <v>165</v>
+        <v>90</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
-        <v>166</v>
+        <v>20</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45" s="1" t="s">
+        <v>143</v>
+      </c>
       <c r="B45" s="1" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
-        <v>66</v>
+        <v>44</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
-        <v>91</v>
+        <v>37</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
-        <v>126</v>
+        <v>145</v>
       </c>
       <c r="B48" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A49" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A50" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="B50" s="1" t="s">
         <v>331</v>
       </c>
-      <c r="C48" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
+      <c r="C50" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A51" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="B49" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
-        <v>154</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>334</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
-        <v>103</v>
-      </c>
       <c r="B51" s="1" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>94</v>
+        <v>3</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
-        <v>124</v>
+      <c r="A52" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>336</v>
+        <v>350</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>94</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A53" t="s">
-        <v>135</v>
+      <c r="A53" s="1" t="s">
+        <v>281</v>
       </c>
       <c r="B53" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A54" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A55" s="1" t="s">
         <v>337</v>
       </c>
-      <c r="C53" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A54" t="s">
+      <c r="B55" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A56" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A57" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A58" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A59" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A60" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A61" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A62" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A63" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A64" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A65" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A66" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A67" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A68" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A69" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A70" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A71" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A72" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A73" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A74" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A75" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A76" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A77" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A78" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A79" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="B54" s="1" t="s">
-        <v>338</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A55" t="s">
-        <v>88</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>339</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A56" t="s">
+      <c r="B79" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A80" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A81" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A82" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A83" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A84" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A85" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A86" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A87" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A88" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A89" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A90" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D90" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A91" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D91" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A92" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D92" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A93" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D93" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A94" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="B56" s="1" t="s">
-        <v>340</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A57" t="s">
-        <v>141</v>
-      </c>
-      <c r="B57" s="1" t="s">
-        <v>341</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A58" t="s">
-        <v>97</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>342</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A59" t="s">
-        <v>276</v>
-      </c>
-      <c r="B59" s="1" t="s">
-        <v>343</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D59" s="1" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A60" t="s">
-        <v>71</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>344</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A61" t="s">
+      <c r="B94" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D94" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A95" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="B61" s="1" t="s">
-        <v>345</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D61" s="1" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A62" t="s">
-        <v>63</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>346</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D62" s="1" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A63" t="s">
-        <v>59</v>
-      </c>
-      <c r="B63" s="1" t="s">
-        <v>347</v>
-      </c>
-      <c r="C63" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D63" s="1" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A64" t="s">
-        <v>277</v>
-      </c>
-      <c r="B64" s="1" t="s">
+      <c r="B95" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D95" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A96" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D96" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A97" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D97" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A98" s="1" t="s">
         <v>348</v>
       </c>
-      <c r="C64" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D64" s="1" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A65" t="s">
-        <v>128</v>
-      </c>
-      <c r="B65" s="1" t="s">
+      <c r="B98" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D98" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B99" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D99" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A100" s="1" t="s">
         <v>349</v>
       </c>
-      <c r="C65" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D65" s="1" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A66" t="s">
-        <v>57</v>
-      </c>
-      <c r="B66" s="1" t="s">
-        <v>350</v>
-      </c>
-      <c r="C66" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D66" s="1" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A67" t="s">
-        <v>129</v>
-      </c>
-      <c r="B67" s="1" t="s">
-        <v>351</v>
-      </c>
-      <c r="C67" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D67" s="1" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A68" t="s">
-        <v>105</v>
-      </c>
-      <c r="B68" s="1" t="s">
-        <v>352</v>
-      </c>
-      <c r="C68" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D68" s="1" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A69" t="s">
-        <v>61</v>
-      </c>
-      <c r="B69" s="1" t="s">
-        <v>353</v>
-      </c>
-      <c r="C69" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D69" s="1" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A70" t="s">
-        <v>110</v>
-      </c>
-      <c r="B70" s="1" t="s">
-        <v>354</v>
-      </c>
-      <c r="C70" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D70" s="1" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A71" t="s">
-        <v>155</v>
-      </c>
-      <c r="B71" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="C71" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D71" s="1" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A72" t="s">
-        <v>86</v>
-      </c>
-      <c r="B72" s="1" t="s">
-        <v>356</v>
-      </c>
-      <c r="C72" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D72" s="1" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A73" t="s">
+      <c r="B100" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D100" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A101" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B73" s="1" t="s">
-        <v>357</v>
-      </c>
-      <c r="C73" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D73" s="1" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A74" t="s">
-        <v>53</v>
-      </c>
-      <c r="B74" s="1" t="s">
-        <v>358</v>
-      </c>
-      <c r="C74" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D74" s="1" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A75" t="s">
-        <v>106</v>
-      </c>
-      <c r="B75" s="1" t="s">
-        <v>359</v>
-      </c>
-      <c r="C75" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D75" s="1" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A76" t="s">
-        <v>108</v>
-      </c>
-      <c r="B76" s="1" t="s">
-        <v>360</v>
-      </c>
-      <c r="C76" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D76" s="1" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A77" t="s">
-        <v>64</v>
-      </c>
-      <c r="B77" s="1" t="s">
-        <v>361</v>
-      </c>
-      <c r="C77" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D77" s="1" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A78" t="s">
-        <v>131</v>
-      </c>
-      <c r="B78" s="1" t="s">
-        <v>362</v>
-      </c>
-      <c r="C78" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D78" s="1" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A79" t="s">
-        <v>55</v>
-      </c>
-      <c r="B79" s="1" t="s">
-        <v>363</v>
-      </c>
-      <c r="C79" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D79" s="1" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A80" t="s">
-        <v>85</v>
-      </c>
-      <c r="B80" s="1" t="s">
-        <v>364</v>
-      </c>
-      <c r="C80" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D80" s="1" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A81" t="s">
-        <v>81</v>
-      </c>
-      <c r="B81" s="1" t="s">
-        <v>365</v>
-      </c>
-      <c r="C81" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D81" s="1" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A82" t="s">
-        <v>83</v>
-      </c>
-      <c r="B82" s="1" t="s">
-        <v>366</v>
-      </c>
-      <c r="C82" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D82" s="1" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A83" t="s">
-        <v>68</v>
-      </c>
-      <c r="B83" s="1" t="s">
-        <v>367</v>
-      </c>
-      <c r="C83" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D83" s="1" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A84" t="s">
+      <c r="B101" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D101" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A102" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B84" s="1" t="s">
-        <v>368</v>
-      </c>
-      <c r="C84" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D84" s="1" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A85" t="s">
-        <v>113</v>
-      </c>
-      <c r="B85" s="1" t="s">
-        <v>369</v>
-      </c>
-      <c r="C85" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D85" s="1" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A86" t="s">
-        <v>118</v>
-      </c>
-      <c r="B86" s="1" t="s">
-        <v>370</v>
-      </c>
-      <c r="C86" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D86" s="1" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A87" t="s">
-        <v>75</v>
-      </c>
-      <c r="B87" s="1" t="s">
-        <v>371</v>
-      </c>
-      <c r="C87" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D87" s="1" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A88" t="s">
-        <v>278</v>
-      </c>
-      <c r="B88" s="1" t="s">
-        <v>372</v>
-      </c>
-      <c r="C88" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D88" s="1" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A89" t="s">
-        <v>215</v>
-      </c>
-      <c r="B89" s="1" t="s">
-        <v>373</v>
-      </c>
-      <c r="C89" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D89" s="1" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A90" t="s">
-        <v>279</v>
-      </c>
-      <c r="B90" s="1" t="s">
-        <v>374</v>
-      </c>
-      <c r="C90" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D90" s="1" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A91" t="s">
-        <v>332</v>
-      </c>
-      <c r="B91" s="1" t="s">
-        <v>375</v>
-      </c>
-      <c r="C91" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D91" s="1" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A92" t="s">
-        <v>134</v>
-      </c>
-      <c r="B92" s="1" t="s">
-        <v>376</v>
-      </c>
-      <c r="C92" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D92" s="1" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A93" t="s">
-        <v>79</v>
-      </c>
-      <c r="B93" s="1" t="s">
-        <v>377</v>
-      </c>
-      <c r="C93" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D93" s="1" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A94" t="s">
-        <v>280</v>
-      </c>
-      <c r="B94" s="1" t="s">
-        <v>378</v>
-      </c>
-      <c r="C94" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D94" s="1" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A95" t="s">
-        <v>281</v>
-      </c>
-      <c r="B95" s="1" t="s">
-        <v>379</v>
-      </c>
-      <c r="C95" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D95" s="1" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A96" t="s">
-        <v>282</v>
-      </c>
-      <c r="B96" s="1" t="s">
-        <v>380</v>
-      </c>
-      <c r="C96" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D96" s="1" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A97" t="s">
-        <v>283</v>
-      </c>
-      <c r="B97" s="1" t="s">
-        <v>381</v>
-      </c>
-      <c r="C97" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D97" s="1" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A98"/>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A99"/>
+      <c r="B102" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D102" s="1" t="s">
+        <v>165</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3450,23 +3571,23 @@
         <v>1</v>
       </c>
       <c r="F4" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="H4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="I4" t="str">
         <f t="shared" ref="I4:I51" si="0">_xlfn.CONCAT(H4:H4)</f>
         <v>elioo_06</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="Q4" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="R4" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="S4" t="str">
         <f>_xlfn.CONCAT(Q4:R4)</f>
@@ -3482,7 +3603,7 @@
         <v>19</v>
       </c>
       <c r="H5" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="I5" t="str">
         <f t="shared" si="0"/>
@@ -3495,7 +3616,7 @@
         <v>154</v>
       </c>
       <c r="R5" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="S5" t="str">
         <f t="shared" ref="S5:S53" si="1">_xlfn.CONCAT(Q5:R5)</f>
@@ -3511,7 +3632,7 @@
         <v>4</v>
       </c>
       <c r="H6" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="I6" t="str">
         <f t="shared" si="0"/>
@@ -3524,7 +3645,7 @@
         <v>103</v>
       </c>
       <c r="R6" s="1" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="S6" t="str">
         <f t="shared" si="1"/>
@@ -3540,7 +3661,7 @@
         <v>9</v>
       </c>
       <c r="H7" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="I7" t="str">
         <f t="shared" si="0"/>
@@ -3553,7 +3674,7 @@
         <v>124</v>
       </c>
       <c r="R7" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="S7" t="str">
         <f t="shared" si="1"/>
@@ -3569,7 +3690,7 @@
         <v>38</v>
       </c>
       <c r="H8" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="I8" t="str">
         <f t="shared" si="0"/>
@@ -3582,7 +3703,7 @@
         <v>135</v>
       </c>
       <c r="R8" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="S8" t="str">
         <f t="shared" si="1"/>
@@ -3595,10 +3716,10 @@
       </c>
       <c r="E9" s="1"/>
       <c r="F9" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="H9" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="I9" t="str">
         <f t="shared" si="0"/>
@@ -3611,7 +3732,7 @@
         <v>101</v>
       </c>
       <c r="R9" s="1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="S9" t="str">
         <f t="shared" si="1"/>
@@ -3624,10 +3745,10 @@
       </c>
       <c r="E10" s="1"/>
       <c r="F10" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="H10" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="I10" t="str">
         <f t="shared" si="0"/>
@@ -3640,7 +3761,7 @@
         <v>88</v>
       </c>
       <c r="R10" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="S10" t="str">
         <f t="shared" si="1"/>
@@ -3656,20 +3777,20 @@
         <v>50</v>
       </c>
       <c r="H11" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="I11" t="str">
         <f t="shared" si="0"/>
         <v>Ale_Mare93</v>
       </c>
       <c r="P11" s="1" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="Q11" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="R11" s="1" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="S11" t="str">
         <f t="shared" si="1"/>
@@ -3685,7 +3806,7 @@
         <v>13</v>
       </c>
       <c r="H12" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="I12" t="str">
         <f t="shared" si="0"/>
@@ -3698,7 +3819,7 @@
         <v>141</v>
       </c>
       <c r="R12" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="S12" t="str">
         <f t="shared" si="1"/>
@@ -3727,7 +3848,7 @@
         <v>97</v>
       </c>
       <c r="R13" s="1" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="S13" t="str">
         <f t="shared" si="1"/>
@@ -3743,20 +3864,20 @@
         <v>32</v>
       </c>
       <c r="H14" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="I14" t="str">
         <f t="shared" si="0"/>
         <v>DaMoops</v>
       </c>
       <c r="P14" s="1" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="Q14" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="R14" s="1" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="S14" t="str">
         <f t="shared" si="1"/>
@@ -3772,7 +3893,7 @@
         <v>47</v>
       </c>
       <c r="H15" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="I15" t="str">
         <f t="shared" si="0"/>
@@ -3785,7 +3906,7 @@
         <v>71</v>
       </c>
       <c r="R15" s="1" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="S15" t="str">
         <f t="shared" si="1"/>
@@ -3801,7 +3922,7 @@
         <v>45</v>
       </c>
       <c r="H16" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="I16" t="str">
         <f t="shared" si="0"/>
@@ -3814,7 +3935,7 @@
         <v>133</v>
       </c>
       <c r="R16" s="1" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="S16" t="str">
         <f t="shared" si="1"/>
@@ -3830,7 +3951,7 @@
         <v>39</v>
       </c>
       <c r="H17" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="I17" t="str">
         <f t="shared" si="0"/>
@@ -3843,7 +3964,7 @@
         <v>63</v>
       </c>
       <c r="R17" s="1" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="S17" t="str">
         <f t="shared" si="1"/>
@@ -3869,7 +3990,7 @@
         <v>59</v>
       </c>
       <c r="R18" s="1" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="S18" t="str">
         <f t="shared" si="1"/>
@@ -3885,20 +4006,20 @@
         <v>15</v>
       </c>
       <c r="H19" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="I19" t="str">
         <f t="shared" si="0"/>
         <v>riccalso</v>
       </c>
       <c r="P19" s="1" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="Q19" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="R19" s="1" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="S19" t="str">
         <f t="shared" si="1"/>
@@ -3914,7 +4035,7 @@
         <v>24</v>
       </c>
       <c r="H20" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="I20" t="str">
         <f t="shared" si="0"/>
@@ -3927,7 +4048,7 @@
         <v>128</v>
       </c>
       <c r="R20" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="S20" t="str">
         <f t="shared" si="1"/>
@@ -3956,7 +4077,7 @@
         <v>57</v>
       </c>
       <c r="R21" s="1" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="S21" t="str">
         <f t="shared" si="1"/>
@@ -3972,7 +4093,7 @@
         <v>17</v>
       </c>
       <c r="H22" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="I22" t="str">
         <f t="shared" si="0"/>
@@ -3985,7 +4106,7 @@
         <v>99</v>
       </c>
       <c r="R22" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="S22" t="str">
         <f t="shared" si="1"/>
@@ -4001,7 +4122,7 @@
         <v>144</v>
       </c>
       <c r="H23" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="I23" t="str">
         <f t="shared" si="0"/>
@@ -4014,7 +4135,7 @@
         <v>129</v>
       </c>
       <c r="R23" s="1" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="S23" t="str">
         <f t="shared" si="1"/>
@@ -4030,7 +4151,7 @@
         <v>138</v>
       </c>
       <c r="H24" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="I24" t="str">
         <f t="shared" si="0"/>
@@ -4043,7 +4164,7 @@
         <v>105</v>
       </c>
       <c r="R24" s="1" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="S24" t="str">
         <f t="shared" si="1"/>
@@ -4072,7 +4193,7 @@
         <v>61</v>
       </c>
       <c r="R25" s="1" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="S25" t="str">
         <f t="shared" si="1"/>
@@ -4088,7 +4209,7 @@
         <v>6</v>
       </c>
       <c r="H26" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="I26" t="str">
         <f t="shared" si="0"/>
@@ -4101,7 +4222,7 @@
         <v>110</v>
       </c>
       <c r="R26" s="1" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="S26" t="str">
         <f t="shared" si="1"/>
@@ -4117,7 +4238,7 @@
         <v>51</v>
       </c>
       <c r="H27" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="I27" t="str">
         <f t="shared" si="0"/>
@@ -4130,7 +4251,7 @@
         <v>155</v>
       </c>
       <c r="R27" s="1" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="S27" t="str">
         <f t="shared" si="1"/>
@@ -4146,7 +4267,7 @@
         <v>28</v>
       </c>
       <c r="H28" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="I28" t="str">
         <f t="shared" si="0"/>
@@ -4159,7 +4280,7 @@
         <v>86</v>
       </c>
       <c r="R28" s="1" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="S28" t="str">
         <f t="shared" si="1"/>
@@ -4175,7 +4296,7 @@
         <v>115</v>
       </c>
       <c r="H29" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="I29" t="str">
         <f t="shared" si="0"/>
@@ -4188,7 +4309,7 @@
         <v>73</v>
       </c>
       <c r="R29" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="S29" t="str">
         <f t="shared" si="1"/>
@@ -4204,7 +4325,7 @@
         <v>36</v>
       </c>
       <c r="H30" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="I30" t="str">
         <f t="shared" si="0"/>
@@ -4217,7 +4338,7 @@
         <v>53</v>
       </c>
       <c r="R30" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="S30" t="str">
         <f t="shared" si="1"/>
@@ -4233,20 +4354,20 @@
         <v>98</v>
       </c>
       <c r="H31" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="I31" t="str">
         <f t="shared" si="0"/>
         <v>ralfone01</v>
       </c>
       <c r="P31" s="1" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="Q31" t="s">
         <v>106</v>
       </c>
       <c r="R31" s="1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="S31" t="str">
         <f t="shared" si="1"/>
@@ -4262,7 +4383,7 @@
         <v>34</v>
       </c>
       <c r="H32" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="I32" t="str">
         <f t="shared" si="0"/>
@@ -4275,7 +4396,7 @@
         <v>108</v>
       </c>
       <c r="R32" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="S32" t="str">
         <f t="shared" si="1"/>
@@ -4291,7 +4412,7 @@
         <v>89</v>
       </c>
       <c r="H33" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="I33" t="str">
         <f t="shared" si="0"/>
@@ -4304,7 +4425,7 @@
         <v>64</v>
       </c>
       <c r="R33" s="1" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="S33" t="str">
         <f t="shared" si="1"/>
@@ -4317,10 +4438,10 @@
       </c>
       <c r="E34" s="1"/>
       <c r="F34" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="H34" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="I34" t="str">
         <f t="shared" si="0"/>
@@ -4333,7 +4454,7 @@
         <v>131</v>
       </c>
       <c r="R34" s="1" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="S34" t="str">
         <f t="shared" si="1"/>
@@ -4362,7 +4483,7 @@
         <v>55</v>
       </c>
       <c r="R35" s="1" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="S35" t="str">
         <f t="shared" si="1"/>
@@ -4378,7 +4499,7 @@
         <v>121</v>
       </c>
       <c r="H36" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="I36" t="str">
         <f t="shared" si="0"/>
@@ -4391,7 +4512,7 @@
         <v>85</v>
       </c>
       <c r="R36" s="1" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="S36" t="str">
         <f t="shared" si="1"/>
@@ -4407,7 +4528,7 @@
         <v>43</v>
       </c>
       <c r="H37" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="I37" t="str">
         <f t="shared" si="0"/>
@@ -4420,7 +4541,7 @@
         <v>81</v>
       </c>
       <c r="R37" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="S37" t="str">
         <f t="shared" si="1"/>
@@ -4436,7 +4557,7 @@
         <v>136</v>
       </c>
       <c r="H38" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="I38" t="str">
         <f t="shared" si="0"/>
@@ -4449,7 +4570,7 @@
         <v>83</v>
       </c>
       <c r="R38" s="1" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="S38" t="str">
         <f t="shared" si="1"/>
@@ -4465,7 +4586,7 @@
         <v>95</v>
       </c>
       <c r="H39" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="I39" t="str">
         <f t="shared" si="0"/>
@@ -4478,7 +4599,7 @@
         <v>68</v>
       </c>
       <c r="R39" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="S39" t="str">
         <f t="shared" si="1"/>
@@ -4493,7 +4614,7 @@
         <v>119</v>
       </c>
       <c r="H40" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="I40" t="str">
         <f t="shared" si="0"/>
@@ -4506,7 +4627,7 @@
         <v>77</v>
       </c>
       <c r="R40" s="1" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="S40" t="str">
         <f t="shared" si="1"/>
@@ -4521,7 +4642,7 @@
         <v>157</v>
       </c>
       <c r="H41" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="I41" t="str">
         <f t="shared" si="0"/>
@@ -4534,7 +4655,7 @@
         <v>113</v>
       </c>
       <c r="R41" s="1" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="S41" t="str">
         <f t="shared" si="1"/>
@@ -4549,7 +4670,7 @@
         <v>158</v>
       </c>
       <c r="H42" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="I42" t="str">
         <f t="shared" si="0"/>
@@ -4562,7 +4683,7 @@
         <v>118</v>
       </c>
       <c r="R42" s="1" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="S42" t="str">
         <f t="shared" si="1"/>
@@ -4577,7 +4698,7 @@
         <v>11</v>
       </c>
       <c r="H43" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="I43" t="str">
         <f t="shared" si="0"/>
@@ -4590,7 +4711,7 @@
         <v>75</v>
       </c>
       <c r="R43" s="1" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="S43" t="str">
         <f t="shared" si="1"/>
@@ -4605,20 +4726,20 @@
         <v>159</v>
       </c>
       <c r="H44" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="I44" t="str">
         <f t="shared" si="0"/>
         <v>BACWasTaken</v>
       </c>
       <c r="P44" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="Q44" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="R44" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="S44" t="str">
         <f t="shared" si="1"/>
@@ -4633,7 +4754,7 @@
         <v>21</v>
       </c>
       <c r="H45" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="I45" t="str">
         <f t="shared" si="0"/>
@@ -4643,7 +4764,7 @@
         <v>151</v>
       </c>
       <c r="Q45" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="R45" s="1"/>
       <c r="S45" t="str">
@@ -4659,20 +4780,20 @@
         <v>160</v>
       </c>
       <c r="H46" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="I46" t="str">
         <f t="shared" si="0"/>
         <v>aless_io98</v>
       </c>
       <c r="P46" s="1" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="Q46" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="R46" s="1" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="S46" t="str">
         <f t="shared" si="1"/>
@@ -4687,7 +4808,7 @@
         <v>161</v>
       </c>
       <c r="H47" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="I47" t="str">
         <f t="shared" si="0"/>
@@ -4700,7 +4821,7 @@
         <v>156</v>
       </c>
       <c r="R47" s="1" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="S47" t="str">
         <f t="shared" si="1"/>
@@ -4712,20 +4833,20 @@
         <v>46</v>
       </c>
       <c r="F48" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="I48" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="P48" s="1" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="Q48" t="s">
         <v>134</v>
       </c>
       <c r="R48" s="1" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="S48" t="str">
         <f t="shared" si="1"/>
@@ -4740,7 +4861,7 @@
         <v>65</v>
       </c>
       <c r="H49" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="I49" t="str">
         <f t="shared" si="0"/>
@@ -4765,23 +4886,23 @@
         <v>48</v>
       </c>
       <c r="F50" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="H50" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="I50" t="str">
         <f t="shared" si="0"/>
         <v>cicciovolley91</v>
       </c>
       <c r="P50" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="Q50" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="R50" s="1" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="S50" t="str">
         <f t="shared" si="1"/>
@@ -4793,7 +4914,7 @@
         <v>49</v>
       </c>
       <c r="F51" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="H51" t="s">
         <v>125</v>
@@ -4803,13 +4924,13 @@
         <v>begghich</v>
       </c>
       <c r="P51" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="Q51" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="R51" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="S51" t="str">
         <f t="shared" si="1"/>
@@ -4819,13 +4940,13 @@
     <row r="52" spans="1:19" x14ac:dyDescent="0.3">
       <c r="F52" s="1"/>
       <c r="P52" s="1" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="Q52" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="R52" s="1" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="S52" t="str">
         <f t="shared" si="1"/>
@@ -4835,13 +4956,13 @@
     <row r="53" spans="1:19" x14ac:dyDescent="0.3">
       <c r="F53" s="1"/>
       <c r="P53" s="1" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="Q53" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="R53" s="1" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="S53" t="str">
         <f t="shared" si="1"/>

</xml_diff>

<commit_message>
convocazioni 1 stagione 125
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stefa\Link-clan\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7ee4892a2dd36b84/Desktop/Link-clan/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FCDD52C-4DCE-46C4-BB20-7F2264BA0663}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="13_ncr:1_{9FCDD52C-4DCE-46C4-BB20-7F2264BA0663}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{850E0488-124F-4429-8FDF-458B59134D3B}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{FECCDA54-7594-4EB7-ABFB-2C408C6461DD}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="738" uniqueCount="435">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="641" uniqueCount="337">
   <si>
     <t>TagTelegram</t>
   </si>
@@ -66,9 +66,6 @@
     <t>ＡＲ♠️＠ｌｅｍａｎ</t>
   </si>
   <si>
-    <t>@elioo_06</t>
-  </si>
-  <si>
     <t>ＡＲ♠️Ｆｅｄｅ</t>
   </si>
   <si>
@@ -225,9 +222,6 @@
     <t>Nico</t>
   </si>
   <si>
-    <t>@niflash</t>
-  </si>
-  <si>
     <t>riccardo</t>
   </si>
   <si>
@@ -309,9 +303,6 @@
     <t>Lubbro95 C.B.</t>
   </si>
   <si>
-    <t>Ce Magnamm</t>
-  </si>
-  <si>
     <t>YATO51</t>
   </si>
   <si>
@@ -453,9 +444,6 @@
     <t>alabatia89</t>
   </si>
   <si>
-    <t>@alabatia89</t>
-  </si>
-  <si>
     <t>sid</t>
   </si>
   <si>
@@ -519,9 +507,6 @@
     <t>@MaspicDigital</t>
   </si>
   <si>
-    <t>si</t>
-  </si>
-  <si>
     <t>elioo_06</t>
   </si>
   <si>
@@ -870,141 +855,9 @@
     <t>@GoofyGooberr</t>
   </si>
   <si>
-    <t xml:space="preserve">Antonio96 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">_SINA22_ </t>
-  </si>
-  <si>
-    <t xml:space="preserve">begghich </t>
-  </si>
-  <si>
-    <t xml:space="preserve">simo99 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kekko03 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Domenico </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Don Michele </t>
-  </si>
-  <si>
-    <t xml:space="preserve">\GuyFawkes/ </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ＡＲ♦️Ｎｉｃｏ </t>
-  </si>
-  <si>
-    <t xml:space="preserve">tala </t>
-  </si>
-  <si>
-    <t xml:space="preserve">LATIN WARRIOR™ </t>
-  </si>
-  <si>
-    <t xml:space="preserve">AR♣️OMA </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ＡＲ♠️Ｆｅｄｅ </t>
-  </si>
-  <si>
-    <t xml:space="preserve">GaiaScienza </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lore_98 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">christian98 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">shinigami </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ＡＲ♠️Ɛ Ɩ ɪ Ơ </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Daniele </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Qliff </t>
-  </si>
-  <si>
-    <t xml:space="preserve">mrdeath75 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sandiokan </t>
-  </si>
-  <si>
-    <t xml:space="preserve">AR ♦️Goldenboy </t>
-  </si>
-  <si>
-    <t xml:space="preserve">crezyred </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ＡＲ♥️Ｍａｚｚｉｔｏ </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Geeno </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ＡＲ♣️Ｒｉｃｃａｌｓｏ </t>
-  </si>
-  <si>
-    <t xml:space="preserve">aleman(statale) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Damo </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ＡＲ♠️Ｏｘｈａｔｒｅｓ </t>
-  </si>
-  <si>
-    <t xml:space="preserve">DOCCC </t>
-  </si>
-  <si>
-    <t xml:space="preserve">bughy </t>
-  </si>
-  <si>
-    <t xml:space="preserve">bo </t>
-  </si>
-  <si>
-    <t xml:space="preserve">MARCHIO </t>
-  </si>
-  <si>
-    <t xml:space="preserve">BrokerTony </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ａｒ❤️Ｓａｍｕｅｌｅ </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ＡＲ ❤️ＡＬＥＸ </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ＡＲ♦️Ｅ＄ </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ＡＲ♦️Ｂｌａｚｏｒ１１１ </t>
-  </si>
-  <si>
-    <t xml:space="preserve">alabatia89 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Peppone91 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">sid </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Luigi13 </t>
-  </si>
-  <si>
     <t>HTL I EBDP</t>
   </si>
   <si>
-    <t xml:space="preserve">coraz </t>
-  </si>
-  <si>
     <t>@totino96</t>
   </si>
   <si>
@@ -1014,9 +867,6 @@
     <t>@Gaia951</t>
   </si>
   <si>
-    <t>@Balliver</t>
-  </si>
-  <si>
     <t>@Mannito92</t>
   </si>
   <si>
@@ -1026,9 +876,6 @@
     <t>@MerMet92</t>
   </si>
   <si>
-    <t>@T0N1003</t>
-  </si>
-  <si>
     <t>@ciuler</t>
   </si>
   <si>
@@ -1053,192 +900,12 @@
     <t>@srd_rce</t>
   </si>
   <si>
-    <t xml:space="preserve">Ahmed </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wolfdale </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cry </t>
-  </si>
-  <si>
-    <t xml:space="preserve">AR♠️alfone </t>
-  </si>
-  <si>
-    <t xml:space="preserve">YATO51 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Big </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Luca01 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cicciovolley91 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Meru </t>
-  </si>
-  <si>
-    <t xml:space="preserve">lord Tony </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nico </t>
-  </si>
-  <si>
-    <t xml:space="preserve">dani_lanc </t>
-  </si>
-  <si>
-    <t xml:space="preserve">khmer BM⚡️ </t>
-  </si>
-  <si>
-    <t xml:space="preserve">TexWiller </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ar♦️KingSupremo </t>
-  </si>
-  <si>
-    <t xml:space="preserve">vinz </t>
-  </si>
-  <si>
-    <t xml:space="preserve">⭐️Marco⭐️ </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ＡＲ❤️♣️ＧＯＤ９８♠️♦️ </t>
-  </si>
-  <si>
-    <t xml:space="preserve">AR♦️ᴍᴀᴛᴛᴇᴏ </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bombazza </t>
-  </si>
-  <si>
-    <t xml:space="preserve">●SUMATRA● </t>
-  </si>
-  <si>
-    <t xml:space="preserve">AnUbIs </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Arsenio </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Angeloxf7 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ＡＲ♣️Ｓｕｎｄｒｉｐｓ </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ＢＲ♠️ＤｏＮ </t>
-  </si>
-  <si>
-    <t xml:space="preserve">nevio lostirato </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lubbro95 C.B. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">lil_wally </t>
-  </si>
-  <si>
-    <t xml:space="preserve">pro </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zokum </t>
-  </si>
-  <si>
-    <t xml:space="preserve">⚡️MAJOR⚡️ </t>
-  </si>
-  <si>
-    <t xml:space="preserve">superfede </t>
-  </si>
-  <si>
-    <t xml:space="preserve">sebabigo </t>
-  </si>
-  <si>
-    <t xml:space="preserve">OneLeggedJack </t>
-  </si>
-  <si>
-    <t xml:space="preserve">•fury™• </t>
-  </si>
-  <si>
-    <t xml:space="preserve">random guy </t>
-  </si>
-  <si>
-    <t xml:space="preserve">frankye73 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zumpy </t>
-  </si>
-  <si>
-    <t xml:space="preserve">REMIDA </t>
-  </si>
-  <si>
-    <t xml:space="preserve">kingmike </t>
-  </si>
-  <si>
-    <t xml:space="preserve">orso86 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lore </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eric </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Just_Dodo </t>
-  </si>
-  <si>
-    <t xml:space="preserve">DonPunta </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dino </t>
-  </si>
-  <si>
-    <t xml:space="preserve">teo </t>
-  </si>
-  <si>
-    <t xml:space="preserve">NIMBLE MONGOOSE </t>
-  </si>
-  <si>
     <t>ＡＲ♠️ｓｐｅｚｉａ</t>
   </si>
   <si>
-    <t xml:space="preserve">Raffaele11 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fogu </t>
-  </si>
-  <si>
-    <t xml:space="preserve">manuel1903 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">BwonE </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Basco </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spartaco1966 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Two ciamela </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fabrizio </t>
-  </si>
-  <si>
-    <t xml:space="preserve">El Gladiator </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Frenci </t>
-  </si>
-  <si>
     <t>@sunnering</t>
   </si>
   <si>
-    <t>@X_teo</t>
-  </si>
-  <si>
     <t>@mangusta_agile</t>
   </si>
   <si>
@@ -1254,91 +921,130 @@
     <t>@Basco3</t>
   </si>
   <si>
-    <t>@ag0_96</t>
-  </si>
-  <si>
-    <t>@Giggi_A</t>
-  </si>
-  <si>
-    <t>@Fabrizio2418</t>
-  </si>
-  <si>
-    <t>@Marcotghy</t>
-  </si>
-  <si>
     <t>@Cisco00001</t>
   </si>
   <si>
-    <t>Dog Rider</t>
-  </si>
-  <si>
-    <t>Zenel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Torsiz </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Enriic </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Quizzz </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pinguino </t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;c5&gt;0hAnd4 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">tiau </t>
-  </si>
-  <si>
-    <t>simosuper</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RETROWAV3R™️ </t>
-  </si>
-  <si>
     <t>@Torsiz007</t>
   </si>
   <si>
-    <t>@BACWasTaken</t>
-  </si>
-  <si>
     <t>@RETROWAV3R</t>
   </si>
   <si>
-    <t xml:space="preserve">ＡＲ❤️ｉＳＡＭｕ </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ＡＲ♣️Ｃｉｃｃｉｏ </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ＡＲ♦️道路軍Wåyne </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ａ Ｒ ♠️ ＦＥＤＥＲＩＣＯ </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ＡＲ♠️＠ｌｅｍａｎ </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thor ⚡️ </t>
-  </si>
-  <si>
-    <t>@Lokkah</t>
-  </si>
-  <si>
-    <t>@robu99</t>
-  </si>
-  <si>
-    <t>Robu</t>
-  </si>
-  <si>
     <t>Christian</t>
   </si>
   <si>
     <t>@Christian00007</t>
+  </si>
+  <si>
+    <t>@sorridetemi</t>
+  </si>
+  <si>
+    <t>@Fox_0265</t>
+  </si>
+  <si>
+    <t>@Davidone11</t>
+  </si>
+  <si>
+    <t>&lt;c5&gt;0hAnd4</t>
+  </si>
+  <si>
+    <t>Antonio96</t>
+  </si>
+  <si>
+    <t>arKaiba❤️Sparky</t>
+  </si>
+  <si>
+    <t>Cry</t>
+  </si>
+  <si>
+    <t>Eric</t>
+  </si>
+  <si>
+    <t>frenci</t>
+  </si>
+  <si>
+    <t>Lore</t>
+  </si>
+  <si>
+    <t>Luca01</t>
+  </si>
+  <si>
+    <t>manuel1903</t>
+  </si>
+  <si>
+    <t>Mr.Fox</t>
+  </si>
+  <si>
+    <t>NIMBLE MONGOOSE</t>
+  </si>
+  <si>
+    <t>RETROWAV3R™️</t>
+  </si>
+  <si>
+    <t>Royal Army</t>
+  </si>
+  <si>
+    <t>superfede</t>
+  </si>
+  <si>
+    <t>tiau</t>
+  </si>
+  <si>
+    <t>Zumpy</t>
+  </si>
+  <si>
+    <t>I Tori Feroci</t>
+  </si>
+  <si>
+    <t>Si</t>
+  </si>
+  <si>
+    <t>@cvbalibre</t>
+  </si>
+  <si>
+    <t>@Robu99</t>
+  </si>
+  <si>
+    <t>Ａ Ｒ ♠️ ＦＥＤＥＲＩＣＯ</t>
+  </si>
+  <si>
+    <t>GaiaScienza</t>
+  </si>
+  <si>
+    <t>AR♣️Cuba</t>
+  </si>
+  <si>
+    <t>Torsiz</t>
+  </si>
+  <si>
+    <t>Meru</t>
+  </si>
+  <si>
+    <t>_SINA22_</t>
+  </si>
+  <si>
+    <t>Dino</t>
+  </si>
+  <si>
+    <t>Geeno</t>
+  </si>
+  <si>
+    <t>●SUMATRA●</t>
+  </si>
+  <si>
+    <t>Cicciovolley91</t>
+  </si>
+  <si>
+    <t>BwonE</t>
+  </si>
+  <si>
+    <t>Basco</t>
+  </si>
+  <si>
+    <t>khmer BM⚡</t>
+  </si>
+  <si>
+    <t>\GuyFawkes/</t>
   </si>
 </sst>
 </file>
@@ -2202,10 +1908,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EE2B0F9-AC31-464B-B046-53CB033C8615}">
-  <dimension ref="A1:D125"/>
+  <dimension ref="A1:D100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2233,1728 +1939,1387 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>93</v>
+        <v>130</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>343</v>
+        <v>303</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>411</v>
+        <v>319</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>161</v>
+        <v>320</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>332</v>
+        <v>127</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>359</v>
+        <v>251</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>411</v>
+        <v>319</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>161</v>
+        <v>320</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>118</v>
+        <v>285</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>350</v>
+        <v>105</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>411</v>
+        <v>319</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>161</v>
+        <v>320</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>54</v>
+        <v>95</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>352</v>
+        <v>94</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>411</v>
+        <v>319</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>161</v>
+        <v>320</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>70</v>
+        <v>274</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>383</v>
+        <v>304</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>411</v>
+        <v>319</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>161</v>
+        <v>320</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>52</v>
+        <v>102</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>344</v>
+        <v>101</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>411</v>
+        <v>319</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>161</v>
+        <v>320</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>399</v>
-      </c>
       <c r="B8" s="1" t="s">
-        <v>385</v>
+        <v>288</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>411</v>
+        <v>319</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>161</v>
+        <v>320</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>367</v>
+        <v>253</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>411</v>
+        <v>319</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>161</v>
+        <v>320</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>98</v>
+        <v>78</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>362</v>
+        <v>77</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>411</v>
+        <v>319</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>161</v>
+        <v>320</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>333</v>
+        <v>300</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>361</v>
+        <v>305</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>411</v>
+        <v>319</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>161</v>
+        <v>320</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>58</v>
+        <v>282</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>368</v>
+        <v>64</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>411</v>
+        <v>319</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>161</v>
+        <v>320</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>85</v>
+        <v>119</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>287</v>
+        <v>118</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>411</v>
+        <v>319</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>161</v>
+        <v>320</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>83</v>
+        <v>299</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>366</v>
+        <v>298</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>411</v>
+        <v>319</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>161</v>
+        <v>320</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>152</v>
+        <v>49</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>364</v>
+        <v>48</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>411</v>
+        <v>319</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>161</v>
+        <v>320</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>103</v>
+        <v>264</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>355</v>
+        <v>215</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>411</v>
+        <v>319</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>161</v>
+        <v>320</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>94</v>
+        <v>277</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>365</v>
+        <v>306</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>411</v>
+        <v>319</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>161</v>
+        <v>320</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>400</v>
+        <v>115</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>386</v>
+        <v>114</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>411</v>
+        <v>319</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>161</v>
+        <v>320</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>124</v>
+        <v>263</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>363</v>
+        <v>260</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>411</v>
+        <v>319</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>161</v>
+        <v>320</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>102</v>
+        <v>72</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>356</v>
+        <v>71</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>411</v>
+        <v>319</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>161</v>
+        <v>320</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>327</v>
+        <v>287</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>341</v>
+        <v>307</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>411</v>
+        <v>319</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>161</v>
+        <v>320</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>268</v>
+        <v>295</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>284</v>
+        <v>308</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>411</v>
+        <v>319</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>161</v>
+        <v>320</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>369</v>
+        <v>67</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>411</v>
+        <v>319</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>161</v>
+        <v>320</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>82</v>
+        <v>113</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>380</v>
+        <v>112</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>411</v>
+        <v>319</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>161</v>
+        <v>320</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>56</v>
+        <v>269</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>320</v>
+        <v>255</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>411</v>
+        <v>319</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>161</v>
+        <v>320</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>272</v>
+        <v>122</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>372</v>
+        <v>139</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>411</v>
+        <v>319</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>161</v>
+        <v>320</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>111</v>
+        <v>266</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>303</v>
+        <v>247</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>411</v>
+        <v>319</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>161</v>
+        <v>320</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>130</v>
+        <v>286</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>370</v>
+        <v>309</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>411</v>
+        <v>319</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>161</v>
+        <v>320</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>334</v>
+        <v>81</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>371</v>
+        <v>88</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>411</v>
+        <v>319</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>161</v>
+        <v>320</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>137</v>
+        <v>278</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>354</v>
+        <v>310</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>411</v>
+        <v>319</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>161</v>
+        <v>320</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>96</v>
+        <v>55</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>342</v>
+        <v>54</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>411</v>
+        <v>319</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>161</v>
+        <v>320</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>401</v>
+        <v>292</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>387</v>
+        <v>311</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>411</v>
+        <v>319</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>161</v>
+        <v>320</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
+        <v>301</v>
+      </c>
       <c r="B33" s="1" t="s">
-        <v>388</v>
+        <v>312</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>411</v>
+        <v>319</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>161</v>
+        <v>320</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>43</v>
+        <v>91</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>389</v>
+        <v>138</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>411</v>
+        <v>319</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>161</v>
+        <v>320</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>402</v>
+        <v>290</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>390</v>
+        <v>313</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>411</v>
+        <v>319</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>161</v>
+        <v>320</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>403</v>
+        <v>284</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>391</v>
+        <v>69</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>411</v>
+        <v>319</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>161</v>
+        <v>320</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
-        <v>404</v>
+        <v>80</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>392</v>
+        <v>79</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>411</v>
+        <v>319</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>161</v>
+        <v>320</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>405</v>
+        <v>111</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>393</v>
+        <v>110</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>411</v>
+        <v>319</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>161</v>
+        <v>320</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
-        <v>406</v>
+        <v>57</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>394</v>
+        <v>56</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>411</v>
+        <v>319</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>161</v>
+        <v>320</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
-        <v>407</v>
+        <v>60</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>395</v>
+        <v>87</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>411</v>
+        <v>319</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>161</v>
+        <v>320</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
-        <v>408</v>
+        <v>126</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>396</v>
+        <v>125</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>411</v>
+        <v>319</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>161</v>
+        <v>320</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
-        <v>409</v>
+        <v>297</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>397</v>
+        <v>314</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>411</v>
+        <v>319</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>161</v>
+        <v>320</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
-        <v>410</v>
+        <v>302</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>398</v>
+        <v>315</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>411</v>
+        <v>319</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>161</v>
+        <v>320</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
-        <v>434</v>
+        <v>267</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>433</v>
+        <v>248</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>411</v>
+        <v>319</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>161</v>
+        <v>320</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
-        <v>324</v>
+        <v>137</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>279</v>
+        <v>136</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>91</v>
+        <v>319</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>161</v>
+        <v>320</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
-        <v>323</v>
+        <v>117</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>278</v>
+        <v>116</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>91</v>
+        <v>319</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>161</v>
+        <v>320</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47" s="1" t="s">
+        <v>283</v>
+      </c>
       <c r="B47" s="1" t="s">
-        <v>412</v>
+        <v>316</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>91</v>
+        <v>319</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>161</v>
+        <v>320</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
-        <v>421</v>
+        <v>53</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>413</v>
+        <v>52</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>91</v>
+        <v>319</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>161</v>
+        <v>320</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
-        <v>122</v>
+        <v>291</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>280</v>
+        <v>317</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>91</v>
+        <v>319</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>161</v>
+        <v>320</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
-        <v>329</v>
+        <v>134</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>347</v>
+        <v>133</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>91</v>
+        <v>319</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>161</v>
+        <v>320</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
-        <v>328</v>
+        <v>271</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>345</v>
+        <v>258</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>91</v>
+        <v>319</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>161</v>
+        <v>320</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
-        <v>120</v>
+        <v>90</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>281</v>
+        <v>89</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>91</v>
+        <v>319</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>161</v>
+        <v>320</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
-        <v>116</v>
+        <v>76</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>282</v>
+        <v>75</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>91</v>
+        <v>319</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>161</v>
+        <v>320</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
-        <v>63</v>
+        <v>265</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>349</v>
+        <v>318</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>91</v>
+        <v>319</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>161</v>
+        <v>320</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
-        <v>326</v>
+        <v>11</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>307</v>
+        <v>323</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>91</v>
+        <v>3</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>161</v>
+        <v>320</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
-        <v>331</v>
+        <v>155</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>351</v>
+        <v>152</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>91</v>
+        <v>3</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>161</v>
+        <v>320</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>339</v>
+        <v>46</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>91</v>
+        <v>3</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>161</v>
+        <v>320</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
-        <v>110</v>
+        <v>5</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>283</v>
+        <v>9</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>91</v>
+        <v>3</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>161</v>
+        <v>320</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
-        <v>277</v>
+        <v>156</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>285</v>
+        <v>153</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>91</v>
+        <v>3</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>161</v>
+        <v>320</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
-        <v>131</v>
+        <v>13</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>286</v>
+        <v>12</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>91</v>
+        <v>3</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>161</v>
+        <v>320</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
-        <v>88</v>
+        <v>15</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>346</v>
+        <v>14</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>91</v>
+        <v>3</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>161</v>
+        <v>320</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
-        <v>127</v>
+        <v>17</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>414</v>
+        <v>16</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>91</v>
+        <v>3</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>161</v>
+        <v>320</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
-        <v>105</v>
+        <v>19</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>360</v>
+        <v>18</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>91</v>
+        <v>3</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>161</v>
+        <v>320</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
-        <v>125</v>
+        <v>85</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>288</v>
+        <v>84</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>91</v>
+        <v>3</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>161</v>
+        <v>320</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
-        <v>269</v>
+        <v>21</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>322</v>
+        <v>20</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>91</v>
+        <v>3</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>161</v>
+        <v>320</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
-        <v>76</v>
+        <v>22</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>376</v>
+        <v>198</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>91</v>
+        <v>3</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>161</v>
+        <v>320</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
-        <v>74</v>
+        <v>24</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>384</v>
+        <v>23</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>91</v>
+        <v>3</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>161</v>
+        <v>320</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
-        <v>274</v>
+        <v>26</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>379</v>
+        <v>25</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>91</v>
+        <v>3</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>161</v>
+        <v>320</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
-        <v>422</v>
+        <v>28</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>415</v>
+        <v>27</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>91</v>
+        <v>3</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>161</v>
+        <v>320</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
-        <v>68</v>
+        <v>30</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>358</v>
+        <v>29</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>91</v>
+        <v>3</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>161</v>
+        <v>320</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
-        <v>336</v>
+        <v>32</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>374</v>
+        <v>31</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>91</v>
+        <v>3</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>161</v>
+        <v>320</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
-        <v>61</v>
+        <v>34</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>375</v>
+        <v>33</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>91</v>
+        <v>3</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>161</v>
+        <v>320</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
-        <v>337</v>
+        <v>132</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>381</v>
+        <v>131</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>91</v>
+        <v>3</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>161</v>
+        <v>320</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
-        <v>335</v>
+        <v>276</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>373</v>
+        <v>324</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>91</v>
+        <v>3</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>161</v>
+        <v>320</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A75" s="1" t="s">
-        <v>270</v>
-      </c>
       <c r="B75" s="1" t="s">
-        <v>377</v>
+        <v>273</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>91</v>
+        <v>3</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>161</v>
+        <v>320</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
-        <v>50</v>
+        <v>97</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>293</v>
+        <v>96</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>91</v>
+        <v>3</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>161</v>
+        <v>320</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
-        <v>129</v>
+        <v>38</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>378</v>
+        <v>37</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>91</v>
+        <v>3</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>161</v>
+        <v>320</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>357</v>
+        <v>39</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>91</v>
+        <v>3</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>161</v>
+        <v>320</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
-        <v>114</v>
+        <v>42</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>416</v>
+        <v>41</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>91</v>
+        <v>3</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>161</v>
+        <v>320</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
-        <v>276</v>
+        <v>44</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>340</v>
+        <v>43</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>91</v>
+        <v>3</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>161</v>
+        <v>320</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
-        <v>338</v>
+        <v>154</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>382</v>
+        <v>149</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>91</v>
+        <v>3</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>161</v>
+        <v>320</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
-        <v>139</v>
+        <v>321</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>317</v>
+        <v>325</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>91</v>
+        <v>3</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>161</v>
+        <v>320</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
-        <v>133</v>
+        <v>296</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>417</v>
+        <v>326</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>91</v>
+        <v>3</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>161</v>
+        <v>320</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
-        <v>141</v>
+        <v>279</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>319</v>
+        <v>327</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>91</v>
+        <v>3</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>161</v>
+        <v>320</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
-        <v>402</v>
+        <v>275</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>418</v>
+        <v>328</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>91</v>
+        <v>3</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>161</v>
+        <v>320</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A86" s="1" t="s">
+        <v>289</v>
+      </c>
       <c r="B86" s="1" t="s">
-        <v>147</v>
+        <v>329</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>91</v>
+        <v>3</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>161</v>
+        <v>320</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A87" s="1" t="s">
+        <v>108</v>
+      </c>
       <c r="B87" s="1" t="s">
-        <v>419</v>
+        <v>330</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>91</v>
+        <v>3</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>161</v>
+        <v>320</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="s">
-        <v>403</v>
+        <v>281</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>391</v>
+        <v>331</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>91</v>
+        <v>3</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>161</v>
+        <v>320</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
-        <v>273</v>
+        <v>322</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>353</v>
+        <v>45</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>91</v>
+        <v>3</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>161</v>
+        <v>320</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
-        <v>423</v>
+        <v>66</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>420</v>
+        <v>65</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>91</v>
+        <v>3</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>161</v>
+        <v>320</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
-        <v>431</v>
+        <v>86</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>432</v>
+        <v>332</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>91</v>
+        <v>3</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>161</v>
+        <v>320</v>
       </c>
     </row>
     <row r="92" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="s">
-        <v>12</v>
+        <v>293</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>294</v>
+        <v>333</v>
       </c>
       <c r="C92" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>161</v>
+        <v>320</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
-        <v>12</v>
+        <v>294</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>290</v>
+        <v>334</v>
       </c>
       <c r="C93" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>161</v>
+        <v>320</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="s">
-        <v>430</v>
+        <v>83</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>424</v>
+        <v>82</v>
       </c>
       <c r="C94" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>161</v>
+        <v>320</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="s">
-        <v>14</v>
+        <v>51</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>289</v>
+        <v>50</v>
       </c>
       <c r="C95" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>161</v>
+        <v>320</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="s">
-        <v>10</v>
+        <v>121</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>295</v>
+        <v>120</v>
       </c>
       <c r="C96" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>161</v>
+        <v>320</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97" s="1" t="s">
-        <v>325</v>
+        <v>107</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>291</v>
+        <v>106</v>
       </c>
       <c r="C97" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>161</v>
+        <v>320</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="s">
-        <v>45</v>
+        <v>7</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>297</v>
+        <v>6</v>
       </c>
       <c r="C98" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>161</v>
+        <v>320</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
-        <v>41</v>
+        <v>280</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>298</v>
+        <v>335</v>
       </c>
       <c r="C99" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>161</v>
+        <v>320</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="s">
-        <v>100</v>
+        <v>272</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>292</v>
+        <v>336</v>
       </c>
       <c r="C100" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A101" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B101" s="1" t="s">
-        <v>296</v>
-      </c>
-      <c r="C101" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D101" s="1" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A102" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B102" s="1" t="s">
-        <v>301</v>
-      </c>
-      <c r="C102" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D102" s="1" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A103" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B103" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="C103" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D103" s="1" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A104" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B104" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="C104" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D104" s="1" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A105" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B105" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="C105" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D105" s="1" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A106" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="B106" s="1" t="s">
-        <v>299</v>
-      </c>
-      <c r="C106" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D106" s="1" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A107" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B107" s="1" t="s">
-        <v>310</v>
-      </c>
-      <c r="C107" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D107" s="1" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A108" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B108" s="1" t="s">
-        <v>302</v>
-      </c>
-      <c r="C108" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D108" s="1" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A109" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="B109" s="1" t="s">
-        <v>425</v>
-      </c>
-      <c r="C109" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D109" s="1" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A110" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B110" s="1" t="s">
-        <v>305</v>
-      </c>
-      <c r="C110" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D110" s="1" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A111" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="B111" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="C111" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D111" s="1" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A112" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="B112" s="1" t="s">
-        <v>308</v>
-      </c>
-      <c r="C112" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D112" s="1" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A113" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B113" s="1" t="s">
-        <v>313</v>
-      </c>
-      <c r="C113" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D113" s="1" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A114" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="B114" s="1" t="s">
-        <v>315</v>
-      </c>
-      <c r="C114" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D114" s="1" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A115" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B115" s="1" t="s">
-        <v>311</v>
-      </c>
-      <c r="C115" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D115" s="1" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A116" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B116" s="1" t="s">
-        <v>426</v>
-      </c>
-      <c r="C116" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D116" s="1" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A117" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B117" s="1" t="s">
-        <v>314</v>
-      </c>
-      <c r="C117" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D117" s="1" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A118" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B118" s="1" t="s">
-        <v>316</v>
-      </c>
-      <c r="C118" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D118" s="1" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A119" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B119" s="1" t="s">
-        <v>312</v>
-      </c>
-      <c r="C119" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D119" s="1" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A120" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B120" s="1" t="s">
-        <v>427</v>
-      </c>
-      <c r="C120" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D120" s="1" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A121" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B121" s="1" t="s">
-        <v>428</v>
-      </c>
-      <c r="C121" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D121" s="1" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A122" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B122" s="1" t="s">
-        <v>429</v>
-      </c>
-      <c r="C122" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D122" s="1" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A123" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B123" s="1" t="s">
-        <v>318</v>
-      </c>
-      <c r="C123" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D123" s="1" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B124" s="1" t="s">
-        <v>321</v>
-      </c>
-      <c r="C124" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D124" s="1" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A125" s="1" t="s">
-        <v>330</v>
-      </c>
-      <c r="B125" s="1" t="s">
-        <v>348</v>
-      </c>
-      <c r="C125" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D125" s="1" t="s">
-        <v>161</v>
+        <v>320</v>
       </c>
     </row>
   </sheetData>
@@ -3986,23 +3351,23 @@
         <v>1</v>
       </c>
       <c r="F4" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="H4" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="I4" t="str">
         <f t="shared" ref="I4:I51" si="0">_xlfn.CONCAT(H4:H4)</f>
         <v>elioo_06</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="Q4" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="R4" s="1" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="S4" t="str">
         <f>_xlfn.CONCAT(Q4:R4)</f>
@@ -4015,23 +3380,23 @@
       </c>
       <c r="E5" s="1"/>
       <c r="F5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H5" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="I5" t="str">
         <f t="shared" si="0"/>
         <v>Blazor111</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="Q5" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="R5" s="1" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="S5" t="str">
         <f t="shared" ref="S5:S53" si="1">_xlfn.CONCAT(Q5:R5)</f>
@@ -4047,20 +3412,20 @@
         <v>4</v>
       </c>
       <c r="H6" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="I6" t="str">
         <f t="shared" si="0"/>
         <v>aleman7273</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="Q6" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="R6" s="1" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="S6" t="str">
         <f t="shared" si="1"/>
@@ -4076,20 +3441,20 @@
         <v>9</v>
       </c>
       <c r="H7" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="I7" t="str">
         <f t="shared" si="0"/>
         <v>aleman7273</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="Q7" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="R7" s="1" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="S7" t="str">
         <f t="shared" si="1"/>
@@ -4102,23 +3467,23 @@
       </c>
       <c r="E8" s="1"/>
       <c r="F8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H8" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="I8" t="str">
         <f t="shared" si="0"/>
         <v>FORTEX09</v>
       </c>
       <c r="P8" s="1" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="Q8" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="R8" s="1" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="S8" t="str">
         <f t="shared" si="1"/>
@@ -4131,23 +3496,23 @@
       </c>
       <c r="E9" s="1"/>
       <c r="F9" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="H9" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="I9" t="str">
         <f t="shared" si="0"/>
         <v>BuldzS</v>
       </c>
       <c r="P9" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="Q9" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="R9" s="1" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="S9" t="str">
         <f t="shared" si="1"/>
@@ -4160,23 +3525,23 @@
       </c>
       <c r="E10" s="1"/>
       <c r="F10" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="H10" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="I10" t="str">
         <f t="shared" si="0"/>
         <v>Alestrega22</v>
       </c>
       <c r="P10" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="Q10" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="R10" s="1" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="S10" t="str">
         <f t="shared" si="1"/>
@@ -4189,23 +3554,23 @@
       </c>
       <c r="E11" s="1"/>
       <c r="F11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H11" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="I11" t="str">
         <f t="shared" si="0"/>
         <v>Ale_Mare93</v>
       </c>
       <c r="P11" s="1" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="Q11" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="R11" s="1" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="S11" t="str">
         <f t="shared" si="1"/>
@@ -4218,23 +3583,23 @@
       </c>
       <c r="E12" s="1"/>
       <c r="F12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H12" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="I12" t="str">
         <f t="shared" si="0"/>
         <v>Romas10</v>
       </c>
       <c r="P12" s="1" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="Q12" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="R12" s="1" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="S12" t="str">
         <f t="shared" si="1"/>
@@ -4247,23 +3612,23 @@
       </c>
       <c r="E13" s="1"/>
       <c r="F13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I13" t="str">
         <f t="shared" si="0"/>
         <v>crezyred</v>
       </c>
       <c r="P13" s="1" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="Q13" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="R13" s="1" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="S13" t="str">
         <f t="shared" si="1"/>
@@ -4276,23 +3641,23 @@
       </c>
       <c r="E14" s="1"/>
       <c r="F14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H14" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="I14" t="str">
         <f t="shared" si="0"/>
         <v>DaMoops</v>
       </c>
       <c r="P14" s="1" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="Q14" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="R14" s="1" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="S14" t="str">
         <f t="shared" si="1"/>
@@ -4305,23 +3670,23 @@
       </c>
       <c r="E15" s="1"/>
       <c r="F15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H15" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="I15" t="str">
         <f t="shared" si="0"/>
         <v>Robu99</v>
       </c>
       <c r="P15" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="Q15" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="R15" s="1" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="S15" t="str">
         <f t="shared" si="1"/>
@@ -4334,23 +3699,23 @@
       </c>
       <c r="E16" s="1"/>
       <c r="F16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H16" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="I16" t="str">
         <f t="shared" si="0"/>
         <v>Punk_ake</v>
       </c>
       <c r="P16" s="1" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="Q16" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="R16" s="1" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="S16" t="str">
         <f t="shared" si="1"/>
@@ -4363,23 +3728,23 @@
       </c>
       <c r="E17" s="1"/>
       <c r="F17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H17" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="I17" t="str">
         <f t="shared" si="0"/>
         <v>Marchio04</v>
       </c>
       <c r="P17" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q17" t="s">
         <v>59</v>
       </c>
-      <c r="Q17" t="s">
-        <v>60</v>
-      </c>
       <c r="R17" s="1" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="S17" t="str">
         <f t="shared" si="1"/>
@@ -4392,20 +3757,20 @@
       </c>
       <c r="E18" s="1"/>
       <c r="F18" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="I18" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="P18" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q18" t="s">
         <v>55</v>
       </c>
-      <c r="Q18" t="s">
-        <v>56</v>
-      </c>
       <c r="R18" s="1" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="S18" t="str">
         <f t="shared" si="1"/>
@@ -4418,23 +3783,23 @@
       </c>
       <c r="E19" s="1"/>
       <c r="F19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H19" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="I19" t="str">
         <f t="shared" si="0"/>
         <v>riccalso</v>
       </c>
       <c r="P19" s="1" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="Q19" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="R19" s="1" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="S19" t="str">
         <f t="shared" si="1"/>
@@ -4447,23 +3812,23 @@
       </c>
       <c r="E20" s="1"/>
       <c r="F20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H20" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="I20" t="str">
         <f t="shared" si="0"/>
         <v>BO_CRL</v>
       </c>
       <c r="P20" s="1" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="Q20" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="R20" s="1" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="S20" t="str">
         <f t="shared" si="1"/>
@@ -4476,23 +3841,23 @@
       </c>
       <c r="E21" s="1"/>
       <c r="F21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I21" t="str">
         <f t="shared" si="0"/>
         <v>BrokerTony</v>
       </c>
       <c r="P21" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q21" t="s">
         <v>53</v>
       </c>
-      <c r="Q21" t="s">
-        <v>54</v>
-      </c>
       <c r="R21" s="1" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="S21" t="str">
         <f t="shared" si="1"/>
@@ -4505,23 +3870,23 @@
       </c>
       <c r="E22" s="1"/>
       <c r="F22" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H22" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="I22" t="str">
         <f t="shared" si="0"/>
         <v>Mazzito</v>
       </c>
       <c r="P22" s="1" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="Q22" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="R22" s="1" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="S22" t="str">
         <f t="shared" si="1"/>
@@ -4534,23 +3899,23 @@
       </c>
       <c r="E23" s="1"/>
       <c r="F23" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="H23" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="I23" t="str">
         <f t="shared" si="0"/>
         <v>NicoSkev98</v>
       </c>
       <c r="P23" s="1" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="Q23" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="R23" s="1" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="S23" t="str">
         <f t="shared" si="1"/>
@@ -4563,23 +3928,23 @@
       </c>
       <c r="E24" s="1"/>
       <c r="F24" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="H24" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="I24" t="str">
         <f t="shared" si="0"/>
         <v>pietro_actis</v>
       </c>
       <c r="P24" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="Q24" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="R24" s="1" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="S24" t="str">
         <f t="shared" si="1"/>
@@ -4592,23 +3957,23 @@
       </c>
       <c r="E25" s="1"/>
       <c r="F25" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H25" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I25" t="str">
         <f t="shared" si="0"/>
         <v>mrdeath75</v>
       </c>
       <c r="P25" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q25" t="s">
         <v>57</v>
       </c>
-      <c r="Q25" t="s">
-        <v>58</v>
-      </c>
       <c r="R25" s="1" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="S25" t="str">
         <f t="shared" si="1"/>
@@ -4624,20 +3989,20 @@
         <v>6</v>
       </c>
       <c r="H26" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="I26" t="str">
         <f t="shared" si="0"/>
         <v>Ahmed_Eliow</v>
       </c>
       <c r="P26" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="Q26" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="R26" s="1" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="S26" t="str">
         <f t="shared" si="1"/>
@@ -4650,23 +4015,23 @@
       </c>
       <c r="E27" s="1"/>
       <c r="F27" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H27" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="I27" t="str">
         <f t="shared" si="0"/>
         <v>Madara_2912</v>
       </c>
       <c r="P27" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="Q27" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="R27" s="1" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="S27" t="str">
         <f t="shared" si="1"/>
@@ -4679,23 +4044,23 @@
       </c>
       <c r="E28" s="1"/>
       <c r="F28" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H28" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="I28" t="str">
         <f t="shared" si="0"/>
         <v>ArBughy</v>
       </c>
       <c r="P28" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="Q28" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="R28" s="1" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="S28" t="str">
         <f t="shared" si="1"/>
@@ -4708,23 +4073,23 @@
       </c>
       <c r="E29" s="1"/>
       <c r="F29" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="H29" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="I29" t="str">
         <f t="shared" si="0"/>
         <v>Tanjim041</v>
       </c>
       <c r="P29" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="Q29" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="R29" s="1" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="S29" t="str">
         <f t="shared" si="1"/>
@@ -4737,23 +4102,23 @@
       </c>
       <c r="E30" s="1"/>
       <c r="F30" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H30" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="I30" t="str">
         <f t="shared" si="0"/>
         <v>Sz66603</v>
       </c>
       <c r="P30" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q30" t="s">
         <v>49</v>
       </c>
-      <c r="Q30" t="s">
-        <v>50</v>
-      </c>
       <c r="R30" s="1" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="S30" t="str">
         <f t="shared" si="1"/>
@@ -4766,23 +4131,23 @@
       </c>
       <c r="E31" s="1"/>
       <c r="F31" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="H31" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="I31" t="str">
         <f t="shared" si="0"/>
         <v>ralfone01</v>
       </c>
       <c r="P31" s="1" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="Q31" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="R31" s="1" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="S31" t="str">
         <f t="shared" si="1"/>
@@ -4795,23 +4160,23 @@
       </c>
       <c r="E32" s="1"/>
       <c r="F32" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H32" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="I32" t="str">
         <f t="shared" si="0"/>
         <v>yvngdanyy</v>
       </c>
       <c r="P32" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="Q32" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="R32" s="1" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="S32" t="str">
         <f t="shared" si="1"/>
@@ -4824,23 +4189,23 @@
       </c>
       <c r="E33" s="1"/>
       <c r="F33" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H33" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="I33" t="str">
         <f t="shared" si="0"/>
         <v>rkomi99</v>
       </c>
       <c r="P33" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="Q33" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="R33" s="1" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="S33" t="str">
         <f t="shared" si="1"/>
@@ -4853,23 +4218,23 @@
       </c>
       <c r="E34" s="1"/>
       <c r="F34" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="H34" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="I34" t="str">
         <f t="shared" si="0"/>
         <v>sunnering41</v>
       </c>
       <c r="P34" s="1" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="Q34" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="R34" s="1" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="S34" t="str">
         <f t="shared" si="1"/>
@@ -4882,23 +4247,23 @@
       </c>
       <c r="E35" s="1"/>
       <c r="F35" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="H35" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="I35" t="str">
         <f t="shared" si="0"/>
         <v>alabatia89</v>
       </c>
       <c r="P35" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q35" t="s">
         <v>51</v>
       </c>
-      <c r="Q35" t="s">
-        <v>52</v>
-      </c>
       <c r="R35" s="1" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="S35" t="str">
         <f t="shared" si="1"/>
@@ -4911,23 +4276,23 @@
       </c>
       <c r="E36" s="1"/>
       <c r="F36" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="H36" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="I36" t="str">
         <f t="shared" si="0"/>
         <v>asso_nr</v>
       </c>
       <c r="P36" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="Q36" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="R36" s="1" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="S36" t="str">
         <f t="shared" si="1"/>
@@ -4940,23 +4305,23 @@
       </c>
       <c r="E37" s="1"/>
       <c r="F37" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H37" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="I37" t="str">
         <f t="shared" si="0"/>
         <v>PepponeB91</v>
       </c>
       <c r="P37" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="Q37" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="R37" s="1" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="S37" t="str">
         <f t="shared" si="1"/>
@@ -4969,23 +4334,23 @@
       </c>
       <c r="E38" s="1"/>
       <c r="F38" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="H38" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="I38" t="str">
         <f t="shared" si="0"/>
         <v>OhAnd4</v>
       </c>
       <c r="P38" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="Q38" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="R38" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="S38" t="str">
         <f t="shared" si="1"/>
@@ -4998,23 +4363,23 @@
       </c>
       <c r="E39" s="1"/>
       <c r="F39" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="H39" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="I39" t="str">
         <f t="shared" si="0"/>
         <v>Lilyan51</v>
       </c>
       <c r="P39" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="Q39" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="R39" s="1" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="S39" t="str">
         <f t="shared" si="1"/>
@@ -5026,23 +4391,23 @@
         <v>38</v>
       </c>
       <c r="F40" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="H40" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="I40" t="str">
         <f t="shared" si="0"/>
         <v>K3kk07</v>
       </c>
       <c r="P40" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="Q40" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="R40" s="1" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="S40" t="str">
         <f t="shared" si="1"/>
@@ -5054,23 +4419,23 @@
         <v>39</v>
       </c>
       <c r="F41" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="H41" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="I41" t="str">
         <f t="shared" si="0"/>
         <v>Mastrolivo</v>
       </c>
       <c r="P41" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="Q41" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="R41" s="1" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="S41" t="str">
         <f t="shared" si="1"/>
@@ -5082,23 +4447,23 @@
         <v>40</v>
       </c>
       <c r="F42" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="H42" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="I42" t="str">
         <f t="shared" si="0"/>
         <v>Sibinpopzz</v>
       </c>
       <c r="P42" s="1" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="Q42" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="R42" s="1" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="S42" t="str">
         <f t="shared" si="1"/>
@@ -5110,23 +4475,23 @@
         <v>41</v>
       </c>
       <c r="F43" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H43" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="I43" t="str">
         <f t="shared" si="0"/>
         <v>FedericoBello03</v>
       </c>
       <c r="P43" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="Q43" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="R43" s="1" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="S43" t="str">
         <f t="shared" si="1"/>
@@ -5138,23 +4503,23 @@
         <v>42</v>
       </c>
       <c r="F44" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="H44" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="I44" t="str">
         <f t="shared" si="0"/>
         <v>BACWasTaken</v>
       </c>
       <c r="P44" s="1" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="Q44" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="R44" s="1" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="S44" t="str">
         <f t="shared" si="1"/>
@@ -5166,20 +4531,20 @@
         <v>43</v>
       </c>
       <c r="F45" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H45" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="I45" t="str">
         <f t="shared" si="0"/>
         <v>wa1n8</v>
       </c>
       <c r="P45" s="1" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="Q45" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="R45" s="1"/>
       <c r="S45" t="str">
@@ -5192,23 +4557,23 @@
         <v>44</v>
       </c>
       <c r="F46" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="H46" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="I46" t="str">
         <f t="shared" si="0"/>
         <v>aless_io98</v>
       </c>
       <c r="P46" s="1" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="Q46" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="R46" s="1" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="S46" t="str">
         <f t="shared" si="1"/>
@@ -5220,23 +4585,23 @@
         <v>45</v>
       </c>
       <c r="F47" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="H47" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="I47" t="str">
         <f t="shared" si="0"/>
         <v>MaspicDigital</v>
       </c>
       <c r="P47" s="1" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="Q47" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="R47" s="1" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="S47" t="str">
         <f t="shared" si="1"/>
@@ -5248,20 +4613,20 @@
         <v>46</v>
       </c>
       <c r="F48" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="I48" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="P48" s="1" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="Q48" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="R48" s="1" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="S48" t="str">
         <f t="shared" si="1"/>
@@ -5273,23 +4638,23 @@
         <v>47</v>
       </c>
       <c r="F49" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H49" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="I49" t="str">
         <f t="shared" si="0"/>
         <v>niflash</v>
       </c>
       <c r="P49" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="Q49" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="R49" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="S49" t="str">
         <f t="shared" si="1"/>
@@ -5301,23 +4666,23 @@
         <v>48</v>
       </c>
       <c r="F50" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="H50" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="I50" t="str">
         <f t="shared" si="0"/>
         <v>cicciovolley91</v>
       </c>
       <c r="P50" s="1" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="Q50" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="R50" s="1" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="S50" t="str">
         <f t="shared" si="1"/>
@@ -5329,23 +4694,23 @@
         <v>49</v>
       </c>
       <c r="F51" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="H51" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="I51" t="str">
         <f t="shared" si="0"/>
         <v>begghich</v>
       </c>
       <c r="P51" s="1" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="Q51" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="R51" s="1" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="S51" t="str">
         <f t="shared" si="1"/>
@@ -5355,13 +4720,13 @@
     <row r="52" spans="1:19" x14ac:dyDescent="0.3">
       <c r="F52" s="1"/>
       <c r="P52" s="1" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="Q52" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="R52" s="1" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="S52" t="str">
         <f t="shared" si="1"/>
@@ -5371,13 +4736,13 @@
     <row r="53" spans="1:19" x14ac:dyDescent="0.3">
       <c r="F53" s="1"/>
       <c r="P53" s="1" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="Q53" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="R53" s="1" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="S53" t="str">
         <f t="shared" si="1"/>

</xml_diff>

<commit_message>
convocazioni armata stagione 125 - 2
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7ee4892a2dd36b84/Desktop/Link-clan/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="11" documentId="13_ncr:1_{9FCDD52C-4DCE-46C4-BB20-7F2264BA0663}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{850E0488-124F-4429-8FDF-458B59134D3B}"/>
+  <xr:revisionPtr revIDLastSave="18" documentId="13_ncr:1_{9FCDD52C-4DCE-46C4-BB20-7F2264BA0663}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D8290DC1-52C1-497E-B125-230673D4F98E}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{FECCDA54-7594-4EB7-ABFB-2C408C6461DD}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="641" uniqueCount="337">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="290">
   <si>
     <t>TagTelegram</t>
   </si>
@@ -93,9 +93,6 @@
     <t>ＡＲ♦️Ｂｌａｚｏｒ１１１</t>
   </si>
   <si>
-    <t>@Blazor111</t>
-  </si>
-  <si>
     <t>ＡＲ♦️道路軍Wåyne</t>
   </si>
   <si>
@@ -291,9 +288,6 @@
     <t>ＡＲ♦️Ｅ＄</t>
   </si>
   <si>
-    <t>@rkomi99</t>
-  </si>
-  <si>
     <t>@cicciovolley91</t>
   </si>
   <si>
@@ -360,9 +354,6 @@
     <t>@domenico_9</t>
   </si>
   <si>
-    <t>@Alestrega22</t>
-  </si>
-  <si>
     <t>J.O.K.E.R</t>
   </si>
   <si>
@@ -375,15 +366,9 @@
     <t>Kekko03</t>
   </si>
   <si>
-    <t>@K3kk07</t>
-  </si>
-  <si>
     <t>dani_lanc</t>
   </si>
   <si>
-    <t>@asso_nr</t>
-  </si>
-  <si>
     <t>simo99</t>
   </si>
   <si>
@@ -426,9 +411,6 @@
     <t>&lt;c5&gt;OhAnd4</t>
   </si>
   <si>
-    <t>@OhAnd4</t>
-  </si>
-  <si>
     <t>DOCCC</t>
   </si>
   <si>
@@ -858,153 +840,33 @@
     <t>HTL I EBDP</t>
   </si>
   <si>
-    <t>@totino96</t>
-  </si>
-  <si>
     <t>@RickySina22</t>
   </si>
   <si>
     <t>@Gaia951</t>
   </si>
   <si>
-    <t>@Mannito92</t>
-  </si>
-  <si>
-    <t>@luca3689</t>
-  </si>
-  <si>
     <t>@MerMet92</t>
   </si>
   <si>
-    <t>@ciuler</t>
-  </si>
-  <si>
     <t>@Sas0800</t>
   </si>
   <si>
-    <t>@arsenapoli</t>
-  </si>
-  <si>
-    <t>@superfede2</t>
-  </si>
-  <si>
-    <t>@Oneleggedjack</t>
-  </si>
-  <si>
-    <t>@Manu2365</t>
-  </si>
-  <si>
-    <t>@usernamepersonalee</t>
-  </si>
-  <si>
-    <t>@srd_rce</t>
-  </si>
-  <si>
-    <t>ＡＲ♠️ｓｐｅｚｉａ</t>
-  </si>
-  <si>
-    <t>@sunnering</t>
-  </si>
-  <si>
-    <t>@mangusta_agile</t>
-  </si>
-  <si>
-    <t>@BBCTR3</t>
-  </si>
-  <si>
-    <t>@manuel190396</t>
-  </si>
-  <si>
-    <t>@BwoneJ</t>
-  </si>
-  <si>
-    <t>@Basco3</t>
-  </si>
-  <si>
     <t>@Cisco00001</t>
   </si>
   <si>
     <t>@Torsiz007</t>
   </si>
   <si>
-    <t>@RETROWAV3R</t>
-  </si>
-  <si>
-    <t>Christian</t>
-  </si>
-  <si>
-    <t>@Christian00007</t>
-  </si>
-  <si>
-    <t>@sorridetemi</t>
-  </si>
-  <si>
-    <t>@Fox_0265</t>
-  </si>
-  <si>
-    <t>@Davidone11</t>
-  </si>
-  <si>
-    <t>&lt;c5&gt;0hAnd4</t>
-  </si>
-  <si>
-    <t>Antonio96</t>
-  </si>
-  <si>
-    <t>arKaiba❤️Sparky</t>
-  </si>
-  <si>
-    <t>Cry</t>
-  </si>
-  <si>
-    <t>Eric</t>
-  </si>
-  <si>
     <t>frenci</t>
   </si>
   <si>
-    <t>Lore</t>
-  </si>
-  <si>
-    <t>Luca01</t>
-  </si>
-  <si>
-    <t>manuel1903</t>
-  </si>
-  <si>
-    <t>Mr.Fox</t>
-  </si>
-  <si>
-    <t>NIMBLE MONGOOSE</t>
-  </si>
-  <si>
-    <t>RETROWAV3R™️</t>
-  </si>
-  <si>
-    <t>Royal Army</t>
-  </si>
-  <si>
-    <t>superfede</t>
-  </si>
-  <si>
-    <t>tiau</t>
-  </si>
-  <si>
-    <t>Zumpy</t>
-  </si>
-  <si>
-    <t>I Tori Feroci</t>
-  </si>
-  <si>
     <t>Si</t>
   </si>
   <si>
     <t>@cvbalibre</t>
   </si>
   <si>
-    <t>@Robu99</t>
-  </si>
-  <si>
     <t>Ａ Ｒ ♠️ ＦＥＤＥＲＩＣＯ</t>
   </si>
   <si>
@@ -1023,28 +885,25 @@
     <t>_SINA22_</t>
   </si>
   <si>
-    <t>Dino</t>
-  </si>
-  <si>
-    <t>Geeno</t>
-  </si>
-  <si>
     <t>●SUMATRA●</t>
   </si>
   <si>
     <t>Cicciovolley91</t>
   </si>
   <si>
-    <t>BwonE</t>
-  </si>
-  <si>
-    <t>Basco</t>
-  </si>
-  <si>
-    <t>khmer BM⚡</t>
-  </si>
-  <si>
     <t>\GuyFawkes/</t>
+  </si>
+  <si>
+    <t>Ａｒ❤Ｓａｍｕｅｌｅ</t>
+  </si>
+  <si>
+    <t>Lind L. Taylor</t>
+  </si>
+  <si>
+    <t>@PharmaShooter</t>
+  </si>
+  <si>
+    <t>@niflash</t>
   </si>
 </sst>
 </file>
@@ -1908,10 +1767,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EE2B0F9-AC31-464B-B046-53CB033C8615}">
-  <dimension ref="A1:D100"/>
+  <dimension ref="A1:D92"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="C46" sqref="C2:D46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1939,1391 +1798,640 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>130</v>
+        <v>273</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>303</v>
+        <v>280</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>320</v>
+        <v>275</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>127</v>
+        <v>31</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>251</v>
+        <v>30</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>320</v>
+        <v>275</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>285</v>
+        <v>39</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>105</v>
+        <v>38</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>320</v>
+        <v>275</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>95</v>
+        <v>23</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>94</v>
+        <v>22</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>320</v>
+        <v>275</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>274</v>
+        <v>11</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>304</v>
+        <v>277</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>320</v>
+        <v>275</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>102</v>
+        <v>21</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>101</v>
+        <v>286</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>320</v>
+        <v>275</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="B8" s="1" t="s">
-        <v>288</v>
+        <v>32</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>320</v>
+        <v>275</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>268</v>
+        <v>150</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>253</v>
+        <v>147</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>320</v>
+        <v>275</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>78</v>
+        <v>270</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>77</v>
+        <v>281</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>320</v>
+        <v>275</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>300</v>
+        <v>271</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>305</v>
+        <v>283</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>320</v>
+        <v>275</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>282</v>
+        <v>15</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>64</v>
+        <v>14</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>320</v>
+        <v>275</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>119</v>
+        <v>17</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>118</v>
+        <v>16</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>320</v>
+        <v>275</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>299</v>
+        <v>37</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>298</v>
+        <v>36</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>320</v>
+        <v>275</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>49</v>
+        <v>276</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>48</v>
+        <v>279</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>320</v>
+        <v>275</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>264</v>
+        <v>13</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>215</v>
+        <v>12</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>320</v>
+        <v>275</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
-        <v>277</v>
-      </c>
       <c r="B17" s="1" t="s">
-        <v>306</v>
+        <v>267</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>320</v>
+        <v>275</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>115</v>
+        <v>268</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>114</v>
+        <v>282</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>320</v>
+        <v>275</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>263</v>
+        <v>105</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>260</v>
+        <v>104</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>320</v>
+        <v>275</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>72</v>
+        <v>8</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>71</v>
+        <v>45</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>320</v>
+        <v>275</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>287</v>
+        <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>307</v>
+        <v>19</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>320</v>
+        <v>275</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>295</v>
+        <v>5</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>308</v>
+        <v>9</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>320</v>
+        <v>275</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>68</v>
+        <v>41</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>67</v>
+        <v>40</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>320</v>
+        <v>275</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>113</v>
+        <v>27</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>112</v>
+        <v>26</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>320</v>
+        <v>275</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>269</v>
+        <v>116</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>255</v>
+        <v>115</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>320</v>
+        <v>275</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>122</v>
+        <v>29</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>139</v>
+        <v>28</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>320</v>
+        <v>275</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>266</v>
+        <v>43</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>247</v>
+        <v>42</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>320</v>
+        <v>275</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>286</v>
+        <v>7</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>309</v>
+        <v>6</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>320</v>
+        <v>275</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>81</v>
+        <v>266</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>88</v>
+        <v>285</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>320</v>
+        <v>275</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>278</v>
+        <v>84</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>310</v>
+        <v>284</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>320</v>
+        <v>275</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>55</v>
+        <v>149</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>54</v>
+        <v>146</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>320</v>
+        <v>275</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>292</v>
+        <v>148</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>311</v>
+        <v>143</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>320</v>
+        <v>275</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>301</v>
+        <v>126</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>312</v>
+        <v>125</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>320</v>
+        <v>275</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>91</v>
+        <v>269</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>138</v>
+        <v>278</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>320</v>
+        <v>275</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>290</v>
+        <v>114</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>313</v>
+        <v>113</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>320</v>
+        <v>275</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>284</v>
+        <v>95</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>69</v>
+        <v>94</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>320</v>
+        <v>275</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
-        <v>80</v>
+        <v>25</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>79</v>
+        <v>24</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>320</v>
+        <v>275</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>111</v>
+        <v>288</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>110</v>
+        <v>287</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>320</v>
+        <v>275</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
-        <v>57</v>
+        <v>88</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>56</v>
+        <v>87</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>320</v>
+        <v>275</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
-        <v>60</v>
+        <v>272</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>87</v>
+        <v>274</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>320</v>
+        <v>275</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
-        <v>126</v>
+        <v>48</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>125</v>
+        <v>47</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>320</v>
+        <v>275</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
-        <v>297</v>
+        <v>258</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>314</v>
+        <v>209</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>320</v>
+        <v>275</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
-        <v>302</v>
+        <v>131</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>315</v>
+        <v>130</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>320</v>
+        <v>275</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
-        <v>267</v>
+        <v>80</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>248</v>
+        <v>86</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>320</v>
+        <v>275</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
-        <v>137</v>
+        <v>77</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>136</v>
+        <v>76</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>320</v>
+        <v>275</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
-        <v>117</v>
+        <v>289</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>116</v>
+        <v>60</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A47" s="1" t="s">
-        <v>283</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>316</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>319</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A48" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>319</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A49" s="1" t="s">
-        <v>291</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>317</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>319</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A50" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>319</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A51" s="1" t="s">
-        <v>271</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>258</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>319</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A52" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>319</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A53" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>319</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A54" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>318</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>319</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A55" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>323</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A56" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A57" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B57" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A58" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A59" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="B59" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D59" s="1" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A60" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A61" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B61" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D61" s="1" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A62" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D62" s="1" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A63" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B63" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C63" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D63" s="1" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A64" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B64" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="C64" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D64" s="1" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A65" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B65" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C65" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D65" s="1" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A66" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B66" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="C66" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D66" s="1" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A67" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B67" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C67" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D67" s="1" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A68" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B68" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C68" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D68" s="1" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A69" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B69" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C69" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D69" s="1" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A70" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B70" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C70" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D70" s="1" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A71" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B71" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C71" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D71" s="1" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A72" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B72" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C72" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D72" s="1" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A73" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="B73" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="C73" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D73" s="1" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A74" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="B74" s="1" t="s">
-        <v>324</v>
-      </c>
-      <c r="C74" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D74" s="1" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B75" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="C75" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D75" s="1" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A76" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="B76" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="C76" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D76" s="1" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A77" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B77" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C77" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D77" s="1" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A78" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B78" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C78" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D78" s="1" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A79" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B79" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C79" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D79" s="1" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A80" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B80" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C80" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D80" s="1" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A81" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="B81" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="C81" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D81" s="1" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A82" s="1" t="s">
-        <v>321</v>
-      </c>
-      <c r="B82" s="1" t="s">
-        <v>325</v>
-      </c>
-      <c r="C82" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D82" s="1" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A83" s="1" t="s">
-        <v>296</v>
-      </c>
-      <c r="B83" s="1" t="s">
-        <v>326</v>
-      </c>
-      <c r="C83" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D83" s="1" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A84" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="B84" s="1" t="s">
-        <v>327</v>
-      </c>
-      <c r="C84" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D84" s="1" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A85" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="B85" s="1" t="s">
-        <v>328</v>
-      </c>
-      <c r="C85" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D85" s="1" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A86" s="1" t="s">
-        <v>289</v>
-      </c>
-      <c r="B86" s="1" t="s">
-        <v>329</v>
-      </c>
-      <c r="C86" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D86" s="1" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A87" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="B87" s="1" t="s">
-        <v>330</v>
-      </c>
-      <c r="C87" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D87" s="1" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A88" s="1" t="s">
-        <v>281</v>
-      </c>
-      <c r="B88" s="1" t="s">
-        <v>331</v>
-      </c>
-      <c r="C88" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D88" s="1" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A89" s="1" t="s">
-        <v>322</v>
-      </c>
-      <c r="B89" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C89" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D89" s="1" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A90" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="B90" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C90" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D90" s="1" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A91" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="B91" s="1" t="s">
-        <v>332</v>
-      </c>
-      <c r="C91" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D91" s="1" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A92" s="1" t="s">
-        <v>293</v>
-      </c>
-      <c r="B92" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="C92" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D92" s="1" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A93" s="1" t="s">
-        <v>294</v>
-      </c>
-      <c r="B93" s="1" t="s">
-        <v>334</v>
-      </c>
-      <c r="C93" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D93" s="1" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A94" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="B94" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C94" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D94" s="1" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A95" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B95" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C95" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D95" s="1" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A96" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="B96" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="C96" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D96" s="1" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A97" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="B97" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C97" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D97" s="1" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A98" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B98" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C98" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D98" s="1" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A99" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="B99" s="1" t="s">
-        <v>335</v>
-      </c>
-      <c r="C99" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D99" s="1" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A100" s="1" t="s">
-        <v>272</v>
-      </c>
-      <c r="B100" s="1" t="s">
-        <v>336</v>
-      </c>
-      <c r="C100" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D100" s="1" t="s">
-        <v>320</v>
-      </c>
-    </row>
+        <v>275</v>
+      </c>
+    </row>
+    <row r="92" ht="22.2" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3331,7 +2439,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{523DE1FE-2557-4F28-A82F-4FEA694BECD3}">
   <dimension ref="A4:S56"/>
   <sheetViews>
-    <sheetView topLeftCell="I26" zoomScale="113" workbookViewId="0">
+    <sheetView zoomScale="89" workbookViewId="0">
       <selection activeCell="Q4" sqref="Q4:Q53"/>
     </sheetView>
   </sheetViews>
@@ -3351,23 +2459,23 @@
         <v>1</v>
       </c>
       <c r="F4" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="H4" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="I4" t="str">
         <f t="shared" ref="I4:I51" si="0">_xlfn.CONCAT(H4:H4)</f>
         <v>elioo_06</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="Q4" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="R4" s="1" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="S4" t="str">
         <f>_xlfn.CONCAT(Q4:R4)</f>
@@ -3383,20 +2491,20 @@
         <v>18</v>
       </c>
       <c r="H5" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="I5" t="str">
         <f t="shared" si="0"/>
         <v>Blazor111</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="Q5" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="R5" s="1" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="S5" t="str">
         <f t="shared" ref="S5:S53" si="1">_xlfn.CONCAT(Q5:R5)</f>
@@ -3412,20 +2520,20 @@
         <v>4</v>
       </c>
       <c r="H6" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="I6" t="str">
         <f t="shared" si="0"/>
         <v>aleman7273</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="Q6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="R6" s="1" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="S6" t="str">
         <f t="shared" si="1"/>
@@ -3441,20 +2549,20 @@
         <v>9</v>
       </c>
       <c r="H7" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="I7" t="str">
         <f t="shared" si="0"/>
         <v>aleman7273</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="Q7" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="R7" s="1" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="S7" t="str">
         <f t="shared" si="1"/>
@@ -3467,23 +2575,23 @@
       </c>
       <c r="E8" s="1"/>
       <c r="F8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H8" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="I8" t="str">
         <f t="shared" si="0"/>
         <v>FORTEX09</v>
       </c>
       <c r="P8" s="1" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="Q8" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="R8" s="1" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="S8" t="str">
         <f t="shared" si="1"/>
@@ -3496,23 +2604,23 @@
       </c>
       <c r="E9" s="1"/>
       <c r="F9" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="H9" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="I9" t="str">
         <f t="shared" si="0"/>
         <v>BuldzS</v>
       </c>
       <c r="P9" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="Q9" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="R9" s="1" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="S9" t="str">
         <f t="shared" si="1"/>
@@ -3525,23 +2633,23 @@
       </c>
       <c r="E10" s="1"/>
       <c r="F10" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="H10" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="I10" t="str">
         <f t="shared" si="0"/>
         <v>Alestrega22</v>
       </c>
       <c r="P10" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q10" t="s">
         <v>82</v>
       </c>
-      <c r="Q10" t="s">
-        <v>83</v>
-      </c>
       <c r="R10" s="1" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="S10" t="str">
         <f t="shared" si="1"/>
@@ -3554,23 +2662,23 @@
       </c>
       <c r="E11" s="1"/>
       <c r="F11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H11" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="I11" t="str">
         <f t="shared" si="0"/>
         <v>Ale_Mare93</v>
       </c>
       <c r="P11" s="1" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="Q11" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="R11" s="1" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="S11" t="str">
         <f t="shared" si="1"/>
@@ -3586,20 +2694,20 @@
         <v>12</v>
       </c>
       <c r="H12" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="I12" t="str">
         <f t="shared" si="0"/>
         <v>Romas10</v>
       </c>
       <c r="P12" s="1" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="Q12" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="R12" s="1" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="S12" t="str">
         <f t="shared" si="1"/>
@@ -3612,23 +2720,23 @@
       </c>
       <c r="E13" s="1"/>
       <c r="F13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I13" t="str">
         <f t="shared" si="0"/>
         <v>crezyred</v>
       </c>
       <c r="P13" s="1" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="Q13" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="R13" s="1" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="S13" t="str">
         <f t="shared" si="1"/>
@@ -3641,23 +2749,23 @@
       </c>
       <c r="E14" s="1"/>
       <c r="F14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H14" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="I14" t="str">
         <f t="shared" si="0"/>
         <v>DaMoops</v>
       </c>
       <c r="P14" s="1" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="Q14" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="R14" s="1" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="S14" t="str">
         <f t="shared" si="1"/>
@@ -3670,23 +2778,23 @@
       </c>
       <c r="E15" s="1"/>
       <c r="F15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H15" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="I15" t="str">
         <f t="shared" si="0"/>
         <v>Robu99</v>
       </c>
       <c r="P15" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q15" t="s">
         <v>65</v>
       </c>
-      <c r="Q15" t="s">
-        <v>66</v>
-      </c>
       <c r="R15" s="1" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="S15" t="str">
         <f t="shared" si="1"/>
@@ -3699,23 +2807,23 @@
       </c>
       <c r="E16" s="1"/>
       <c r="F16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H16" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="I16" t="str">
         <f t="shared" si="0"/>
         <v>Punk_ake</v>
       </c>
       <c r="P16" s="1" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="Q16" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="R16" s="1" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="S16" t="str">
         <f t="shared" si="1"/>
@@ -3728,23 +2836,23 @@
       </c>
       <c r="E17" s="1"/>
       <c r="F17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H17" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="I17" t="str">
         <f t="shared" si="0"/>
         <v>Marchio04</v>
       </c>
       <c r="P17" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q17" t="s">
         <v>58</v>
       </c>
-      <c r="Q17" t="s">
-        <v>59</v>
-      </c>
       <c r="R17" s="1" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="S17" t="str">
         <f t="shared" si="1"/>
@@ -3757,20 +2865,20 @@
       </c>
       <c r="E18" s="1"/>
       <c r="F18" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="I18" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="P18" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q18" t="s">
         <v>54</v>
       </c>
-      <c r="Q18" t="s">
-        <v>55</v>
-      </c>
       <c r="R18" s="1" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="S18" t="str">
         <f t="shared" si="1"/>
@@ -3786,20 +2894,20 @@
         <v>14</v>
       </c>
       <c r="H19" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="I19" t="str">
         <f t="shared" si="0"/>
         <v>riccalso</v>
       </c>
       <c r="P19" s="1" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="Q19" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="R19" s="1" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="S19" t="str">
         <f t="shared" si="1"/>
@@ -3812,23 +2920,23 @@
       </c>
       <c r="E20" s="1"/>
       <c r="F20" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H20" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="I20" t="str">
         <f t="shared" si="0"/>
         <v>BO_CRL</v>
       </c>
       <c r="P20" s="1" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="Q20" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="R20" s="1" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="S20" t="str">
         <f t="shared" si="1"/>
@@ -3841,23 +2949,23 @@
       </c>
       <c r="E21" s="1"/>
       <c r="F21" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H21" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I21" t="str">
         <f t="shared" si="0"/>
         <v>BrokerTony</v>
       </c>
       <c r="P21" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q21" t="s">
         <v>52</v>
       </c>
-      <c r="Q21" t="s">
-        <v>53</v>
-      </c>
       <c r="R21" s="1" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="S21" t="str">
         <f t="shared" si="1"/>
@@ -3873,20 +2981,20 @@
         <v>16</v>
       </c>
       <c r="H22" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="I22" t="str">
         <f t="shared" si="0"/>
         <v>Mazzito</v>
       </c>
       <c r="P22" s="1" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="Q22" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="R22" s="1" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="S22" t="str">
         <f t="shared" si="1"/>
@@ -3899,23 +3007,23 @@
       </c>
       <c r="E23" s="1"/>
       <c r="F23" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="H23" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="I23" t="str">
         <f t="shared" si="0"/>
         <v>NicoSkev98</v>
       </c>
       <c r="P23" s="1" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="Q23" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="R23" s="1" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="S23" t="str">
         <f t="shared" si="1"/>
@@ -3928,23 +3036,23 @@
       </c>
       <c r="E24" s="1"/>
       <c r="F24" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="H24" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="I24" t="str">
         <f t="shared" si="0"/>
         <v>pietro_actis</v>
       </c>
       <c r="P24" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="Q24" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="R24" s="1" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="S24" t="str">
         <f t="shared" si="1"/>
@@ -3957,23 +3065,23 @@
       </c>
       <c r="E25" s="1"/>
       <c r="F25" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H25" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I25" t="str">
         <f t="shared" si="0"/>
         <v>mrdeath75</v>
       </c>
       <c r="P25" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q25" t="s">
         <v>56</v>
       </c>
-      <c r="Q25" t="s">
-        <v>57</v>
-      </c>
       <c r="R25" s="1" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="S25" t="str">
         <f t="shared" si="1"/>
@@ -3989,20 +3097,20 @@
         <v>6</v>
       </c>
       <c r="H26" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="I26" t="str">
         <f t="shared" si="0"/>
         <v>Ahmed_Eliow</v>
       </c>
       <c r="P26" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="Q26" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="R26" s="1" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="S26" t="str">
         <f t="shared" si="1"/>
@@ -4015,23 +3123,23 @@
       </c>
       <c r="E27" s="1"/>
       <c r="F27" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H27" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="I27" t="str">
         <f t="shared" si="0"/>
         <v>Madara_2912</v>
       </c>
       <c r="P27" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="Q27" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="R27" s="1" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="S27" t="str">
         <f t="shared" si="1"/>
@@ -4044,23 +3152,23 @@
       </c>
       <c r="E28" s="1"/>
       <c r="F28" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H28" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="I28" t="str">
         <f t="shared" si="0"/>
         <v>ArBughy</v>
       </c>
       <c r="P28" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="Q28" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="R28" s="1" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="S28" t="str">
         <f t="shared" si="1"/>
@@ -4073,23 +3181,23 @@
       </c>
       <c r="E29" s="1"/>
       <c r="F29" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="H29" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="I29" t="str">
         <f t="shared" si="0"/>
         <v>Tanjim041</v>
       </c>
       <c r="P29" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q29" t="s">
         <v>67</v>
       </c>
-      <c r="Q29" t="s">
-        <v>68</v>
-      </c>
       <c r="R29" s="1" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="S29" t="str">
         <f t="shared" si="1"/>
@@ -4102,23 +3210,23 @@
       </c>
       <c r="E30" s="1"/>
       <c r="F30" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H30" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="I30" t="str">
         <f t="shared" si="0"/>
         <v>Sz66603</v>
       </c>
       <c r="P30" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q30" t="s">
         <v>48</v>
       </c>
-      <c r="Q30" t="s">
-        <v>49</v>
-      </c>
       <c r="R30" s="1" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="S30" t="str">
         <f t="shared" si="1"/>
@@ -4131,23 +3239,23 @@
       </c>
       <c r="E31" s="1"/>
       <c r="F31" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="H31" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="I31" t="str">
         <f t="shared" si="0"/>
         <v>ralfone01</v>
       </c>
       <c r="P31" s="1" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="Q31" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="R31" s="1" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="S31" t="str">
         <f t="shared" si="1"/>
@@ -4160,23 +3268,23 @@
       </c>
       <c r="E32" s="1"/>
       <c r="F32" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H32" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="I32" t="str">
         <f t="shared" si="0"/>
         <v>yvngdanyy</v>
       </c>
       <c r="P32" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="Q32" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="R32" s="1" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="S32" t="str">
         <f t="shared" si="1"/>
@@ -4189,23 +3297,23 @@
       </c>
       <c r="E33" s="1"/>
       <c r="F33" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H33" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="I33" t="str">
         <f t="shared" si="0"/>
         <v>rkomi99</v>
       </c>
       <c r="P33" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="Q33" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="R33" s="1" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="S33" t="str">
         <f t="shared" si="1"/>
@@ -4218,23 +3326,23 @@
       </c>
       <c r="E34" s="1"/>
       <c r="F34" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="H34" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="I34" t="str">
         <f t="shared" si="0"/>
         <v>sunnering41</v>
       </c>
       <c r="P34" s="1" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="Q34" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="R34" s="1" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="S34" t="str">
         <f t="shared" si="1"/>
@@ -4247,23 +3355,23 @@
       </c>
       <c r="E35" s="1"/>
       <c r="F35" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="H35" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="I35" t="str">
         <f t="shared" si="0"/>
         <v>alabatia89</v>
       </c>
       <c r="P35" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q35" t="s">
         <v>50</v>
       </c>
-      <c r="Q35" t="s">
-        <v>51</v>
-      </c>
       <c r="R35" s="1" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="S35" t="str">
         <f t="shared" si="1"/>
@@ -4276,23 +3384,23 @@
       </c>
       <c r="E36" s="1"/>
       <c r="F36" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="H36" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="I36" t="str">
         <f t="shared" si="0"/>
         <v>asso_nr</v>
       </c>
       <c r="P36" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q36" t="s">
         <v>79</v>
       </c>
-      <c r="Q36" t="s">
-        <v>80</v>
-      </c>
       <c r="R36" s="1" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="S36" t="str">
         <f t="shared" si="1"/>
@@ -4305,23 +3413,23 @@
       </c>
       <c r="E37" s="1"/>
       <c r="F37" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H37" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="I37" t="str">
         <f t="shared" si="0"/>
         <v>PepponeB91</v>
       </c>
       <c r="P37" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q37" t="s">
         <v>75</v>
       </c>
-      <c r="Q37" t="s">
-        <v>76</v>
-      </c>
       <c r="R37" s="1" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="S37" t="str">
         <f t="shared" si="1"/>
@@ -4334,23 +3442,23 @@
       </c>
       <c r="E38" s="1"/>
       <c r="F38" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="H38" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="I38" t="str">
         <f t="shared" si="0"/>
         <v>OhAnd4</v>
       </c>
       <c r="P38" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q38" t="s">
         <v>77</v>
       </c>
-      <c r="Q38" t="s">
-        <v>78</v>
-      </c>
       <c r="R38" s="1" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="S38" t="str">
         <f t="shared" si="1"/>
@@ -4363,23 +3471,23 @@
       </c>
       <c r="E39" s="1"/>
       <c r="F39" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H39" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="I39" t="str">
         <f t="shared" si="0"/>
         <v>Lilyan51</v>
       </c>
       <c r="P39" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q39" t="s">
         <v>62</v>
       </c>
-      <c r="Q39" t="s">
-        <v>63</v>
-      </c>
       <c r="R39" s="1" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="S39" t="str">
         <f t="shared" si="1"/>
@@ -4391,23 +3499,23 @@
         <v>38</v>
       </c>
       <c r="F40" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="H40" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="I40" t="str">
         <f t="shared" si="0"/>
         <v>K3kk07</v>
       </c>
       <c r="P40" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q40" t="s">
         <v>71</v>
       </c>
-      <c r="Q40" t="s">
-        <v>72</v>
-      </c>
       <c r="R40" s="1" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="S40" t="str">
         <f t="shared" si="1"/>
@@ -4419,23 +3527,23 @@
         <v>39</v>
       </c>
       <c r="F41" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="H41" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="I41" t="str">
         <f t="shared" si="0"/>
         <v>Mastrolivo</v>
       </c>
       <c r="P41" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="Q41" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="R41" s="1" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="S41" t="str">
         <f t="shared" si="1"/>
@@ -4447,23 +3555,23 @@
         <v>40</v>
       </c>
       <c r="F42" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="H42" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="I42" t="str">
         <f t="shared" si="0"/>
         <v>Sibinpopzz</v>
       </c>
       <c r="P42" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="Q42" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="R42" s="1" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="S42" t="str">
         <f t="shared" si="1"/>
@@ -4478,20 +3586,20 @@
         <v>10</v>
       </c>
       <c r="H43" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="I43" t="str">
         <f t="shared" si="0"/>
         <v>FedericoBello03</v>
       </c>
       <c r="P43" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q43" t="s">
         <v>69</v>
       </c>
-      <c r="Q43" t="s">
-        <v>70</v>
-      </c>
       <c r="R43" s="1" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="S43" t="str">
         <f t="shared" si="1"/>
@@ -4503,23 +3611,23 @@
         <v>42</v>
       </c>
       <c r="F44" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="H44" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="I44" t="str">
         <f t="shared" si="0"/>
         <v>BACWasTaken</v>
       </c>
       <c r="P44" s="1" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="Q44" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="R44" s="1" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="S44" t="str">
         <f t="shared" si="1"/>
@@ -4531,20 +3639,20 @@
         <v>43</v>
       </c>
       <c r="F45" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H45" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="I45" t="str">
         <f t="shared" si="0"/>
         <v>wa1n8</v>
       </c>
       <c r="P45" s="1" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="Q45" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="R45" s="1"/>
       <c r="S45" t="str">
@@ -4557,23 +3665,23 @@
         <v>44</v>
       </c>
       <c r="F46" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="H46" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="I46" t="str">
         <f t="shared" si="0"/>
         <v>aless_io98</v>
       </c>
       <c r="P46" s="1" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="Q46" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="R46" s="1" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="S46" t="str">
         <f t="shared" si="1"/>
@@ -4585,23 +3693,23 @@
         <v>45</v>
       </c>
       <c r="F47" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="H47" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="I47" t="str">
         <f t="shared" si="0"/>
         <v>MaspicDigital</v>
       </c>
       <c r="P47" s="1" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="Q47" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="R47" s="1" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="S47" t="str">
         <f t="shared" si="1"/>
@@ -4613,20 +3721,20 @@
         <v>46</v>
       </c>
       <c r="F48" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="I48" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="P48" s="1" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="Q48" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="R48" s="1" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="S48" t="str">
         <f t="shared" si="1"/>
@@ -4638,23 +3746,23 @@
         <v>47</v>
       </c>
       <c r="F49" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H49" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="I49" t="str">
         <f t="shared" si="0"/>
         <v>niflash</v>
       </c>
       <c r="P49" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q49" t="s">
         <v>73</v>
       </c>
-      <c r="Q49" t="s">
-        <v>74</v>
-      </c>
       <c r="R49" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="S49" t="str">
         <f t="shared" si="1"/>
@@ -4666,23 +3774,23 @@
         <v>48</v>
       </c>
       <c r="F50" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="H50" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="I50" t="str">
         <f t="shared" si="0"/>
         <v>cicciovolley91</v>
       </c>
       <c r="P50" s="1" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="Q50" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="R50" s="1" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="S50" t="str">
         <f t="shared" si="1"/>
@@ -4694,23 +3802,23 @@
         <v>49</v>
       </c>
       <c r="F51" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="H51" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="I51" t="str">
         <f t="shared" si="0"/>
         <v>begghich</v>
       </c>
       <c r="P51" s="1" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="Q51" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="R51" s="1" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="S51" t="str">
         <f t="shared" si="1"/>
@@ -4720,13 +3828,13 @@
     <row r="52" spans="1:19" x14ac:dyDescent="0.3">
       <c r="F52" s="1"/>
       <c r="P52" s="1" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="Q52" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="R52" s="1" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="S52" t="str">
         <f t="shared" si="1"/>
@@ -4736,13 +3844,13 @@
     <row r="53" spans="1:19" x14ac:dyDescent="0.3">
       <c r="F53" s="1"/>
       <c r="P53" s="1" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="Q53" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="R53" s="1" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="S53" t="str">
         <f t="shared" si="1"/>

</xml_diff>

<commit_message>
convocazioni stagione 125 3
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7ee4892a2dd36b84/Desktop/Link-clan/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="18" documentId="13_ncr:1_{9FCDD52C-4DCE-46C4-BB20-7F2264BA0663}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D8290DC1-52C1-497E-B125-230673D4F98E}"/>
+  <xr:revisionPtr revIDLastSave="29" documentId="13_ncr:1_{9FCDD52C-4DCE-46C4-BB20-7F2264BA0663}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{431AFCDF-3040-432E-8D8D-59C5FED6F4DE}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{FECCDA54-7594-4EB7-ABFB-2C408C6461DD}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="13776" xr2:uid="{FECCDA54-7594-4EB7-ABFB-2C408C6461DD}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="627" uniqueCount="338">
   <si>
     <t>TagTelegram</t>
   </si>
@@ -843,24 +843,15 @@
     <t>@RickySina22</t>
   </si>
   <si>
-    <t>@Gaia951</t>
-  </si>
-  <si>
     <t>@MerMet92</t>
   </si>
   <si>
     <t>@Sas0800</t>
   </si>
   <si>
-    <t>@Cisco00001</t>
-  </si>
-  <si>
     <t>@Torsiz007</t>
   </si>
   <si>
-    <t>frenci</t>
-  </si>
-  <si>
     <t>Si</t>
   </si>
   <si>
@@ -870,9 +861,6 @@
     <t>Ａ Ｒ ♠️ ＦＥＤＥＲＩＣＯ</t>
   </si>
   <si>
-    <t>GaiaScienza</t>
-  </si>
-  <si>
     <t>AR♣️Cuba</t>
   </si>
   <si>
@@ -904,6 +892,162 @@
   </si>
   <si>
     <t>@niflash</t>
+  </si>
+  <si>
+    <t>Antonio96</t>
+  </si>
+  <si>
+    <t>Zumpy</t>
+  </si>
+  <si>
+    <t>Eric</t>
+  </si>
+  <si>
+    <t>Dino</t>
+  </si>
+  <si>
+    <t>Geeno</t>
+  </si>
+  <si>
+    <t>Frenk8</t>
+  </si>
+  <si>
+    <t>Fabrizio</t>
+  </si>
+  <si>
+    <t>Luca01</t>
+  </si>
+  <si>
+    <t>⚡MAJOR⚡</t>
+  </si>
+  <si>
+    <t>two ciamela</t>
+  </si>
+  <si>
+    <t>Royal Army</t>
+  </si>
+  <si>
+    <t>superfede</t>
+  </si>
+  <si>
+    <t>Andrea</t>
+  </si>
+  <si>
+    <t>RETROWAV3R™️</t>
+  </si>
+  <si>
+    <t>fogu</t>
+  </si>
+  <si>
+    <t>IL DISTRUTTORE</t>
+  </si>
+  <si>
+    <t>ＮＯＴＯＲＩＯＵＳ Ｂ.Ｉ.Ｇ</t>
+  </si>
+  <si>
+    <t>NIMBLE MONGOOSE</t>
+  </si>
+  <si>
+    <t>tiau</t>
+  </si>
+  <si>
+    <t>arKaiba❤️Sparky</t>
+  </si>
+  <si>
+    <t>lord Tony</t>
+  </si>
+  <si>
+    <t>@totino96</t>
+  </si>
+  <si>
+    <t>@K3kk07</t>
+  </si>
+  <si>
+    <t>@srd_rce</t>
+  </si>
+  <si>
+    <t>@sunnering</t>
+  </si>
+  <si>
+    <t>@arsenapoli</t>
+  </si>
+  <si>
+    <t>@Alestrega22</t>
+  </si>
+  <si>
+    <t>@Freenk8</t>
+  </si>
+  <si>
+    <t>@Fabrizio2418</t>
+  </si>
+  <si>
+    <t>@luca3689</t>
+  </si>
+  <si>
+    <t>@Giggi_A</t>
+  </si>
+  <si>
+    <t>@Oneleggedjack</t>
+  </si>
+  <si>
+    <t>@Davidone11</t>
+  </si>
+  <si>
+    <t>@superfede2</t>
+  </si>
+  <si>
+    <t>@Manu2365</t>
+  </si>
+  <si>
+    <t>@RETROWAV3R</t>
+  </si>
+  <si>
+    <t>@BBCTR3</t>
+  </si>
+  <si>
+    <t>@mangusta_agile</t>
+  </si>
+  <si>
+    <t>@asso_nr</t>
+  </si>
+  <si>
+    <t>@sorridetemi</t>
+  </si>
+  <si>
+    <t>@T0N1003</t>
+  </si>
+  <si>
+    <t>Dog Rider</t>
+  </si>
+  <si>
+    <t>khmer BM⚡</t>
+  </si>
+  <si>
+    <t>Lore</t>
+  </si>
+  <si>
+    <t>⭐Marco⭐</t>
+  </si>
+  <si>
+    <t>IceMan</t>
+  </si>
+  <si>
+    <t>@ciuler</t>
+  </si>
+  <si>
+    <t>@usernamepersonalee</t>
+  </si>
+  <si>
+    <t>@alabatia89</t>
+  </si>
+  <si>
+    <t>@Robu99</t>
+  </si>
+  <si>
+    <t>@IceManLTD</t>
+  </si>
+  <si>
+    <t>@BACWasTaken</t>
   </si>
 </sst>
 </file>
@@ -1767,10 +1911,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EE2B0F9-AC31-464B-B046-53CB033C8615}">
-  <dimension ref="A1:D92"/>
+  <dimension ref="A1:D97"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C46" sqref="C2:D46"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1803,559 +1947,553 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>273</v>
+        <v>307</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>280</v>
+        <v>286</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>3</v>
+        <v>327</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>31</v>
+        <v>89</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>30</v>
+        <v>132</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>3</v>
+        <v>327</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>39</v>
+        <v>308</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>38</v>
+        <v>109</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>3</v>
+        <v>327</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>23</v>
+        <v>259</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>22</v>
+        <v>287</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>3</v>
+        <v>327</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>11</v>
+        <v>309</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>277</v>
+        <v>288</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>3</v>
+        <v>327</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>21</v>
+        <v>310</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>3</v>
+        <v>327</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>33</v>
+        <v>311</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>32</v>
+        <v>63</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>3</v>
+        <v>327</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>150</v>
+        <v>312</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>147</v>
+        <v>290</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>3</v>
+        <v>327</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>270</v>
+        <v>313</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>281</v>
+        <v>291</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>3</v>
+        <v>327</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>271</v>
+        <v>314</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>283</v>
+        <v>292</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>3</v>
+        <v>327</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>15</v>
+        <v>315</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>14</v>
+        <v>293</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>3</v>
+        <v>327</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>17</v>
+        <v>122</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>16</v>
+        <v>294</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>3</v>
+        <v>327</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>37</v>
+        <v>65</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>36</v>
+        <v>64</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>3</v>
+        <v>327</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>276</v>
+        <v>75</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>279</v>
+        <v>74</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>3</v>
+        <v>327</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>13</v>
+        <v>316</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>12</v>
+        <v>295</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>3</v>
+        <v>327</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>317</v>
+      </c>
       <c r="B17" s="1" t="s">
-        <v>267</v>
+        <v>68</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>3</v>
+        <v>327</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>282</v>
+        <v>242</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>3</v>
+        <v>327</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>105</v>
+        <v>318</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>104</v>
+        <v>296</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>3</v>
+        <v>327</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>8</v>
+        <v>319</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>45</v>
+        <v>297</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>3</v>
+        <v>327</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>20</v>
+        <v>320</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>19</v>
+        <v>103</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>3</v>
+        <v>327</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="1" t="s">
-        <v>5</v>
-      </c>
       <c r="B22" s="1" t="s">
-        <v>9</v>
+        <v>298</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>3</v>
+        <v>327</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>41</v>
+        <v>100</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>40</v>
+        <v>99</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>3</v>
+        <v>327</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>27</v>
+        <v>56</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>26</v>
+        <v>55</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>3</v>
+        <v>327</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>116</v>
+        <v>52</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>115</v>
+        <v>51</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>3</v>
+        <v>327</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>29</v>
+        <v>321</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>28</v>
+        <v>299</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>3</v>
+        <v>327</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>43</v>
+        <v>257</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>42</v>
+        <v>254</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>3</v>
+        <v>327</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>7</v>
+        <v>93</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>6</v>
+        <v>92</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>3</v>
+        <v>327</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>266</v>
+        <v>80</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>285</v>
+        <v>86</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>3</v>
+        <v>327</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>84</v>
+        <v>322</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>284</v>
+        <v>300</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>3</v>
+        <v>327</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>149</v>
+        <v>112</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>146</v>
+        <v>111</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>3</v>
+        <v>327</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" s="1" t="s">
-        <v>148</v>
-      </c>
       <c r="B32" s="1" t="s">
-        <v>143</v>
+        <v>301</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>3</v>
+        <v>327</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>3</v>
+        <v>327</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" s="1" t="s">
-        <v>269</v>
-      </c>
       <c r="B34" s="1" t="s">
-        <v>278</v>
+        <v>302</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>3</v>
+        <v>327</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>114</v>
+        <v>54</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>113</v>
+        <v>53</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>3</v>
+        <v>327</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>95</v>
+        <v>323</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>94</v>
+        <v>303</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>3</v>
+        <v>327</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
-        <v>25</v>
+        <v>322</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>24</v>
+        <v>304</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>3</v>
+        <v>327</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>288</v>
+        <v>84</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>3</v>
+        <v>327</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
-        <v>88</v>
+        <v>48</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>87</v>
+        <v>47</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>3</v>
+        <v>327</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
-        <v>272</v>
+        <v>131</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>274</v>
+        <v>130</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>3</v>
+        <v>327</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>47</v>
+        <v>6</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>3</v>
+        <v>327</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
@@ -2366,69 +2504,779 @@
         <v>209</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>3</v>
+        <v>327</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
-        <v>131</v>
+        <v>67</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>130</v>
+        <v>66</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>3</v>
+        <v>327</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
-        <v>80</v>
+        <v>114</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>86</v>
+        <v>113</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>3</v>
+        <v>327</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
-        <v>77</v>
+        <v>324</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>76</v>
+        <v>110</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>3</v>
+        <v>327</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
-        <v>289</v>
+        <v>323</v>
       </c>
       <c r="B46" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A48" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A49" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A50" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A51" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A52" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A53" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A54" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A55" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A56" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A57" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A58" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A59" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A60" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A61" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A62" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A63" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A64" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A65" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A66" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A67" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A68" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A69" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A70" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A71" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A72" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A73" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A74" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A75" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A76" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A77" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A78" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A79" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A80" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B81" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A82" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A83" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A84" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A85" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A86" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="B86" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C46" s="1" t="s">
+      <c r="C86" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D46" s="1" t="s">
+      <c r="D86" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A87" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A88" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A89" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A90" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="B90" s="1" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="92" ht="22.2" customHeight="1" x14ac:dyDescent="0.3"/>
+      <c r="C90" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D90" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A91" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D91" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A92" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D92" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A93" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D93" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A94" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D94" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A95" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D95" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A96" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D96" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A97" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D97" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
convocazioni stagione 126 war 1
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7ee4892a2dd36b84/Desktop/Link-clan/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="45" documentId="13_ncr:1_{9FCDD52C-4DCE-46C4-BB20-7F2264BA0663}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{042812D9-6459-4841-B302-D6C89AE84766}"/>
+  <xr:revisionPtr revIDLastSave="59" documentId="13_ncr:1_{9FCDD52C-4DCE-46C4-BB20-7F2264BA0663}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{90FA87AE-8E4C-4AFA-9CFB-2AB7005DEE02}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{FECCDA54-7594-4EB7-ABFB-2C408C6461DD}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="788" uniqueCount="386">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="767" uniqueCount="378">
   <si>
     <t>TagTelegram</t>
   </si>
@@ -855,9 +855,6 @@
     <t>@cvbalibre</t>
   </si>
   <si>
-    <t>AR♣️Cuba</t>
-  </si>
-  <si>
     <t>Torsiz</t>
   </si>
   <si>
@@ -876,12 +873,6 @@
     <t>\GuyFawkes/</t>
   </si>
   <si>
-    <t>Lind L. Taylor</t>
-  </si>
-  <si>
-    <t>@PharmaShooter</t>
-  </si>
-  <si>
     <t>@niflash</t>
   </si>
   <si>
@@ -999,9 +990,6 @@
     <t>@T0N1003</t>
   </si>
   <si>
-    <t>Dog Rider</t>
-  </si>
-  <si>
     <t>Lore</t>
   </si>
   <si>
@@ -1038,12 +1026,6 @@
     <t>@Gaia951</t>
   </si>
   <si>
-    <t>@Filantropo1010</t>
-  </si>
-  <si>
-    <t>@Lokkah</t>
-  </si>
-  <si>
     <t>Cry</t>
   </si>
   <si>
@@ -1053,15 +1035,6 @@
     <t>shinigami</t>
   </si>
   <si>
-    <t>Thor⚡️</t>
-  </si>
-  <si>
-    <t>ＡＲ♦️Ｆ❗️Ｌｏ</t>
-  </si>
-  <si>
-    <t>ＡＲ❤️ｉＳＡＭｕ</t>
-  </si>
-  <si>
     <t>@Andrew260903</t>
   </si>
   <si>
@@ -1080,12 +1053,6 @@
     <t>@BwoneJ</t>
   </si>
   <si>
-    <t>@ag0_96</t>
-  </si>
-  <si>
-    <t>@Christian00007</t>
-  </si>
-  <si>
     <t>@Augu05</t>
   </si>
   <si>
@@ -1107,12 +1074,6 @@
     <t>BwonE</t>
   </si>
   <si>
-    <t>SPARTACO_1996</t>
-  </si>
-  <si>
-    <t>christian</t>
-  </si>
-  <si>
     <t>Augu05</t>
   </si>
   <si>
@@ -1122,21 +1083,6 @@
     <t>Teodoro⠀Mapuzzi</t>
   </si>
   <si>
-    <t>Quizzz</t>
-  </si>
-  <si>
-    <t>PIZZALILLO</t>
-  </si>
-  <si>
-    <t>ＡＲ♠️Ｐｅｒｓｅｕｓ</t>
-  </si>
-  <si>
-    <t>ＡＲ♣️Ｃａｐｏｎｅ⚡️</t>
-  </si>
-  <si>
-    <t>ＡＲ♣️ＳｎｏｏｐＲｏｚｚ☘️</t>
-  </si>
-  <si>
     <t>@AndreaB2005</t>
   </si>
   <si>
@@ -1146,12 +1092,6 @@
     <t>@of_mike</t>
   </si>
   <si>
-    <t>@Deso121</t>
-  </si>
-  <si>
-    <t>@Lucky_Puere</t>
-  </si>
-  <si>
     <t>@Basco3</t>
   </si>
   <si>
@@ -1161,21 +1101,9 @@
     <t>@Cisco00001</t>
   </si>
   <si>
-    <t>@capo</t>
-  </si>
-  <si>
-    <t>khmer BM⚡️</t>
-  </si>
-  <si>
     <t>of_mike</t>
   </si>
   <si>
-    <t>Deso_JR</t>
-  </si>
-  <si>
-    <t>Lucky Luciano</t>
-  </si>
-  <si>
     <t>Basco</t>
   </si>
   <si>
@@ -1188,10 +1116,58 @@
     <t>teo</t>
   </si>
   <si>
-    <t>♦️Ｅｌ Ｍａｔａｒｏｚｚ™️</t>
-  </si>
-  <si>
     <t>I Tori Feroci</t>
+  </si>
+  <si>
+    <t>@kedelu27</t>
+  </si>
+  <si>
+    <t>@Poddybig</t>
+  </si>
+  <si>
+    <t>Cuba❤️Eren</t>
+  </si>
+  <si>
+    <t>Ａｒ❤Ｓａｍｕｅｌｅ</t>
+  </si>
+  <si>
+    <t>⭐Marco⭐</t>
+  </si>
+  <si>
+    <t>AR♣️KeDelu</t>
+  </si>
+  <si>
+    <t>Poddy big</t>
+  </si>
+  <si>
+    <t>Sønサル•D•Lůffy</t>
+  </si>
+  <si>
+    <t>Thor⚡</t>
+  </si>
+  <si>
+    <t>⚡MAJOR⚡</t>
+  </si>
+  <si>
+    <t>IronMan</t>
+  </si>
+  <si>
+    <t>gilbe03</t>
+  </si>
+  <si>
+    <t>Bregs!</t>
+  </si>
+  <si>
+    <t>Dani</t>
+  </si>
+  <si>
+    <t>@ElTibe</t>
+  </si>
+  <si>
+    <t>khmer BM⚡</t>
+  </si>
+  <si>
+    <t>Warlosing</t>
   </si>
 </sst>
 </file>
@@ -2055,10 +2031,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EE2B0F9-AC31-464B-B046-53CB033C8615}">
-  <dimension ref="A1:D137"/>
+  <dimension ref="A1:D132"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="C101" sqref="C52:C101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2091,10 +2067,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>330</v>
+        <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>274</v>
+        <v>4</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>3</v>
@@ -2105,10 +2081,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>23</v>
+        <v>326</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>22</v>
+        <v>273</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>3</v>
@@ -2119,10 +2095,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>91</v>
+        <v>31</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>136</v>
+        <v>30</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>3</v>
@@ -2133,10 +2109,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>30</v>
+        <v>332</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>3</v>
@@ -2147,10 +2123,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>21</v>
+        <v>272</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>192</v>
+        <v>363</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>3</v>
@@ -2161,10 +2137,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>126</v>
+        <v>27</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>125</v>
+        <v>26</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>3</v>
@@ -2175,10 +2151,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>105</v>
+        <v>23</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>104</v>
+        <v>22</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>3</v>
@@ -2189,10 +2165,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>268</v>
+        <v>5</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>276</v>
+        <v>9</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>3</v>
@@ -2203,10 +2179,10 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>5</v>
+        <v>269</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>9</v>
+        <v>274</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>3</v>
@@ -2217,10 +2193,10 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>269</v>
+        <v>33</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>275</v>
+        <v>32</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>3</v>
@@ -2245,10 +2221,10 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>325</v>
+        <v>126</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>322</v>
+        <v>125</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>3</v>
@@ -2259,10 +2235,10 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>27</v>
+        <v>88</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>26</v>
+        <v>87</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>3</v>
@@ -2287,10 +2263,10 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>272</v>
+        <v>91</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>273</v>
+        <v>136</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>3</v>
@@ -2301,10 +2277,10 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>33</v>
+        <v>327</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>32</v>
+        <v>330</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>3</v>
@@ -2315,10 +2291,10 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>270</v>
+        <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>277</v>
+        <v>16</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>3</v>
@@ -2329,10 +2305,10 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>266</v>
+        <v>37</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>279</v>
+        <v>36</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>3</v>
@@ -2343,10 +2319,10 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>98</v>
+        <v>41</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>227</v>
+        <v>40</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>3</v>
@@ -2357,10 +2333,10 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>331</v>
+        <v>21</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>336</v>
+        <v>364</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>3</v>
@@ -2371,10 +2347,10 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>29</v>
+        <v>328</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>3</v>
@@ -2385,10 +2361,10 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>88</v>
+        <v>105</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>87</v>
+        <v>104</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>3</v>
@@ -2399,10 +2375,10 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>8</v>
+        <v>268</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>45</v>
+        <v>275</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>3</v>
@@ -2413,10 +2389,10 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>13</v>
+        <v>266</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>12</v>
+        <v>278</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>3</v>
@@ -2427,10 +2403,10 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>3</v>
@@ -2441,10 +2417,10 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>43</v>
+        <v>260</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>42</v>
+        <v>241</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>3</v>
@@ -2455,10 +2431,10 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>3</v>
@@ -2468,11 +2444,8 @@
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" s="1" t="s">
-        <v>25</v>
-      </c>
       <c r="B29" s="1" t="s">
-        <v>24</v>
+        <v>267</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>3</v>
@@ -2482,8 +2455,11 @@
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="B30" s="1" t="s">
-        <v>267</v>
+        <v>12</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>3</v>
@@ -2494,10 +2470,10 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>332</v>
+        <v>98</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>18</v>
+        <v>365</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>3</v>
@@ -2508,10 +2484,10 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>148</v>
+        <v>361</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>143</v>
+        <v>366</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>3</v>
@@ -2522,10 +2498,10 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>41</v>
+        <v>279</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>40</v>
+        <v>347</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>3</v>
@@ -2536,10 +2512,10 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>333</v>
+        <v>303</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>337</v>
+        <v>63</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>3</v>
@@ -2550,10 +2526,10 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>11</v>
+        <v>339</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>338</v>
+        <v>346</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>3</v>
@@ -2564,10 +2540,10 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>5</v>
+        <v>317</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>4</v>
+        <v>298</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>3</v>
@@ -2578,10 +2554,10 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
-        <v>20</v>
+        <v>349</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>19</v>
+        <v>291</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>3</v>
@@ -2592,10 +2568,10 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>150</v>
+        <v>362</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>147</v>
+        <v>367</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>3</v>
@@ -2606,10 +2582,10 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
-        <v>11</v>
+        <v>300</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>10</v>
+        <v>109</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>3</v>
@@ -2620,10 +2596,10 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>339</v>
+        <v>10</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>3</v>
@@ -2634,10 +2610,10 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
-        <v>329</v>
+        <v>20</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>145</v>
+        <v>368</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>3</v>
@@ -2648,10 +2624,10 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
-        <v>334</v>
+        <v>20</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>340</v>
+        <v>369</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>3</v>
@@ -2662,10 +2638,10 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
-        <v>335</v>
+        <v>325</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>341</v>
+        <v>145</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>3</v>
@@ -2676,13 +2652,13 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
-        <v>77</v>
+        <v>340</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>76</v>
+        <v>138</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>321</v>
+        <v>3</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>271</v>
@@ -2690,13 +2666,13 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
-        <v>306</v>
+        <v>8</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>321</v>
+        <v>3</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>271</v>
@@ -2704,13 +2680,13 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
-        <v>82</v>
+        <v>354</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>81</v>
+        <v>358</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>321</v>
+        <v>3</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>271</v>
@@ -2718,13 +2694,13 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
-        <v>114</v>
+        <v>270</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>113</v>
+        <v>276</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>321</v>
+        <v>3</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>271</v>
@@ -2732,13 +2708,13 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
-        <v>84</v>
+        <v>108</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>278</v>
+        <v>107</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>321</v>
+        <v>3</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>271</v>
@@ -2746,13 +2722,13 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
-        <v>319</v>
+        <v>334</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>300</v>
+        <v>342</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>321</v>
+        <v>3</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>271</v>
@@ -2760,13 +2736,13 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
-        <v>303</v>
+        <v>71</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>109</v>
+        <v>70</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>321</v>
+        <v>3</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>271</v>
@@ -2774,13 +2750,13 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
-        <v>316</v>
+        <v>75</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>296</v>
+        <v>74</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>321</v>
+        <v>3</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>271</v>
@@ -2788,13 +2764,13 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
-        <v>108</v>
+        <v>316</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>107</v>
+        <v>297</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>321</v>
+        <v>360</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>271</v>
@@ -2802,13 +2778,13 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
-        <v>342</v>
+        <v>73</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>352</v>
+        <v>72</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>321</v>
+        <v>360</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>271</v>
@@ -2816,13 +2792,13 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
-        <v>93</v>
+        <v>333</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>92</v>
+        <v>341</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>321</v>
+        <v>360</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>271</v>
@@ -2830,13 +2806,13 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
-        <v>343</v>
+        <v>265</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>353</v>
+        <v>252</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>321</v>
+        <v>360</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>271</v>
@@ -2844,13 +2820,13 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
-        <v>308</v>
+        <v>122</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>288</v>
+        <v>370</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>321</v>
+        <v>360</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>271</v>
@@ -2858,13 +2834,13 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
-        <v>305</v>
+        <v>315</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>286</v>
+        <v>110</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>321</v>
+        <v>360</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>271</v>
@@ -2872,13 +2848,13 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>321</v>
+        <v>360</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>271</v>
@@ -2886,13 +2862,13 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
-        <v>112</v>
+        <v>305</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>111</v>
+        <v>285</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>321</v>
+        <v>360</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>271</v>
@@ -2900,13 +2876,13 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
-        <v>41</v>
+        <v>307</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>354</v>
+        <v>288</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>321</v>
+        <v>360</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>271</v>
@@ -2914,13 +2890,13 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
-        <v>344</v>
+        <v>299</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>355</v>
+        <v>280</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>321</v>
+        <v>360</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>271</v>
@@ -2928,13 +2904,13 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
-        <v>345</v>
+        <v>112</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>289</v>
+        <v>111</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>321</v>
+        <v>360</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>271</v>
@@ -2942,13 +2918,13 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
-        <v>121</v>
+        <v>324</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>120</v>
+        <v>319</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>321</v>
+        <v>360</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>271</v>
@@ -2956,13 +2932,13 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
-        <v>312</v>
+        <v>302</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>292</v>
+        <v>283</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>321</v>
+        <v>360</v>
       </c>
       <c r="D64" s="1" t="s">
         <v>271</v>
@@ -2970,13 +2946,13 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
-        <v>128</v>
+        <v>350</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>127</v>
+        <v>294</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>321</v>
+        <v>360</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>271</v>
@@ -2984,13 +2960,13 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>68</v>
+        <v>287</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>321</v>
+        <v>360</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>271</v>
@@ -2998,13 +2974,13 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
-        <v>52</v>
+        <v>148</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>51</v>
+        <v>348</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>321</v>
+        <v>360</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>271</v>
@@ -3012,13 +2988,13 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
-        <v>100</v>
+        <v>261</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>99</v>
+        <v>242</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>321</v>
+        <v>360</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>271</v>
@@ -3026,13 +3002,13 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
-        <v>317</v>
+        <v>93</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>298</v>
+        <v>92</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>321</v>
+        <v>360</v>
       </c>
       <c r="D69" s="1" t="s">
         <v>271</v>
@@ -3040,13 +3016,13 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
-        <v>263</v>
+        <v>336</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>249</v>
+        <v>286</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>321</v>
+        <v>360</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>271</v>
@@ -3054,13 +3030,13 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
-        <v>89</v>
+        <v>301</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>132</v>
+        <v>282</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>321</v>
+        <v>360</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>271</v>
@@ -3068,13 +3044,13 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
-        <v>346</v>
+        <v>308</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>83</v>
+        <v>68</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>321</v>
+        <v>360</v>
       </c>
       <c r="D72" s="1" t="s">
         <v>271</v>
@@ -3082,13 +3058,13 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
-        <v>59</v>
+        <v>79</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>321</v>
+        <v>360</v>
       </c>
       <c r="D73" s="1" t="s">
         <v>271</v>
@@ -3096,13 +3072,13 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
-        <v>265</v>
+        <v>353</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>252</v>
+        <v>357</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>321</v>
+        <v>360</v>
       </c>
       <c r="D74" s="1" t="s">
         <v>271</v>
@@ -3110,13 +3086,13 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
-        <v>347</v>
+        <v>52</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>356</v>
+        <v>51</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>321</v>
+        <v>360</v>
       </c>
       <c r="D75" s="1" t="s">
         <v>271</v>
@@ -3124,13 +3100,13 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
-        <v>116</v>
+        <v>80</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>115</v>
+        <v>86</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>321</v>
+        <v>360</v>
       </c>
       <c r="D76" s="1" t="s">
         <v>271</v>
@@ -3138,13 +3114,13 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
-        <v>348</v>
+        <v>309</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>357</v>
+        <v>289</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>321</v>
+        <v>360</v>
       </c>
       <c r="D77" s="1" t="s">
         <v>271</v>
@@ -3152,13 +3128,13 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
-        <v>349</v>
+        <v>257</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>358</v>
+        <v>254</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>321</v>
+        <v>360</v>
       </c>
       <c r="D78" s="1" t="s">
         <v>271</v>
@@ -3166,13 +3142,13 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
-        <v>350</v>
+        <v>311</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>359</v>
+        <v>103</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>321</v>
+        <v>360</v>
       </c>
       <c r="D79" s="1" t="s">
         <v>271</v>
@@ -3180,13 +3156,13 @@
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
-        <v>282</v>
+        <v>121</v>
       </c>
       <c r="B80" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C80" s="1" t="s">
         <v>360</v>
-      </c>
-      <c r="C80" s="1" t="s">
-        <v>321</v>
       </c>
       <c r="D80" s="1" t="s">
         <v>271</v>
@@ -3194,13 +3170,13 @@
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
-        <v>351</v>
+        <v>56</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>138</v>
+        <v>55</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>321</v>
+        <v>360</v>
       </c>
       <c r="D81" s="1" t="s">
         <v>271</v>
@@ -3208,13 +3184,13 @@
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
-        <v>326</v>
+        <v>312</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>129</v>
+        <v>292</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>321</v>
+        <v>360</v>
       </c>
       <c r="D82" s="1" t="s">
         <v>271</v>
@@ -3222,13 +3198,13 @@
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
-        <v>148</v>
+        <v>259</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>361</v>
+        <v>281</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>321</v>
+        <v>360</v>
       </c>
       <c r="D83" s="1" t="s">
         <v>271</v>
@@ -3236,13 +3212,13 @@
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
-        <v>329</v>
+        <v>128</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>362</v>
+        <v>127</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>321</v>
+        <v>360</v>
       </c>
       <c r="D84" s="1" t="s">
         <v>271</v>
@@ -3250,13 +3226,13 @@
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
-        <v>329</v>
+        <v>100</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>363</v>
+        <v>99</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>321</v>
+        <v>360</v>
       </c>
       <c r="D85" s="1" t="s">
         <v>271</v>
@@ -3264,35 +3240,41 @@
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
-        <v>329</v>
+        <v>310</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>364</v>
+        <v>290</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>321</v>
+        <v>360</v>
       </c>
       <c r="D86" s="1" t="s">
         <v>271</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A87" s="1" t="s">
+        <v>263</v>
+      </c>
       <c r="B87" s="1" t="s">
-        <v>365</v>
+        <v>249</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>321</v>
+        <v>360</v>
       </c>
       <c r="D87" s="1" t="s">
         <v>271</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A88" s="1" t="s">
+        <v>117</v>
+      </c>
       <c r="B88" s="1" t="s">
-        <v>366</v>
+        <v>133</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>321</v>
+        <v>360</v>
       </c>
       <c r="D88" s="1" t="s">
         <v>271</v>
@@ -3300,13 +3282,13 @@
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
-        <v>281</v>
+        <v>314</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>280</v>
+        <v>295</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>385</v>
+        <v>360</v>
       </c>
       <c r="D89" s="1" t="s">
         <v>271</v>
@@ -3314,13 +3296,13 @@
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
-        <v>324</v>
+        <v>351</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>376</v>
+        <v>355</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>385</v>
+        <v>360</v>
       </c>
       <c r="D90" s="1" t="s">
         <v>271</v>
@@ -3328,13 +3310,13 @@
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
-        <v>282</v>
+        <v>89</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>60</v>
+        <v>132</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>385</v>
+        <v>360</v>
       </c>
       <c r="D91" s="1" t="s">
         <v>271</v>
@@ -3342,13 +3324,13 @@
     </row>
     <row r="92" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="s">
-        <v>318</v>
+        <v>41</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>110</v>
+        <v>343</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>385</v>
+        <v>360</v>
       </c>
       <c r="D92" s="1" t="s">
         <v>271</v>
@@ -3356,27 +3338,24 @@
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
-        <v>327</v>
+        <v>335</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>44</v>
+        <v>344</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>385</v>
+        <v>360</v>
       </c>
       <c r="D93" s="1" t="s">
         <v>271</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A94" s="1" t="s">
-        <v>258</v>
-      </c>
       <c r="B94" s="1" t="s">
-        <v>209</v>
+        <v>371</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>385</v>
+        <v>360</v>
       </c>
       <c r="D94" s="1" t="s">
         <v>271</v>
@@ -3384,13 +3363,13 @@
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="s">
-        <v>328</v>
+        <v>54</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>323</v>
+        <v>53</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>385</v>
+        <v>360</v>
       </c>
       <c r="D95" s="1" t="s">
         <v>271</v>
@@ -3398,41 +3377,35 @@
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="s">
-        <v>7</v>
+        <v>375</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>6</v>
+        <v>372</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>385</v>
+        <v>360</v>
       </c>
       <c r="D96" s="1" t="s">
         <v>271</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A97" s="1" t="s">
-        <v>131</v>
-      </c>
       <c r="B97" s="1" t="s">
-        <v>130</v>
+        <v>373</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>385</v>
+        <v>360</v>
       </c>
       <c r="D97" s="1" t="s">
         <v>271</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A98" s="1" t="s">
-        <v>75</v>
-      </c>
       <c r="B98" s="1" t="s">
-        <v>74</v>
+        <v>374</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>385</v>
+        <v>360</v>
       </c>
       <c r="D98" s="1" t="s">
         <v>271</v>
@@ -3440,13 +3413,13 @@
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
-        <v>67</v>
+        <v>340</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>66</v>
+        <v>359</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>385</v>
+        <v>360</v>
       </c>
       <c r="D99" s="1" t="s">
         <v>271</v>
@@ -3454,13 +3427,13 @@
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="s">
-        <v>71</v>
+        <v>313</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>70</v>
+        <v>293</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>385</v>
+        <v>360</v>
       </c>
       <c r="D100" s="1" t="s">
         <v>271</v>
@@ -3468,13 +3441,13 @@
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101" s="1" t="s">
-        <v>302</v>
+        <v>313</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>283</v>
+        <v>296</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>385</v>
+        <v>360</v>
       </c>
       <c r="D101" s="1" t="s">
         <v>271</v>
@@ -3482,13 +3455,13 @@
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102" s="1" t="s">
-        <v>304</v>
+        <v>8</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>285</v>
+        <v>45</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>385</v>
+        <v>377</v>
       </c>
       <c r="D102" s="1" t="s">
         <v>271</v>
@@ -3496,13 +3469,13 @@
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103" s="1" t="s">
-        <v>367</v>
+        <v>43</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>294</v>
+        <v>42</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>385</v>
+        <v>377</v>
       </c>
       <c r="D103" s="1" t="s">
         <v>271</v>
@@ -3510,13 +3483,13 @@
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104" s="1" t="s">
-        <v>122</v>
+        <v>354</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>245</v>
+        <v>358</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>385</v>
+        <v>377</v>
       </c>
       <c r="D104" s="1" t="s">
         <v>271</v>
@@ -3524,13 +3497,13 @@
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105" s="1" t="s">
-        <v>65</v>
+        <v>270</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>64</v>
+        <v>276</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>385</v>
+        <v>377</v>
       </c>
       <c r="D105" s="1" t="s">
         <v>271</v>
@@ -3538,13 +3511,13 @@
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106" s="1" t="s">
-        <v>310</v>
+        <v>114</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>291</v>
+        <v>113</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>385</v>
+        <v>377</v>
       </c>
       <c r="D106" s="1" t="s">
         <v>271</v>
@@ -3552,13 +3525,13 @@
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107" s="1" t="s">
-        <v>368</v>
+        <v>322</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>297</v>
+        <v>129</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>385</v>
+        <v>377</v>
       </c>
       <c r="D107" s="1" t="s">
         <v>271</v>
@@ -3566,13 +3539,13 @@
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108" s="1" t="s">
-        <v>80</v>
+        <v>116</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>86</v>
+        <v>115</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>385</v>
+        <v>377</v>
       </c>
       <c r="D108" s="1" t="s">
         <v>271</v>
@@ -3580,13 +3553,13 @@
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A109" s="1" t="s">
-        <v>259</v>
+        <v>95</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>284</v>
+        <v>94</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>385</v>
+        <v>377</v>
       </c>
       <c r="D109" s="1" t="s">
         <v>271</v>
@@ -3594,13 +3567,13 @@
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110" s="1" t="s">
-        <v>149</v>
+        <v>329</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>146</v>
+        <v>331</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>385</v>
+        <v>377</v>
       </c>
       <c r="D110" s="1" t="s">
         <v>271</v>
@@ -3608,13 +3581,13 @@
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A111" s="1" t="s">
-        <v>257</v>
+        <v>148</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>254</v>
+        <v>143</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>385</v>
+        <v>377</v>
       </c>
       <c r="D111" s="1" t="s">
         <v>271</v>
@@ -3622,13 +3595,13 @@
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112" s="1" t="s">
-        <v>314</v>
+        <v>258</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>103</v>
+        <v>209</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>385</v>
+        <v>377</v>
       </c>
       <c r="D112" s="1" t="s">
         <v>271</v>
@@ -3636,13 +3609,13 @@
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A113" s="1" t="s">
-        <v>117</v>
+        <v>324</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>133</v>
+        <v>319</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>385</v>
+        <v>377</v>
       </c>
       <c r="D113" s="1" t="s">
         <v>271</v>
@@ -3650,13 +3623,13 @@
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A114" s="1" t="s">
-        <v>315</v>
+        <v>77</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>295</v>
+        <v>76</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>385</v>
+        <v>377</v>
       </c>
       <c r="D114" s="1" t="s">
         <v>271</v>
@@ -3664,13 +3637,13 @@
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A115" s="1" t="s">
-        <v>261</v>
+        <v>279</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>242</v>
+        <v>60</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>385</v>
+        <v>377</v>
       </c>
       <c r="D115" s="1" t="s">
         <v>271</v>
@@ -3678,13 +3651,13 @@
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A116" s="1" t="s">
-        <v>56</v>
+        <v>7</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>55</v>
+        <v>6</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>385</v>
+        <v>377</v>
       </c>
       <c r="D116" s="1" t="s">
         <v>271</v>
@@ -3692,13 +3665,13 @@
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A117" s="1" t="s">
-        <v>313</v>
+        <v>82</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>293</v>
+        <v>81</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>385</v>
+        <v>377</v>
       </c>
       <c r="D117" s="1" t="s">
         <v>271</v>
@@ -3706,13 +3679,13 @@
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A118" s="1" t="s">
-        <v>369</v>
+        <v>321</v>
       </c>
       <c r="B118" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="C118" s="1" t="s">
         <v>377</v>
-      </c>
-      <c r="C118" s="1" t="s">
-        <v>385</v>
       </c>
       <c r="D118" s="1" t="s">
         <v>271</v>
@@ -3720,13 +3693,13 @@
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A119" s="1" t="s">
-        <v>54</v>
+        <v>338</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>53</v>
+        <v>345</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>385</v>
+        <v>377</v>
       </c>
       <c r="D119" s="1" t="s">
         <v>271</v>
@@ -3734,13 +3707,13 @@
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A120" s="1" t="s">
-        <v>370</v>
+        <v>323</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>378</v>
+        <v>44</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>385</v>
+        <v>377</v>
       </c>
       <c r="D120" s="1" t="s">
         <v>271</v>
@@ -3748,13 +3721,13 @@
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A121" s="1" t="s">
-        <v>371</v>
+        <v>84</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>379</v>
+        <v>277</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>385</v>
+        <v>377</v>
       </c>
       <c r="D121" s="1" t="s">
         <v>271</v>
@@ -3762,13 +3735,13 @@
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A122" s="1" t="s">
-        <v>73</v>
+        <v>131</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>72</v>
+        <v>130</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>385</v>
+        <v>377</v>
       </c>
       <c r="D122" s="1" t="s">
         <v>271</v>
@@ -3776,13 +3749,13 @@
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A123" s="1" t="s">
-        <v>372</v>
+        <v>337</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>380</v>
+        <v>83</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>385</v>
+        <v>377</v>
       </c>
       <c r="D123" s="1" t="s">
         <v>271</v>
@@ -3790,13 +3763,13 @@
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A124" s="1" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>385</v>
+        <v>377</v>
       </c>
       <c r="D124" s="1" t="s">
         <v>271</v>
@@ -3804,13 +3777,13 @@
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A125" s="1" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>385</v>
+        <v>377</v>
       </c>
       <c r="D125" s="1" t="s">
         <v>271</v>
@@ -3818,13 +3791,13 @@
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A126" s="1" t="s">
-        <v>97</v>
+        <v>48</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>96</v>
+        <v>47</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>385</v>
+        <v>377</v>
       </c>
       <c r="D126" s="1" t="s">
         <v>271</v>
@@ -3832,13 +3805,13 @@
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A127" s="1" t="s">
-        <v>373</v>
+        <v>320</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>385</v>
+        <v>377</v>
       </c>
       <c r="D127" s="1" t="s">
         <v>271</v>
@@ -3846,13 +3819,13 @@
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A128" s="1" t="s">
-        <v>309</v>
+        <v>352</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>290</v>
+        <v>356</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>385</v>
+        <v>377</v>
       </c>
       <c r="D128" s="1" t="s">
         <v>271</v>
@@ -3860,13 +3833,13 @@
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A129" s="1" t="s">
-        <v>316</v>
+        <v>50</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>299</v>
+        <v>49</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>385</v>
+        <v>377</v>
       </c>
       <c r="D129" s="1" t="s">
         <v>271</v>
@@ -3874,13 +3847,13 @@
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A130" s="1" t="s">
-        <v>260</v>
+        <v>149</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>241</v>
+        <v>146</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>385</v>
+        <v>377</v>
       </c>
       <c r="D130" s="1" t="s">
         <v>271</v>
@@ -3888,13 +3861,13 @@
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A131" s="1" t="s">
-        <v>95</v>
+        <v>150</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>94</v>
+        <v>147</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>385</v>
+        <v>377</v>
       </c>
       <c r="D131" s="1" t="s">
         <v>271</v>
@@ -3902,85 +3875,15 @@
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A132" s="1" t="s">
-        <v>142</v>
+        <v>43</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>139</v>
+        <v>42</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>385</v>
+        <v>377</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A133" s="1" t="s">
-        <v>320</v>
-      </c>
-      <c r="B133" s="1" t="s">
-        <v>301</v>
-      </c>
-      <c r="C133" s="1" t="s">
-        <v>385</v>
-      </c>
-      <c r="D133" s="1" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A134" s="1" t="s">
-        <v>374</v>
-      </c>
-      <c r="B134" s="1" t="s">
-        <v>382</v>
-      </c>
-      <c r="C134" s="1" t="s">
-        <v>385</v>
-      </c>
-      <c r="D134" s="1" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A135" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B135" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C135" s="1" t="s">
-        <v>385</v>
-      </c>
-      <c r="D135" s="1" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A136" s="1" t="s">
-        <v>351</v>
-      </c>
-      <c r="B136" s="1" t="s">
-        <v>383</v>
-      </c>
-      <c r="C136" s="1" t="s">
-        <v>385</v>
-      </c>
-      <c r="D136" s="1" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A137" s="1" t="s">
-        <v>375</v>
-      </c>
-      <c r="B137" s="1" t="s">
-        <v>384</v>
-      </c>
-      <c r="C137" s="1" t="s">
-        <v>385</v>
-      </c>
-      <c r="D137" s="1" t="s">
         <v>271</v>
       </c>
     </row>

</xml_diff>

<commit_message>
convocazioni stagione 126 - 2
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7ee4892a2dd36b84/Desktop/Link-clan/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="71" documentId="13_ncr:1_{9FCDD52C-4DCE-46C4-BB20-7F2264BA0663}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F54EDF6A-C457-47CE-B928-815F4147E13C}"/>
+  <xr:revisionPtr revIDLastSave="92" documentId="13_ncr:1_{9FCDD52C-4DCE-46C4-BB20-7F2264BA0663}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A402727E-ED37-40B6-A952-BF879D789044}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{FECCDA54-7594-4EB7-ABFB-2C408C6461DD}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="747" uniqueCount="378">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="747" uniqueCount="384">
   <si>
     <t>TagTelegram</t>
   </si>
@@ -879,15 +879,9 @@
     <t>Antonio96</t>
   </si>
   <si>
-    <t>Zumpy</t>
-  </si>
-  <si>
     <t>Eric</t>
   </si>
   <si>
-    <t>Dino</t>
-  </si>
-  <si>
     <t>Geeno</t>
   </si>
   <si>
@@ -906,15 +900,6 @@
     <t>Royal Army</t>
   </si>
   <si>
-    <t>superfede</t>
-  </si>
-  <si>
-    <t>Andrea</t>
-  </si>
-  <si>
-    <t>RETROWAV3R™️</t>
-  </si>
-  <si>
     <t>fogu</t>
   </si>
   <si>
@@ -942,12 +927,6 @@
     <t>@srd_rce</t>
   </si>
   <si>
-    <t>@sunnering</t>
-  </si>
-  <si>
-    <t>@arsenapoli</t>
-  </si>
-  <si>
     <t>@Alestrega22</t>
   </si>
   <si>
@@ -966,15 +945,9 @@
     <t>@Davidone11</t>
   </si>
   <si>
-    <t>@superfede2</t>
-  </si>
-  <si>
     <t>@Manu2365</t>
   </si>
   <si>
-    <t>@RETROWAV3R</t>
-  </si>
-  <si>
     <t>@BBCTR3</t>
   </si>
   <si>
@@ -1065,9 +1038,6 @@
     <t>Mr.Fox</t>
   </si>
   <si>
-    <t>Raffaele11</t>
-  </si>
-  <si>
     <t>manuel1903</t>
   </si>
   <si>
@@ -1083,15 +1053,9 @@
     <t>Teodoro⠀Mapuzzi</t>
   </si>
   <si>
-    <t>@AndreaB2005</t>
-  </si>
-  <si>
     <t>@gioee_e27</t>
   </si>
   <si>
-    <t>@of_mike</t>
-  </si>
-  <si>
     <t>@Basco3</t>
   </si>
   <si>
@@ -1101,9 +1065,6 @@
     <t>@Cisco00001</t>
   </si>
   <si>
-    <t>of_mike</t>
-  </si>
-  <si>
     <t>Basco</t>
   </si>
   <si>
@@ -1128,12 +1089,6 @@
     <t>Cuba❤️Eren</t>
   </si>
   <si>
-    <t>Ａｒ❤Ｓａｍｕｅｌｅ</t>
-  </si>
-  <si>
-    <t>⭐Marco⭐</t>
-  </si>
-  <si>
     <t>AR♣️KeDelu</t>
   </si>
   <si>
@@ -1143,38 +1098,101 @@
     <t>Sønサル•D•Lůffy</t>
   </si>
   <si>
-    <t>Thor⚡</t>
-  </si>
-  <si>
-    <t>⚡MAJOR⚡</t>
-  </si>
-  <si>
-    <t>IronMan</t>
-  </si>
-  <si>
-    <t>gilbe03</t>
-  </si>
-  <si>
     <t>Bregs!</t>
   </si>
   <si>
-    <t>Dani</t>
-  </si>
-  <si>
-    <t>@ElTibe</t>
-  </si>
-  <si>
-    <t>khmer BM⚡</t>
-  </si>
-  <si>
     <t>Warlosing</t>
+  </si>
+  <si>
+    <t>ＡＲ❤️Ｔｅｆａｎｏｓ</t>
+  </si>
+  <si>
+    <t>Thor⚡️</t>
+  </si>
+  <si>
+    <t>Gianlomb</t>
+  </si>
+  <si>
+    <t>@Gianlomb</t>
+  </si>
+  <si>
+    <t>khmer BM⚡️</t>
+  </si>
+  <si>
+    <t>mastro olivo</t>
+  </si>
+  <si>
+    <t>ItsMeYUKKI</t>
+  </si>
+  <si>
+    <t>@Yukki1_618</t>
+  </si>
+  <si>
+    <t>Lind L. Taylor</t>
+  </si>
+  <si>
+    <t>TOTAL DISASTER</t>
+  </si>
+  <si>
+    <t>Quizzz</t>
+  </si>
+  <si>
+    <t>cech04</t>
+  </si>
+  <si>
+    <t>a.j</t>
+  </si>
+  <si>
+    <t>SbranaClash300#</t>
+  </si>
+  <si>
+    <t>Maradona</t>
+  </si>
+  <si>
+    <t>jamino</t>
+  </si>
+  <si>
+    <t>long island</t>
+  </si>
+  <si>
+    <t>RedShift</t>
+  </si>
+  <si>
+    <t>GXSALVO08</t>
+  </si>
+  <si>
+    <t>Nik</t>
+  </si>
+  <si>
+    <t>@PharmaShooter</t>
+  </si>
+  <si>
+    <t>@The_Lore27</t>
+  </si>
+  <si>
+    <t>@X_teo</t>
+  </si>
+  <si>
+    <t>@SranaClash300</t>
+  </si>
+  <si>
+    <t>@fabri1010</t>
+  </si>
+  <si>
+    <t>@Longisland02</t>
+  </si>
+  <si>
+    <t>@GXSALVO08</t>
+  </si>
+  <si>
+    <t>@hehehejs</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1308,6 +1326,12 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="33">
@@ -1651,9 +1675,15 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1701,7 +1731,7 @@
     <cellStyle name="Valore non valido" xfId="7" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Valore valido" xfId="6" builtinId="26" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="11">
+  <dxfs count="5">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1723,58 +1753,12 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
       <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1789,10 +1773,12 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
       <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2126,10 +2112,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EE2B0F9-AC31-464B-B046-53CB033C8615}">
-  <dimension ref="A1:D127"/>
+  <dimension ref="A1:D128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A123" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B63" sqref="B63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2162,13 +2148,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>6</v>
+        <v>353</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>377</v>
+        <v>3</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>271</v>
@@ -2176,13 +2162,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>322</v>
+        <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>129</v>
+        <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>377</v>
+        <v>3</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>271</v>
@@ -2190,10 +2176,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>45</v>
+        <v>323</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>3</v>
@@ -2204,10 +2190,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>5</v>
+        <v>317</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>4</v>
+        <v>273</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>3</v>
@@ -2218,10 +2204,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>3</v>
@@ -2232,27 +2218,24 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>149</v>
+        <v>272</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>146</v>
+        <v>350</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>377</v>
+        <v>3</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>271</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>304</v>
-      </c>
       <c r="B8" s="1" t="s">
-        <v>284</v>
+        <v>356</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>377</v>
+        <v>3</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>271</v>
@@ -2260,10 +2243,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>349</v>
+        <v>11</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>291</v>
+        <v>10</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>3</v>
@@ -2274,13 +2257,13 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>333</v>
+        <v>33</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>341</v>
+        <v>32</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>360</v>
+        <v>3</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>271</v>
@@ -2288,13 +2271,13 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>93</v>
+        <v>269</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>92</v>
+        <v>274</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>360</v>
+        <v>3</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>271</v>
@@ -2302,10 +2285,10 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>26</v>
+        <v>357</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>3</v>
@@ -2316,10 +2299,10 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>303</v>
+        <v>21</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>63</v>
+        <v>192</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>3</v>
@@ -2330,13 +2313,13 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>315</v>
+        <v>279</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>110</v>
+        <v>337</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>360</v>
+        <v>3</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>271</v>
@@ -2344,10 +2327,10 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>339</v>
+        <v>37</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>346</v>
+        <v>36</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>3</v>
@@ -2358,10 +2341,10 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>325</v>
+        <v>319</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>145</v>
+        <v>18</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>3</v>
@@ -2372,10 +2355,10 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>340</v>
+        <v>270</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>138</v>
+        <v>276</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>3</v>
@@ -2386,13 +2369,13 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>340</v>
+        <v>126</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>359</v>
+        <v>125</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>360</v>
+        <v>3</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>271</v>
@@ -2400,13 +2383,13 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>352</v>
+        <v>331</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>356</v>
+        <v>138</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>377</v>
+        <v>3</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>271</v>
@@ -2414,13 +2397,13 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>313</v>
+        <v>27</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>293</v>
+        <v>26</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>360</v>
+        <v>3</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>271</v>
@@ -2428,13 +2411,13 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>313</v>
+        <v>39</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>296</v>
+        <v>38</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>360</v>
+        <v>3</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>271</v>
@@ -2442,13 +2425,13 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>114</v>
+        <v>88</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>113</v>
+        <v>87</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>377</v>
+        <v>3</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>271</v>
@@ -2456,10 +2439,10 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>328</v>
+        <v>29</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>3</v>
@@ -2470,10 +2453,10 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>23</v>
+        <v>348</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>22</v>
+        <v>351</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>3</v>
@@ -2484,13 +2467,13 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>261</v>
+        <v>318</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>242</v>
+        <v>321</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>360</v>
+        <v>3</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>271</v>
@@ -2498,10 +2481,10 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>3</v>
@@ -2512,10 +2495,10 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>21</v>
+        <v>316</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>364</v>
+        <v>145</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>3</v>
@@ -2526,13 +2509,13 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>338</v>
+        <v>91</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>345</v>
+        <v>136</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>377</v>
+        <v>3</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>271</v>
@@ -2540,13 +2523,13 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>377</v>
+        <v>3</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>271</v>
@@ -2554,13 +2537,13 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>84</v>
+        <v>330</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>277</v>
+        <v>336</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>377</v>
+        <v>3</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>271</v>
@@ -2568,13 +2551,13 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>354</v>
+        <v>266</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>358</v>
+        <v>278</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>377</v>
+        <v>3</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>271</v>
@@ -2582,13 +2565,13 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>320</v>
+        <v>260</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>376</v>
+        <v>241</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>377</v>
+        <v>3</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>271</v>
@@ -2596,13 +2579,13 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>258</v>
+        <v>15</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>209</v>
+        <v>14</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>377</v>
+        <v>3</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>271</v>
@@ -2610,10 +2593,10 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>3</v>
@@ -2624,10 +2607,10 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>272</v>
+        <v>98</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>363</v>
+        <v>227</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>3</v>
@@ -2638,10 +2621,10 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>31</v>
+        <v>349</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>30</v>
+        <v>352</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>3</v>
@@ -2652,13 +2635,13 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
-        <v>309</v>
+        <v>17</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>289</v>
+        <v>16</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>360</v>
+        <v>3</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>271</v>
@@ -2666,13 +2649,13 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>52</v>
+        <v>325</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>51</v>
+        <v>333</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>360</v>
+        <v>3</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>271</v>
@@ -2680,10 +2663,10 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
-        <v>105</v>
+        <v>75</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>104</v>
+        <v>74</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>3</v>
@@ -2693,14 +2676,11 @@
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A40" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>254</v>
+      <c r="B40" s="2" t="s">
+        <v>267</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>360</v>
+        <v>3</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>271</v>
@@ -2708,13 +2688,13 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
-        <v>67</v>
+        <v>108</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>66</v>
+        <v>107</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>360</v>
+        <v>3</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>271</v>
@@ -2722,13 +2702,13 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
-        <v>375</v>
+        <v>306</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>372</v>
+        <v>110</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>360</v>
+        <v>3</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>271</v>
@@ -2736,13 +2716,13 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
-        <v>259</v>
+        <v>299</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>360</v>
+        <v>3</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>271</v>
@@ -2750,10 +2730,10 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
-        <v>11</v>
+        <v>73</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>332</v>
+        <v>72</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>3</v>
@@ -2764,10 +2744,10 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
-        <v>11</v>
+        <v>303</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>10</v>
+        <v>103</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>3</v>
@@ -2778,10 +2758,10 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
-        <v>334</v>
+        <v>307</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>342</v>
+        <v>292</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>3</v>
@@ -2792,13 +2772,13 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
-        <v>73</v>
+        <v>359</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>72</v>
+        <v>358</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>360</v>
+        <v>3</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>271</v>
@@ -2806,13 +2786,13 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
-        <v>305</v>
+        <v>296</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>360</v>
+        <v>3</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>271</v>
@@ -2820,13 +2800,13 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
-        <v>329</v>
+        <v>6</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>331</v>
+        <v>7</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>377</v>
+        <v>355</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>271</v>
@@ -2834,13 +2814,13 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
-        <v>307</v>
+        <v>129</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>288</v>
+        <v>313</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>271</v>
@@ -2848,13 +2828,13 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
-        <v>350</v>
+        <v>146</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>294</v>
+        <v>149</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>271</v>
@@ -2862,13 +2842,13 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
-        <v>75</v>
+        <v>282</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>74</v>
+        <v>297</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>3</v>
+        <v>355</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>271</v>
@@ -2876,13 +2856,13 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
-        <v>266</v>
+        <v>343</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>278</v>
+        <v>340</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>3</v>
+        <v>355</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>271</v>
@@ -2890,13 +2870,13 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
-        <v>265</v>
+        <v>113</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>252</v>
+        <v>114</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>271</v>
@@ -2904,13 +2884,13 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
-        <v>324</v>
+        <v>335</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>319</v>
+        <v>329</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>271</v>
@@ -2918,13 +2898,13 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
-        <v>112</v>
+        <v>47</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>111</v>
+        <v>48</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>271</v>
@@ -2932,13 +2912,13 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
-        <v>300</v>
+        <v>277</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>109</v>
+        <v>84</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>3</v>
+        <v>355</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>271</v>
@@ -2946,13 +2926,13 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
-        <v>361</v>
+        <v>345</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>3</v>
+        <v>355</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>271</v>
@@ -2960,13 +2940,13 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
-        <v>263</v>
+        <v>360</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>249</v>
+        <v>311</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>271</v>
@@ -2974,13 +2954,13 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
-        <v>89</v>
+        <v>209</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>132</v>
+        <v>258</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>271</v>
@@ -2988,13 +2968,13 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
-        <v>95</v>
+        <v>322</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>94</v>
+        <v>320</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>377</v>
+        <v>355</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>271</v>
@@ -3002,13 +2982,13 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
-        <v>117</v>
+        <v>94</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>133</v>
+        <v>95</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>271</v>
@@ -3016,13 +2996,13 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
-        <v>260</v>
+        <v>147</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>241</v>
+        <v>150</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>3</v>
+        <v>355</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>271</v>
@@ -3030,13 +3010,13 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
-        <v>88</v>
+        <v>143</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>87</v>
+        <v>148</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>3</v>
+        <v>355</v>
       </c>
       <c r="D64" s="1" t="s">
         <v>271</v>
@@ -3044,13 +3024,13 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
-        <v>108</v>
+        <v>64</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>107</v>
+        <v>65</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>3</v>
+        <v>355</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>271</v>
@@ -3058,13 +3038,13 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
-        <v>306</v>
+        <v>130</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>287</v>
+        <v>131</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>271</v>
@@ -3072,13 +3052,13 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>86</v>
+        <v>279</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>271</v>
@@ -3086,13 +3066,13 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>271</v>
@@ -3100,13 +3080,13 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
-        <v>122</v>
+        <v>83</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>370</v>
+        <v>328</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
       <c r="D69" s="1" t="s">
         <v>271</v>
@@ -3114,13 +3094,13 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B70" s="1" t="s">
         <v>314</v>
       </c>
-      <c r="B70" s="1" t="s">
-        <v>295</v>
-      </c>
       <c r="C70" s="1" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>271</v>
@@ -3128,13 +3108,13 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
-        <v>327</v>
+        <v>115</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>330</v>
+        <v>116</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>3</v>
+        <v>355</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>271</v>
@@ -3142,13 +3122,13 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
-        <v>311</v>
+        <v>81</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>103</v>
+        <v>82</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
       <c r="D72" s="1" t="s">
         <v>271</v>
@@ -3156,13 +3136,13 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
-        <v>335</v>
+        <v>309</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>344</v>
+        <v>312</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
       <c r="D73" s="1" t="s">
         <v>271</v>
@@ -3170,13 +3150,13 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>3</v>
+        <v>355</v>
       </c>
       <c r="D74" s="1" t="s">
         <v>271</v>
@@ -3184,13 +3164,13 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
-        <v>98</v>
+        <v>76</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>365</v>
+        <v>77</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>3</v>
+        <v>355</v>
       </c>
       <c r="D75" s="1" t="s">
         <v>271</v>
@@ -3198,13 +3178,13 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
-        <v>150</v>
+        <v>361</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>377</v>
+        <v>355</v>
       </c>
       <c r="D76" s="1" t="s">
         <v>271</v>
@@ -3212,13 +3192,13 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
-        <v>148</v>
+        <v>22</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>348</v>
+        <v>23</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
       <c r="D77" s="1" t="s">
         <v>271</v>
@@ -3226,13 +3206,13 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
-        <v>148</v>
+        <v>293</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>143</v>
+        <v>308</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>377</v>
+        <v>355</v>
       </c>
       <c r="D78" s="1" t="s">
         <v>271</v>
@@ -3240,13 +3220,13 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
-        <v>17</v>
+        <v>362</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>16</v>
+        <v>363</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>3</v>
+        <v>355</v>
       </c>
       <c r="D79" s="1" t="s">
         <v>271</v>
@@ -3254,13 +3234,13 @@
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
-        <v>269</v>
+        <v>109</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>274</v>
+        <v>295</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>3</v>
+        <v>355</v>
       </c>
       <c r="D80" s="1" t="s">
         <v>271</v>
@@ -3268,13 +3248,13 @@
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
-        <v>56</v>
+        <v>275</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>55</v>
+        <v>268</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
       <c r="D81" s="1" t="s">
         <v>271</v>
@@ -3282,13 +3262,13 @@
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>38</v>
+        <v>8</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>3</v>
+        <v>355</v>
       </c>
       <c r="D82" s="1" t="s">
         <v>271</v>
@@ -3296,13 +3276,13 @@
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
-        <v>353</v>
+        <v>89</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>357</v>
+        <v>132</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>360</v>
+        <v>347</v>
       </c>
       <c r="D83" s="1" t="s">
         <v>271</v>
@@ -3310,13 +3290,13 @@
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
-        <v>65</v>
+        <v>376</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>64</v>
+        <v>364</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>377</v>
+        <v>347</v>
       </c>
       <c r="D84" s="1" t="s">
         <v>271</v>
@@ -3324,13 +3304,13 @@
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
-        <v>131</v>
+        <v>300</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>130</v>
+        <v>286</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>377</v>
+        <v>347</v>
       </c>
       <c r="D85" s="1" t="s">
         <v>271</v>
@@ -3338,13 +3318,13 @@
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
-        <v>279</v>
+        <v>339</v>
       </c>
       <c r="B86" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="C86" s="1" t="s">
         <v>347</v>
-      </c>
-      <c r="C86" s="1" t="s">
-        <v>3</v>
       </c>
       <c r="D86" s="1" t="s">
         <v>271</v>
@@ -3352,13 +3332,13 @@
     </row>
     <row r="87" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
-        <v>279</v>
+        <v>148</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>60</v>
+        <v>338</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>377</v>
+        <v>347</v>
       </c>
       <c r="D87" s="1" t="s">
         <v>271</v>
@@ -3366,13 +3346,13 @@
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="s">
-        <v>351</v>
+        <v>80</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>355</v>
+        <v>86</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>360</v>
+        <v>347</v>
       </c>
       <c r="D88" s="1" t="s">
         <v>271</v>
@@ -3380,13 +3360,13 @@
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
-        <v>308</v>
+        <v>67</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>360</v>
+        <v>347</v>
       </c>
       <c r="D89" s="1" t="s">
         <v>271</v>
@@ -3394,13 +3374,13 @@
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
-        <v>79</v>
+        <v>54</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>78</v>
+        <v>53</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>360</v>
+        <v>347</v>
       </c>
       <c r="D90" s="1" t="s">
         <v>271</v>
@@ -3408,13 +3388,13 @@
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
-        <v>41</v>
+        <v>305</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>40</v>
+        <v>290</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>3</v>
+        <v>347</v>
       </c>
       <c r="D91" s="1" t="s">
         <v>271</v>
@@ -3422,13 +3402,13 @@
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="s">
-        <v>41</v>
+        <v>79</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>343</v>
+        <v>78</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>360</v>
+        <v>347</v>
       </c>
       <c r="D92" s="1" t="s">
         <v>271</v>
@@ -3436,13 +3416,13 @@
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
-        <v>126</v>
+        <v>298</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>125</v>
+        <v>283</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>3</v>
+        <v>347</v>
       </c>
       <c r="D93" s="1" t="s">
         <v>271</v>
@@ -3450,13 +3430,13 @@
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="s">
-        <v>362</v>
+        <v>377</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>3</v>
+        <v>347</v>
       </c>
       <c r="D94" s="1" t="s">
         <v>271</v>
@@ -3464,13 +3444,13 @@
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="s">
-        <v>43</v>
+        <v>117</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>42</v>
+        <v>133</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>377</v>
+        <v>347</v>
       </c>
       <c r="D95" s="1" t="s">
         <v>271</v>
@@ -3478,13 +3458,13 @@
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="s">
-        <v>91</v>
+        <v>112</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>136</v>
+        <v>111</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>3</v>
+        <v>347</v>
       </c>
       <c r="D96" s="1" t="s">
         <v>271</v>
@@ -3492,13 +3472,13 @@
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97" s="1" t="s">
-        <v>121</v>
+        <v>378</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>120</v>
+        <v>346</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>360</v>
+        <v>347</v>
       </c>
       <c r="D97" s="1" t="s">
         <v>271</v>
@@ -3506,13 +3486,13 @@
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="s">
-        <v>312</v>
+        <v>93</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>292</v>
+        <v>92</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>360</v>
+        <v>347</v>
       </c>
       <c r="D98" s="1" t="s">
         <v>271</v>
@@ -3520,27 +3500,24 @@
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
-        <v>15</v>
+        <v>301</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>14</v>
+        <v>68</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>3</v>
+        <v>347</v>
       </c>
       <c r="D99" s="1" t="s">
         <v>271</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A100" s="1" t="s">
-        <v>268</v>
-      </c>
       <c r="B100" s="1" t="s">
-        <v>275</v>
+        <v>245</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>3</v>
+        <v>347</v>
       </c>
       <c r="D100" s="1" t="s">
         <v>271</v>
@@ -3548,13 +3525,13 @@
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101" s="1" t="s">
-        <v>337</v>
+        <v>302</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>83</v>
+        <v>287</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>377</v>
+        <v>347</v>
       </c>
       <c r="D101" s="1" t="s">
         <v>271</v>
@@ -3562,13 +3539,13 @@
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102" s="1" t="s">
-        <v>323</v>
+        <v>327</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>44</v>
+        <v>284</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>377</v>
+        <v>347</v>
       </c>
       <c r="D102" s="1" t="s">
         <v>271</v>
@@ -3576,13 +3553,13 @@
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103" s="1" t="s">
-        <v>13</v>
+        <v>257</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>12</v>
+        <v>254</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>3</v>
+        <v>347</v>
       </c>
       <c r="D103" s="1" t="s">
         <v>271</v>
@@ -3590,13 +3567,13 @@
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104" s="1" t="s">
-        <v>100</v>
+        <v>304</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>99</v>
+        <v>288</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>360</v>
+        <v>347</v>
       </c>
       <c r="D104" s="1" t="s">
         <v>271</v>
@@ -3604,27 +3581,24 @@
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105" s="1" t="s">
-        <v>270</v>
+        <v>316</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>276</v>
+        <v>366</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>3</v>
+        <v>347</v>
       </c>
       <c r="D105" s="1" t="s">
         <v>271</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A106" s="1" t="s">
-        <v>316</v>
-      </c>
       <c r="B106" s="1" t="s">
-        <v>297</v>
+        <v>354</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>360</v>
+        <v>347</v>
       </c>
       <c r="D106" s="1" t="s">
         <v>271</v>
@@ -3632,13 +3606,13 @@
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107" s="1" t="s">
-        <v>301</v>
+        <v>52</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>282</v>
+        <v>51</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>360</v>
+        <v>347</v>
       </c>
       <c r="D107" s="1" t="s">
         <v>271</v>
@@ -3646,41 +3620,35 @@
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108" s="1" t="s">
-        <v>116</v>
+        <v>315</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>115</v>
+        <v>310</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>377</v>
+        <v>347</v>
       </c>
       <c r="D108" s="1" t="s">
         <v>271</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A109" s="1" t="s">
-        <v>302</v>
-      </c>
       <c r="B109" s="1" t="s">
-        <v>283</v>
+        <v>367</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>360</v>
+        <v>347</v>
       </c>
       <c r="D109" s="1" t="s">
         <v>271</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A110" s="1" t="s">
-        <v>310</v>
-      </c>
       <c r="B110" s="1" t="s">
-        <v>290</v>
+        <v>368</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>360</v>
+        <v>347</v>
       </c>
       <c r="D110" s="1" t="s">
         <v>271</v>
@@ -3688,13 +3656,13 @@
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A111" s="1" t="s">
-        <v>317</v>
+        <v>341</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>298</v>
+        <v>344</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>3</v>
+        <v>347</v>
       </c>
       <c r="D111" s="1" t="s">
         <v>271</v>
@@ -3702,13 +3670,13 @@
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112" s="1" t="s">
-        <v>82</v>
+        <v>294</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>81</v>
+        <v>280</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>377</v>
+        <v>347</v>
       </c>
       <c r="D112" s="1" t="s">
         <v>271</v>
@@ -3716,13 +3684,13 @@
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A113" s="1" t="s">
-        <v>326</v>
+        <v>100</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>273</v>
+        <v>99</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>3</v>
+        <v>347</v>
       </c>
       <c r="D113" s="1" t="s">
         <v>271</v>
@@ -3730,13 +3698,13 @@
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A114" s="1" t="s">
-        <v>299</v>
+        <v>379</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>280</v>
+        <v>369</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>360</v>
+        <v>347</v>
       </c>
       <c r="D114" s="1" t="s">
         <v>271</v>
@@ -3744,13 +3712,13 @@
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A115" s="1" t="s">
-        <v>336</v>
+        <v>128</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>286</v>
+        <v>127</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>360</v>
+        <v>347</v>
       </c>
       <c r="D115" s="1" t="s">
         <v>271</v>
@@ -3758,13 +3726,13 @@
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A116" s="1" t="s">
-        <v>321</v>
+        <v>56</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>318</v>
+        <v>55</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>377</v>
+        <v>347</v>
       </c>
       <c r="D116" s="1" t="s">
         <v>271</v>
@@ -3772,13 +3740,13 @@
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A117" s="1" t="s">
-        <v>128</v>
+        <v>326</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>127</v>
+        <v>334</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>360</v>
+        <v>347</v>
       </c>
       <c r="D117" s="1" t="s">
         <v>271</v>
@@ -3786,13 +3754,13 @@
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A118" s="1" t="s">
-        <v>20</v>
+        <v>261</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>368</v>
+        <v>242</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>3</v>
+        <v>347</v>
       </c>
       <c r="D118" s="1" t="s">
         <v>271</v>
@@ -3800,13 +3768,13 @@
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A119" s="1" t="s">
-        <v>20</v>
+        <v>304</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>369</v>
+        <v>291</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>3</v>
+        <v>347</v>
       </c>
       <c r="D119" s="1" t="s">
         <v>271</v>
@@ -3814,13 +3782,13 @@
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A120" s="1" t="s">
-        <v>71</v>
+        <v>324</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>70</v>
+        <v>332</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>3</v>
+        <v>347</v>
       </c>
       <c r="D120" s="1" t="s">
         <v>271</v>
@@ -3828,41 +3796,38 @@
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A121" s="1" t="s">
-        <v>50</v>
+        <v>380</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>49</v>
+        <v>370</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>377</v>
+        <v>347</v>
       </c>
       <c r="D121" s="1" t="s">
         <v>271</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A122" s="1" t="s">
-        <v>77</v>
-      </c>
       <c r="B122" s="1" t="s">
-        <v>76</v>
+        <v>371</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>377</v>
+        <v>347</v>
       </c>
       <c r="D122" s="1" t="s">
         <v>271</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A123" s="1" t="s">
-        <v>33</v>
+      <c r="A123" s="3" t="s">
+        <v>381</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>32</v>
+        <v>372</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>3</v>
+        <v>347</v>
       </c>
       <c r="D123" s="1" t="s">
         <v>271</v>
@@ -3870,57 +3835,83 @@
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B124" s="1" t="s">
-        <v>267</v>
+        <v>373</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>3</v>
+        <v>347</v>
       </c>
       <c r="D124" s="1" t="s">
         <v>271</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A125" s="1" t="s">
+        <v>382</v>
+      </c>
       <c r="B125" s="1" t="s">
-        <v>371</v>
+        <v>374</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>360</v>
+        <v>347</v>
       </c>
       <c r="D125" s="1" t="s">
         <v>271</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A126" s="1" t="s">
+        <v>383</v>
+      </c>
       <c r="B126" s="1" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>360</v>
+        <v>347</v>
       </c>
       <c r="D126" s="1" t="s">
         <v>271</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A127" s="1" t="s">
+        <v>105</v>
+      </c>
       <c r="B127" s="1" t="s">
-        <v>374</v>
+        <v>104</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>360</v>
+        <v>347</v>
       </c>
       <c r="D127" s="1" t="s">
         <v>271</v>
       </c>
     </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A128" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B128" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C128" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="D128" s="1" t="s">
+        <v>271</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D127">
-    <sortCondition ref="A2:A127"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D123">
+    <sortCondition ref="C2:C123"/>
   </sortState>
-  <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+  <conditionalFormatting sqref="B1:B48 B83:B1048576">
+    <cfRule type="duplicateValues" dxfId="4" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B3:B127 B1">
-    <cfRule type="duplicateValues" dxfId="0" priority="19"/>
+  <conditionalFormatting sqref="B3:B48 B1 B83:B127">
+    <cfRule type="duplicateValues" dxfId="3" priority="20"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2:B128">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
aggiunta nuovui tag da baby
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7ee4892a2dd36b84/Desktop/Link-clan/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="92" documentId="13_ncr:1_{9FCDD52C-4DCE-46C4-BB20-7F2264BA0663}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A402727E-ED37-40B6-A952-BF879D789044}"/>
+  <xr:revisionPtr revIDLastSave="99" documentId="13_ncr:1_{9FCDD52C-4DCE-46C4-BB20-7F2264BA0663}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{570247C6-4325-4BEE-B9B9-D099128B7D5B}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{FECCDA54-7594-4EB7-ABFB-2C408C6461DD}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="747" uniqueCount="384">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="751" uniqueCount="387">
   <si>
     <t>TagTelegram</t>
   </si>
@@ -1186,6 +1186,15 @@
   </si>
   <si>
     <t>@hehehejs</t>
+  </si>
+  <si>
+    <t>@Cech04</t>
+  </si>
+  <si>
+    <t>@Immajamino</t>
+  </si>
+  <si>
+    <t>@CR_redshift</t>
   </si>
 </sst>
 </file>
@@ -1675,12 +1684,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1731,27 +1737,7 @@
     <cellStyle name="Valore non valido" xfId="7" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Valore valido" xfId="6" builtinId="26" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="5">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -2115,7 +2101,7 @@
   <dimension ref="A1:D128"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B63" sqref="B63"/>
+      <selection activeCell="B111" sqref="B111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2676,7 +2662,7 @@
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B40" s="2" t="s">
+      <c r="B40" s="1" t="s">
         <v>267</v>
       </c>
       <c r="C40" s="1" t="s">
@@ -3513,6 +3499,9 @@
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A100" s="1" t="s">
+        <v>122</v>
+      </c>
       <c r="B100" s="1" t="s">
         <v>245</v>
       </c>
@@ -3633,6 +3622,9 @@
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A109" s="1" t="s">
+        <v>384</v>
+      </c>
       <c r="B109" s="1" t="s">
         <v>367</v>
       </c>
@@ -3809,6 +3801,9 @@
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A122" s="1" t="s">
+        <v>385</v>
+      </c>
       <c r="B122" s="1" t="s">
         <v>371</v>
       </c>
@@ -3820,7 +3815,7 @@
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A123" s="3" t="s">
+      <c r="A123" s="2" t="s">
         <v>381</v>
       </c>
       <c r="B123" s="1" t="s">
@@ -3834,6 +3829,9 @@
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A124" s="1" t="s">
+        <v>386</v>
+      </c>
       <c r="B124" s="1" t="s">
         <v>373</v>
       </c>
@@ -3905,13 +3903,13 @@
     <sortCondition ref="C2:C123"/>
   </sortState>
   <conditionalFormatting sqref="B1:B48 B83:B1048576">
-    <cfRule type="duplicateValues" dxfId="4" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2:B128">
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:B48 B1 B83:B127">
-    <cfRule type="duplicateValues" dxfId="3" priority="20"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B2:B128">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="20"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
convocazioni stagione 126 - 4
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7ee4892a2dd36b84/Desktop/Link-clan/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="168" documentId="13_ncr:1_{9FCDD52C-4DCE-46C4-BB20-7F2264BA0663}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{27046D0D-FB94-4BC2-8D50-40A436833DDF}"/>
+  <xr:revisionPtr revIDLastSave="202" documentId="13_ncr:1_{9FCDD52C-4DCE-46C4-BB20-7F2264BA0663}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8FDD939E-5F09-4653-A762-46C813883B9E}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{FECCDA54-7594-4EB7-ABFB-2C408C6461DD}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="274">
   <si>
     <t>TagTelegram</t>
   </si>
@@ -638,9 +638,6 @@
     <t>Sønサル•D•Lůffy</t>
   </si>
   <si>
-    <t>Warlosing</t>
-  </si>
-  <si>
     <t>Gianlomb</t>
   </si>
   <si>
@@ -686,26 +683,185 @@
     <t>calumet</t>
   </si>
   <si>
-    <t>IvanKing</t>
-  </si>
-  <si>
     <t>@Calumett</t>
   </si>
   <si>
-    <t>@Ivanking97</t>
-  </si>
-  <si>
     <t>khmer BM⚡</t>
   </si>
   <si>
     <t>Thor⚡</t>
+  </si>
+  <si>
+    <t>Ａ Ｒ ♠️ ＦＥＤＥＲＩＣＯ</t>
+  </si>
+  <si>
+    <t>ＡＲ♥️Ｐｏｎｃｉｏ９９</t>
+  </si>
+  <si>
+    <t>ＡＲ♥️Ｓｔｅｆａｎｏ</t>
+  </si>
+  <si>
+    <t>ＡＲ❤️Ｔｅｆａｎｏｓ</t>
+  </si>
+  <si>
+    <t>ＡＲ♦️Ｂｏｓｏ</t>
+  </si>
+  <si>
+    <t>AR❤️TORIAS</t>
+  </si>
+  <si>
+    <t>ᴀʀ♥️ᴍᴏɴɪᴀ</t>
+  </si>
+  <si>
+    <t>ＡＲ♦️ｏＢ❗Ｒ</t>
+  </si>
+  <si>
+    <t>ＡＲ♥️Ｌｏｒｙ９９ｍｉｎｅ</t>
+  </si>
+  <si>
+    <t>ＡＲ♥️ＬｅＬｅ</t>
+  </si>
+  <si>
+    <t>ＡＲ♠️Ｍｉｃｈａｅｌ</t>
+  </si>
+  <si>
+    <t>⚡Polis⚡</t>
+  </si>
+  <si>
+    <t>ＡＲ♦️Ｆ❗️Ｌｏ</t>
+  </si>
+  <si>
+    <t>@tefanoss</t>
+  </si>
+  <si>
+    <t>@Boso_7</t>
+  </si>
+  <si>
+    <t>@micro723</t>
+  </si>
+  <si>
+    <t>@Filantropo1010</t>
+  </si>
+  <si>
+    <t>•fury™•</t>
+  </si>
+  <si>
+    <t>Luigi13</t>
+  </si>
+  <si>
+    <t>Dino</t>
+  </si>
+  <si>
+    <t>⚡MAJOR⚡</t>
+  </si>
+  <si>
+    <t>Quizzz</t>
+  </si>
+  <si>
+    <t>SbranaClash300#</t>
+  </si>
+  <si>
+    <t>Dado has 200 iq</t>
+  </si>
+  <si>
+    <t>@Manu2365</t>
+  </si>
+  <si>
+    <t>@luigi134</t>
+  </si>
+  <si>
+    <t>@sunnering</t>
+  </si>
+  <si>
+    <t>@MAJOR992</t>
+  </si>
+  <si>
+    <t>@SranaClash300</t>
+  </si>
+  <si>
+    <t>@Dadoisonfire</t>
+  </si>
+  <si>
+    <t>DOCCC</t>
+  </si>
+  <si>
+    <t>Zokum</t>
+  </si>
+  <si>
+    <t>vinz</t>
+  </si>
+  <si>
+    <t>Maradona</t>
+  </si>
+  <si>
+    <t>Zumpy</t>
+  </si>
+  <si>
+    <t>superfede</t>
+  </si>
+  <si>
+    <t>Sfidante</t>
+  </si>
+  <si>
+    <t>RETROWAV3R™️</t>
+  </si>
+  <si>
+    <t>GXSALVO08</t>
+  </si>
+  <si>
+    <t>Andyfantasy98</t>
+  </si>
+  <si>
+    <t>IronMan</t>
+  </si>
+  <si>
+    <t>Arsenio</t>
+  </si>
+  <si>
+    <t>@pietro_actis</t>
+  </si>
+  <si>
+    <t>@usernamepersonalee</t>
+  </si>
+  <si>
+    <t>@Giovicor</t>
+  </si>
+  <si>
+    <t>@vinz9898</t>
+  </si>
+  <si>
+    <t>@fabri1010</t>
+  </si>
+  <si>
+    <t>@FabioZumpy77</t>
+  </si>
+  <si>
+    <t>@superfede2</t>
+  </si>
+  <si>
+    <t>@Sgrillo97</t>
+  </si>
+  <si>
+    <t>@RETROWAV3R</t>
+  </si>
+  <si>
+    <t>@GXSALVO08</t>
+  </si>
+  <si>
+    <t>@AndyFantasy</t>
+  </si>
+  <si>
+    <t>@arsenapoli</t>
+  </si>
+  <si>
+    <t>Ce Magnamm</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -839,12 +995,6 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="33">
@@ -1188,12 +1338,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1241,67 +1388,7 @@
     <cellStyle name="Valore non valido" xfId="7" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Valore valido" xfId="6" builtinId="26" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="7">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1642,10 +1729,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EE2B0F9-AC31-464B-B046-53CB033C8615}">
-  <dimension ref="A1:D123"/>
+  <dimension ref="A1:D143"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
-      <selection activeCell="F104" sqref="F104"/>
+    <sheetView tabSelected="1" topLeftCell="A124" workbookViewId="0">
+      <selection activeCell="B128" sqref="B128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1657,9 +1744,8 @@
     <col min="5" max="5" width="8.88671875" style="1"/>
     <col min="6" max="6" width="22.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.88671875" style="1"/>
+    <col min="8" max="8" width="20" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -1678,13 +1764,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>92</v>
+        <v>10</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>91</v>
+        <v>219</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>201</v>
+        <v>3</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>120</v>
@@ -1692,13 +1778,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>61</v>
+        <v>108</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>60</v>
+        <v>105</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>201</v>
+        <v>3</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>120</v>
@@ -1706,13 +1792,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>201</v>
+        <v>3</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>120</v>
@@ -1720,13 +1806,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>41</v>
+        <v>170</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>201</v>
+        <v>3</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>120</v>
@@ -1734,13 +1820,13 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>28</v>
+        <v>218</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>201</v>
+        <v>3</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>120</v>
@@ -1748,13 +1834,13 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>201</v>
+        <v>3</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>120</v>
@@ -1762,13 +1848,13 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>117</v>
+        <v>167</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>124</v>
+        <v>169</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>201</v>
+        <v>3</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>120</v>
@@ -1776,13 +1862,13 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>82</v>
+        <v>164</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>81</v>
+        <v>122</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>201</v>
+        <v>3</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>120</v>
@@ -1790,13 +1876,13 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>75</v>
+        <v>18</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>74</v>
+        <v>200</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>201</v>
+        <v>3</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>120</v>
@@ -1804,13 +1890,13 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>128</v>
+        <v>107</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>50</v>
+        <v>104</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>201</v>
+        <v>3</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>120</v>
@@ -1818,13 +1904,13 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>161</v>
+        <v>16</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>201</v>
+        <v>3</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>120</v>
@@ -1832,13 +1918,13 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>156</v>
+        <v>31</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>142</v>
+        <v>30</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>201</v>
+        <v>3</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>120</v>
@@ -1846,13 +1932,13 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>206</v>
+        <v>7</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>205</v>
+        <v>6</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>201</v>
+        <v>3</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>120</v>
@@ -1860,13 +1946,13 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>144</v>
+        <v>12</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>85</v>
+        <v>11</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>201</v>
+        <v>3</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>120</v>
@@ -1874,13 +1960,13 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>201</v>
+        <v>3</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>120</v>
@@ -1888,13 +1974,13 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>214</v>
+        <v>14</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>78</v>
+        <v>13</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>194</v>
+        <v>3</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>120</v>
@@ -1902,13 +1988,13 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>129</v>
+        <v>35</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>143</v>
+        <v>34</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>194</v>
+        <v>3</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>120</v>
@@ -1916,13 +2002,13 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>194</v>
+        <v>3</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>120</v>
@@ -1930,13 +2016,13 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>215</v>
+        <v>178</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>19</v>
+        <v>101</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>194</v>
+        <v>3</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>120</v>
@@ -1944,13 +2030,13 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>183</v>
+        <v>72</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>177</v>
+        <v>97</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>194</v>
+        <v>3</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>120</v>
@@ -1958,13 +2044,13 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>44</v>
+        <v>166</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>194</v>
+        <v>3</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>120</v>
@@ -1972,13 +2058,13 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>51</v>
+        <v>23</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>52</v>
+        <v>22</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>194</v>
+        <v>3</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>120</v>
@@ -1986,13 +2072,13 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>182</v>
+        <v>121</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>176</v>
+        <v>197</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>194</v>
+        <v>3</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>120</v>
@@ -2000,13 +2086,13 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>216</v>
+        <v>148</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>218</v>
+        <v>134</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>194</v>
+        <v>3</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>120</v>
@@ -2014,13 +2100,13 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>209</v>
+        <v>39</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>213</v>
+        <v>38</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>194</v>
+        <v>3</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>120</v>
@@ -2028,13 +2114,13 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>126</v>
+        <v>195</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>68</v>
+        <v>198</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>194</v>
+        <v>3</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>120</v>
@@ -2042,13 +2128,13 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>191</v>
+        <v>209</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>188</v>
+        <v>206</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>194</v>
+        <v>3</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>120</v>
@@ -2056,13 +2142,13 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>111</v>
+        <v>27</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>112</v>
+        <v>26</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>194</v>
+        <v>3</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>120</v>
@@ -2070,13 +2156,13 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>56</v>
+        <v>25</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>57</v>
+        <v>24</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>194</v>
+        <v>3</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>120</v>
@@ -2084,13 +2170,13 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>130</v>
+        <v>165</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>145</v>
+        <v>168</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>194</v>
+        <v>3</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>120</v>
@@ -2098,13 +2184,13 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>133</v>
+        <v>73</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>174</v>
+        <v>100</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>194</v>
+        <v>3</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>120</v>
@@ -2112,13 +2198,13 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>152</v>
+        <v>184</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>194</v>
+        <v>3</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>120</v>
@@ -2126,13 +2212,13 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>132</v>
+        <v>177</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>147</v>
+        <v>183</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>194</v>
+        <v>3</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>120</v>
@@ -2140,13 +2226,13 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>202</v>
+        <v>232</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>203</v>
+        <v>220</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>194</v>
+        <v>3</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>120</v>
@@ -2154,10 +2240,13 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>116</v>
+        <v>232</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>221</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>194</v>
+        <v>3</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>120</v>
@@ -2165,13 +2254,13 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
-        <v>158</v>
+        <v>232</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>162</v>
+        <v>222</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>194</v>
+        <v>3</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>120</v>
@@ -2179,13 +2268,13 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>138</v>
+        <v>233</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>186</v>
+        <v>223</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>194</v>
+        <v>3</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>120</v>
@@ -2193,13 +2282,13 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
-        <v>217</v>
+        <v>233</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>219</v>
+        <v>224</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>194</v>
+        <v>3</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>120</v>
@@ -2207,13 +2296,13 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
-        <v>53</v>
+        <v>233</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>54</v>
+        <v>225</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>194</v>
+        <v>3</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>120</v>
@@ -2221,13 +2310,13 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
-        <v>98</v>
+        <v>233</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>93</v>
+        <v>226</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>194</v>
+        <v>3</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>120</v>
@@ -2235,13 +2324,13 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
-        <v>109</v>
+        <v>233</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>113</v>
+        <v>227</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>194</v>
+        <v>3</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>120</v>
@@ -2249,13 +2338,13 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
-        <v>207</v>
+        <v>233</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>210</v>
+        <v>228</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>194</v>
+        <v>3</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>120</v>
@@ -2263,13 +2352,13 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
-        <v>69</v>
+        <v>163</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>64</v>
+        <v>103</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>194</v>
+        <v>3</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>120</v>
@@ -2277,13 +2366,13 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
-        <v>181</v>
+        <v>37</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>173</v>
+        <v>36</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>194</v>
+        <v>3</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>120</v>
@@ -2291,13 +2380,13 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
-        <v>204</v>
+        <v>234</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>106</v>
+        <v>229</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>194</v>
+        <v>3</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>120</v>
@@ -2305,13 +2394,13 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
-        <v>180</v>
+        <v>234</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>172</v>
+        <v>230</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>194</v>
+        <v>3</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>120</v>
@@ -2319,13 +2408,13 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
-        <v>97</v>
+        <v>106</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>72</v>
+        <v>203</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>194</v>
+        <v>3</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>120</v>
@@ -2333,13 +2422,13 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
-        <v>139</v>
+        <v>235</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>153</v>
+        <v>231</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>194</v>
+        <v>3</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>120</v>
@@ -2347,13 +2436,13 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
-        <v>55</v>
+        <v>19</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>150</v>
+        <v>214</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>194</v>
+        <v>3</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>120</v>
@@ -2361,13 +2450,13 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
-        <v>62</v>
+        <v>78</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>63</v>
+        <v>213</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>194</v>
+        <v>3</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>120</v>
@@ -2375,10 +2464,10 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>84</v>
+        <v>154</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>194</v>
@@ -2389,10 +2478,10 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
-        <v>199</v>
+        <v>58</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>196</v>
+        <v>59</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>194</v>
@@ -2403,10 +2492,10 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
-        <v>48</v>
+        <v>236</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>49</v>
+        <v>243</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>194</v>
@@ -2417,10 +2506,10 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>194</v>
@@ -2431,10 +2520,10 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>114</v>
+        <v>145</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>194</v>
@@ -2445,10 +2534,10 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
-        <v>95</v>
+        <v>135</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>96</v>
+        <v>149</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>194</v>
@@ -2459,10 +2548,10 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
-        <v>87</v>
+        <v>138</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>88</v>
+        <v>186</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>194</v>
@@ -2473,10 +2562,10 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>171</v>
+        <v>106</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>194</v>
@@ -2487,10 +2576,10 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>194</v>
@@ -2501,10 +2590,10 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
-        <v>193</v>
+        <v>53</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>212</v>
+        <v>54</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>194</v>
@@ -2515,10 +2604,10 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
-        <v>185</v>
+        <v>237</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>106</v>
+        <v>244</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>194</v>
@@ -2529,10 +2618,10 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
-        <v>46</v>
+        <v>139</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>47</v>
+        <v>153</v>
       </c>
       <c r="C63" s="1" t="s">
         <v>194</v>
@@ -2543,10 +2632,10 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
-        <v>140</v>
+        <v>62</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>152</v>
+        <v>63</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>194</v>
@@ -2557,10 +2646,10 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
-        <v>208</v>
+        <v>238</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>211</v>
+        <v>245</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>194</v>
@@ -2571,10 +2660,10 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>194</v>
@@ -2585,13 +2674,13 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
-        <v>4</v>
+        <v>207</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>5</v>
+        <v>210</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>3</v>
+        <v>194</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>120</v>
@@ -2599,13 +2688,13 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
-        <v>30</v>
+        <v>98</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>31</v>
+        <v>93</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>3</v>
+        <v>194</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>120</v>
@@ -2613,13 +2702,13 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
-        <v>122</v>
+        <v>87</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>164</v>
+        <v>88</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>3</v>
+        <v>194</v>
       </c>
       <c r="D69" s="1" t="s">
         <v>120</v>
@@ -2627,13 +2716,13 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
-        <v>123</v>
+        <v>193</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>118</v>
+        <v>211</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>3</v>
+        <v>194</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>120</v>
@@ -2641,13 +2730,13 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
-        <v>11</v>
+        <v>74</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>12</v>
+        <v>75</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>3</v>
+        <v>194</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>120</v>
@@ -2655,13 +2744,13 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
-        <v>15</v>
+        <v>55</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>16</v>
+        <v>150</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>3</v>
+        <v>194</v>
       </c>
       <c r="D72" s="1" t="s">
         <v>120</v>
@@ -2669,13 +2758,13 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
-        <v>197</v>
+        <v>239</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>121</v>
+        <v>246</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>3</v>
+        <v>194</v>
       </c>
       <c r="D73" s="1" t="s">
         <v>120</v>
@@ -2683,13 +2772,13 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
-        <v>34</v>
+        <v>136</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>35</v>
+        <v>151</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>3</v>
+        <v>194</v>
       </c>
       <c r="D74" s="1" t="s">
         <v>120</v>
@@ -2697,13 +2786,13 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
-        <v>26</v>
+        <v>133</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>27</v>
+        <v>174</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>3</v>
+        <v>194</v>
       </c>
       <c r="D75" s="1" t="s">
         <v>120</v>
@@ -2711,13 +2800,13 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
-        <v>13</v>
+        <v>111</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>14</v>
+        <v>112</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>3</v>
+        <v>194</v>
       </c>
       <c r="D76" s="1" t="s">
         <v>120</v>
@@ -2725,13 +2814,13 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
-        <v>125</v>
+        <v>137</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>119</v>
+        <v>152</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>3</v>
+        <v>194</v>
       </c>
       <c r="D77" s="1" t="s">
         <v>120</v>
@@ -2739,13 +2828,13 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
-        <v>134</v>
+        <v>240</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>148</v>
+        <v>163</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>3</v>
+        <v>194</v>
       </c>
       <c r="D78" s="1" t="s">
         <v>120</v>
@@ -2753,13 +2842,13 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
-        <v>17</v>
+        <v>46</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>166</v>
+        <v>47</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>3</v>
+        <v>194</v>
       </c>
       <c r="D79" s="1" t="s">
         <v>120</v>
@@ -2767,13 +2856,13 @@
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
-        <v>32</v>
+        <v>158</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>33</v>
+        <v>162</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>3</v>
+        <v>194</v>
       </c>
       <c r="D80" s="1" t="s">
         <v>120</v>
@@ -2781,13 +2870,13 @@
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
-        <v>184</v>
+        <v>208</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>128</v>
+        <v>212</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>3</v>
+        <v>194</v>
       </c>
       <c r="D81" s="1" t="s">
         <v>120</v>
@@ -2795,13 +2884,13 @@
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
-        <v>168</v>
+        <v>191</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>165</v>
+        <v>188</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>3</v>
+        <v>194</v>
       </c>
       <c r="D82" s="1" t="s">
         <v>120</v>
@@ -2809,13 +2898,13 @@
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
-        <v>22</v>
+        <v>129</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>23</v>
+        <v>143</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>3</v>
+        <v>194</v>
       </c>
       <c r="D83" s="1" t="s">
         <v>120</v>
@@ -2823,13 +2912,13 @@
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
-        <v>198</v>
+        <v>79</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>195</v>
+        <v>80</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>3</v>
+        <v>194</v>
       </c>
       <c r="D84" s="1" t="s">
         <v>120</v>
@@ -2837,13 +2926,13 @@
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
-        <v>141</v>
+        <v>91</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>155</v>
+        <v>92</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>3</v>
+        <v>194</v>
       </c>
       <c r="D85" s="1" t="s">
         <v>120</v>
@@ -2851,13 +2940,13 @@
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>3</v>
+        <v>194</v>
       </c>
       <c r="D86" s="1" t="s">
         <v>120</v>
@@ -2865,13 +2954,13 @@
     </row>
     <row r="87" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
-        <v>6</v>
+        <v>201</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>7</v>
+        <v>202</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>3</v>
+        <v>194</v>
       </c>
       <c r="D87" s="1" t="s">
         <v>120</v>
@@ -2879,13 +2968,13 @@
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="s">
-        <v>94</v>
+        <v>241</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>160</v>
+        <v>247</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>3</v>
+        <v>194</v>
       </c>
       <c r="D88" s="1" t="s">
         <v>120</v>
@@ -2893,13 +2982,13 @@
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
-        <v>104</v>
+        <v>181</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>107</v>
+        <v>173</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>3</v>
+        <v>194</v>
       </c>
       <c r="D89" s="1" t="s">
         <v>120</v>
@@ -2907,13 +2996,13 @@
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
-        <v>131</v>
+        <v>109</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>146</v>
+        <v>113</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>3</v>
+        <v>194</v>
       </c>
       <c r="D90" s="1" t="s">
         <v>120</v>
@@ -2921,13 +3010,13 @@
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
-        <v>190</v>
+        <v>242</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>187</v>
+        <v>248</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>3</v>
+        <v>194</v>
       </c>
       <c r="D91" s="1" t="s">
         <v>120</v>
@@ -2935,13 +3024,13 @@
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>3</v>
+        <v>194</v>
       </c>
       <c r="D92" s="1" t="s">
         <v>120</v>
@@ -2949,13 +3038,13 @@
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
-        <v>42</v>
+        <v>83</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>43</v>
+        <v>84</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>3</v>
+        <v>194</v>
       </c>
       <c r="D93" s="1" t="s">
         <v>120</v>
@@ -2963,13 +3052,13 @@
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="s">
-        <v>192</v>
+        <v>126</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>189</v>
+        <v>68</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>3</v>
+        <v>194</v>
       </c>
       <c r="D94" s="1" t="s">
         <v>120</v>
@@ -2977,13 +3066,13 @@
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="s">
-        <v>220</v>
+        <v>56</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>159</v>
+        <v>57</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>3</v>
+        <v>194</v>
       </c>
       <c r="D95" s="1" t="s">
         <v>120</v>
@@ -2991,13 +3080,10 @@
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="B96" s="1" t="s">
-        <v>167</v>
+        <v>116</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>3</v>
+        <v>194</v>
       </c>
       <c r="D96" s="1" t="s">
         <v>120</v>
@@ -3005,13 +3091,13 @@
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97" s="1" t="s">
-        <v>76</v>
+        <v>131</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>77</v>
+        <v>146</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>3</v>
+        <v>194</v>
       </c>
       <c r="D97" s="1" t="s">
         <v>120</v>
@@ -3019,13 +3105,13 @@
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="s">
-        <v>105</v>
+        <v>192</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>108</v>
+        <v>189</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>3</v>
+        <v>273</v>
       </c>
       <c r="D98" s="1" t="s">
         <v>120</v>
@@ -3033,13 +3119,13 @@
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
-        <v>102</v>
+        <v>127</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>106</v>
+        <v>115</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>3</v>
+        <v>273</v>
       </c>
       <c r="D99" s="1" t="s">
         <v>120</v>
@@ -3047,13 +3133,13 @@
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="s">
-        <v>38</v>
+        <v>124</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>39</v>
+        <v>117</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>3</v>
+        <v>273</v>
       </c>
       <c r="D100" s="1" t="s">
         <v>120</v>
@@ -3061,13 +3147,13 @@
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101" s="1" t="s">
-        <v>200</v>
+        <v>125</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>18</v>
+        <v>119</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>3</v>
+        <v>273</v>
       </c>
       <c r="D101" s="1" t="s">
         <v>120</v>
@@ -3075,13 +3161,13 @@
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102" s="1" t="s">
-        <v>170</v>
+        <v>94</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>10</v>
+        <v>160</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>3</v>
+        <v>273</v>
       </c>
       <c r="D102" s="1" t="s">
         <v>120</v>
@@ -3089,13 +3175,13 @@
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103" s="1" t="s">
-        <v>9</v>
+        <v>41</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>3</v>
+        <v>273</v>
       </c>
       <c r="D103" s="1" t="s">
         <v>120</v>
@@ -3103,13 +3189,13 @@
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104" s="1" t="s">
-        <v>221</v>
+        <v>67</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>18</v>
+        <v>175</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>3</v>
+        <v>273</v>
       </c>
       <c r="D104" s="1" t="s">
         <v>120</v>
@@ -3117,13 +3203,13 @@
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105" s="1" t="s">
-        <v>101</v>
+        <v>190</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>178</v>
+        <v>187</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>3</v>
+        <v>273</v>
       </c>
       <c r="D105" s="1" t="s">
         <v>120</v>
@@ -3131,13 +3217,13 @@
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106" s="1" t="s">
-        <v>36</v>
+        <v>89</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>37</v>
+        <v>90</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>3</v>
+        <v>273</v>
       </c>
       <c r="D106" s="1" t="s">
         <v>120</v>
@@ -3145,13 +3231,13 @@
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107" s="1" t="s">
-        <v>103</v>
+        <v>20</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>163</v>
+        <v>21</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>3</v>
+        <v>273</v>
       </c>
       <c r="D107" s="1" t="s">
         <v>120</v>
@@ -3159,13 +3245,13 @@
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108" s="1" t="s">
-        <v>100</v>
+        <v>42</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>73</v>
+        <v>43</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>3</v>
+        <v>273</v>
       </c>
       <c r="D108" s="1" t="s">
         <v>120</v>
@@ -3173,13 +3259,13 @@
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A109" s="1" t="s">
-        <v>67</v>
+        <v>28</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>175</v>
+        <v>29</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>3</v>
+        <v>273</v>
       </c>
       <c r="D109" s="1" t="s">
         <v>120</v>
@@ -3187,13 +3273,13 @@
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110" s="1" t="s">
-        <v>86</v>
+        <v>249</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>154</v>
+        <v>261</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>3</v>
+        <v>273</v>
       </c>
       <c r="D110" s="1" t="s">
         <v>120</v>
@@ -3201,13 +3287,13 @@
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A111" s="1" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>59</v>
+        <v>82</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>3</v>
+        <v>273</v>
       </c>
       <c r="D111" s="1" t="s">
         <v>120</v>
@@ -3215,24 +3301,455 @@
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="C112" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="D112" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A113" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C113" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="D113" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A114" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="B114" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="C114" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="D114" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A115" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C115" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="D115" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A116" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="C112" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D112" s="1" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A123" s="2"/>
+      <c r="B116" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="C116" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="D116" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A117" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B117" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C117" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="D117" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A118" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B118" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C118" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="D118" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A119" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B119" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C119" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="D119" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A120" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B120" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C120" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="D120" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A121" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="B121" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="C121" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="D121" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A122" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B122" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C122" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="D122" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A123" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="B123" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="C123" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="D123" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A124" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="B124" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="C124" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="D124" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A125" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B125" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C125" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="D125" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A126" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="B126" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="C126" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="D126" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A127" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B127" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C127" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="D127" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A128" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B128" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C128" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="D128" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A129" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="B129" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="C129" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="D129" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A130" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="B130" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="C130" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="D130" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A131" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="B131" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="C131" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="D131" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A132" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B132" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C132" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="D132" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A133" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="B133" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="C133" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="D133" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A134" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B134" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C134" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="D134" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A135" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="B135" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C135" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="D135" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A136" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B136" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="C136" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="D136" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A137" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="B137" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="C137" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="D137" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A138" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="B138" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="C138" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="D138" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A139" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B139" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="C139" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="D139" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A140" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B140" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C140" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="D140" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A141" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="B141" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="C141" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="D141" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A142" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="C142" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="D142" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A143" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="B143" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="C143" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="D143" s="1" t="s">
+        <v>120</v>
+      </c>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D123">
     <sortCondition ref="C2:C123"/>
   </sortState>
-  <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  <conditionalFormatting sqref="A1 A144:A1048576">
+    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
convocazioni stagione 127 - 1
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7ee4892a2dd36b84/Desktop/Link-clan/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="209" documentId="13_ncr:1_{9FCDD52C-4DCE-46C4-BB20-7F2264BA0663}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{11D8B094-1B95-43EC-9DBA-2EAB1B66BBAC}"/>
+  <xr:revisionPtr revIDLastSave="234" documentId="13_ncr:1_{9FCDD52C-4DCE-46C4-BB20-7F2264BA0663}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A5DD4C87-2080-4F06-A494-E36B5461E6E7}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{FECCDA54-7594-4EB7-ABFB-2C408C6461DD}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{FECCDA54-7594-4EB7-ABFB-2C408C6461DD}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="257">
   <si>
     <t>TagTelegram</t>
   </si>
@@ -62,9 +62,6 @@
     <t>@Ale_Mare93</t>
   </si>
   <si>
-    <t>ＡＲ♠️Ｆｅｄｅ</t>
-  </si>
-  <si>
     <t>@FedericoBello03</t>
   </si>
   <si>
@@ -215,12 +212,6 @@
     <t>@frankye73</t>
   </si>
   <si>
-    <t>AR♦️ᴍᴀᴛᴛᴇᴏ</t>
-  </si>
-  <si>
-    <t>@xmatte0x</t>
-  </si>
-  <si>
     <t>orso86</t>
   </si>
   <si>
@@ -338,9 +329,6 @@
     <t>AR♠️alfone</t>
   </si>
   <si>
-    <t>ＡＲ♠️Ｏｘｈａｔｒｅｓ</t>
-  </si>
-  <si>
     <t>Sandiokan</t>
   </si>
   <si>
@@ -554,9 +542,6 @@
     <t>@Fox_0265</t>
   </si>
   <si>
-    <t>@manuel190396</t>
-  </si>
-  <si>
     <t>@User32418</t>
   </si>
   <si>
@@ -578,9 +563,6 @@
     <t>Mr.Fox</t>
   </si>
   <si>
-    <t>manuel1903</t>
-  </si>
-  <si>
     <t>BwonE</t>
   </si>
   <si>
@@ -659,21 +641,12 @@
     <t>TOTAL DISASTER</t>
   </si>
   <si>
-    <t>cech04</t>
-  </si>
-  <si>
     <t>@PharmaShooter</t>
   </si>
   <si>
     <t>@The_Lore27</t>
   </si>
   <si>
-    <t>@X_teo</t>
-  </si>
-  <si>
-    <t>@Cech04</t>
-  </si>
-  <si>
     <t>⭐Marco⭐</t>
   </si>
   <si>
@@ -695,66 +668,12 @@
     <t>Ａ Ｒ ♠️ ＦＥＤＥＲＩＣＯ</t>
   </si>
   <si>
-    <t>ＡＲ♥️Ｐｏｎｃｉｏ９９</t>
-  </si>
-  <si>
-    <t>ＡＲ♥️Ｓｔｅｆａｎｏ</t>
-  </si>
-  <si>
-    <t>ＡＲ❤️Ｔｅｆａｎｏｓ</t>
-  </si>
-  <si>
-    <t>ＡＲ♦️Ｂｏｓｏ</t>
-  </si>
-  <si>
-    <t>AR❤️TORIAS</t>
-  </si>
-  <si>
-    <t>ᴀʀ♥️ᴍᴏɴɪᴀ</t>
-  </si>
-  <si>
-    <t>ＡＲ♦️ｏＢ❗Ｒ</t>
-  </si>
-  <si>
-    <t>ＡＲ♥️Ｌｏｒｙ９９ｍｉｎｅ</t>
-  </si>
-  <si>
-    <t>ＡＲ♥️ＬｅＬｅ</t>
-  </si>
-  <si>
-    <t>ＡＲ♠️Ｍｉｃｈａｅｌ</t>
-  </si>
-  <si>
-    <t>⚡Polis⚡</t>
-  </si>
-  <si>
-    <t>ＡＲ♦️Ｆ❗️Ｌｏ</t>
-  </si>
-  <si>
-    <t>@tefanoss</t>
-  </si>
-  <si>
-    <t>@Boso_7</t>
-  </si>
-  <si>
-    <t>@micro723</t>
-  </si>
-  <si>
-    <t>@Filantropo1010</t>
-  </si>
-  <si>
     <t>•fury™•</t>
   </si>
   <si>
-    <t>Luigi13</t>
-  </si>
-  <si>
     <t>Dino</t>
   </si>
   <si>
-    <t>⚡MAJOR⚡</t>
-  </si>
-  <si>
     <t>Quizzz</t>
   </si>
   <si>
@@ -767,15 +686,9 @@
     <t>@Manu2365</t>
   </si>
   <si>
-    <t>@luigi134</t>
-  </si>
-  <si>
     <t>@sunnering</t>
   </si>
   <si>
-    <t>@MAJOR992</t>
-  </si>
-  <si>
     <t>@SranaClash300</t>
   </si>
   <si>
@@ -785,9 +698,6 @@
     <t>DOCCC</t>
   </si>
   <si>
-    <t>Zokum</t>
-  </si>
-  <si>
     <t>vinz</t>
   </si>
   <si>
@@ -800,9 +710,6 @@
     <t>superfede</t>
   </si>
   <si>
-    <t>Sfidante</t>
-  </si>
-  <si>
     <t>RETROWAV3R™️</t>
   </si>
   <si>
@@ -824,9 +731,6 @@
     <t>@usernamepersonalee</t>
   </si>
   <si>
-    <t>@Giovicor</t>
-  </si>
-  <si>
     <t>@vinz9898</t>
   </si>
   <si>
@@ -839,9 +743,6 @@
     <t>@superfede2</t>
   </si>
   <si>
-    <t>@Sgrillo97</t>
-  </si>
-  <si>
     <t>@RETROWAV3R</t>
   </si>
   <si>
@@ -855,6 +756,54 @@
   </si>
   <si>
     <t>Ce Magnamm</t>
+  </si>
+  <si>
+    <t>SistemaS</t>
+  </si>
+  <si>
+    <t>Money_rain</t>
+  </si>
+  <si>
+    <t>MaLuMa</t>
+  </si>
+  <si>
+    <t>IvanKing</t>
+  </si>
+  <si>
+    <t>@tentationtop</t>
+  </si>
+  <si>
+    <t>@Pacca2317</t>
+  </si>
+  <si>
+    <t>@Ivanking97</t>
+  </si>
+  <si>
+    <t>kingmike</t>
+  </si>
+  <si>
+    <t>PIZZALILLO</t>
+  </si>
+  <si>
+    <t>cablo</t>
+  </si>
+  <si>
+    <t>sfidante</t>
+  </si>
+  <si>
+    <t>testosterone ma</t>
+  </si>
+  <si>
+    <t>@Kingmike1592</t>
+  </si>
+  <si>
+    <t>@ziobenni26</t>
+  </si>
+  <si>
+    <t>@christian363</t>
+  </si>
+  <si>
+    <t>@GRQJ8VL02</t>
   </si>
 </sst>
 </file>
@@ -1729,16 +1678,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EE2B0F9-AC31-464B-B046-53CB033C8615}">
-  <dimension ref="A1:D143"/>
+  <dimension ref="A1:D133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A134" zoomScale="143" workbookViewId="0">
-      <selection activeCell="F142" sqref="F142"/>
+    <sheetView tabSelected="1" zoomScale="137" workbookViewId="0">
+      <selection activeCell="A71" sqref="A71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="27.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.77734375" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.88671875" style="1"/>
@@ -1759,320 +1708,320 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>10</v>
+        <v>34</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>219</v>
+        <v>33</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>108</v>
+        <v>117</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>105</v>
+        <v>191</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>10</v>
+        <v>104</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>9</v>
+        <v>101</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>170</v>
+        <v>205</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>18</v>
+        <v>189</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>218</v>
+        <v>192</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>4</v>
+        <v>166</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>167</v>
+        <v>24</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>169</v>
+        <v>23</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>164</v>
+        <v>202</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>122</v>
+        <v>200</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>200</v>
+        <v>35</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>107</v>
+        <v>13</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>104</v>
+        <v>12</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>15</v>
+        <v>210</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>31</v>
+        <v>5</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>7</v>
+        <v>160</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>6</v>
+        <v>118</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>12</v>
+        <v>114</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>11</v>
+        <v>119</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>118</v>
+        <v>103</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>123</v>
+        <v>100</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>14</v>
+        <v>38</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>76</v>
+        <v>204</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>178</v>
+        <v>11</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>101</v>
+        <v>10</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>72</v>
+        <v>30</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>97</v>
+        <v>29</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>17</v>
+        <v>164</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>23</v>
+        <v>140</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>22</v>
+        <v>82</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>121</v>
+        <v>102</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>197</v>
@@ -2081,1667 +2030,1527 @@
         <v>3</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>148</v>
+        <v>15</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>134</v>
+        <v>14</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>39</v>
+        <v>159</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>38</v>
+        <v>99</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>195</v>
+        <v>70</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>198</v>
+        <v>97</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>209</v>
+        <v>17</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>206</v>
+        <v>194</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>27</v>
+        <v>124</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>26</v>
+        <v>178</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="B31" s="1" t="s">
-        <v>168</v>
-      </c>
       <c r="C31" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>73</v>
+        <v>162</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>100</v>
+        <v>16</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>128</v>
+        <v>172</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>177</v>
+        <v>17</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>183</v>
+        <v>209</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>232</v>
+        <v>115</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>220</v>
+        <v>121</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>232</v>
+        <v>113</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>221</v>
+        <v>120</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
-        <v>232</v>
+        <v>170</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>222</v>
+        <v>64</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>233</v>
+        <v>20</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>223</v>
+        <v>19</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
-        <v>233</v>
+        <v>65</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>224</v>
+        <v>122</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
-        <v>233</v>
+        <v>28</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>225</v>
+        <v>27</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
-        <v>233</v>
+        <v>142</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>226</v>
+        <v>127</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
-        <v>233</v>
+        <v>63</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>227</v>
+        <v>62</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
-        <v>233</v>
+        <v>63</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>228</v>
+        <v>112</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
-        <v>163</v>
+        <v>199</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>103</v>
+        <v>198</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
-        <v>37</v>
+        <v>152</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>36</v>
+        <v>138</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
-        <v>234</v>
+        <v>32</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>229</v>
+        <v>31</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
-        <v>234</v>
+        <v>157</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>230</v>
+        <v>39</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
-        <v>106</v>
+        <v>85</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>203</v>
+        <v>84</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
-        <v>235</v>
+        <v>144</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>231</v>
+        <v>130</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>3</v>
+        <v>240</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>214</v>
+        <v>6</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>3</v>
+        <v>240</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
-        <v>78</v>
+        <v>149</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>213</v>
+        <v>135</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>3</v>
+        <v>240</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
-        <v>154</v>
+        <v>51</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>86</v>
+        <v>50</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>194</v>
+        <v>240</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>58</v>
+        <v>76</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>194</v>
+        <v>240</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
-        <v>243</v>
+        <v>124</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>236</v>
+        <v>49</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>194</v>
+        <v>240</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
-        <v>155</v>
+        <v>87</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>141</v>
+        <v>86</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>194</v>
+        <v>240</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
-        <v>145</v>
+        <v>58</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>130</v>
+        <v>57</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>194</v>
+        <v>240</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>194</v>
+        <v>240</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
-        <v>186</v>
+        <v>155</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>138</v>
+        <v>208</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>194</v>
+        <v>240</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
-        <v>106</v>
+        <v>145</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>185</v>
+        <v>131</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>194</v>
+        <v>240</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
-        <v>64</v>
+        <v>156</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>69</v>
+        <v>91</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>194</v>
+        <v>240</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
-        <v>54</v>
+        <v>79</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>53</v>
+        <v>78</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>194</v>
+        <v>240</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
-        <v>244</v>
+        <v>53</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>237</v>
+        <v>52</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>194</v>
+        <v>240</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
-        <v>153</v>
+        <v>183</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>139</v>
+        <v>186</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>194</v>
+        <v>240</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
-        <v>63</v>
+        <v>239</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>62</v>
+        <v>229</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>194</v>
+        <v>240</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
-        <v>245</v>
+        <v>93</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>238</v>
+        <v>92</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>194</v>
+        <v>240</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
-        <v>147</v>
+        <v>102</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>132</v>
+        <v>179</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>194</v>
+        <v>240</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
-        <v>210</v>
+        <v>233</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>207</v>
+        <v>222</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>194</v>
+        <v>240</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
-        <v>93</v>
+        <v>109</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>194</v>
+        <v>240</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
-        <v>88</v>
+        <v>146</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>87</v>
+        <v>54</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>194</v>
+        <v>240</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
-        <v>211</v>
+        <v>150</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>193</v>
+        <v>83</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>194</v>
+        <v>240</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A71" s="1" t="s">
-        <v>75</v>
-      </c>
       <c r="B71" s="1" t="s">
-        <v>74</v>
+        <v>241</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>194</v>
+        <v>240</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
-        <v>150</v>
+        <v>89</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>55</v>
+        <v>88</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>194</v>
+        <v>240</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
-        <v>246</v>
+        <v>72</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>239</v>
+        <v>71</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>194</v>
+        <v>240</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
-        <v>151</v>
+        <v>56</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>136</v>
+        <v>55</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>194</v>
+        <v>240</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
-        <v>174</v>
+        <v>48</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>133</v>
+        <v>47</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>194</v>
+        <v>240</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
-        <v>112</v>
+        <v>234</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>111</v>
+        <v>223</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>194</v>
+        <v>240</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
-        <v>152</v>
+        <v>159</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>137</v>
+        <v>213</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>194</v>
+        <v>240</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>240</v>
+        <v>174</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>194</v>
+        <v>240</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
-        <v>47</v>
+        <v>245</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>46</v>
+        <v>242</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>194</v>
+        <v>240</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
-        <v>162</v>
+        <v>219</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>158</v>
+        <v>215</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>194</v>
+        <v>240</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
-        <v>212</v>
+        <v>110</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>208</v>
+        <v>106</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>194</v>
+        <v>240</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
-        <v>188</v>
+        <v>207</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>191</v>
+        <v>206</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>194</v>
+        <v>240</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
-        <v>143</v>
+        <v>237</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>129</v>
+        <v>226</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>194</v>
+        <v>240</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
-        <v>80</v>
+        <v>217</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>79</v>
+        <v>212</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>194</v>
+        <v>240</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
-        <v>92</v>
+        <v>171</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>91</v>
+        <v>176</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>194</v>
+        <v>240</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
-        <v>61</v>
+        <v>238</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>60</v>
+        <v>227</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>194</v>
+        <v>240</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
-        <v>202</v>
+        <v>171</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>201</v>
+        <v>176</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>194</v>
+        <v>240</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>194</v>
+        <v>240</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
-        <v>173</v>
+        <v>247</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>181</v>
+        <v>244</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>194</v>
+        <v>240</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
-        <v>113</v>
+        <v>8</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>109</v>
+        <v>40</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>194</v>
+        <v>240</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
-        <v>248</v>
+        <v>74</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>242</v>
+        <v>73</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="s">
-        <v>96</v>
+        <v>68</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>95</v>
+        <v>67</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
-        <v>84</v>
+        <v>108</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>83</v>
+        <v>107</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="s">
-        <v>68</v>
+        <v>173</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>126</v>
+        <v>187</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="s">
-        <v>57</v>
+        <v>102</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>56</v>
+        <v>98</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A96" s="1" t="s">
+        <v>196</v>
+      </c>
       <c r="B96" s="1" t="s">
-        <v>116</v>
+        <v>195</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97" s="1" t="s">
-        <v>146</v>
+        <v>216</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>131</v>
+        <v>211</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="s">
-        <v>189</v>
+        <v>46</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>192</v>
+        <v>45</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>273</v>
+        <v>188</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
-        <v>115</v>
+        <v>253</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>127</v>
+        <v>248</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>273</v>
+        <v>188</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="s">
-        <v>117</v>
+        <v>232</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>124</v>
+        <v>221</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>273</v>
+        <v>188</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101" s="1" t="s">
-        <v>119</v>
+        <v>61</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>125</v>
+        <v>66</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>273</v>
+        <v>188</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102" s="1" t="s">
-        <v>160</v>
+        <v>111</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>94</v>
+        <v>123</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>273</v>
+        <v>188</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103" s="1" t="s">
-        <v>8</v>
+        <v>42</v>
       </c>
       <c r="B103" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>273</v>
+        <v>188</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104" s="1" t="s">
-        <v>175</v>
+        <v>235</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>67</v>
+        <v>224</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>273</v>
+        <v>188</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105" s="1" t="s">
-        <v>187</v>
+        <v>231</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>190</v>
+        <v>153</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>273</v>
+        <v>188</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106" s="1" t="s">
-        <v>90</v>
+        <v>203</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>89</v>
+        <v>201</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>273</v>
+        <v>188</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107" s="1" t="s">
-        <v>21</v>
+        <v>143</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>20</v>
+        <v>128</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>273</v>
+        <v>188</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108" s="1" t="s">
-        <v>43</v>
+        <v>190</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>42</v>
+        <v>193</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>273</v>
+        <v>188</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A109" s="1" t="s">
-        <v>29</v>
+        <v>230</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>28</v>
+        <v>220</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>273</v>
+        <v>188</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110" s="1" t="s">
-        <v>261</v>
+        <v>218</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>249</v>
+        <v>214</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>273</v>
+        <v>188</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A111" s="1" t="s">
-        <v>82</v>
+        <v>180</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>81</v>
+        <v>134</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>273</v>
+        <v>188</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112" s="1" t="s">
-        <v>205</v>
+        <v>168</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>204</v>
+        <v>175</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>273</v>
+        <v>188</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A113" s="1" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>85</v>
+        <v>125</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>273</v>
+        <v>188</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A114" s="1" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>217</v>
+        <v>132</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>273</v>
+        <v>188</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A115" s="1" t="s">
-        <v>156</v>
+        <v>81</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>142</v>
+        <v>80</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>273</v>
+        <v>188</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A116" s="1" t="s">
-        <v>262</v>
+        <v>158</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>273</v>
+        <v>188</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A117" s="1" t="s">
-        <v>33</v>
+        <v>148</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>32</v>
+        <v>136</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>273</v>
+        <v>188</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A118" s="1" t="s">
-        <v>161</v>
+        <v>60</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>40</v>
+        <v>59</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>273</v>
+        <v>188</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A119" s="1" t="s">
-        <v>106</v>
+        <v>181</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>102</v>
+        <v>184</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>273</v>
+        <v>188</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A120" s="1" t="s">
-        <v>71</v>
+        <v>159</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>70</v>
+        <v>249</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>273</v>
+        <v>188</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A121" s="1" t="s">
-        <v>263</v>
+        <v>182</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>250</v>
+        <v>185</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>273</v>
+        <v>188</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A122" s="1" t="s">
-        <v>128</v>
+        <v>148</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>50</v>
+        <v>133</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>273</v>
+        <v>188</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A123" s="1" t="s">
-        <v>264</v>
-      </c>
       <c r="B123" s="1" t="s">
-        <v>251</v>
+        <v>228</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>273</v>
+        <v>188</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A124" s="1" t="s">
-        <v>265</v>
+        <v>169</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>252</v>
+        <v>129</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>273</v>
+        <v>188</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A125" s="1" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>273</v>
+        <v>188</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A126" s="1" t="s">
-        <v>266</v>
+        <v>236</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>253</v>
+        <v>225</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>273</v>
+        <v>188</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A127" s="1" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>140</v>
+        <v>126</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>273</v>
+        <v>188</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A128" s="1" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>65</v>
+        <v>94</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>273</v>
+        <v>188</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A129" s="1" t="s">
-        <v>267</v>
+        <v>254</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>273</v>
+        <v>188</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A130" s="1" t="s">
-        <v>171</v>
+        <v>255</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>179</v>
+        <v>251</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>273</v>
+        <v>188</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A131" s="1" t="s">
-        <v>268</v>
+        <v>256</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>273</v>
+        <v>188</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A132" s="1" t="s">
-        <v>114</v>
+        <v>44</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>110</v>
+        <v>43</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>273</v>
+        <v>188</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A133" s="1" t="s">
-        <v>269</v>
+        <v>90</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>256</v>
+        <v>95</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>273</v>
+        <v>188</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A134" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B134" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C134" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="D134" s="1" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A135" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="B135" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="C135" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="D135" s="1" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A136" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="B136" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="C136" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="D136" s="1" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A137" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="B137" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="C137" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="D137" s="1" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A138" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="B138" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="C138" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="D138" s="1" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A139" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="B139" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="C139" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="D139" s="1" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A140" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B140" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C140" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="D140" s="1" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A141" s="1" t="s">
-        <v>271</v>
-      </c>
-      <c r="B141" s="1" t="s">
-        <v>258</v>
-      </c>
-      <c r="C141" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="D141" s="1" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B142" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="C142" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="D142" s="1" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A143" s="1" t="s">
-        <v>272</v>
-      </c>
-      <c r="B143" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="C143" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="D143" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
convocazioni stagione 127 - 2
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7ee4892a2dd36b84/Desktop/Link-clan/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="238" documentId="13_ncr:1_{9FCDD52C-4DCE-46C4-BB20-7F2264BA0663}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2766DF29-402F-459B-A540-89741764BC92}"/>
+  <xr:revisionPtr revIDLastSave="261" documentId="13_ncr:1_{9FCDD52C-4DCE-46C4-BB20-7F2264BA0663}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5759B8EC-F8F8-4413-97A0-785724A5EB43}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{FECCDA54-7594-4EB7-ABFB-2C408C6461DD}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="263">
   <si>
     <t>TagTelegram</t>
   </si>
@@ -92,12 +92,6 @@
     <t>@BuldzS</t>
   </si>
   <si>
-    <t>bo</t>
-  </si>
-  <si>
-    <t>@BO_CRL</t>
-  </si>
-  <si>
     <t>BrokerTony</t>
   </si>
   <si>
@@ -530,9 +524,6 @@
     <t>GaiaScienza</t>
   </si>
   <si>
-    <t>shinigami</t>
-  </si>
-  <si>
     <t>@Andrew260903</t>
   </si>
   <si>
@@ -656,9 +647,6 @@
     <t>khmer BM⚡</t>
   </si>
   <si>
-    <t>Thor⚡</t>
-  </si>
-  <si>
     <t>Ａ Ｒ ♠️ ＦＥＤＥＲＩＣＯ</t>
   </si>
   <si>
@@ -668,9 +656,6 @@
     <t>Dino</t>
   </si>
   <si>
-    <t>Quizzz</t>
-  </si>
-  <si>
     <t>SbranaClash300#</t>
   </si>
   <si>
@@ -749,24 +734,12 @@
     <t>@arsenapoli</t>
   </si>
   <si>
-    <t>Ce Magnamm</t>
-  </si>
-  <si>
-    <t>SistemaS</t>
-  </si>
-  <si>
-    <t>Money_rain</t>
-  </si>
-  <si>
     <t>MaLuMa</t>
   </si>
   <si>
     <t>IvanKing</t>
   </si>
   <si>
-    <t>@tentationtop</t>
-  </si>
-  <si>
     <t>@Pacca2317</t>
   </si>
   <si>
@@ -776,15 +749,9 @@
     <t>kingmike</t>
   </si>
   <si>
-    <t>PIZZALILLO</t>
-  </si>
-  <si>
     <t>cablo</t>
   </si>
   <si>
-    <t>sfidante</t>
-  </si>
-  <si>
     <t>testosterone ma</t>
   </si>
   <si>
@@ -794,16 +761,67 @@
     <t>@ziobenni26</t>
   </si>
   <si>
-    <t>@christian363</t>
-  </si>
-  <si>
     <t>@GRQJ8VL02</t>
   </si>
   <si>
     <t>Dog Rider</t>
   </si>
   <si>
-    <t>no</t>
+    <t>Thor⚡️</t>
+  </si>
+  <si>
+    <t>Si</t>
+  </si>
+  <si>
+    <t>Alex Hunter</t>
+  </si>
+  <si>
+    <t>Raffockij</t>
+  </si>
+  <si>
+    <t>Gervasio</t>
+  </si>
+  <si>
+    <t>lilpezzo300</t>
+  </si>
+  <si>
+    <t>jamino</t>
+  </si>
+  <si>
+    <t>@giraffaele</t>
+  </si>
+  <si>
+    <t>@Melqiades</t>
+  </si>
+  <si>
+    <t>@Immajamino</t>
+  </si>
+  <si>
+    <t>Sfidante</t>
+  </si>
+  <si>
+    <t>YouLose</t>
+  </si>
+  <si>
+    <t>FrankoBot</t>
+  </si>
+  <si>
+    <t>KOKODEWA</t>
+  </si>
+  <si>
+    <t>@Sgrillo97</t>
+  </si>
+  <si>
+    <t>@YL1272</t>
+  </si>
+  <si>
+    <t>@shu4pppp</t>
+  </si>
+  <si>
+    <t>@Anti47394</t>
+  </si>
+  <si>
+    <t>Warlosing</t>
   </si>
 </sst>
 </file>
@@ -1287,10 +1305,13 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1337,7 +1358,27 @@
     <cellStyle name="Valore non valido" xfId="7" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Valore valido" xfId="6" builtinId="26" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1681,15 +1722,16 @@
   <dimension ref="A1:D133"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="137" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D133"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D133" sqref="D2:D133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.88671875" style="1"/>
     <col min="6" max="6" width="22.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19.33203125" style="1" bestFit="1" customWidth="1"/>
@@ -1708,1849 +1750,1844 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="2"/>
+      <c r="B19" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B37" s="2" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
+      <c r="C37" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
+      <c r="B39" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
+      <c r="C39" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B45" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A36" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A37" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A38" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A40" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A42" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A43" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A45" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>137</v>
-      </c>
       <c r="C45" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A46" s="1" t="s">
-        <v>32</v>
-      </c>
       <c r="B46" s="1" t="s">
-        <v>31</v>
+        <v>246</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>3</v>
+        <v>243</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
-        <v>156</v>
+        <v>185</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>39</v>
+        <v>188</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>3</v>
+        <v>243</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
-        <v>85</v>
+        <v>138</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>84</v>
+        <v>123</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>3</v>
+        <v>243</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
-        <v>143</v>
+        <v>153</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
-        <v>7</v>
+        <v>176</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>6</v>
+        <v>131</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
-        <v>148</v>
+        <v>211</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>134</v>
+        <v>207</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
-        <v>51</v>
+        <v>77</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>50</v>
+        <v>76</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
-        <v>77</v>
+        <v>148</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>76</v>
+        <v>134</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
-        <v>123</v>
+        <v>198</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>49</v>
+        <v>196</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
-        <v>87</v>
+        <v>49</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>86</v>
+        <v>48</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
-        <v>58</v>
+        <v>226</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>57</v>
+        <v>215</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
-        <v>150</v>
+        <v>87</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>136</v>
+        <v>86</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
-        <v>154</v>
+        <v>142</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>206</v>
+        <v>128</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
-        <v>155</v>
+        <v>242</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>91</v>
+        <v>239</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
-        <v>79</v>
+        <v>251</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>78</v>
+        <v>247</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
-        <v>53</v>
+        <v>121</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
-        <v>182</v>
+        <v>167</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>185</v>
+        <v>172</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>227</v>
+        <v>233</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
-        <v>93</v>
+        <v>252</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>92</v>
+        <v>248</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
-        <v>102</v>
+        <v>54</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>178</v>
+        <v>53</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
-        <v>231</v>
+        <v>109</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>220</v>
+        <v>120</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
-        <v>109</v>
+        <v>191</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>105</v>
+        <v>190</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
-        <v>145</v>
+        <v>100</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>54</v>
+        <v>175</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
-        <v>149</v>
+        <v>46</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>83</v>
+        <v>45</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A71" s="1" t="s">
+        <v>209</v>
+      </c>
       <c r="B71" s="1" t="s">
-        <v>239</v>
+        <v>205</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
-        <v>89</v>
+        <v>155</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>88</v>
+        <v>151</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A75" s="1" t="s">
-        <v>48</v>
-      </c>
       <c r="B75" s="1" t="s">
-        <v>47</v>
+        <v>249</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
-        <v>158</v>
+        <v>165</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>211</v>
+        <v>126</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
-        <v>166</v>
+        <v>106</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>173</v>
+        <v>105</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
-        <v>217</v>
+        <v>143</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>213</v>
+        <v>52</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
-        <v>110</v>
+        <v>232</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>106</v>
+        <v>222</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
-        <v>205</v>
+        <v>179</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>204</v>
+        <v>182</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
-        <v>235</v>
+        <v>40</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>224</v>
+        <v>39</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
-        <v>215</v>
+        <v>230</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>210</v>
+        <v>219</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
-        <v>170</v>
+        <v>152</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>175</v>
+        <v>203</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
-        <v>236</v>
+        <v>163</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>225</v>
+        <v>170</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
-        <v>170</v>
+        <v>202</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>175</v>
+        <v>201</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="s">
-        <v>244</v>
+        <v>210</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>241</v>
+        <v>206</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
-        <v>245</v>
+        <v>177</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>242</v>
+        <v>180</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>40</v>
+        <v>64</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
-        <v>74</v>
+        <v>224</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>73</v>
+        <v>150</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>255</v>
+        <v>243</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="s">
-        <v>68</v>
+        <v>253</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>67</v>
+        <v>250</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>255</v>
+        <v>243</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
-        <v>108</v>
+        <v>91</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>107</v>
+        <v>90</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>255</v>
+        <v>243</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="s">
-        <v>172</v>
+        <v>42</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>186</v>
+        <v>41</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>255</v>
+        <v>243</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="s">
-        <v>102</v>
+        <v>169</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>98</v>
+        <v>183</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>255</v>
+        <v>243</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="s">
-        <v>194</v>
+        <v>227</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>193</v>
+        <v>216</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>255</v>
+        <v>243</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97" s="1" t="s">
-        <v>214</v>
+        <v>141</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>209</v>
+        <v>127</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>255</v>
+        <v>243</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="s">
-        <v>46</v>
+        <v>147</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>45</v>
+        <v>81</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>255</v>
+        <v>243</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
-        <v>251</v>
+        <v>72</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>246</v>
+        <v>71</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>255</v>
+        <v>243</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="s">
-        <v>230</v>
+        <v>85</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>219</v>
+        <v>84</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>255</v>
+        <v>243</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101" s="1" t="s">
-        <v>61</v>
+        <v>107</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>66</v>
+        <v>103</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>255</v>
+        <v>262</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A102" s="1" t="s">
-        <v>111</v>
-      </c>
       <c r="B102" s="1" t="s">
-        <v>122</v>
+        <v>221</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>255</v>
+        <v>262</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103" s="1" t="s">
-        <v>42</v>
+        <v>212</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>41</v>
+        <v>208</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>255</v>
+        <v>262</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104" s="1" t="s">
-        <v>233</v>
+        <v>44</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>222</v>
+        <v>43</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>255</v>
+        <v>262</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105" s="1" t="s">
-        <v>229</v>
+        <v>70</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>152</v>
+        <v>69</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>255</v>
+        <v>262</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106" s="1" t="s">
-        <v>201</v>
+        <v>108</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>199</v>
+        <v>104</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>255</v>
+        <v>262</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107" s="1" t="s">
-        <v>142</v>
+        <v>258</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>127</v>
+        <v>254</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>255</v>
+        <v>262</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108" s="1" t="s">
-        <v>188</v>
+        <v>241</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>191</v>
+        <v>238</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>255</v>
+        <v>262</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A109" s="1" t="s">
-        <v>228</v>
+        <v>164</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>218</v>
+        <v>171</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>255</v>
+        <v>262</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110" s="1" t="s">
-        <v>216</v>
+        <v>231</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>212</v>
+        <v>220</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>255</v>
+        <v>262</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A111" s="1" t="s">
-        <v>179</v>
+        <v>225</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>133</v>
+        <v>214</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>255</v>
+        <v>262</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112" s="1" t="s">
-        <v>167</v>
+        <v>240</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>174</v>
+        <v>237</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>255</v>
+        <v>262</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A113" s="1" t="s">
-        <v>138</v>
+        <v>229</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>124</v>
+        <v>218</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>255</v>
+        <v>262</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A114" s="1" t="s">
-        <v>146</v>
+        <v>79</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>131</v>
+        <v>78</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>255</v>
+        <v>262</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A115" s="1" t="s">
-        <v>81</v>
+        <v>178</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>80</v>
+        <v>181</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>255</v>
+        <v>262</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A116" s="1" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>153</v>
+        <v>130</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>255</v>
+        <v>262</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A117" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>255</v>
+        <v>262</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A118" s="1" t="s">
-        <v>60</v>
+        <v>259</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>59</v>
+        <v>255</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>255</v>
+        <v>262</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A119" s="1" t="s">
-        <v>180</v>
+        <v>58</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>183</v>
+        <v>57</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>255</v>
+        <v>262</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A120" s="1" t="s">
-        <v>158</v>
+        <v>260</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>247</v>
+        <v>256</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>255</v>
+        <v>262</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A121" s="1" t="s">
-        <v>181</v>
+        <v>144</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>184</v>
+        <v>129</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>255</v>
+        <v>262</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A122" s="1" t="s">
-        <v>147</v>
+        <v>66</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>132</v>
+        <v>65</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>255</v>
+        <v>262</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A123" s="1" t="s">
+        <v>111</v>
+      </c>
       <c r="B123" s="1" t="s">
-        <v>226</v>
+        <v>117</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>255</v>
+        <v>262</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A124" s="1" t="s">
-        <v>168</v>
+        <v>113</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>255</v>
+        <v>262</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A125" s="1" t="s">
-        <v>63</v>
+        <v>168</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>62</v>
+        <v>173</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>255</v>
+        <v>262</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A126" s="1" t="s">
-        <v>234</v>
+        <v>63</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>223</v>
+        <v>119</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>255</v>
+        <v>262</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A127" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>255</v>
+        <v>262</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A128" s="1" t="s">
-        <v>69</v>
+        <v>261</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>94</v>
+        <v>257</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>255</v>
+        <v>262</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A129" s="1" t="s">
-        <v>252</v>
+        <v>149</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>248</v>
+        <v>135</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>255</v>
+        <v>262</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A130" s="1" t="s">
-        <v>253</v>
+        <v>67</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>249</v>
+        <v>92</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>255</v>
+        <v>262</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A131" s="1" t="s">
-        <v>254</v>
+        <v>17</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>250</v>
+        <v>189</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>255</v>
+        <v>262</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A132" s="1" t="s">
-        <v>44</v>
+        <v>61</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>255</v>
+        <v>262</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A133" s="1" t="s">
-        <v>90</v>
+        <v>166</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>95</v>
+        <v>62</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>255</v>
+        <v>262</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
     </row>
   </sheetData>
@@ -3558,7 +3595,10 @@
     <sortCondition ref="C2:C123"/>
   </sortState>
   <conditionalFormatting sqref="A1 A144:A1048576">
-    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="4"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B98:B100">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
convocazioni stagione 127 - 4
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7ee4892a2dd36b84/Desktop/Link-clan/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="261" documentId="13_ncr:1_{9FCDD52C-4DCE-46C4-BB20-7F2264BA0663}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5759B8EC-F8F8-4413-97A0-785724A5EB43}"/>
+  <xr:revisionPtr revIDLastSave="280" documentId="13_ncr:1_{9FCDD52C-4DCE-46C4-BB20-7F2264BA0663}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{85686EE5-831D-45C9-A0EE-477F5E4A5EB6}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{FECCDA54-7594-4EB7-ABFB-2C408C6461DD}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{FECCDA54-7594-4EB7-ABFB-2C408C6461DD}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="227">
   <si>
     <t>TagTelegram</t>
   </si>
@@ -200,36 +200,15 @@
     <t>@Wazito888</t>
   </si>
   <si>
-    <t>frankye73</t>
-  </si>
-  <si>
-    <t>@frankye73</t>
-  </si>
-  <si>
-    <t>orso86</t>
-  </si>
-  <si>
-    <t>@orso_86</t>
-  </si>
-  <si>
-    <t>@Lucaser95</t>
-  </si>
-  <si>
     <t>tala</t>
   </si>
   <si>
     <t>@Tala91111</t>
   </si>
   <si>
-    <t>ＡＲ♦️Ｅ＄</t>
-  </si>
-  <si>
     <t>@cicciovolley91</t>
   </si>
   <si>
-    <t>Lubbro95 C.B.</t>
-  </si>
-  <si>
     <t>YATO51</t>
   </si>
   <si>
@@ -242,12 +221,6 @@
     <t>@ralfone01</t>
   </si>
   <si>
-    <t>Angeloxf7</t>
-  </si>
-  <si>
-    <t>@angang37</t>
-  </si>
-  <si>
     <t>Lore_98</t>
   </si>
   <si>
@@ -269,12 +242,6 @@
     <t>@domenico_9</t>
   </si>
   <si>
-    <t>Pinguino</t>
-  </si>
-  <si>
-    <t>@lorenzocastaldii</t>
-  </si>
-  <si>
     <t>Kekko03</t>
   </si>
   <si>
@@ -416,9 +383,6 @@
     <t>Fabrizio</t>
   </si>
   <si>
-    <t>Luca01</t>
-  </si>
-  <si>
     <t>two ciamela</t>
   </si>
   <si>
@@ -458,9 +422,6 @@
     <t>@Freenk8</t>
   </si>
   <si>
-    <t>@luca3689</t>
-  </si>
-  <si>
     <t>@Giggi_A</t>
   </si>
   <si>
@@ -491,9 +452,6 @@
     <t>IceMan</t>
   </si>
   <si>
-    <t>@ciuler</t>
-  </si>
-  <si>
     <t>@alabatia89</t>
   </si>
   <si>
@@ -527,33 +485,15 @@
     <t>@Andrew260903</t>
   </si>
   <si>
-    <t>@Fox_0265</t>
-  </si>
-  <si>
     <t>@User32418</t>
   </si>
   <si>
-    <t>@rkomi99</t>
-  </si>
-  <si>
-    <t>@BwoneJ</t>
-  </si>
-  <si>
     <t>@Augu05</t>
   </si>
   <si>
-    <t>@Balliver</t>
-  </si>
-  <si>
     <t>star</t>
   </si>
   <si>
-    <t>Mr.Fox</t>
-  </si>
-  <si>
-    <t>BwonE</t>
-  </si>
-  <si>
     <t>Augu05</t>
   </si>
   <si>
@@ -569,18 +509,12 @@
     <t>@Basco3</t>
   </si>
   <si>
-    <t>@Napless1926</t>
-  </si>
-  <si>
     <t>@Cisco00001</t>
   </si>
   <si>
     <t>Basco</t>
   </si>
   <si>
-    <t>D10S</t>
-  </si>
-  <si>
     <t>frenci</t>
   </si>
   <si>
@@ -644,12 +578,6 @@
     <t>@Calumett</t>
   </si>
   <si>
-    <t>khmer BM⚡</t>
-  </si>
-  <si>
-    <t>Ａ Ｒ ♠️ ＦＥＤＥＲＩＣＯ</t>
-  </si>
-  <si>
     <t>•fury™•</t>
   </si>
   <si>
@@ -677,30 +605,15 @@
     <t>DOCCC</t>
   </si>
   <si>
-    <t>vinz</t>
-  </si>
-  <si>
     <t>Maradona</t>
   </si>
   <si>
-    <t>Zumpy</t>
-  </si>
-  <si>
     <t>superfede</t>
   </si>
   <si>
-    <t>RETROWAV3R™️</t>
-  </si>
-  <si>
     <t>GXSALVO08</t>
   </si>
   <si>
-    <t>Andyfantasy98</t>
-  </si>
-  <si>
-    <t>IronMan</t>
-  </si>
-  <si>
     <t>Arsenio</t>
   </si>
   <si>
@@ -710,72 +623,36 @@
     <t>@usernamepersonalee</t>
   </si>
   <si>
-    <t>@vinz9898</t>
-  </si>
-  <si>
     <t>@fabri1010</t>
   </si>
   <si>
-    <t>@FabioZumpy77</t>
-  </si>
-  <si>
     <t>@superfede2</t>
   </si>
   <si>
-    <t>@RETROWAV3R</t>
-  </si>
-  <si>
     <t>@GXSALVO08</t>
   </si>
   <si>
-    <t>@AndyFantasy</t>
-  </si>
-  <si>
     <t>@arsenapoli</t>
   </si>
   <si>
     <t>MaLuMa</t>
   </si>
   <si>
-    <t>IvanKing</t>
-  </si>
-  <si>
     <t>@Pacca2317</t>
   </si>
   <si>
-    <t>@Ivanking97</t>
-  </si>
-  <si>
-    <t>kingmike</t>
-  </si>
-  <si>
-    <t>cablo</t>
-  </si>
-  <si>
     <t>testosterone ma</t>
   </si>
   <si>
-    <t>@Kingmike1592</t>
-  </si>
-  <si>
-    <t>@ziobenni26</t>
-  </si>
-  <si>
     <t>@GRQJ8VL02</t>
   </si>
   <si>
     <t>Dog Rider</t>
   </si>
   <si>
-    <t>Thor⚡️</t>
-  </si>
-  <si>
     <t>Si</t>
   </si>
   <si>
-    <t>Alex Hunter</t>
-  </si>
-  <si>
     <t>Raffockij</t>
   </si>
   <si>
@@ -785,43 +662,58 @@
     <t>lilpezzo300</t>
   </si>
   <si>
-    <t>jamino</t>
-  </si>
-  <si>
     <t>@giraffaele</t>
   </si>
   <si>
     <t>@Melqiades</t>
   </si>
   <si>
-    <t>@Immajamino</t>
-  </si>
-  <si>
-    <t>Sfidante</t>
-  </si>
-  <si>
-    <t>YouLose</t>
-  </si>
-  <si>
-    <t>FrankoBot</t>
-  </si>
-  <si>
     <t>KOKODEWA</t>
   </si>
   <si>
-    <t>@Sgrillo97</t>
-  </si>
-  <si>
-    <t>@YL1272</t>
-  </si>
-  <si>
-    <t>@shu4pppp</t>
-  </si>
-  <si>
     <t>@Anti47394</t>
   </si>
   <si>
     <t>Warlosing</t>
+  </si>
+  <si>
+    <t>ＡＲ♠️Ｆｅｄｅ</t>
+  </si>
+  <si>
+    <t>shinigami</t>
+  </si>
+  <si>
+    <t>Thor⚡</t>
+  </si>
+  <si>
+    <t>ＡＲ♠️ｓｐｅｚｉａ</t>
+  </si>
+  <si>
+    <t>@X_teo</t>
+  </si>
+  <si>
+    <t>Syfor</t>
+  </si>
+  <si>
+    <t>DADDA</t>
+  </si>
+  <si>
+    <t>-roger8-</t>
+  </si>
+  <si>
+    <t>@WarWorz</t>
+  </si>
+  <si>
+    <t>PaoloTheBest</t>
+  </si>
+  <si>
+    <t>@PaoloTh3Best</t>
+  </si>
+  <si>
+    <t>vincy</t>
+  </si>
+  <si>
+    <t>@VincyR70</t>
   </si>
 </sst>
 </file>
@@ -1305,13 +1197,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1358,27 +1247,7 @@
     <cellStyle name="Valore non valido" xfId="7" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Valore valido" xfId="6" builtinId="26" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1719,11 +1588,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EE2B0F9-AC31-464B-B046-53CB033C8615}">
-  <dimension ref="A1:D133"/>
+  <dimension ref="A1:D116"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="137" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D133" sqref="D2:D133"/>
+      <selection pane="bottomLeft" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1750,1844 +1619,1605 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>186</v>
+      <c r="A2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>214</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>245</v>
+        <v>205</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+      <c r="B4" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
+      <c r="C7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B11" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="B7" s="2" t="s">
+      <c r="C11" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="B11" s="2" t="s">
+      <c r="C12" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
+      <c r="C14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B22" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B43" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" s="2" t="s">
+      <c r="C43" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="B29" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>244</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A36" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A37" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A38" s="2" t="s">
-        <v>223</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A40" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A42" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A43" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A45" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B46" s="1" t="s">
-        <v>246</v>
+        <v>189</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>243</v>
+        <v>3</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>245</v>
+        <v>205</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A47" s="1" t="s">
-        <v>185</v>
-      </c>
       <c r="B47" s="1" t="s">
-        <v>188</v>
+        <v>217</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>243</v>
+        <v>3</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>245</v>
+        <v>205</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
-        <v>138</v>
+        <v>98</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>123</v>
+        <v>109</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>243</v>
+        <v>3</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>245</v>
+        <v>205</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
-        <v>153</v>
+        <v>127</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>89</v>
+        <v>113</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>243</v>
+        <v>213</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>245</v>
+        <v>205</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
-        <v>176</v>
+        <v>136</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>243</v>
+        <v>213</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>245</v>
+        <v>205</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
-        <v>211</v>
+        <v>151</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>207</v>
+        <v>153</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>243</v>
+        <v>213</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>245</v>
+        <v>205</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
-        <v>77</v>
+        <v>140</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>76</v>
+        <v>37</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>243</v>
+        <v>213</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>245</v>
+        <v>205</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
-        <v>148</v>
+        <v>102</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>134</v>
+        <v>107</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>243</v>
+        <v>213</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>245</v>
+        <v>205</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
-        <v>198</v>
+        <v>74</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>196</v>
+        <v>73</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>243</v>
+        <v>213</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>245</v>
+        <v>205</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
-        <v>49</v>
+        <v>100</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>48</v>
+        <v>106</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>243</v>
+        <v>213</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>245</v>
+        <v>205</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
-        <v>226</v>
+        <v>128</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>215</v>
+        <v>114</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>243</v>
+        <v>213</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>245</v>
+        <v>205</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
-        <v>87</v>
+        <v>56</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>86</v>
+        <v>55</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>243</v>
+        <v>213</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>245</v>
+        <v>205</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
-        <v>142</v>
+        <v>212</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>128</v>
+        <v>211</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>243</v>
+        <v>213</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>245</v>
+        <v>205</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
-        <v>136</v>
+        <v>57</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>243</v>
+        <v>213</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>245</v>
+        <v>205</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
-        <v>242</v>
+        <v>132</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>239</v>
+        <v>121</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>243</v>
+        <v>213</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>245</v>
+        <v>205</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
-        <v>251</v>
+        <v>40</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>247</v>
+        <v>39</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>243</v>
+        <v>213</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>245</v>
+        <v>205</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>47</v>
+        <v>116</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>243</v>
+        <v>213</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>245</v>
+        <v>205</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
-        <v>167</v>
+        <v>180</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>172</v>
+        <v>179</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>243</v>
+        <v>213</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>245</v>
+        <v>205</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
-        <v>235</v>
+        <v>163</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>233</v>
+        <v>166</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>243</v>
+        <v>204</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>245</v>
+        <v>205</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
-        <v>252</v>
+        <v>139</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>248</v>
+        <v>78</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>243</v>
+        <v>204</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>245</v>
+        <v>205</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
-        <v>54</v>
+        <v>169</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>53</v>
+        <v>168</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>243</v>
+        <v>204</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>245</v>
+        <v>205</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
-        <v>109</v>
+        <v>49</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>120</v>
+        <v>48</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>243</v>
+        <v>204</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>245</v>
+        <v>205</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
-        <v>191</v>
+        <v>210</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>190</v>
+        <v>207</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>243</v>
+        <v>204</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>245</v>
+        <v>205</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
-        <v>100</v>
+        <v>185</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>243</v>
+        <v>204</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>245</v>
+        <v>205</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
-        <v>46</v>
+        <v>135</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>45</v>
+        <v>122</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>243</v>
+        <v>204</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>245</v>
+        <v>205</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
-        <v>209</v>
+        <v>197</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>205</v>
+        <v>191</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>243</v>
+        <v>204</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>245</v>
+        <v>205</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
-        <v>155</v>
+        <v>195</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>151</v>
+        <v>137</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>243</v>
+        <v>204</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>245</v>
+        <v>205</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
-        <v>56</v>
+        <v>201</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>55</v>
+        <v>200</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>243</v>
+        <v>204</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>245</v>
+        <v>205</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>243</v>
+        <v>204</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>245</v>
+        <v>205</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A75" s="1" t="s">
+        <v>157</v>
+      </c>
       <c r="B75" s="1" t="s">
-        <v>249</v>
+        <v>159</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>243</v>
+        <v>204</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>245</v>
+        <v>205</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
-        <v>228</v>
+        <v>68</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>217</v>
+        <v>67</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>243</v>
+        <v>204</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>245</v>
+        <v>205</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>243</v>
+        <v>204</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>245</v>
+        <v>205</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
-        <v>106</v>
+        <v>54</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>105</v>
+        <v>53</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>243</v>
+        <v>204</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>245</v>
+        <v>205</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
-        <v>236</v>
+        <v>42</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>234</v>
+        <v>41</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>243</v>
+        <v>204</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>245</v>
+        <v>205</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
-        <v>143</v>
+        <v>218</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>52</v>
+        <v>161</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>243</v>
+        <v>204</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>245</v>
+        <v>205</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
-        <v>232</v>
+        <v>110</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>222</v>
+        <v>47</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>243</v>
+        <v>204</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>245</v>
+        <v>205</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
-        <v>179</v>
+        <v>51</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>182</v>
+        <v>50</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>243</v>
+        <v>204</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>245</v>
+        <v>205</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>243</v>
+        <v>204</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>245</v>
+        <v>205</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
-        <v>230</v>
+        <v>76</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>219</v>
+        <v>75</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>243</v>
+        <v>204</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>245</v>
+        <v>205</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
-        <v>152</v>
+        <v>158</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>203</v>
+        <v>160</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>243</v>
+        <v>204</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>245</v>
+        <v>205</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A86" s="1" t="s">
-        <v>163</v>
-      </c>
       <c r="B86" s="1" t="s">
-        <v>170</v>
+        <v>219</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>243</v>
+        <v>204</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>245</v>
+        <v>205</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>201</v>
+        <v>190</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>243</v>
+        <v>204</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>245</v>
+        <v>205</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>206</v>
+        <v>220</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>243</v>
+        <v>204</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>245</v>
+        <v>205</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
-        <v>177</v>
+        <v>203</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>180</v>
+        <v>202</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>243</v>
+        <v>204</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>245</v>
+        <v>205</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
-        <v>59</v>
+        <v>89</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>64</v>
+        <v>155</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>243</v>
+        <v>204</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>245</v>
+        <v>205</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A91" s="1" t="s">
-        <v>224</v>
-      </c>
       <c r="B91" s="1" t="s">
-        <v>150</v>
+        <v>208</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>243</v>
+        <v>204</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>245</v>
+        <v>205</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="s">
-        <v>253</v>
+        <v>209</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>250</v>
+        <v>206</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>243</v>
+        <v>204</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>245</v>
+        <v>205</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
-        <v>91</v>
+        <v>150</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>90</v>
+        <v>115</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>243</v>
+        <v>204</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>245</v>
+        <v>205</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="s">
-        <v>42</v>
+        <v>149</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>41</v>
+        <v>152</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>243</v>
+        <v>204</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>245</v>
+        <v>205</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="s">
-        <v>169</v>
+        <v>95</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>183</v>
+        <v>94</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>243</v>
+        <v>204</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>245</v>
+        <v>205</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="s">
-        <v>227</v>
+        <v>141</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>216</v>
+        <v>138</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>243</v>
+        <v>204</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>245</v>
+        <v>205</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97" s="1" t="s">
-        <v>141</v>
+        <v>80</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>127</v>
+        <v>79</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>243</v>
+        <v>204</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>245</v>
+        <v>205</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="s">
-        <v>147</v>
+        <v>199</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>81</v>
+        <v>193</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>243</v>
+        <v>204</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>245</v>
+        <v>205</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
-        <v>72</v>
+        <v>124</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>71</v>
+        <v>111</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>243</v>
+        <v>204</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>245</v>
+        <v>205</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="s">
-        <v>85</v>
+        <v>96</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>243</v>
+        <v>204</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>245</v>
+        <v>205</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101" s="1" t="s">
-        <v>107</v>
+        <v>126</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>103</v>
+        <v>112</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>262</v>
+        <v>204</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>245</v>
+        <v>205</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A102" s="1" t="s">
+        <v>176</v>
+      </c>
       <c r="B102" s="1" t="s">
-        <v>221</v>
+        <v>174</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>262</v>
+        <v>204</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>245</v>
+        <v>205</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103" s="1" t="s">
-        <v>212</v>
+        <v>134</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>208</v>
+        <v>70</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>262</v>
+        <v>204</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>245</v>
+        <v>205</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104" s="1" t="s">
-        <v>44</v>
+        <v>130</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>262</v>
+        <v>204</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>245</v>
+        <v>205</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105" s="1" t="s">
-        <v>70</v>
+        <v>187</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>69</v>
+        <v>183</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>262</v>
+        <v>204</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>245</v>
+        <v>205</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106" s="1" t="s">
-        <v>108</v>
+        <v>186</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>104</v>
+        <v>182</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>262</v>
+        <v>204</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>245</v>
+        <v>205</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107" s="1" t="s">
-        <v>258</v>
+        <v>97</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>254</v>
+        <v>93</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>262</v>
+        <v>204</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>245</v>
+        <v>205</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108" s="1" t="s">
-        <v>241</v>
+        <v>198</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>238</v>
+        <v>192</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>262</v>
+        <v>204</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>245</v>
+        <v>205</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A109" s="1" t="s">
-        <v>164</v>
+        <v>188</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>171</v>
+        <v>184</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>262</v>
+        <v>204</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>245</v>
+        <v>205</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110" s="1" t="s">
-        <v>231</v>
+        <v>44</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>220</v>
+        <v>43</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>262</v>
+        <v>204</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>245</v>
+        <v>205</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A111" s="1" t="s">
-        <v>225</v>
+        <v>132</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>214</v>
+        <v>118</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>262</v>
+        <v>204</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>245</v>
+        <v>205</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112" s="1" t="s">
-        <v>240</v>
+        <v>131</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>237</v>
+        <v>117</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>262</v>
+        <v>204</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>245</v>
+        <v>205</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A113" s="1" t="s">
-        <v>229</v>
+        <v>59</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>218</v>
+        <v>58</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>262</v>
+        <v>204</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>245</v>
+        <v>205</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A114" s="1" t="s">
-        <v>79</v>
+        <v>222</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>78</v>
+        <v>221</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>262</v>
+        <v>204</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>245</v>
+        <v>205</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A115" s="1" t="s">
-        <v>178</v>
+        <v>224</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>181</v>
+        <v>223</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>262</v>
+        <v>204</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>245</v>
+        <v>205</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A116" s="1" t="s">
-        <v>145</v>
+        <v>226</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>130</v>
+        <v>225</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>262</v>
+        <v>204</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A117" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="B117" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="C117" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="D117" s="1" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A118" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="B118" s="1" t="s">
-        <v>255</v>
-      </c>
-      <c r="C118" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="D118" s="1" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A119" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B119" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C119" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="D119" s="1" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A120" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="B120" s="1" t="s">
-        <v>256</v>
-      </c>
-      <c r="C120" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="D120" s="1" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A121" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="B121" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="C121" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="D121" s="1" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A122" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="B122" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C122" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="D122" s="1" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A123" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="B123" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="C123" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="D123" s="1" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A124" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="B124" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="C124" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="D124" s="1" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A125" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B125" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="C125" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="D125" s="1" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A126" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B126" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="C126" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="D126" s="1" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A127" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="B127" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="C127" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="D127" s="1" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A128" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="B128" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="C128" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="D128" s="1" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A129" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="B129" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="C129" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="D129" s="1" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A130" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="B130" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="C130" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="D130" s="1" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A131" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B131" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="C131" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="D131" s="1" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A132" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B132" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C132" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="D132" s="1" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A133" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="B133" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C133" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="D133" s="1" t="s">
-        <v>245</v>
+        <v>205</v>
       </c>
     </row>
   </sheetData>
@@ -3595,10 +3225,7 @@
     <sortCondition ref="C2:C123"/>
   </sortState>
   <conditionalFormatting sqref="A1 A144:A1048576">
-    <cfRule type="duplicateValues" dxfId="2" priority="4"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B98:B100">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="4"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
convocazioni stagione 128 - 1
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7ee4892a2dd36b84/Desktop/Link-clan/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="301" documentId="13_ncr:1_{9FCDD52C-4DCE-46C4-BB20-7F2264BA0663}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B43B81DB-062D-4A39-93A6-17925289AABA}"/>
+  <xr:revisionPtr revIDLastSave="341" documentId="13_ncr:1_{9FCDD52C-4DCE-46C4-BB20-7F2264BA0663}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2C211A67-27F2-44E8-8353-4DBF65AC2E18}"/>
   <bookViews>
     <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="13776" xr2:uid="{FECCDA54-7594-4EB7-ABFB-2C408C6461DD}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="248">
   <si>
     <t>TagTelegram</t>
   </si>
@@ -149,12 +149,6 @@
     <t>ＡＲ ❤️ＡＬＥＸ</t>
   </si>
   <si>
-    <t>christian98</t>
-  </si>
-  <si>
-    <t>@chri98757</t>
-  </si>
-  <si>
     <t>Big</t>
   </si>
   <si>
@@ -167,12 +161,6 @@
     <t>@dm996mazz</t>
   </si>
   <si>
-    <t>pro</t>
-  </si>
-  <si>
-    <t>@moretti000</t>
-  </si>
-  <si>
     <t>Bombazza</t>
   </si>
   <si>
@@ -209,9 +197,6 @@
     <t>@Lilyan51</t>
   </si>
   <si>
-    <t>@kvaradona997</t>
-  </si>
-  <si>
     <t>@ralfone01</t>
   </si>
   <si>
@@ -272,9 +257,6 @@
     <t>@NicoSkev98</t>
   </si>
   <si>
-    <t>nevio lostirato</t>
-  </si>
-  <si>
     <t>LATIN WARRIOR™</t>
   </si>
   <si>
@@ -338,9 +320,6 @@
     <t>_SINA22_</t>
   </si>
   <si>
-    <t>●SUMATRA●</t>
-  </si>
-  <si>
     <t>Cicciovolley91</t>
   </si>
   <si>
@@ -380,9 +359,6 @@
     <t>tiau</t>
   </si>
   <si>
-    <t>arKaiba❤️Sparky</t>
-  </si>
-  <si>
     <t>lord Tony</t>
   </si>
   <si>
@@ -419,9 +395,6 @@
     <t>@asso_nr</t>
   </si>
   <si>
-    <t>@sorridetemi</t>
-  </si>
-  <si>
     <t>@T0N1003</t>
   </si>
   <si>
@@ -488,9 +461,6 @@
     <t>frenci</t>
   </si>
   <si>
-    <t>teo</t>
-  </si>
-  <si>
     <t>@kedelu27</t>
   </si>
   <si>
@@ -542,9 +512,6 @@
     <t>SbranaClash300#</t>
   </si>
   <si>
-    <t>Dado has 200 iq</t>
-  </si>
-  <si>
     <t>@Manu2365</t>
   </si>
   <si>
@@ -554,9 +521,6 @@
     <t>@SranaClash300</t>
   </si>
   <si>
-    <t>@Dadoisonfire</t>
-  </si>
-  <si>
     <t>DOCCC</t>
   </si>
   <si>
@@ -590,9 +554,6 @@
     <t>Gervasio</t>
   </si>
   <si>
-    <t>lilpezzo300</t>
-  </si>
-  <si>
     <t>@giraffaele</t>
   </si>
   <si>
@@ -605,24 +566,9 @@
     <t>ＡＲ♠️Ｆｅｄｅ</t>
   </si>
   <si>
-    <t>shinigami</t>
-  </si>
-  <si>
     <t>ＡＲ♠️ｓｐｅｚｉａ</t>
   </si>
   <si>
-    <t>Syfor</t>
-  </si>
-  <si>
-    <t>DADDA</t>
-  </si>
-  <si>
-    <t>-roger8-</t>
-  </si>
-  <si>
-    <t>@WarWorz</t>
-  </si>
-  <si>
     <t>PaoloTheBest</t>
   </si>
   <si>
@@ -674,9 +620,6 @@
     <t>@Sgrillo97</t>
   </si>
   <si>
-    <t>@ziobenni26</t>
-  </si>
-  <si>
     <t>@vinz9898</t>
   </si>
   <si>
@@ -722,9 +665,6 @@
     <t>Sfidante</t>
   </si>
   <si>
-    <t>cablo</t>
-  </si>
-  <si>
     <t>vinz</t>
   </si>
   <si>
@@ -743,24 +683,9 @@
     <t>I Tori Feroci</t>
   </si>
   <si>
-    <t>@Balliver</t>
-  </si>
-  <si>
-    <t>@An_dr3a51</t>
-  </si>
-  <si>
-    <t>@danielylo</t>
-  </si>
-  <si>
     <t>@Lucaser95</t>
   </si>
   <si>
-    <t>ＡＲ❤️Ｄａｒｋ Ａｎｇｅｌ</t>
-  </si>
-  <si>
-    <t>ＡＲ❤️Ｎｉｃｏ</t>
-  </si>
-  <si>
     <t>Lubbro95 C.B.</t>
   </si>
   <si>
@@ -773,49 +698,85 @@
     <t>@Boso_7</t>
   </si>
   <si>
-    <t>@tefanoss</t>
-  </si>
-  <si>
-    <t>⭐️Marco⭐️</t>
-  </si>
-  <si>
-    <t>ＡＲ♦️Ｌ．Ｌａｗｌｉｅｔ</t>
-  </si>
-  <si>
-    <t>ＡＲ♦️ＣＲＥＺＹＲＥＤ</t>
-  </si>
-  <si>
-    <t>AR❤️Nicoflash</t>
-  </si>
-  <si>
-    <t>Ａｒ❤️Ｓａｍｕｅｌｅ</t>
-  </si>
-  <si>
     <t>ＡＲ♦️Ｅ＄</t>
   </si>
   <si>
     <t>Chri</t>
   </si>
   <si>
+    <t>ＡＲ♦️Ｂｏｓｏ</t>
+  </si>
+  <si>
+    <t>ＡＲ♥️Ｓｔｅｆａｎｏ</t>
+  </si>
+  <si>
+    <t>⭐Marco⭐</t>
+  </si>
+  <si>
+    <t>Lind L. Taylor</t>
+  </si>
+  <si>
+    <t>crezyred</t>
+  </si>
+  <si>
+    <t>Thor⚡</t>
+  </si>
+  <si>
+    <t>nicoflash</t>
+  </si>
+  <si>
+    <t>Ａｒ❤Ｓａｍｕｅｌｅ</t>
+  </si>
+  <si>
+    <t>ＡＲ❤️ＳＵＭＡＴＲＡ</t>
+  </si>
+  <si>
+    <t>@tefanosss</t>
+  </si>
+  <si>
+    <t>Beéle</t>
+  </si>
+  <si>
+    <t>SPARTACO_1996</t>
+  </si>
+  <si>
+    <t>testosterone ma</t>
+  </si>
+  <si>
+    <t>Nico</t>
+  </si>
+  <si>
+    <t>@ZuMoOoO</t>
+  </si>
+  <si>
+    <t>@ag0_96</t>
+  </si>
+  <si>
+    <t>@GRQJ8VL02</t>
+  </si>
+  <si>
+    <t>@Melqiades</t>
+  </si>
+  <si>
+    <t>Frittu</t>
+  </si>
+  <si>
+    <t>IL DISTRUTTORE</t>
+  </si>
+  <si>
+    <t>DAI HOPP</t>
+  </si>
+  <si>
+    <t>@Frittuuu</t>
+  </si>
+  <si>
+    <t>@gioee_e27</t>
+  </si>
+  <si>
+    <t>@andrea_cop</t>
+  </si>
+  <si>
     <t>Ａ Ｒ ♠️ ＦＥＤＥＲＩＣＯ</t>
-  </si>
-  <si>
-    <t>ＡＲ♠️Ｏｘｈａｔｒｅｓ</t>
-  </si>
-  <si>
-    <t>ＡＲ♦️Ｂｏｓｏ</t>
-  </si>
-  <si>
-    <t>AR❤️TORIAS</t>
-  </si>
-  <si>
-    <t>ＡＲ♥️Ｓｔｅｆａｎｏ</t>
-  </si>
-  <si>
-    <t>ＡＲ❤️Ｔｅｆａｎｏｓ</t>
-  </si>
-  <si>
-    <t>ＡＲ♥️Ｐｏｎｃｉｏ９９</t>
   </si>
 </sst>
 </file>
@@ -1690,11 +1651,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EE2B0F9-AC31-464B-B046-53CB033C8615}">
-  <dimension ref="A1:D135"/>
+  <dimension ref="A1:D125"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="137" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A97" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D135" sqref="D2:D135"/>
+    <sheetView tabSelected="1" zoomScale="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A115" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D126" sqref="D126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1721,1872 +1682,1744 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>72</v>
+        <v>9</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>71</v>
+        <v>176</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>235</v>
+        <v>3</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>172</v>
+        <v>27</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>168</v>
+        <v>26</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>235</v>
+        <v>3</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>91</v>
+        <v>112</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>235</v>
+        <v>3</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>171</v>
+        <v>232</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>167</v>
+        <v>224</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>235</v>
+        <v>3</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>165</v>
+        <v>59</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>163</v>
+        <v>58</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>235</v>
+        <v>3</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>181</v>
+        <v>22</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>177</v>
+        <v>21</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>235</v>
+        <v>3</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>203</v>
+        <v>17</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>219</v>
+        <v>147</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>235</v>
+        <v>3</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>204</v>
+        <v>31</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>220</v>
+        <v>30</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>235</v>
+        <v>3</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>205</v>
+        <v>91</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>221</v>
+        <v>144</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>235</v>
+        <v>3</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>206</v>
+        <v>142</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>222</v>
+        <v>145</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>235</v>
+        <v>3</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>207</v>
+        <v>126</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>223</v>
+        <v>92</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>235</v>
+        <v>3</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>235</v>
+        <v>3</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>197</v>
+        <v>57</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>196</v>
+        <v>225</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>235</v>
+        <v>3</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>209</v>
+        <v>220</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>235</v>
+        <v>3</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>210</v>
+        <v>13</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>226</v>
+        <v>12</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>235</v>
+        <v>3</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>211</v>
+        <v>219</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>235</v>
+        <v>3</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>43</v>
+        <v>81</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>42</v>
+        <v>79</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>235</v>
+        <v>3</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>212</v>
+        <v>154</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>235</v>
+        <v>3</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>213</v>
+        <v>89</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>229</v>
+        <v>93</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>235</v>
+        <v>3</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>125</v>
+        <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>114</v>
+        <v>19</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>235</v>
+        <v>3</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>195</v>
+        <v>23</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>194</v>
+        <v>227</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>235</v>
+        <v>3</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>112</v>
+        <v>131</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>235</v>
+        <v>3</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>214</v>
+        <v>5</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>230</v>
+        <v>4</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>235</v>
+        <v>3</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>215</v>
+        <v>17</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>235</v>
+        <v>3</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>216</v>
+        <v>35</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>232</v>
+        <v>34</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>235</v>
+        <v>3</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>217</v>
+        <v>80</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>233</v>
+        <v>150</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>235</v>
+        <v>3</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>218</v>
+        <v>8</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>234</v>
+        <v>37</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>235</v>
+        <v>3</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>201</v>
+        <v>11</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>200</v>
+        <v>10</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>235</v>
+        <v>3</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>57</v>
+        <v>134</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>56</v>
+        <v>136</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>235</v>
+        <v>3</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>124</v>
+        <v>25</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>111</v>
+        <v>24</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>235</v>
+        <v>3</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>139</v>
+        <v>16</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>235</v>
+        <v>3</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>129</v>
+        <v>70</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>116</v>
+        <v>74</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>235</v>
+        <v>3</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>54</v>
+        <v>33</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>53</v>
+        <v>32</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>235</v>
+        <v>3</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>188</v>
+        <v>125</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>187</v>
+        <v>78</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>235</v>
+        <v>3</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>55</v>
+        <v>80</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>102</v>
+        <v>77</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>235</v>
+        <v>184</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
-        <v>58</v>
+        <v>97</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>79</v>
+        <v>229</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>235</v>
+        <v>3</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>96</v>
+        <v>65</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>101</v>
+        <v>64</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>235</v>
+        <v>184</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>50</v>
+        <v>106</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>235</v>
+        <v>184</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>28</v>
+        <v>230</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>235</v>
+        <v>184</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41" s="1" t="s">
+        <v>152</v>
+      </c>
       <c r="B41" s="1" t="s">
-        <v>191</v>
+        <v>151</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>202</v>
+        <v>184</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
-        <v>92</v>
+        <v>123</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>103</v>
+        <v>36</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>202</v>
+        <v>184</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
-        <v>121</v>
+        <v>39</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>108</v>
+        <v>38</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>202</v>
+        <v>3</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44" s="1" t="s">
+        <v>86</v>
+      </c>
       <c r="B44" s="1" t="s">
-        <v>185</v>
+        <v>96</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>202</v>
+        <v>3</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>202</v>
+        <v>3</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>202</v>
+        <v>3</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
-        <v>153</v>
+        <v>90</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>156</v>
+        <v>231</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>202</v>
+        <v>3</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
-        <v>159</v>
+        <v>186</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>158</v>
+        <v>201</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>202</v>
+        <v>3</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
-        <v>170</v>
+        <v>149</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>166</v>
+        <v>148</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>202</v>
+        <v>184</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
-        <v>131</v>
+        <v>51</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>76</v>
+        <v>95</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>202</v>
+        <v>184</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A51" s="1" t="s">
-        <v>128</v>
-      </c>
       <c r="B51" s="1" t="s">
-        <v>115</v>
+        <v>177</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>202</v>
+        <v>3</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A52" s="1" t="s">
-        <v>178</v>
-      </c>
       <c r="B52" s="1" t="s">
-        <v>174</v>
+        <v>87</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>202</v>
+        <v>184</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
-        <v>41</v>
+        <v>216</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>40</v>
+        <v>217</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>202</v>
+        <v>184</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
-        <v>199</v>
+        <v>175</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>198</v>
+        <v>174</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>202</v>
+        <v>184</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A55" s="1" t="s">
+        <v>237</v>
+      </c>
       <c r="B55" s="1" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>202</v>
+        <v>184</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
-        <v>236</v>
+        <v>195</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>151</v>
+        <v>210</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>202</v>
+        <v>184</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
-        <v>122</v>
+        <v>54</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>110</v>
+        <v>76</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>202</v>
+        <v>184</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A58" s="1" t="s">
+        <v>61</v>
+      </c>
       <c r="B58" s="1" t="s">
-        <v>241</v>
+        <v>60</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>202</v>
+        <v>184</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
-        <v>52</v>
+        <v>194</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>51</v>
+        <v>209</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>202</v>
+        <v>184</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>100</v>
+        <v>72</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>202</v>
+        <v>184</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>184</v>
+        <v>234</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>202</v>
+        <v>184</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
-        <v>66</v>
+        <v>192</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>65</v>
+        <v>207</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>202</v>
+        <v>184</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
-        <v>148</v>
+        <v>119</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>150</v>
+        <v>63</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>202</v>
+        <v>184</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
-        <v>78</v>
+        <v>109</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>77</v>
+        <v>98</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>202</v>
+        <v>184</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
-        <v>49</v>
+        <v>159</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>48</v>
+        <v>156</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>202</v>
+        <v>184</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
-        <v>180</v>
+        <v>166</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>176</v>
+        <v>162</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>202</v>
+        <v>184</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
-        <v>90</v>
+        <v>167</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>89</v>
+        <v>163</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>202</v>
+        <v>184</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
-        <v>45</v>
+        <v>187</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>44</v>
+        <v>202</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>202</v>
+        <v>184</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
-        <v>74</v>
+        <v>179</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>73</v>
+        <v>178</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>202</v>
+        <v>184</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
-        <v>39</v>
+        <v>115</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>202</v>
+        <v>184</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A71" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="B71" s="1" t="s">
-        <v>192</v>
+        <v>28</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>202</v>
+        <v>184</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
-        <v>86</v>
+        <v>239</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>146</v>
+        <v>235</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>202</v>
+        <v>184</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
-        <v>173</v>
+        <v>48</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>169</v>
+        <v>47</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>202</v>
+        <v>184</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
-        <v>133</v>
+        <v>15</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>130</v>
+        <v>14</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>202</v>
+        <v>184</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
-        <v>179</v>
+        <v>188</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>175</v>
+        <v>203</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>202</v>
+        <v>184</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
-        <v>238</v>
+        <v>173</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>193</v>
+        <v>171</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>202</v>
+        <v>184</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>109</v>
+        <v>140</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>202</v>
+        <v>184</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
-        <v>141</v>
+        <v>88</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>144</v>
+        <v>94</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>202</v>
+        <v>184</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
-        <v>119</v>
+        <v>168</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>106</v>
+        <v>164</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>202</v>
+        <v>184</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
-        <v>147</v>
+        <v>127</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>149</v>
+        <v>130</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>202</v>
+        <v>184</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
-        <v>239</v>
+        <v>56</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>242</v>
+        <v>55</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>202</v>
+        <v>184</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>68</v>
+        <v>103</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>202</v>
+        <v>184</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
-        <v>186</v>
+        <v>161</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>183</v>
+        <v>158</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>202</v>
+        <v>184</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
-        <v>117</v>
+        <v>181</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>105</v>
+        <v>180</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>202</v>
+        <v>184</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A85" s="1" t="s">
+        <v>120</v>
+      </c>
       <c r="B85" s="1" t="s">
-        <v>93</v>
+        <v>108</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>202</v>
+        <v>184</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
-        <v>15</v>
+        <v>196</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>14</v>
+        <v>211</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>202</v>
+        <v>184</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
-        <v>7</v>
+        <v>110</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>6</v>
+        <v>62</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>202</v>
+        <v>184</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="s">
-        <v>97</v>
+        <v>124</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>154</v>
+        <v>121</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>3</v>
+        <v>184</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
-        <v>152</v>
+        <v>97</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>155</v>
+        <v>236</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>3</v>
+        <v>184</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
-        <v>22</v>
+        <v>143</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>21</v>
+        <v>146</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>3</v>
+        <v>184</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
-        <v>135</v>
+        <v>67</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>98</v>
+        <v>66</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>3</v>
+        <v>184</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="s">
-        <v>27</v>
+        <v>183</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>26</v>
+        <v>182</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>3</v>
+        <v>215</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
-        <v>31</v>
+        <v>69</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>30</v>
+        <v>68</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>3</v>
+        <v>215</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="s">
-        <v>62</v>
+        <v>80</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>247</v>
+        <v>137</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>3</v>
+        <v>215</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="s">
-        <v>118</v>
+        <v>240</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>67</v>
+        <v>172</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>3</v>
+        <v>184</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="s">
-        <v>164</v>
+        <v>199</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>248</v>
+        <v>214</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>3</v>
+        <v>215</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97" s="1" t="s">
-        <v>23</v>
+        <v>113</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>249</v>
+        <v>101</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>3</v>
+        <v>215</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="s">
-        <v>137</v>
+        <v>7</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>3</v>
+        <v>215</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
-        <v>126</v>
+        <v>45</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>113</v>
+        <v>44</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>3</v>
+        <v>215</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="s">
-        <v>5</v>
+        <v>122</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>4</v>
+        <v>71</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>3</v>
+        <v>215</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101" s="1" t="s">
-        <v>11</v>
+        <v>191</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>10</v>
+        <v>206</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>3</v>
+        <v>215</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102" s="1" t="s">
-        <v>87</v>
+        <v>190</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>85</v>
+        <v>205</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>3</v>
+        <v>215</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103" s="1" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>3</v>
+        <v>215</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104" s="1" t="s">
-        <v>35</v>
+        <v>244</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>34</v>
+        <v>241</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>3</v>
+        <v>215</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105" s="1" t="s">
-        <v>143</v>
+        <v>169</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>145</v>
+        <v>165</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>3</v>
+        <v>215</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106" s="1" t="s">
-        <v>25</v>
+        <v>116</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>24</v>
+        <v>104</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>3</v>
+        <v>215</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107" s="1" t="s">
-        <v>20</v>
+        <v>245</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>19</v>
+        <v>242</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>3</v>
+        <v>215</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108" s="1" t="s">
-        <v>8</v>
+        <v>155</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>37</v>
+        <v>153</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>3</v>
+        <v>215</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A109" s="1" t="s">
-        <v>162</v>
+        <v>185</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>161</v>
+        <v>200</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>3</v>
+        <v>215</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110" s="1" t="s">
-        <v>86</v>
+        <v>139</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>83</v>
+        <v>141</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>3</v>
+        <v>215</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A111" s="1" t="s">
-        <v>33</v>
+        <v>197</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>32</v>
+        <v>212</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>3</v>
+        <v>215</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112" s="1" t="s">
-        <v>13</v>
+        <v>160</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>12</v>
+        <v>157</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>3</v>
+        <v>215</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A113" s="1" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B113" s="1" t="s">
         <v>107</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>3</v>
+        <v>215</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A114" s="1" t="s">
-        <v>64</v>
+        <v>84</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>63</v>
+        <v>83</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>3</v>
+        <v>215</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A115" s="1" t="s">
-        <v>104</v>
+        <v>43</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>250</v>
+        <v>42</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>3</v>
+        <v>215</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A116" s="1" t="s">
-        <v>59</v>
+        <v>198</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>82</v>
+        <v>213</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>3</v>
+        <v>215</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A117" s="1" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>140</v>
+        <v>102</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>3</v>
+        <v>215</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A118" s="1" t="s">
-        <v>132</v>
+        <v>246</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>36</v>
+        <v>243</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>3</v>
+        <v>215</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A119" s="1" t="s">
-        <v>95</v>
+        <v>117</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>3</v>
+        <v>215</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A120" s="1" t="s">
-        <v>18</v>
+        <v>111</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>251</v>
+        <v>99</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>3</v>
+        <v>215</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A121" s="1" t="s">
-        <v>86</v>
+        <v>53</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>160</v>
+        <v>52</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>3</v>
+        <v>215</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A122" s="1" t="s">
-        <v>243</v>
+        <v>132</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>252</v>
+        <v>135</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>3</v>
+        <v>215</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A123" s="1" t="s">
-        <v>244</v>
+        <v>189</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>253</v>
+        <v>204</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>3</v>
+        <v>215</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A124" s="1" t="s">
-        <v>9</v>
+        <v>193</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>189</v>
+        <v>208</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>3</v>
+        <v>215</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A125" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B125" s="1" t="s">
-        <v>190</v>
+      <c r="B125" t="s">
+        <v>247</v>
       </c>
       <c r="C125" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A126" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B126" s="1" t="s">
-        <v>254</v>
-      </c>
-      <c r="C126" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D126" s="1" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A127" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B127" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="C127" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D127" s="1" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A128" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="B128" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="C128" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D128" s="1" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A129" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="B129" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C129" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D129" s="1" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A130" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="B130" s="1" t="s">
-        <v>255</v>
-      </c>
-      <c r="C130" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D130" s="1" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A131" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="B131" s="1" t="s">
-        <v>256</v>
-      </c>
-      <c r="C131" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D131" s="1" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A132" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="B132" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="C132" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D132" s="1" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A133" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="B133" s="1" t="s">
-        <v>258</v>
-      </c>
-      <c r="C133" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D133" s="1" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A134" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="B134" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="C134" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D134" s="1" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A135" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="B135" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="C135" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D135" s="1" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D123">
     <sortCondition ref="C2:C123"/>
   </sortState>
-  <conditionalFormatting sqref="A1 A144:A1048576">
+  <conditionalFormatting sqref="A144:A1048576 A1">
     <cfRule type="duplicateValues" dxfId="0" priority="4"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
convocazioni stagione 128 colosseo
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7ee4892a2dd36b84/Desktop/Link-clan/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="363" documentId="13_ncr:1_{9FCDD52C-4DCE-46C4-BB20-7F2264BA0663}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FB006D64-503F-43F5-B9C3-D5F8781620D4}"/>
+  <xr:revisionPtr revIDLastSave="379" documentId="13_ncr:1_{9FCDD52C-4DCE-46C4-BB20-7F2264BA0663}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7F60BA40-310D-485E-962E-AB2D487634FE}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="13776" xr2:uid="{FECCDA54-7594-4EB7-ABFB-2C408C6461DD}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{FECCDA54-7594-4EB7-ABFB-2C408C6461DD}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="259">
   <si>
     <t>TagTelegram</t>
   </si>
@@ -125,9 +125,6 @@
     <t>@Mastrolivo</t>
   </si>
   <si>
-    <t>HTL I EBDP</t>
-  </si>
-  <si>
     <t>@RickySina22</t>
   </si>
   <si>
@@ -305,9 +302,6 @@
     <t>@Mattia230</t>
   </si>
   <si>
-    <t>@GAB51172</t>
-  </si>
-  <si>
     <t>AR♦️MANGUSTA</t>
   </si>
   <si>
@@ -323,21 +317,12 @@
     <t>XxMattiaxX</t>
   </si>
   <si>
-    <t>pluto</t>
-  </si>
-  <si>
     <t>@begghich</t>
   </si>
   <si>
     <t>@Davide438</t>
   </si>
   <si>
-    <t>@ZuMoOoO</t>
-  </si>
-  <si>
-    <t>Ａｒ❤Ｓａｍｕｅｌｅ</t>
-  </si>
-  <si>
     <t>⭐Marco⭐</t>
   </si>
   <si>
@@ -345,6 +330,486 @@
   </si>
   <si>
     <t>random guy</t>
+  </si>
+  <si>
+    <t>ＡＲ♠️Ｆｅｄｅ</t>
+  </si>
+  <si>
+    <t>ＡＲ♠️Ｏｘｈａｔｒｅｓ</t>
+  </si>
+  <si>
+    <t>AR❤️TORIAS</t>
+  </si>
+  <si>
+    <t>Ａ Ｒ ♠️ ＦＥＤＥＲＩＣＯ</t>
+  </si>
+  <si>
+    <t>ＡＲ❤️ｉＳＡＭｕ</t>
+  </si>
+  <si>
+    <t>ＡＲ♥️Ｌｏｒｙ９９ｍｉｎｅ</t>
+  </si>
+  <si>
+    <t>AR♠️MrDEATH</t>
+  </si>
+  <si>
+    <t>Daniele</t>
+  </si>
+  <si>
+    <t>ＡＲ♠️ｓｐｅｚｉａ</t>
+  </si>
+  <si>
+    <t>Sønサル•D•Lůffy</t>
+  </si>
+  <si>
+    <t>ＡＲ❤️ＳＵＭＡＴＲＡ</t>
+  </si>
+  <si>
+    <t>Qliff</t>
+  </si>
+  <si>
+    <t>Cuba❤️Eren</t>
+  </si>
+  <si>
+    <t>Chri</t>
+  </si>
+  <si>
+    <t>ＡＲ♦️ｏＢ❗️Ｒ</t>
+  </si>
+  <si>
+    <t>ＡＲ♥️Ｐｏｎｃｉｏ９９</t>
+  </si>
+  <si>
+    <t>Itachi Uchiha</t>
+  </si>
+  <si>
+    <t>ＡＲ♠️Ｇｅｅｎｏ</t>
+  </si>
+  <si>
+    <t>AR♠️alfone</t>
+  </si>
+  <si>
+    <t>bughy</t>
+  </si>
+  <si>
+    <t>ＡＲ♠️ＢＡＣ</t>
+  </si>
+  <si>
+    <t>ＡＲ♥️ＬｅＬｅ</t>
+  </si>
+  <si>
+    <t>Kekko03</t>
+  </si>
+  <si>
+    <t>Torsiz</t>
+  </si>
+  <si>
+    <t>ＡＲ ❤️ＡＬＥＸ</t>
+  </si>
+  <si>
+    <t>AR♣️KeDelu</t>
+  </si>
+  <si>
+    <t>Damo</t>
+  </si>
+  <si>
+    <t>ＡＲ♥️Ｍａｚｚｉｔｏ</t>
+  </si>
+  <si>
+    <t>vinz</t>
+  </si>
+  <si>
+    <t>shinigami</t>
+  </si>
+  <si>
+    <t>ＡＲ❤️Ｔｅｆａｎｏｓ</t>
+  </si>
+  <si>
+    <t>aleman(statale)</t>
+  </si>
+  <si>
+    <t>ＡＲ♣️Ｃｉｃｃｉｏ</t>
+  </si>
+  <si>
+    <t>LATIN WARRIOR™</t>
+  </si>
+  <si>
+    <t>ＡＲ♦️Ｌ．Ｌａｗｌｉｅｔ</t>
+  </si>
+  <si>
+    <t>LORD❄️PEZZO</t>
+  </si>
+  <si>
+    <t>AnUbIs</t>
+  </si>
+  <si>
+    <t>AR♣️OMA</t>
+  </si>
+  <si>
+    <t>ᴀʀ♥️ᴍᴏɴɪᴀ</t>
+  </si>
+  <si>
+    <t>BrokerTony</t>
+  </si>
+  <si>
+    <t>PEZZO❄️</t>
+  </si>
+  <si>
+    <t>ＡＲ♦️Ｅ＄</t>
+  </si>
+  <si>
+    <t>Ａｒ❤️Ｓａｍｕｅｌｅ</t>
+  </si>
+  <si>
+    <t>ＡＲ♣️Ｒｉｃｃａｌｓｏ</t>
+  </si>
+  <si>
+    <t>ＡＲ♦️Ｐｅｐｐｏｎｅ９１</t>
+  </si>
+  <si>
+    <t>ＡＲ♦️ＣＲＥＺＹＲＥＤ</t>
+  </si>
+  <si>
+    <t>ＡＲ♦️Ｂｏｓｏ</t>
+  </si>
+  <si>
+    <t>ＡＲ♥️Ｓｔｅｆａｎｏ</t>
+  </si>
+  <si>
+    <t>@FedericoBello03</t>
+  </si>
+  <si>
+    <t>@Balliver</t>
+  </si>
+  <si>
+    <t>@Boso_7</t>
+  </si>
+  <si>
+    <t>@Lokkah</t>
+  </si>
+  <si>
+    <t>@mrdeath75</t>
+  </si>
+  <si>
+    <t>@yvngdanyy</t>
+  </si>
+  <si>
+    <t>@speziaaa</t>
+  </si>
+  <si>
+    <t>@wa1n8</t>
+  </si>
+  <si>
+    <t>@Sas0800</t>
+  </si>
+  <si>
+    <t>@Punk_ake</t>
+  </si>
+  <si>
+    <t>@cvbalibre</t>
+  </si>
+  <si>
+    <t>@Chris_0773</t>
+  </si>
+  <si>
+    <t>@tefanosss</t>
+  </si>
+  <si>
+    <t>@Zumo0o</t>
+  </si>
+  <si>
+    <t>@Alestrega22</t>
+  </si>
+  <si>
+    <t>@ralfone01</t>
+  </si>
+  <si>
+    <t>@ArBughy</t>
+  </si>
+  <si>
+    <t>@BACWasTaken</t>
+  </si>
+  <si>
+    <t>@K3kk07</t>
+  </si>
+  <si>
+    <t>@Torsiz07</t>
+  </si>
+  <si>
+    <t>@Ale_Mare93</t>
+  </si>
+  <si>
+    <t>@kedelu27</t>
+  </si>
+  <si>
+    <t>@DaMoops</t>
+  </si>
+  <si>
+    <t>@Mazzito</t>
+  </si>
+  <si>
+    <t>@vinz9898</t>
+  </si>
+  <si>
+    <t>@aleman7273</t>
+  </si>
+  <si>
+    <t>@MaspicDigital</t>
+  </si>
+  <si>
+    <t>@LatinoCcH</t>
+  </si>
+  <si>
+    <t>@PharmaShooter</t>
+  </si>
+  <si>
+    <t>@RusuA24</t>
+  </si>
+  <si>
+    <t>@Romas10</t>
+  </si>
+  <si>
+    <t>@BrokerTony</t>
+  </si>
+  <si>
+    <t>@rkomi99</t>
+  </si>
+  <si>
+    <t>@riccalso</t>
+  </si>
+  <si>
+    <t>@PepponeB91</t>
+  </si>
+  <si>
+    <t>@crezyred</t>
+  </si>
+  <si>
+    <t>Mr.Fox</t>
+  </si>
+  <si>
+    <t>Meru</t>
+  </si>
+  <si>
+    <t>lord Tony</t>
+  </si>
+  <si>
+    <t>lilpezzo300</t>
+  </si>
+  <si>
+    <t>SistemaS</t>
+  </si>
+  <si>
+    <t>fogu</t>
+  </si>
+  <si>
+    <t>@Fox_0265</t>
+  </si>
+  <si>
+    <t>@ZuMo0o</t>
+  </si>
+  <si>
+    <t>@MerMet92</t>
+  </si>
+  <si>
+    <t>@T0N1003</t>
+  </si>
+  <si>
+    <t>@BBCTR3</t>
+  </si>
+  <si>
+    <t>Ce Magnamm</t>
+  </si>
+  <si>
+    <t>ＡＲ❤️Ｎｉｃｏ</t>
+  </si>
+  <si>
+    <t>Luca01</t>
+  </si>
+  <si>
+    <t>Raffockij</t>
+  </si>
+  <si>
+    <t>kingmike</t>
+  </si>
+  <si>
+    <t>MARCHIO</t>
+  </si>
+  <si>
+    <t>Lubbro95 C.B.</t>
+  </si>
+  <si>
+    <t>Sfidante</t>
+  </si>
+  <si>
+    <t>superfede</t>
+  </si>
+  <si>
+    <t>\GuyFawkes/</t>
+  </si>
+  <si>
+    <t>DonPunta</t>
+  </si>
+  <si>
+    <t>PaoloTheBest</t>
+  </si>
+  <si>
+    <t>christian98</t>
+  </si>
+  <si>
+    <t>ＡＲ❤️Ｄａｒｋ Ａｎｇｅｌ</t>
+  </si>
+  <si>
+    <t>KOKODEWA</t>
+  </si>
+  <si>
+    <t>vincy</t>
+  </si>
+  <si>
+    <t>Pinguino</t>
+  </si>
+  <si>
+    <t>alabatia89</t>
+  </si>
+  <si>
+    <t>ＡＲ♣️Ｓｕｎｄｒｉｐｓ</t>
+  </si>
+  <si>
+    <t>Bombazza</t>
+  </si>
+  <si>
+    <t>calumet</t>
+  </si>
+  <si>
+    <t>Don Michele</t>
+  </si>
+  <si>
+    <t>Eric</t>
+  </si>
+  <si>
+    <t>Frittu</t>
+  </si>
+  <si>
+    <t>IL DISTRUTTORE</t>
+  </si>
+  <si>
+    <t>Just_Dodo</t>
+  </si>
+  <si>
+    <t>-roger8-</t>
+  </si>
+  <si>
+    <t>Royal Army</t>
+  </si>
+  <si>
+    <t>sebabigo</t>
+  </si>
+  <si>
+    <t>Teodoro⠀Mapuzzi</t>
+  </si>
+  <si>
+    <t>tiau</t>
+  </si>
+  <si>
+    <t>two ciamela</t>
+  </si>
+  <si>
+    <t>Uchiha Madara</t>
+  </si>
+  <si>
+    <t>Zumpy</t>
+  </si>
+  <si>
+    <t>@luca3689</t>
+  </si>
+  <si>
+    <t>@giraffaele</t>
+  </si>
+  <si>
+    <t>@Kingmike1592</t>
+  </si>
+  <si>
+    <t>@Marchio04</t>
+  </si>
+  <si>
+    <t>@Lucaser95</t>
+  </si>
+  <si>
+    <t>@Sgrillo97</t>
+  </si>
+  <si>
+    <t>@superfede2</t>
+  </si>
+  <si>
+    <t>@GoofyGooberr</t>
+  </si>
+  <si>
+    <t>@Wazito888</t>
+  </si>
+  <si>
+    <t>@PaoloTh3Best</t>
+  </si>
+  <si>
+    <t>@chri98757</t>
+  </si>
+  <si>
+    <t>@An_dr3a514</t>
+  </si>
+  <si>
+    <t>@Anti47394</t>
+  </si>
+  <si>
+    <t>@VincyR70</t>
+  </si>
+  <si>
+    <t>@lorenzocastaldii</t>
+  </si>
+  <si>
+    <t>@alabatia89</t>
+  </si>
+  <si>
+    <t>@SUNDRIPSYT</t>
+  </si>
+  <si>
+    <t>@nicola3194</t>
+  </si>
+  <si>
+    <t>@Calumett667</t>
+  </si>
+  <si>
+    <t>@Don_Michele_Royale</t>
+  </si>
+  <si>
+    <t>@srd_rce</t>
+  </si>
+  <si>
+    <t>@Frittuuu</t>
+  </si>
+  <si>
+    <t>@gioee_e27</t>
+  </si>
+  <si>
+    <t>@edoogrigo</t>
+  </si>
+  <si>
+    <t>@WarWorz</t>
+  </si>
+  <si>
+    <t>@Davidone11</t>
+  </si>
+  <si>
+    <t>@Bonzifer</t>
+  </si>
+  <si>
+    <t>@Giggi_A</t>
+  </si>
+  <si>
+    <t>@Madara_2912</t>
+  </si>
+  <si>
+    <t>Dog Rider</t>
+  </si>
+  <si>
+    <t>@Cicciovolley91</t>
   </si>
 </sst>
 </file>
@@ -878,7 +1343,37 @@
     <cellStyle name="Valore non valido" xfId="7" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Valore valido" xfId="6" builtinId="26" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="10">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1279,11 +1774,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EE2B0F9-AC31-464B-B046-53CB033C8615}">
-  <dimension ref="A1:D51"/>
+  <dimension ref="A1:D135"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C51" sqref="C2:D51"/>
+      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1315,699 +1810,1866 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>56</v>
+        <v>147</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>57</v>
+        <v>99</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>66</v>
+        <v>148</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>65</v>
+        <v>100</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>39</v>
+        <v>149</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>36</v>
+        <v>101</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>69</v>
+        <v>147</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>67</v>
+        <v>102</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>84</v>
+        <v>150</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>45</v>
+        <v>149</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>43</v>
+        <v>104</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>29</v>
+        <v>151</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>28</v>
+        <v>105</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>47</v>
+        <v>152</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>6</v>
+        <v>106</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>53</v>
+        <v>153</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>55</v>
+        <v>107</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>16</v>
+        <v>154</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>33</v>
+        <v>108</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>7</v>
+        <v>155</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>100</v>
+        <v>109</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>10</v>
+        <v>156</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>9</v>
+        <v>110</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>19</v>
+        <v>157</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>101</v>
+        <v>111</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>78</v>
+        <v>158</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>80</v>
+        <v>112</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>15</v>
+        <v>149</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>14</v>
+        <v>113</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>21</v>
+        <v>159</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>20</v>
+        <v>114</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>44</v>
+        <v>160</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>8</v>
+        <v>115</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>161</v>
+      </c>
       <c r="B19" s="1" t="s">
-        <v>30</v>
+        <v>116</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>52</v>
+        <v>162</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>37</v>
+        <v>117</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>70</v>
+        <v>163</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>68</v>
+        <v>118</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>18</v>
+        <v>164</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>17</v>
+        <v>119</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>34</v>
+        <v>149</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>92</v>
+        <v>120</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>12</v>
+        <v>165</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>11</v>
+        <v>121</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>26</v>
+        <v>166</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>25</v>
+        <v>122</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>42</v>
+        <v>167</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>22</v>
+        <v>123</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>38</v>
+        <v>168</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>35</v>
+        <v>124</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>46</v>
+        <v>169</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>49</v>
+        <v>125</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>73</v>
+        <v>170</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>71</v>
+        <v>126</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>86</v>
+        <v>171</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>85</v>
+        <v>127</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>88</v>
+        <v>147</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>94</v>
+        <v>128</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>64</v>
+        <v>159</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>63</v>
+        <v>129</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>74</v>
+        <v>172</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>72</v>
+        <v>130</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>24</v>
+        <v>173</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>23</v>
+        <v>131</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>41</v>
+        <v>174</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>91</v>
+        <v>132</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>31</v>
+        <v>175</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>32</v>
+        <v>133</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A37" s="1" t="s">
-        <v>61</v>
-      </c>
       <c r="B37" s="1" t="s">
-        <v>60</v>
+        <v>134</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>58</v>
+        <v>176</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>59</v>
+        <v>135</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
-        <v>29</v>
+        <v>177</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>62</v>
+        <v>136</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
-        <v>40</v>
+        <v>149</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>13</v>
+        <v>137</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
-        <v>5</v>
+        <v>178</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>4</v>
+        <v>138</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A42" s="1" t="s">
-        <v>87</v>
-      </c>
       <c r="B42" s="1" t="s">
-        <v>93</v>
+        <v>139</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
-        <v>97</v>
+        <v>47</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>102</v>
+        <v>49</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
-        <v>98</v>
+        <v>179</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>103</v>
+        <v>140</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
-        <v>79</v>
+        <v>7</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>81</v>
+        <v>141</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
-        <v>90</v>
+        <v>46</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>96</v>
+        <v>6</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
-        <v>77</v>
+        <v>180</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>76</v>
+        <v>142</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
-        <v>51</v>
+        <v>181</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>54</v>
+        <v>143</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
-        <v>89</v>
+        <v>182</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>95</v>
+        <v>144</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
-        <v>48</v>
+        <v>149</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>50</v>
+        <v>145</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
-        <v>99</v>
+        <v>159</v>
       </c>
       <c r="B51" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A52" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A53" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A54" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A55" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A56" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A57" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A58" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A59" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A60" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A61" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A62" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A63" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A64" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A65" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A66" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A67" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A68" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A69" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A70" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A71" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A72" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A73" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B73" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C51" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>75</v>
+      <c r="C73" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A74" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A75" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A76" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A77" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A78" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A79" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A80" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A81" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A82" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A83" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A84" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A85" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A86" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A87" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A88" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A89" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A90" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D90" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A91" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D91" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A92" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D92" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A93" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D93" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B94" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D94" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B95" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D95" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A96" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D96" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A97" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="D97" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A98" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="D98" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A99" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="D99" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A100" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="D100" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A101" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="D101" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A102" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="D102" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A103" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="D103" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A104" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="D104" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A105" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="D105" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A106" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="D106" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A107" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="D107" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A108" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="D108" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A109" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="D109" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A110" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="C110" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="D110" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A111" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="D111" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A112" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="C112" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="D112" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A113" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C113" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="D113" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A114" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="B114" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C114" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="D114" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A115" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C115" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="D115" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A116" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="B116" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="C116" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="D116" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A117" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="B117" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="C117" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="D117" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A118" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="B118" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="C118" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="D118" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A119" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="B119" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="C119" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="D119" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A120" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="B120" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="C120" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="D120" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A121" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="B121" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="C121" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="D121" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A122" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="B122" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="C122" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="D122" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A123" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="B123" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="C123" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="D123" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A124" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="B124" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="C124" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="D124" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A125" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="B125" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="C125" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="D125" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A126" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="B126" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="C126" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="D126" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A127" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="B127" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="C127" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="D127" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A128" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="B128" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="C128" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="D128" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A129" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="B129" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="C129" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="D129" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A130" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="B130" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="C130" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="D130" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A131" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B131" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="C131" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="D131" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A132" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="B132" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="C132" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="D132" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A133" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="B133" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="C133" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="D133" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A134" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="B134" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="C134" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="D134" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A135" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="B135" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="C135" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="D135" s="1" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -2015,24 +3677,33 @@
     <sortCondition ref="C2:C118"/>
   </sortState>
   <conditionalFormatting sqref="A137:A1048576 A1">
-    <cfRule type="duplicateValues" dxfId="6" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="13"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B43:B44">
+    <cfRule type="duplicateValues" dxfId="8" priority="9"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B45">
+    <cfRule type="duplicateValues" dxfId="7" priority="8"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B46">
+    <cfRule type="duplicateValues" dxfId="6" priority="7"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B47">
     <cfRule type="duplicateValues" dxfId="5" priority="6"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B45">
+  <conditionalFormatting sqref="B48">
     <cfRule type="duplicateValues" dxfId="4" priority="5"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B46">
+  <conditionalFormatting sqref="B49">
     <cfRule type="duplicateValues" dxfId="3" priority="4"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B47">
-    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
+  <conditionalFormatting sqref="B52:B96">
+    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B48">
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+  <conditionalFormatting sqref="B52:B96">
+    <cfRule type="duplicateValues" dxfId="1" priority="3"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B49">
+  <conditionalFormatting sqref="B52:B96">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
convocazioni stagione 129 - 1
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7ee4892a2dd36b84/Desktop/Link-clan/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="379" documentId="13_ncr:1_{9FCDD52C-4DCE-46C4-BB20-7F2264BA0663}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7F60BA40-310D-485E-962E-AB2D487634FE}"/>
+  <xr:revisionPtr revIDLastSave="395" documentId="13_ncr:1_{9FCDD52C-4DCE-46C4-BB20-7F2264BA0663}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BAAC0644-930B-4C39-8B0C-6C757EAD4FFF}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{FECCDA54-7594-4EB7-ABFB-2C408C6461DD}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="251">
   <si>
     <t>TagTelegram</t>
   </si>
@@ -323,9 +323,6 @@
     <t>@Davide438</t>
   </si>
   <si>
-    <t>⭐Marco⭐</t>
-  </si>
-  <si>
     <t>begghich</t>
   </si>
   <si>
@@ -335,24 +332,9 @@
     <t>ＡＲ♠️Ｆｅｄｅ</t>
   </si>
   <si>
-    <t>ＡＲ♠️Ｏｘｈａｔｒｅｓ</t>
-  </si>
-  <si>
-    <t>AR❤️TORIAS</t>
-  </si>
-  <si>
     <t>Ａ Ｒ ♠️ ＦＥＤＥＲＩＣＯ</t>
   </si>
   <si>
-    <t>ＡＲ❤️ｉＳＡＭｕ</t>
-  </si>
-  <si>
-    <t>ＡＲ♥️Ｌｏｒｙ９９ｍｉｎｅ</t>
-  </si>
-  <si>
-    <t>AR♠️MrDEATH</t>
-  </si>
-  <si>
     <t>Daniele</t>
   </si>
   <si>
@@ -368,15 +350,9 @@
     <t>Qliff</t>
   </si>
   <si>
-    <t>Cuba❤️Eren</t>
-  </si>
-  <si>
     <t>Chri</t>
   </si>
   <si>
-    <t>ＡＲ♦️ｏＢ❗️Ｒ</t>
-  </si>
-  <si>
     <t>ＡＲ♥️Ｐｏｎｃｉｏ９９</t>
   </si>
   <si>
@@ -395,9 +371,6 @@
     <t>ＡＲ♠️ＢＡＣ</t>
   </si>
   <si>
-    <t>ＡＲ♥️ＬｅＬｅ</t>
-  </si>
-  <si>
     <t>Kekko03</t>
   </si>
   <si>
@@ -422,9 +395,6 @@
     <t>shinigami</t>
   </si>
   <si>
-    <t>ＡＲ❤️Ｔｅｆａｎｏｓ</t>
-  </si>
-  <si>
     <t>aleman(statale)</t>
   </si>
   <si>
@@ -437,24 +407,15 @@
     <t>ＡＲ♦️Ｌ．Ｌａｗｌｉｅｔ</t>
   </si>
   <si>
-    <t>LORD❄️PEZZO</t>
-  </si>
-  <si>
     <t>AnUbIs</t>
   </si>
   <si>
     <t>AR♣️OMA</t>
   </si>
   <si>
-    <t>ᴀʀ♥️ᴍᴏɴɪᴀ</t>
-  </si>
-  <si>
     <t>BrokerTony</t>
   </si>
   <si>
-    <t>PEZZO❄️</t>
-  </si>
-  <si>
     <t>ＡＲ♦️Ｅ＄</t>
   </si>
   <si>
@@ -473,21 +434,12 @@
     <t>ＡＲ♦️Ｂｏｓｏ</t>
   </si>
   <si>
-    <t>ＡＲ♥️Ｓｔｅｆａｎｏ</t>
-  </si>
-  <si>
     <t>@FedericoBello03</t>
   </si>
   <si>
-    <t>@Balliver</t>
-  </si>
-  <si>
     <t>@Boso_7</t>
   </si>
   <si>
-    <t>@Lokkah</t>
-  </si>
-  <si>
     <t>@mrdeath75</t>
   </si>
   <si>
@@ -506,9 +458,6 @@
     <t>@Punk_ake</t>
   </si>
   <si>
-    <t>@cvbalibre</t>
-  </si>
-  <si>
     <t>@Chris_0773</t>
   </si>
   <si>
@@ -590,18 +539,6 @@
     <t>Meru</t>
   </si>
   <si>
-    <t>lord Tony</t>
-  </si>
-  <si>
-    <t>lilpezzo300</t>
-  </si>
-  <si>
-    <t>SistemaS</t>
-  </si>
-  <si>
-    <t>fogu</t>
-  </si>
-  <si>
     <t>@Fox_0265</t>
   </si>
   <si>
@@ -611,15 +548,9 @@
     <t>@MerMet92</t>
   </si>
   <si>
-    <t>@T0N1003</t>
-  </si>
-  <si>
     <t>@BBCTR3</t>
   </si>
   <si>
-    <t>Ce Magnamm</t>
-  </si>
-  <si>
     <t>ＡＲ❤️Ｎｉｃｏ</t>
   </si>
   <si>
@@ -806,10 +737,55 @@
     <t>@Madara_2912</t>
   </si>
   <si>
-    <t>Dog Rider</t>
-  </si>
-  <si>
-    <t>@Cicciovolley91</t>
+    <t>mrdeath75</t>
+  </si>
+  <si>
+    <t>⭐️Marco⭐️</t>
+  </si>
+  <si>
+    <t>AR ♦️Goldenboy</t>
+  </si>
+  <si>
+    <t>@aless_io98</t>
+  </si>
+  <si>
+    <t>Gervasio</t>
+  </si>
+  <si>
+    <t>teo</t>
+  </si>
+  <si>
+    <t>DADDA</t>
+  </si>
+  <si>
+    <t>@Melqiades</t>
+  </si>
+  <si>
+    <t>@X_teo</t>
+  </si>
+  <si>
+    <t>@FabioZumpy77</t>
+  </si>
+  <si>
+    <t>@danielylo</t>
+  </si>
+  <si>
+    <t>I Tori Feroci</t>
+  </si>
+  <si>
+    <t>arKaiba❤️Sparky</t>
+  </si>
+  <si>
+    <t>the terminator</t>
+  </si>
+  <si>
+    <t>Thor⚡️</t>
+  </si>
+  <si>
+    <t>@sorridetemi</t>
+  </si>
+  <si>
+    <t>Warlosing</t>
   </si>
 </sst>
 </file>
@@ -1774,11 +1750,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EE2B0F9-AC31-464B-B046-53CB033C8615}">
-  <dimension ref="A1:D135"/>
+  <dimension ref="A1:D126"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
+      <selection pane="bottomLeft" activeCell="F114" sqref="F114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1810,10 +1786,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>147</v>
+        <v>133</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>3</v>
@@ -1824,10 +1800,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>3</v>
@@ -1838,10 +1814,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>149</v>
+        <v>138</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>3</v>
@@ -1852,10 +1828,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>147</v>
+        <v>136</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>3</v>
@@ -1866,10 +1842,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>150</v>
+        <v>7</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>103</v>
+        <v>128</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>3</v>
@@ -1880,10 +1856,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>149</v>
+        <v>163</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>104</v>
+        <v>129</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>3</v>
@@ -1894,10 +1870,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>151</v>
+        <v>161</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>105</v>
+        <v>126</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>3</v>
@@ -1908,10 +1884,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>3</v>
@@ -1922,10 +1898,10 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>107</v>
+        <v>122</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>3</v>
@@ -1936,10 +1912,10 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>108</v>
+        <v>127</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>3</v>
@@ -1950,10 +1926,10 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>3</v>
@@ -1964,10 +1940,10 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>156</v>
+        <v>141</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>3</v>
@@ -1978,10 +1954,10 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>111</v>
+        <v>120</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>3</v>
@@ -1992,10 +1968,10 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>158</v>
+        <v>139</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>3</v>
@@ -2006,10 +1982,10 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>149</v>
+        <v>165</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>113</v>
+        <v>131</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>3</v>
@@ -2020,10 +1996,10 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>114</v>
+        <v>121</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>3</v>
@@ -2034,10 +2010,10 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>160</v>
+        <v>140</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>3</v>
@@ -2048,10 +2024,10 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>161</v>
+        <v>151</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>3</v>
@@ -2062,10 +2038,10 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>162</v>
+        <v>143</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>3</v>
@@ -2076,10 +2052,10 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>163</v>
+        <v>147</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>3</v>
@@ -2090,10 +2066,10 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>164</v>
+        <v>146</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>3</v>
@@ -2104,10 +2080,10 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>149</v>
+        <v>158</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>3</v>
@@ -2118,10 +2094,10 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>3</v>
@@ -2132,10 +2108,10 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>3</v>
@@ -2146,10 +2122,10 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>167</v>
+        <v>150</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>3</v>
@@ -2160,10 +2136,10 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>168</v>
+        <v>135</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>124</v>
+        <v>234</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>3</v>
@@ -2174,10 +2150,10 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>169</v>
+        <v>145</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>125</v>
+        <v>109</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>3</v>
@@ -2188,10 +2164,10 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>170</v>
+        <v>134</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>3</v>
@@ -2202,10 +2178,10 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>171</v>
+        <v>24</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>127</v>
+        <v>23</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>3</v>
@@ -2216,10 +2192,10 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>147</v>
+        <v>63</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>128</v>
+        <v>62</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>3</v>
@@ -2230,10 +2206,10 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>159</v>
+        <v>44</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>129</v>
+        <v>42</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>3</v>
@@ -2244,10 +2220,10 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>172</v>
+        <v>209</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>130</v>
+        <v>177</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>3</v>
@@ -2258,10 +2234,10 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>173</v>
+        <v>29</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>131</v>
+        <v>28</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>3</v>
@@ -2272,10 +2248,10 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>174</v>
+        <v>33</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>132</v>
+        <v>90</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>3</v>
@@ -2286,10 +2262,10 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>175</v>
+        <v>18</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>133</v>
+        <v>17</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>3</v>
@@ -2299,8 +2275,11 @@
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" s="1" t="s">
+        <v>45</v>
+      </c>
       <c r="B37" s="1" t="s">
-        <v>134</v>
+        <v>48</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>3</v>
@@ -2311,10 +2290,10 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>176</v>
+        <v>19</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>135</v>
+        <v>235</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>3</v>
@@ -2325,10 +2304,10 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
-        <v>177</v>
+        <v>228</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>136</v>
+        <v>196</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>3</v>
@@ -2339,10 +2318,10 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
-        <v>149</v>
+        <v>208</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>137</v>
+        <v>176</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>3</v>
@@ -2353,10 +2332,10 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
-        <v>178</v>
+        <v>152</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>138</v>
+        <v>116</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>3</v>
@@ -2366,8 +2345,11 @@
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="B42" s="1" t="s">
-        <v>139</v>
+        <v>35</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>3</v>
@@ -2378,10 +2360,10 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>49</v>
+        <v>8</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>3</v>
@@ -2392,10 +2374,10 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
-        <v>179</v>
+        <v>206</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>140</v>
+        <v>174</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>3</v>
@@ -2406,10 +2388,10 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
-        <v>7</v>
+        <v>226</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>141</v>
+        <v>194</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>3</v>
@@ -2420,10 +2402,10 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
-        <v>46</v>
+        <v>237</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>6</v>
+        <v>236</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>3</v>
@@ -2434,10 +2416,10 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
-        <v>180</v>
+        <v>213</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>142</v>
+        <v>181</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>3</v>
@@ -2448,10 +2430,10 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
-        <v>181</v>
+        <v>210</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>143</v>
+        <v>178</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>3</v>
@@ -2462,10 +2444,10 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
-        <v>182</v>
+        <v>12</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>144</v>
+        <v>11</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>3</v>
@@ -2476,10 +2458,10 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
-        <v>149</v>
+        <v>212</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>145</v>
+        <v>180</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>3</v>
@@ -2490,13 +2472,13 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
-        <v>159</v>
+        <v>68</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>146</v>
+        <v>66</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>3</v>
+        <v>245</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>74</v>
@@ -2504,13 +2486,13 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
-        <v>77</v>
+        <v>5</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>79</v>
+        <v>4</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>194</v>
+        <v>245</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>74</v>
@@ -2518,13 +2500,13 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
-        <v>55</v>
+        <v>30</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>56</v>
+        <v>31</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>194</v>
+        <v>245</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>74</v>
@@ -2532,13 +2514,13 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
-        <v>65</v>
+        <v>95</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>64</v>
+        <v>97</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>194</v>
+        <v>245</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>74</v>
@@ -2546,13 +2528,13 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
-        <v>76</v>
+        <v>218</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>75</v>
+        <v>186</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>194</v>
+        <v>245</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>74</v>
@@ -2566,7 +2548,7 @@
         <v>80</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>194</v>
+        <v>245</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>74</v>
@@ -2574,13 +2556,13 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
-        <v>44</v>
+        <v>233</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>42</v>
+        <v>203</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>194</v>
+        <v>245</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>74</v>
@@ -2588,13 +2570,13 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
-        <v>69</v>
+        <v>219</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>67</v>
+        <v>187</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>194</v>
+        <v>245</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>74</v>
@@ -2602,13 +2584,13 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
-        <v>16</v>
+        <v>94</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>32</v>
+        <v>96</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>194</v>
+        <v>245</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>74</v>
@@ -2616,13 +2598,13 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
-        <v>189</v>
+        <v>40</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>183</v>
+        <v>89</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>194</v>
+        <v>245</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>74</v>
@@ -2630,13 +2612,13 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>194</v>
+        <v>245</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>74</v>
@@ -2644,13 +2626,13 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
-        <v>190</v>
+        <v>170</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>81</v>
+        <v>167</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>194</v>
+        <v>245</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>74</v>
@@ -2658,13 +2640,13 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
-        <v>52</v>
+        <v>207</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>54</v>
+        <v>175</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>194</v>
+        <v>245</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>74</v>
@@ -2672,13 +2654,13 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
-        <v>21</v>
+        <v>205</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>20</v>
+        <v>173</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>194</v>
+        <v>245</v>
       </c>
       <c r="D64" s="1" t="s">
         <v>74</v>
@@ -2686,13 +2668,13 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
-        <v>86</v>
+        <v>241</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>91</v>
+        <v>238</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>194</v>
+        <v>245</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>74</v>
@@ -2700,13 +2682,13 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
-        <v>95</v>
+        <v>215</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>98</v>
+        <v>183</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>194</v>
+        <v>245</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>74</v>
@@ -2714,13 +2696,13 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
-        <v>29</v>
+        <v>169</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>28</v>
+        <v>81</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>194</v>
+        <v>245</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>74</v>
@@ -2728,13 +2710,13 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>66</v>
+        <v>79</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>194</v>
+        <v>245</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>74</v>
@@ -2742,13 +2724,13 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
-        <v>191</v>
+        <v>222</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>194</v>
+        <v>245</v>
       </c>
       <c r="D69" s="1" t="s">
         <v>74</v>
@@ -2756,13 +2738,13 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
-        <v>19</v>
+        <v>224</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>96</v>
+        <v>192</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>194</v>
+        <v>245</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>74</v>
@@ -2770,13 +2752,13 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
-        <v>18</v>
+        <v>69</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>17</v>
+        <v>67</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>194</v>
+        <v>245</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>74</v>
@@ -2784,13 +2766,13 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
-        <v>72</v>
+        <v>29</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>194</v>
+        <v>245</v>
       </c>
       <c r="D72" s="1" t="s">
         <v>74</v>
@@ -2798,13 +2780,13 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
-        <v>83</v>
+        <v>65</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>82</v>
+        <v>64</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>194</v>
+        <v>245</v>
       </c>
       <c r="D73" s="1" t="s">
         <v>74</v>
@@ -2812,13 +2794,13 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
-        <v>38</v>
+        <v>10</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>35</v>
+        <v>9</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>194</v>
+        <v>245</v>
       </c>
       <c r="D74" s="1" t="s">
         <v>74</v>
@@ -2826,13 +2808,13 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
-        <v>10</v>
+        <v>51</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>194</v>
+        <v>245</v>
       </c>
       <c r="D75" s="1" t="s">
         <v>74</v>
@@ -2840,13 +2822,13 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
-        <v>5</v>
+        <v>216</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>4</v>
+        <v>184</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>194</v>
+        <v>245</v>
       </c>
       <c r="D76" s="1" t="s">
         <v>74</v>
@@ -2854,13 +2836,13 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
-        <v>26</v>
+        <v>57</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>25</v>
+        <v>58</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>194</v>
+        <v>245</v>
       </c>
       <c r="D77" s="1" t="s">
         <v>74</v>
@@ -2868,13 +2850,13 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
-        <v>15</v>
+        <v>242</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>14</v>
+        <v>239</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>194</v>
+        <v>245</v>
       </c>
       <c r="D78" s="1" t="s">
         <v>74</v>
@@ -2882,13 +2864,13 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
-        <v>12</v>
+        <v>171</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>11</v>
+        <v>201</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>194</v>
+        <v>245</v>
       </c>
       <c r="D79" s="1" t="s">
         <v>74</v>
@@ -2896,13 +2878,13 @@
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
-        <v>33</v>
+        <v>227</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>90</v>
+        <v>195</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>194</v>
+        <v>245</v>
       </c>
       <c r="D80" s="1" t="s">
         <v>74</v>
@@ -2910,13 +2892,13 @@
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
-        <v>37</v>
+        <v>60</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>34</v>
+        <v>59</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>194</v>
+        <v>245</v>
       </c>
       <c r="D81" s="1" t="s">
         <v>74</v>
@@ -2924,13 +2906,13 @@
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
-        <v>45</v>
+        <v>214</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>48</v>
+        <v>182</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>194</v>
+        <v>245</v>
       </c>
       <c r="D82" s="1" t="s">
         <v>74</v>
@@ -2938,13 +2920,13 @@
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
-        <v>73</v>
+        <v>16</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>71</v>
+        <v>32</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>194</v>
+        <v>245</v>
       </c>
       <c r="D83" s="1" t="s">
         <v>74</v>
@@ -2952,13 +2934,13 @@
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
-        <v>63</v>
+        <v>211</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>62</v>
+        <v>179</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>194</v>
+        <v>245</v>
       </c>
       <c r="D84" s="1" t="s">
         <v>74</v>
@@ -2966,13 +2948,13 @@
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
-        <v>87</v>
+        <v>220</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>92</v>
+        <v>188</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>194</v>
+        <v>245</v>
       </c>
       <c r="D85" s="1" t="s">
         <v>74</v>
@@ -2980,13 +2962,13 @@
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>194</v>
+        <v>245</v>
       </c>
       <c r="D86" s="1" t="s">
         <v>74</v>
@@ -2994,13 +2976,13 @@
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>194</v>
+        <v>245</v>
       </c>
       <c r="D87" s="1" t="s">
         <v>74</v>
@@ -3008,13 +2990,13 @@
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="s">
-        <v>30</v>
+        <v>83</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>31</v>
+        <v>82</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>194</v>
+        <v>245</v>
       </c>
       <c r="D88" s="1" t="s">
         <v>74</v>
@@ -3022,13 +3004,13 @@
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
-        <v>41</v>
+        <v>225</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>22</v>
+        <v>193</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>194</v>
+        <v>245</v>
       </c>
       <c r="D89" s="1" t="s">
         <v>74</v>
@@ -3036,13 +3018,13 @@
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
-        <v>24</v>
+        <v>230</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>23</v>
+        <v>198</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>194</v>
+        <v>245</v>
       </c>
       <c r="D90" s="1" t="s">
         <v>74</v>
@@ -3050,13 +3032,13 @@
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>89</v>
+        <v>22</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>194</v>
+        <v>245</v>
       </c>
       <c r="D91" s="1" t="s">
         <v>74</v>
@@ -3064,13 +3046,13 @@
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="s">
-        <v>192</v>
+        <v>73</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>185</v>
+        <v>71</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>194</v>
+        <v>245</v>
       </c>
       <c r="D92" s="1" t="s">
         <v>74</v>
@@ -3078,35 +3060,41 @@
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>61</v>
+        <v>34</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>194</v>
+        <v>245</v>
       </c>
       <c r="D93" s="1" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A94" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="B94" s="1" t="s">
-        <v>186</v>
+        <v>13</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>194</v>
+        <v>245</v>
       </c>
       <c r="D94" s="1" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A95" s="1" t="s">
+        <v>72</v>
+      </c>
       <c r="B95" s="1" t="s">
-        <v>187</v>
+        <v>70</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>194</v>
+        <v>245</v>
       </c>
       <c r="D95" s="1" t="s">
         <v>74</v>
@@ -3114,13 +3102,13 @@
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="s">
-        <v>193</v>
+        <v>243</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>194</v>
+        <v>245</v>
       </c>
       <c r="D96" s="1" t="s">
         <v>74</v>
@@ -3128,13 +3116,13 @@
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97" s="1" t="s">
-        <v>33</v>
+        <v>244</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>195</v>
+        <v>240</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>257</v>
+        <v>245</v>
       </c>
       <c r="D97" s="1" t="s">
         <v>74</v>
@@ -3142,13 +3130,13 @@
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="s">
-        <v>51</v>
+        <v>87</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>36</v>
+        <v>92</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>257</v>
+        <v>245</v>
       </c>
       <c r="D98" s="1" t="s">
         <v>74</v>
@@ -3156,13 +3144,13 @@
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
-        <v>88</v>
+        <v>223</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>93</v>
+        <v>191</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>257</v>
+        <v>245</v>
       </c>
       <c r="D99" s="1" t="s">
         <v>74</v>
@@ -3170,13 +3158,13 @@
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="s">
-        <v>57</v>
+        <v>15</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>58</v>
+        <v>14</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>257</v>
+        <v>245</v>
       </c>
       <c r="D100" s="1" t="s">
         <v>74</v>
@@ -3184,13 +3172,13 @@
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101" s="1" t="s">
-        <v>228</v>
+        <v>33</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>196</v>
+        <v>172</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="D101" s="1" t="s">
         <v>74</v>
@@ -3198,13 +3186,13 @@
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102" s="1" t="s">
-        <v>229</v>
+        <v>168</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>197</v>
+        <v>166</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="D102" s="1" t="s">
         <v>74</v>
@@ -3212,13 +3200,13 @@
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103" s="1" t="s">
-        <v>230</v>
+        <v>55</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>198</v>
+        <v>56</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="D103" s="1" t="s">
         <v>74</v>
@@ -3226,13 +3214,13 @@
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104" s="1" t="s">
-        <v>231</v>
+        <v>76</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>199</v>
+        <v>75</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="D104" s="1" t="s">
         <v>74</v>
@@ -3240,13 +3228,13 @@
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105" s="1" t="s">
-        <v>232</v>
+        <v>21</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>200</v>
+        <v>20</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="D105" s="1" t="s">
         <v>74</v>
@@ -3254,13 +3242,13 @@
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106" s="1" t="s">
-        <v>233</v>
+        <v>221</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>201</v>
+        <v>189</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="D106" s="1" t="s">
         <v>74</v>
@@ -3268,27 +3256,24 @@
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107" s="1" t="s">
-        <v>234</v>
+        <v>249</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>202</v>
+        <v>246</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="D107" s="1" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A108" s="1" t="s">
-        <v>39</v>
-      </c>
       <c r="B108" s="1" t="s">
-        <v>13</v>
+        <v>247</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="D108" s="1" t="s">
         <v>74</v>
@@ -3296,13 +3281,13 @@
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A109" s="1" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="D109" s="1" t="s">
         <v>74</v>
@@ -3310,13 +3295,13 @@
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110" s="1" t="s">
-        <v>236</v>
+        <v>217</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>204</v>
+        <v>185</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="D110" s="1" t="s">
         <v>74</v>
@@ -3324,13 +3309,13 @@
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A111" s="1" t="s">
-        <v>237</v>
+        <v>88</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>205</v>
+        <v>93</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="D111" s="1" t="s">
         <v>74</v>
@@ -3338,13 +3323,13 @@
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112" s="1" t="s">
-        <v>238</v>
+        <v>85</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>206</v>
+        <v>84</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="D112" s="1" t="s">
         <v>74</v>
@@ -3352,13 +3337,13 @@
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A113" s="1" t="s">
-        <v>50</v>
+        <v>232</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>53</v>
+        <v>202</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="D113" s="1" t="s">
         <v>74</v>
@@ -3366,13 +3351,13 @@
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A114" s="1" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="D114" s="1" t="s">
         <v>74</v>
@@ -3380,13 +3365,13 @@
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A115" s="1" t="s">
-        <v>85</v>
+        <v>138</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>84</v>
+        <v>248</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="D115" s="1" t="s">
         <v>74</v>
@@ -3394,13 +3379,13 @@
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A116" s="1" t="s">
-        <v>240</v>
+        <v>133</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>208</v>
+        <v>99</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="D116" s="1" t="s">
         <v>74</v>
@@ -3408,13 +3393,13 @@
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A117" s="1" t="s">
-        <v>241</v>
+        <v>133</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>209</v>
+        <v>119</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="D117" s="1" t="s">
         <v>74</v>
@@ -3422,13 +3407,13 @@
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A118" s="1" t="s">
-        <v>242</v>
+        <v>52</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>210</v>
+        <v>54</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="D118" s="1" t="s">
         <v>74</v>
@@ -3436,13 +3421,13 @@
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A119" s="1" t="s">
-        <v>243</v>
+        <v>149</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>211</v>
+        <v>113</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="D119" s="1" t="s">
         <v>74</v>
@@ -3450,13 +3435,13 @@
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A120" s="1" t="s">
-        <v>244</v>
+        <v>160</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>212</v>
+        <v>125</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="D120" s="1" t="s">
         <v>74</v>
@@ -3464,13 +3449,13 @@
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A121" s="1" t="s">
-        <v>245</v>
+        <v>148</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>213</v>
+        <v>112</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="D121" s="1" t="s">
         <v>74</v>
@@ -3478,13 +3463,13 @@
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A122" s="1" t="s">
-        <v>246</v>
+        <v>47</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>214</v>
+        <v>49</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="D122" s="1" t="s">
         <v>74</v>
@@ -3492,13 +3477,13 @@
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A123" s="1" t="s">
-        <v>247</v>
+        <v>46</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>215</v>
+        <v>6</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="D123" s="1" t="s">
         <v>74</v>
@@ -3506,13 +3491,13 @@
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A124" s="1" t="s">
-        <v>248</v>
+        <v>164</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>216</v>
+        <v>130</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="D124" s="1" t="s">
         <v>74</v>
@@ -3520,13 +3505,13 @@
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A125" s="1" t="s">
-        <v>249</v>
+        <v>137</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>217</v>
+        <v>101</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="D125" s="1" t="s">
         <v>74</v>
@@ -3534,141 +3519,15 @@
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A126" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B126" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="C126" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="B126" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="C126" s="1" t="s">
-        <v>257</v>
-      </c>
       <c r="D126" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A127" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="B127" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="C127" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="D127" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A128" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="B128" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="C128" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="D128" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A129" s="1" t="s">
-        <v>253</v>
-      </c>
-      <c r="B129" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="C129" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="D129" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A130" s="1" t="s">
-        <v>254</v>
-      </c>
-      <c r="B130" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="C130" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="D130" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A131" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B131" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="C131" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="D131" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A132" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="B132" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="C132" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="D132" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A133" s="1" t="s">
-        <v>255</v>
-      </c>
-      <c r="B133" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="C133" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="D133" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A134" s="1" t="s">
-        <v>256</v>
-      </c>
-      <c r="B134" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="C134" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="D134" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A135" s="1" t="s">
-        <v>258</v>
-      </c>
-      <c r="B135" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="C135" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="D135" s="1" t="s">
         <v>74</v>
       </c>
     </row>
@@ -3698,13 +3557,9 @@
     <cfRule type="duplicateValues" dxfId="3" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B52:B96">
-    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B52:B96">
-    <cfRule type="duplicateValues" dxfId="1" priority="3"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B52:B96">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="3"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
convocazioni stagione 129 - 3
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7ee4892a2dd36b84/Desktop/Link-clan/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="397" documentId="13_ncr:1_{9FCDD52C-4DCE-46C4-BB20-7F2264BA0663}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E61C9DE7-014A-494B-93B2-9C1FE1562B7A}"/>
+  <xr:revisionPtr revIDLastSave="415" documentId="13_ncr:1_{9FCDD52C-4DCE-46C4-BB20-7F2264BA0663}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A077F987-05E5-44E6-A68D-A268E3B6C799}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{FECCDA54-7594-4EB7-ABFB-2C408C6461DD}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{FECCDA54-7594-4EB7-ABFB-2C408C6461DD}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="221">
   <si>
     <t>TagTelegram</t>
   </si>
@@ -155,9 +155,6 @@
     <t>@Oneleggedjack</t>
   </si>
   <si>
-    <t>@mangusta_agile</t>
-  </si>
-  <si>
     <t>@asso_nr</t>
   </si>
   <si>
@@ -194,9 +191,6 @@
     <t>@Augu05</t>
   </si>
   <si>
-    <t>star</t>
-  </si>
-  <si>
     <t>Augu05</t>
   </si>
   <si>
@@ -218,15 +212,6 @@
     <t>@Gianlomb</t>
   </si>
   <si>
-    <t>mastro olivo</t>
-  </si>
-  <si>
-    <t>ItsMeYUKKI</t>
-  </si>
-  <si>
-    <t>@Yukki1_618</t>
-  </si>
-  <si>
     <t>TOTAL DISASTER</t>
   </si>
   <si>
@@ -260,33 +245,15 @@
     <t>Si</t>
   </si>
   <si>
-    <t>Francy</t>
-  </si>
-  <si>
-    <t>@CiccioRex</t>
-  </si>
-  <si>
     <t>@BwoneJ</t>
   </si>
   <si>
-    <t>@orso_86</t>
-  </si>
-  <si>
     <t>BwonE</t>
   </si>
   <si>
-    <t>orso86</t>
-  </si>
-  <si>
     <t>Beéle</t>
   </si>
   <si>
-    <t>SPARTACO_1996</t>
-  </si>
-  <si>
-    <t>@ag0_96</t>
-  </si>
-  <si>
     <t>DAI HOPP</t>
   </si>
   <si>
@@ -302,39 +269,18 @@
     <t>@Mattia230</t>
   </si>
   <si>
-    <t>AR♦️MANGUSTA</t>
-  </si>
-  <si>
-    <t>ＡＲ❤️ＮｉｃｏＦｌａｓｈ</t>
-  </si>
-  <si>
     <t>Tristaban</t>
   </si>
   <si>
-    <t>KAIROS</t>
-  </si>
-  <si>
     <t>XxMattiaxX</t>
   </si>
   <si>
     <t>@begghich</t>
   </si>
   <si>
-    <t>@Davide438</t>
-  </si>
-  <si>
     <t>begghich</t>
   </si>
   <si>
-    <t>random guy</t>
-  </si>
-  <si>
-    <t>ＡＲ♠️Ｆｅｄｅ</t>
-  </si>
-  <si>
-    <t>Ａ Ｒ ♠️ ＦＥＤＥＲＩＣＯ</t>
-  </si>
-  <si>
     <t>Daniele</t>
   </si>
   <si>
@@ -353,15 +299,9 @@
     <t>Chri</t>
   </si>
   <si>
-    <t>ＡＲ♥️Ｐｏｎｃｉｏ９９</t>
-  </si>
-  <si>
     <t>Itachi Uchiha</t>
   </si>
   <si>
-    <t>ＡＲ♠️Ｇｅｅｎｏ</t>
-  </si>
-  <si>
     <t>AR♠️alfone</t>
   </si>
   <si>
@@ -404,9 +344,6 @@
     <t>LATIN WARRIOR™</t>
   </si>
   <si>
-    <t>ＡＲ♦️Ｌ．Ｌａｗｌｉｅｔ</t>
-  </si>
-  <si>
     <t>AnUbIs</t>
   </si>
   <si>
@@ -425,21 +362,12 @@
     <t>ＡＲ♣️Ｒｉｃｃａｌｓｏ</t>
   </si>
   <si>
-    <t>ＡＲ♦️Ｐｅｐｐｏｎｅ９１</t>
-  </si>
-  <si>
     <t>ＡＲ♦️ＣＲＥＺＹＲＥＤ</t>
   </si>
   <si>
-    <t>ＡＲ♦️Ｂｏｓｏ</t>
-  </si>
-  <si>
     <t>@FedericoBello03</t>
   </si>
   <si>
-    <t>@Boso_7</t>
-  </si>
-  <si>
     <t>@mrdeath75</t>
   </si>
   <si>
@@ -461,15 +389,9 @@
     <t>@Chris_0773</t>
   </si>
   <si>
-    <t>@tefanosss</t>
-  </si>
-  <si>
     <t>@Zumo0o</t>
   </si>
   <si>
-    <t>@Alestrega22</t>
-  </si>
-  <si>
     <t>@ralfone01</t>
   </si>
   <si>
@@ -509,9 +431,6 @@
     <t>@LatinoCcH</t>
   </si>
   <si>
-    <t>@PharmaShooter</t>
-  </si>
-  <si>
     <t>@RusuA24</t>
   </si>
   <si>
@@ -527,9 +446,6 @@
     <t>@riccalso</t>
   </si>
   <si>
-    <t>@PepponeB91</t>
-  </si>
-  <si>
     <t>@crezyred</t>
   </si>
   <si>
@@ -620,9 +536,6 @@
     <t>Frittu</t>
   </si>
   <si>
-    <t>IL DISTRUTTORE</t>
-  </si>
-  <si>
     <t>Just_Dodo</t>
   </si>
   <si>
@@ -647,9 +560,6 @@
     <t>Uchiha Madara</t>
   </si>
   <si>
-    <t>Zumpy</t>
-  </si>
-  <si>
     <t>@luca3689</t>
   </si>
   <si>
@@ -716,9 +626,6 @@
     <t>@Frittuuu</t>
   </si>
   <si>
-    <t>@gioee_e27</t>
-  </si>
-  <si>
     <t>@edoogrigo</t>
   </si>
   <si>
@@ -737,55 +644,58 @@
     <t>@Madara_2912</t>
   </si>
   <si>
-    <t>mrdeath75</t>
-  </si>
-  <si>
     <t>⭐️Marco⭐️</t>
   </si>
   <si>
-    <t>AR ♦️Goldenboy</t>
-  </si>
-  <si>
-    <t>@aless_io98</t>
-  </si>
-  <si>
-    <t>Gervasio</t>
-  </si>
-  <si>
     <t>teo</t>
   </si>
   <si>
-    <t>DADDA</t>
-  </si>
-  <si>
-    <t>@Melqiades</t>
-  </si>
-  <si>
-    <t>@X_teo</t>
-  </si>
-  <si>
-    <t>@FabioZumpy77</t>
-  </si>
-  <si>
-    <t>@danielylo</t>
-  </si>
-  <si>
     <t>arKaiba❤️Sparky</t>
   </si>
   <si>
-    <t>the terminator</t>
-  </si>
-  <si>
-    <t>Thor⚡️</t>
-  </si>
-  <si>
     <t>@sorridetemi</t>
   </si>
   <si>
     <t>Warlosing</t>
   </si>
   <si>
-    <t>Ce Magnamm</t>
+    <t>AR♠️MrDEATH</t>
+  </si>
+  <si>
+    <t>MrBabrik</t>
+  </si>
+  <si>
+    <t>@BrikBa</t>
+  </si>
+  <si>
+    <t>ＡＲ♣️ＳＴＡＲ</t>
+  </si>
+  <si>
+    <t>CcH LATINO™️</t>
+  </si>
+  <si>
+    <t>Kairos</t>
+  </si>
+  <si>
+    <t>nevio lostirato</t>
+  </si>
+  <si>
+    <t>prince</t>
+  </si>
+  <si>
+    <t>davide</t>
+  </si>
+  <si>
+    <t>@kvaradona997</t>
+  </si>
+  <si>
+    <t>@gambo84</t>
+  </si>
+  <si>
+    <t>@Balliver</t>
+  </si>
+  <si>
+    <t>@CR0LP0C</t>
   </si>
 </sst>
 </file>
@@ -1750,17 +1660,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EE2B0F9-AC31-464B-B046-53CB033C8615}">
-  <dimension ref="A1:D126"/>
+  <dimension ref="A1:D109"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A76" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B72" sqref="B72"/>
+    <sheetView tabSelected="1" topLeftCell="AM1" zoomScale="124" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A91" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="19.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.88671875" style="1"/>
@@ -1786,716 +1696,716 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>138</v>
+        <v>124</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>136</v>
+        <v>119</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>7</v>
+        <v>121</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>128</v>
+        <v>91</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>163</v>
+        <v>111</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>129</v>
+        <v>208</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>161</v>
+        <v>113</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>126</v>
+        <v>83</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>144</v>
+        <v>130</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>157</v>
+        <v>125</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>122</v>
+        <v>95</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>162</v>
+        <v>133</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>127</v>
+        <v>104</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>141</v>
+        <v>191</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>105</v>
+        <v>161</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>155</v>
+        <v>127</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>120</v>
+        <v>97</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>139</v>
+        <v>45</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>103</v>
+        <v>6</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>165</v>
+        <v>137</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>131</v>
+        <v>109</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>156</v>
+        <v>135</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>121</v>
+        <v>106</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>140</v>
+        <v>33</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>104</v>
+        <v>144</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>151</v>
+        <v>7</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>143</v>
+        <v>115</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>107</v>
+        <v>85</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>147</v>
+        <v>206</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>111</v>
+        <v>205</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>146</v>
+        <v>51</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>110</v>
+        <v>52</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>158</v>
+        <v>10</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>123</v>
+        <v>9</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>154</v>
+        <v>192</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>118</v>
+        <v>162</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>159</v>
+        <v>134</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>124</v>
+        <v>105</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>150</v>
+        <v>120</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>114</v>
+        <v>90</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>135</v>
+        <v>117</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>234</v>
+        <v>87</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>145</v>
+        <v>44</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>109</v>
+        <v>47</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>134</v>
+        <v>74</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>132</v>
+        <v>73</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>24</v>
+        <v>126</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>23</v>
+        <v>96</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>63</v>
+        <v>112</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>62</v>
+        <v>82</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>44</v>
+        <v>21</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>42</v>
+        <v>20</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>209</v>
+        <v>53</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>177</v>
+        <v>54</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>29</v>
+        <v>46</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>33</v>
+        <v>118</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>18</v>
+        <v>122</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>17</v>
+        <v>92</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
-        <v>45</v>
+        <v>131</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>48</v>
+        <v>102</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>19</v>
+        <v>179</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>235</v>
+        <v>149</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
-        <v>228</v>
+        <v>142</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>196</v>
+        <v>139</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
-        <v>208</v>
+        <v>140</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>176</v>
+        <v>138</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
-        <v>152</v>
+        <v>39</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>116</v>
+        <v>13</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
-        <v>38</v>
+        <v>116</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>35</v>
+        <v>86</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
-        <v>43</v>
+        <v>199</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>8</v>
+        <v>169</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
-        <v>206</v>
+        <v>110</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>174</v>
+        <v>99</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
-        <v>226</v>
+        <v>24</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>194</v>
+        <v>23</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
-        <v>237</v>
+        <v>114</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>236</v>
+        <v>84</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
-        <v>213</v>
+        <v>12</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>181</v>
+        <v>11</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
-        <v>210</v>
+        <v>123</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>178</v>
+        <v>93</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
-        <v>12</v>
+        <v>128</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>11</v>
+        <v>98</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
-        <v>212</v>
+        <v>19</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>180</v>
+        <v>203</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
-        <v>68</v>
+        <v>210</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>66</v>
+        <v>209</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>250</v>
+        <v>3</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
-        <v>5</v>
+        <v>182</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>4</v>
+        <v>152</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>250</v>
+        <v>207</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
@@ -2506,1029 +2416,794 @@
         <v>31</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>250</v>
+        <v>207</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
-        <v>95</v>
+        <v>63</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>97</v>
+        <v>61</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>250</v>
+        <v>207</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
-        <v>218</v>
+        <v>5</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>186</v>
+        <v>4</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>250</v>
+        <v>207</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
-        <v>78</v>
+        <v>190</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>80</v>
+        <v>160</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>250</v>
+        <v>207</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
-        <v>233</v>
+        <v>37</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>203</v>
+        <v>34</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>250</v>
+        <v>207</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
-        <v>219</v>
+        <v>49</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>187</v>
+        <v>211</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>250</v>
+        <v>207</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
-        <v>94</v>
+        <v>186</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>96</v>
+        <v>156</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>250</v>
+        <v>207</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
-        <v>40</v>
+        <v>141</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>89</v>
+        <v>72</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>250</v>
+        <v>207</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
-        <v>26</v>
+        <v>80</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>25</v>
+        <v>81</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>250</v>
+        <v>207</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
-        <v>170</v>
+        <v>70</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>167</v>
+        <v>71</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>250</v>
+        <v>207</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
-        <v>207</v>
+        <v>193</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>175</v>
+        <v>163</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>250</v>
+        <v>207</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
-        <v>205</v>
+        <v>131</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>173</v>
+        <v>212</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>250</v>
+        <v>207</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
-        <v>241</v>
+        <v>185</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>238</v>
+        <v>155</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>250</v>
+        <v>207</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
-        <v>215</v>
+        <v>16</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>183</v>
+        <v>32</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>250</v>
+        <v>207</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
-        <v>169</v>
+        <v>40</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>81</v>
+        <v>22</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>250</v>
+        <v>207</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>250</v>
+        <v>207</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
-        <v>222</v>
+        <v>67</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>190</v>
+        <v>65</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>250</v>
+        <v>207</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
-        <v>224</v>
+        <v>194</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>192</v>
+        <v>164</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>250</v>
+        <v>207</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
-        <v>69</v>
+        <v>183</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>67</v>
+        <v>153</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>250</v>
+        <v>207</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
-        <v>29</v>
+        <v>195</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>61</v>
+        <v>165</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>250</v>
+        <v>207</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>64</v>
+        <v>36</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>250</v>
+        <v>207</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
-        <v>10</v>
+        <v>38</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>250</v>
+        <v>207</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
-        <v>51</v>
+        <v>196</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>36</v>
+        <v>166</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>250</v>
+        <v>207</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
-        <v>216</v>
+        <v>58</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>184</v>
+        <v>57</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>250</v>
+        <v>207</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>58</v>
+        <v>41</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>250</v>
+        <v>207</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
-        <v>242</v>
+        <v>197</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>239</v>
+        <v>167</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>250</v>
+        <v>207</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
-        <v>171</v>
+        <v>76</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>201</v>
+        <v>213</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>250</v>
+        <v>207</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
-        <v>227</v>
+        <v>177</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>195</v>
+        <v>147</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>250</v>
+        <v>207</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
-        <v>60</v>
+        <v>187</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>59</v>
+        <v>157</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>250</v>
+        <v>207</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
-        <v>214</v>
+        <v>18</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>182</v>
+        <v>17</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>250</v>
+        <v>207</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
-        <v>16</v>
+        <v>175</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>32</v>
+        <v>145</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>250</v>
+        <v>207</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
-        <v>211</v>
+        <v>68</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>179</v>
+        <v>66</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>250</v>
+        <v>207</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
-        <v>220</v>
+        <v>178</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>188</v>
+        <v>148</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>250</v>
+        <v>207</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
-        <v>50</v>
+        <v>217</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>53</v>
+        <v>214</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>250</v>
+        <v>207</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
-        <v>86</v>
+        <v>184</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>91</v>
+        <v>154</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>250</v>
+        <v>207</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="s">
-        <v>83</v>
+        <v>189</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>82</v>
+        <v>159</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>250</v>
+        <v>207</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
-        <v>225</v>
+        <v>55</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>193</v>
+        <v>56</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>250</v>
+        <v>207</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
-        <v>230</v>
+        <v>218</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>198</v>
+        <v>215</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>250</v>
+        <v>207</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
-        <v>41</v>
+        <v>176</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>22</v>
+        <v>146</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>250</v>
+        <v>207</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="s">
-        <v>73</v>
+        <v>42</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>71</v>
+        <v>8</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>250</v>
+        <v>207</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
-        <v>37</v>
+        <v>198</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>34</v>
+        <v>168</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>250</v>
+        <v>207</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>250</v>
+        <v>207</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="s">
-        <v>72</v>
+        <v>200</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>70</v>
+        <v>170</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>250</v>
+        <v>207</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="s">
-        <v>243</v>
+        <v>180</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>204</v>
+        <v>150</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>250</v>
+        <v>207</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97" s="1" t="s">
-        <v>244</v>
+        <v>26</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>240</v>
+        <v>25</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>250</v>
+        <v>207</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="s">
-        <v>87</v>
+        <v>181</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>92</v>
+        <v>151</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>250</v>
+        <v>207</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
-        <v>223</v>
+        <v>15</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>191</v>
+        <v>14</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>250</v>
+        <v>207</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="s">
-        <v>15</v>
+        <v>219</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>14</v>
+        <v>204</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>250</v>
+        <v>207</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>249</v>
+        <v>207</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102" s="1" t="s">
-        <v>168</v>
+        <v>143</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>249</v>
+        <v>207</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103" s="1" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>249</v>
+        <v>207</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>249</v>
+        <v>207</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105" s="1" t="s">
-        <v>21</v>
+        <v>201</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>20</v>
+        <v>173</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>249</v>
+        <v>207</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106" s="1" t="s">
-        <v>221</v>
+        <v>202</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>189</v>
+        <v>174</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>249</v>
+        <v>207</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107" s="1" t="s">
-        <v>248</v>
+        <v>188</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>245</v>
+        <v>158</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>249</v>
+        <v>207</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A108" s="1" t="s">
+        <v>77</v>
+      </c>
       <c r="B108" s="1" t="s">
-        <v>246</v>
+        <v>79</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>249</v>
+        <v>207</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A109" s="1" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>197</v>
+        <v>216</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>249</v>
+        <v>207</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A110" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="B110" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="C110" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="D110" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A111" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="B111" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C111" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="D111" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A112" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B112" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="C112" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="D112" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A113" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="B113" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="C113" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="D113" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A114" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="B114" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="C114" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="D114" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A115" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="B115" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="C115" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="D115" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A116" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="B116" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="C116" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="D116" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A117" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="B117" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="C117" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="D117" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A118" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B118" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C118" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="D118" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A119" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="B119" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="C119" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="D119" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A120" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="B120" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="C120" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="D120" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A121" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="B121" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="C121" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="D121" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A122" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B122" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C122" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="D122" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A123" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B123" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C123" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="D123" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A124" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="B124" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="C124" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="D124" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A125" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="B125" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="C125" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="D125" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A126" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B126" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="C126" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="D126" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>